<commit_message>
ISA spec update, registers structures defined
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar\Documents\Work\AI\CPU\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E510B45C-49DA-42AD-9562-ECA154B46D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500E006F-DE1F-4DE6-98DB-A5E0E229F33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19118" yWindow="10440" windowWidth="19365" windowHeight="10523" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
+    <workbookView xWindow="-83" yWindow="10440" windowWidth="19366" windowHeight="10523" activeTab="1" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
-    <sheet name="Instructions" sheetId="1" r:id="rId2"/>
+    <sheet name="Foglio2" sheetId="3" r:id="rId2"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="235">
   <si>
     <t>POP</t>
   </si>
@@ -424,6 +425,324 @@
   </si>
   <si>
     <t>R252</t>
+  </si>
+  <si>
+    <t>SRC</t>
+  </si>
+  <si>
+    <t>DST</t>
+  </si>
+  <si>
+    <t>VL</t>
+  </si>
+  <si>
+    <t>ADT</t>
+  </si>
+  <si>
+    <t>ST_RS</t>
+  </si>
+  <si>
+    <t>ST_DST</t>
+  </si>
+  <si>
+    <t>ST_SRC</t>
+  </si>
+  <si>
+    <t>BCS</t>
+  </si>
+  <si>
+    <t>ST_JMP</t>
+  </si>
+  <si>
+    <t>where</t>
+  </si>
+  <si>
+    <t>u8</t>
+  </si>
+  <si>
+    <t>register index for LI, or first ARG of ALU operation</t>
+  </si>
+  <si>
+    <t>second ARG for ALU operation</t>
+  </si>
+  <si>
+    <t>destination register for ALU operation</t>
+  </si>
+  <si>
+    <t>Nibble Selector, current index of nibble for LI instruction</t>
+  </si>
+  <si>
+    <t>should be resetted to zero on each RS change</t>
+  </si>
+  <si>
+    <t>u16</t>
+  </si>
+  <si>
+    <t>ALU Data Type, see table below</t>
+  </si>
+  <si>
+    <t>Vector Length, in ADT units</t>
+  </si>
+  <si>
+    <t>Stride of RS register</t>
+  </si>
+  <si>
+    <t>Stride of DST register</t>
+  </si>
+  <si>
+    <t>Stride of SRC register</t>
+  </si>
+  <si>
+    <t>u24</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Operand Type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>8-bit unsigned integer</t>
+  </si>
+  <si>
+    <t>i8</t>
+  </si>
+  <si>
+    <t>8-bit signed integer</t>
+  </si>
+  <si>
+    <t>0x2</t>
+  </si>
+  <si>
+    <t>16-bit unsigned integer</t>
+  </si>
+  <si>
+    <t>i16</t>
+  </si>
+  <si>
+    <t>16-bit signed integer</t>
+  </si>
+  <si>
+    <t>u32</t>
+  </si>
+  <si>
+    <t>32-bit unsigned integer</t>
+  </si>
+  <si>
+    <t>0x5</t>
+  </si>
+  <si>
+    <t>i32</t>
+  </si>
+  <si>
+    <t>32-bit signed integer</t>
+  </si>
+  <si>
+    <t>u64</t>
+  </si>
+  <si>
+    <t>64-bit unsigned integer</t>
+  </si>
+  <si>
+    <t>f16</t>
+  </si>
+  <si>
+    <t>16-bit floating-point (half-precision)</t>
+  </si>
+  <si>
+    <t>f32</t>
+  </si>
+  <si>
+    <t>32-bit floating-point (single-precision)</t>
+  </si>
+  <si>
+    <t>f64</t>
+  </si>
+  <si>
+    <t>64-bit floating-point (double-precision)</t>
+  </si>
+  <si>
+    <t>i64</t>
+  </si>
+  <si>
+    <t>64-bit signed integer</t>
+  </si>
+  <si>
+    <t>0xB</t>
+  </si>
+  <si>
+    <t>fp4</t>
+  </si>
+  <si>
+    <t>4-bit floating-point</t>
+  </si>
+  <si>
+    <t>fp8</t>
+  </si>
+  <si>
+    <t>8-bit floating-point</t>
+  </si>
+  <si>
+    <t>u1</t>
+  </si>
+  <si>
+    <t>1-bit boolean type</t>
+  </si>
+  <si>
+    <t>i4</t>
+  </si>
+  <si>
+    <t>4-bit int type</t>
+  </si>
+  <si>
+    <t>reserved</t>
+  </si>
+  <si>
+    <t>ALU Data Type definitions</t>
+  </si>
+  <si>
+    <t>Branch Condition Selector</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Always</t>
+  </si>
+  <si>
+    <t>Zero (Z)</t>
+  </si>
+  <si>
+    <t>Not_Zero (NZ)</t>
+  </si>
+  <si>
+    <t>Greater (G)</t>
+  </si>
+  <si>
+    <t>Greater_Or_Equal (GE)</t>
+  </si>
+  <si>
+    <t>Less (L)</t>
+  </si>
+  <si>
+    <t>Less_Or_Equal (LE)</t>
+  </si>
+  <si>
+    <t>Carry (C)</t>
+  </si>
+  <si>
+    <t>Not_Carry (NC)</t>
+  </si>
+  <si>
+    <t>Sign (S)</t>
+  </si>
+  <si>
+    <t>Not_Sign (NS)</t>
+  </si>
+  <si>
+    <t>Overflow (O)</t>
+  </si>
+  <si>
+    <t>Not_Overflow (NO)</t>
+  </si>
+  <si>
+    <t>Parity_Even (PE)</t>
+  </si>
+  <si>
+    <t>Parity_Odd (PO)</t>
+  </si>
+  <si>
+    <t>Interrupt (I)</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>Addition</t>
+  </si>
+  <si>
+    <t>SUB</t>
+  </si>
+  <si>
+    <t>Subtraction</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>Bitwise AND</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>Bitwise OR</t>
+  </si>
+  <si>
+    <t>XOR</t>
+  </si>
+  <si>
+    <t>Bitwise Exclusive OR</t>
+  </si>
+  <si>
+    <t>SHL</t>
+  </si>
+  <si>
+    <t>Shift Left</t>
+  </si>
+  <si>
+    <t>SHR</t>
+  </si>
+  <si>
+    <t>Shift Right Logical</t>
+  </si>
+  <si>
+    <t>MUL</t>
+  </si>
+  <si>
+    <t>Multiplication</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>LOOKUP</t>
+  </si>
+  <si>
+    <t>Lookup slice in vector</t>
+  </si>
+  <si>
+    <t>LOAD</t>
+  </si>
+  <si>
+    <t>Loads nimble, byte or word</t>
+  </si>
+  <si>
+    <t>STORE</t>
+  </si>
+  <si>
+    <t>Saves nimble, byte or word</t>
+  </si>
+  <si>
+    <t>0xC-0xF</t>
+  </si>
+  <si>
+    <t>Reserved</t>
+  </si>
+  <si>
+    <t>ALU Operation Mode Selector</t>
+  </si>
+  <si>
+    <t>AMOD</t>
   </si>
 </sst>
 </file>
@@ -455,7 +774,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -763,11 +1082,156 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -938,6 +1402,28 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1272,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CDEC23-057C-4C1E-AB18-5AC9130DB945}">
-  <dimension ref="B3:G24"/>
+  <dimension ref="B3:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1284,15 +1770,17 @@
     <col min="4" max="4" width="4.9296875" customWidth="1"/>
     <col min="5" max="5" width="2.265625" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.19921875" customWidth="1"/>
+    <col min="7" max="8" width="16.19921875" customWidth="1"/>
+    <col min="10" max="10" width="14.265625" customWidth="1"/>
+    <col min="11" max="18" width="4.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="67" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.45">
       <c r="C4" s="67" t="s">
         <v>104</v>
       </c>
@@ -1302,8 +1790,27 @@
       <c r="F4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="J4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="29">
+        <v>0</v>
+      </c>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25">
+        <v>1</v>
+      </c>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25">
+        <v>2</v>
+      </c>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25">
+        <v>3</v>
+      </c>
+      <c r="R4" s="25"/>
+    </row>
+    <row r="5" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C5" s="67" t="s">
         <v>105</v>
       </c>
@@ -1313,13 +1820,59 @@
       <c r="F5" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="J5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5" s="5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="5">
+        <v>2</v>
+      </c>
+      <c r="N5" s="16">
+        <v>3</v>
+      </c>
+      <c r="O5" s="4">
+        <v>4</v>
+      </c>
+      <c r="P5" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>6</v>
+      </c>
+      <c r="R5" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B8" s="67" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="J8" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" s="22"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
         <v>109</v>
       </c>
@@ -1327,38 +1880,85 @@
         <v>111</v>
       </c>
       <c r="G9" s="31"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="H9" s="68"/>
+      <c r="J9" s="69" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>110</v>
       </c>
       <c r="F10" s="31"/>
       <c r="G10" s="31"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="H10" s="68"/>
+      <c r="K10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" t="s">
+        <v>139</v>
+      </c>
+      <c r="N10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>120</v>
       </c>
       <c r="F11" s="31"/>
       <c r="G11" s="31"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="H11" s="68"/>
+      <c r="K11" t="s">
+        <v>129</v>
+      </c>
+      <c r="L11" t="s">
+        <v>139</v>
+      </c>
+      <c r="N11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="K12" t="s">
+        <v>130</v>
+      </c>
+      <c r="L12" t="s">
+        <v>139</v>
+      </c>
+      <c r="N12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>119</v>
       </c>
       <c r="F13" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="K13" t="s">
+        <v>31</v>
+      </c>
+      <c r="L13" t="s">
+        <v>139</v>
+      </c>
+      <c r="N13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>118</v>
       </c>
       <c r="F14" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="O14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
         <v>117</v>
       </c>
@@ -1366,15 +1966,37 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>116</v>
       </c>
       <c r="F16" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="J16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="K16" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.45">
+      <c r="J17" s="69" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
         <v>121</v>
       </c>
@@ -1382,60 +2004,725 @@
         <v>111</v>
       </c>
       <c r="G18" s="31"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="H18" s="68"/>
+      <c r="K18" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="L18" s="54"/>
+      <c r="M18" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="N18" s="37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>110</v>
       </c>
       <c r="F19" s="31"/>
       <c r="G19" s="31"/>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="H19" s="68"/>
+      <c r="K19" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="L19" s="54"/>
+      <c r="M19" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="N19" s="37" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>128</v>
       </c>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-    </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="H20" s="68"/>
+      <c r="K20" s="54" t="s">
+        <v>134</v>
+      </c>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="N20" s="54" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>127</v>
       </c>
       <c r="F22" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="J22" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="K22" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
         <v>126</v>
       </c>
       <c r="F23" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.45">
+      <c r="J23" s="69" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="3:18" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
         <v>125</v>
       </c>
       <c r="F24" t="s">
         <v>124</v>
       </c>
+      <c r="K24" t="s">
+        <v>133</v>
+      </c>
+      <c r="M24" t="s">
+        <v>145</v>
+      </c>
+      <c r="N24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="3:18" x14ac:dyDescent="0.45">
+      <c r="K25" t="s">
+        <v>135</v>
+      </c>
+      <c r="M25" t="s">
+        <v>145</v>
+      </c>
+      <c r="N25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="3:18" x14ac:dyDescent="0.45">
+      <c r="J28" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="K28" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.45">
+      <c r="J29" s="69" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="3:18" x14ac:dyDescent="0.45">
+      <c r="K30" t="s">
+        <v>136</v>
+      </c>
+      <c r="M30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="3:18" x14ac:dyDescent="0.45">
+      <c r="K31" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="L31" s="54"/>
+      <c r="M31" s="54" t="s">
+        <v>151</v>
+      </c>
+      <c r="N31" s="54"/>
+      <c r="O31" s="54"/>
+      <c r="P31" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="17">
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="O16:R16"/>
     <mergeCell ref="F9:G11"/>
     <mergeCell ref="F18:G20"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:R28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A222D11D-FBDB-42C8-93C4-B5D16645D996}">
+  <dimension ref="A3:D58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="67"/>
+    </row>
+    <row r="5" spans="1:4" s="67" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="81" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="82" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="84" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B6" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="80" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B7" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="74" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="75" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D9" s="75" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="75" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B11" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="75" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B12" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="75" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B13" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D13" s="75" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B15" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15" s="75" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B16" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="75" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B17" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="75" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B18" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="75" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B19" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D19" s="75" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B20" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D20" s="75" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="D21" s="77"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="25" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B25" s="81" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" s="82" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" s="83"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B26" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="79" t="s">
+        <v>190</v>
+      </c>
+      <c r="D26" s="80"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B27" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D27" s="75"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B28" s="74" t="s">
+        <v>158</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" s="75"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B29" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" s="75"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B30" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" s="75"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B31" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D31" s="75"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B32" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="75"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B33" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" s="75"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B34" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D34" s="75"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B35" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D35" s="75"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B36" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D36" s="75"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B37" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D37" s="75"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B38" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D38" s="75"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B39" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="D39" s="75"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B40" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D40" s="75"/>
+    </row>
+    <row r="41" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B41" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="76" t="s">
+        <v>205</v>
+      </c>
+      <c r="D41" s="77"/>
+    </row>
+    <row r="44" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A44" s="67" t="s">
+        <v>234</v>
+      </c>
+      <c r="B44" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="67" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B45" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="C45" s="71" t="s">
+        <v>206</v>
+      </c>
+      <c r="D45" s="72" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B46" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="85" t="s">
+        <v>207</v>
+      </c>
+      <c r="D46" s="73" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B47" s="74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D47" s="75" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B48" s="74" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D48" s="75" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B49" s="74" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D49" s="75" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B50" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D50" s="75" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B51" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D51" s="75" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B52" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D52" s="75" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B53" s="74" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D53" s="75" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B54" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D54" s="75" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B55" s="74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D55" s="75" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B56" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="D56" s="75" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B57" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="D57" s="75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B58" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C58" s="76" t="s">
+        <v>232</v>
+      </c>
+      <c r="D58" s="77"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43404EB-A4C0-4EEB-BCD6-93EC84295AA2}">
   <dimension ref="A4:AD80"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="U79" sqref="U79"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
vm.zig set to 32 bit
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar\Documents\Work\AI\CPU\vcda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aroma\Desktop\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9C0392-CB56-4531-9B3D-C2CC54F199FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FA8F48-84F3-44A6-B9DB-2D3018C6A2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="10440" windowWidth="19366" windowHeight="10523" activeTab="1" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
@@ -1345,7 +1345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1390,142 +1390,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1544,7 +1423,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1553,22 +1454,102 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1905,28 +1886,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CDEC23-057C-4C1E-AB18-5AC9130DB945}">
   <dimension ref="B3:R31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="6.06640625" customWidth="1"/>
-    <col min="4" max="4" width="4.9296875" customWidth="1"/>
-    <col min="5" max="5" width="2.265625" customWidth="1"/>
+    <col min="3" max="3" width="6.109375" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" customWidth="1"/>
+    <col min="5" max="5" width="2.21875" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="8" width="16.19921875" customWidth="1"/>
-    <col min="10" max="10" width="14.265625" customWidth="1"/>
-    <col min="11" max="18" width="4.59765625" customWidth="1"/>
+    <col min="7" max="8" width="16.21875" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" customWidth="1"/>
+    <col min="11" max="18" width="4.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="68" t="s">
+    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="27" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="C4" s="68" t="s">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C4" s="27" t="s">
         <v>103</v>
       </c>
       <c r="D4">
@@ -1938,25 +1919,25 @@
       <c r="J4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4" s="55">
         <v>0</v>
       </c>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25">
+      <c r="L4" s="52"/>
+      <c r="M4" s="52">
         <v>1</v>
       </c>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25">
+      <c r="N4" s="52"/>
+      <c r="O4" s="52">
         <v>2</v>
       </c>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25">
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52">
         <v>3</v>
       </c>
-      <c r="R4" s="25"/>
-    </row>
-    <row r="5" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C5" s="68" t="s">
+      <c r="R4" s="52"/>
+    </row>
+    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="27" t="s">
         <v>104</v>
       </c>
       <c r="D5">
@@ -1993,50 +1974,50 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B8" s="68" t="s">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="27" t="s">
         <v>107</v>
       </c>
       <c r="J8" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22" t="s">
+      <c r="L8" s="53"/>
+      <c r="M8" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22" t="s">
+      <c r="N8" s="53"/>
+      <c r="O8" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22" t="s">
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="R8" s="22"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="R8" s="53"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="69"/>
-      <c r="J9" s="70" t="s">
+      <c r="G9" s="54"/>
+      <c r="H9" s="8"/>
+      <c r="J9" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>109</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="69"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="54"/>
+      <c r="H10" s="8"/>
       <c r="K10" t="s">
         <v>30</v>
       </c>
@@ -2047,13 +2028,13 @@
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>119</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="69"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="8"/>
       <c r="K11" t="s">
         <v>128</v>
       </c>
@@ -2064,7 +2045,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="K12" t="s">
         <v>129</v>
       </c>
@@ -2075,7 +2056,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>118</v>
       </c>
@@ -2092,7 +2073,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>117</v>
       </c>
@@ -2103,7 +2084,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>116</v>
       </c>
@@ -2111,7 +2092,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>115</v>
       </c>
@@ -2121,83 +2102,80 @@
       <c r="J16" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K16" s="53" t="s">
         <v>131</v>
       </c>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22" t="s">
+      <c r="L16" s="53"/>
+      <c r="M16" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22" t="s">
+      <c r="N16" s="53"/>
+      <c r="O16" s="53" t="s">
         <v>133</v>
       </c>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="J17" s="70" t="s">
+      <c r="P16" s="53"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="53"/>
+    </row>
+    <row r="17" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="J17" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="69"/>
-      <c r="K18" s="54" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="8"/>
+      <c r="K18" t="s">
         <v>131</v>
       </c>
-      <c r="L18" s="54"/>
-      <c r="M18" s="37" t="s">
+      <c r="M18" t="s">
         <v>138</v>
       </c>
-      <c r="N18" s="37" t="s">
+      <c r="N18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>109</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="69"/>
-      <c r="K19" s="54" t="s">
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="8"/>
+      <c r="K19" t="s">
         <v>130</v>
       </c>
-      <c r="L19" s="54"/>
-      <c r="M19" s="37" t="s">
+      <c r="M19" t="s">
         <v>138</v>
       </c>
-      <c r="N19" s="37" t="s">
+      <c r="N19" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>127</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="69"/>
-      <c r="K20" s="54" t="s">
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="8"/>
+      <c r="K20" t="s">
         <v>133</v>
       </c>
-      <c r="L20" s="54"/>
-      <c r="M20" s="54" t="s">
+      <c r="M20" t="s">
         <v>144</v>
       </c>
-      <c r="N20" s="54" t="s">
+      <c r="N20" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>126</v>
       </c>
@@ -2207,31 +2185,31 @@
       <c r="J22" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="K22" s="22" t="s">
+      <c r="K22" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22" t="s">
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.45">
+      <c r="P22" s="53"/>
+      <c r="Q22" s="53"/>
+      <c r="R22" s="53"/>
+    </row>
+    <row r="23" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>125</v>
       </c>
       <c r="F23" t="s">
         <v>122</v>
       </c>
-      <c r="J23" s="70" t="s">
+      <c r="J23" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>124</v>
       </c>
@@ -2248,7 +2226,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.3">
       <c r="K25" t="s">
         <v>134</v>
       </c>
@@ -2259,29 +2237,29 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:18" x14ac:dyDescent="0.3">
       <c r="J28" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="K28" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22" t="s">
+      <c r="L28" s="53"/>
+      <c r="M28" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="22"/>
-    </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="J29" s="70" t="s">
+      <c r="N28" s="53"/>
+      <c r="O28" s="53"/>
+      <c r="P28" s="53"/>
+      <c r="Q28" s="53"/>
+      <c r="R28" s="53"/>
+    </row>
+    <row r="29" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="J29" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:18" x14ac:dyDescent="0.3">
       <c r="K30" t="s">
         <v>135</v>
       </c>
@@ -2289,37 +2267,33 @@
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.45">
-      <c r="K31" s="54" t="s">
+    <row r="31" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="K31" t="s">
         <v>136</v>
       </c>
-      <c r="L31" s="54"/>
-      <c r="M31" s="54" t="s">
+      <c r="M31" t="s">
         <v>150</v>
       </c>
-      <c r="N31" s="54"/>
-      <c r="O31" s="54"/>
-      <c r="P31" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:R28"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="O16:R16"/>
+    <mergeCell ref="F9:G11"/>
+    <mergeCell ref="F18:G20"/>
     <mergeCell ref="Q4:R4"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="M8:N8"/>
     <mergeCell ref="O8:P8"/>
     <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="O16:R16"/>
-    <mergeCell ref="F9:G11"/>
-    <mergeCell ref="F18:G20"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:P4"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="O22:R22"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:R28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2329,581 +2303,582 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A222D11D-FBDB-42C8-93C4-B5D16645D996}">
   <dimension ref="A3:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31.796875" customWidth="1"/>
+    <col min="4" max="4" width="34.88671875" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="68" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
         <v>131</v>
       </c>
       <c r="B3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="68"/>
-    </row>
-    <row r="5" spans="1:8" s="68" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="83" t="s">
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="27"/>
+    </row>
+    <row r="5" spans="1:4" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="43" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B6" s="80" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="37" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="34" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B7" s="76" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D7" s="77" t="s">
+      <c r="D7" s="34" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B8" s="76" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="33" t="s">
         <v>157</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="34" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B9" s="76" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="82" t="s">
+      <c r="D9" s="39" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B10" s="76" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="33" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="34" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B11" s="76" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" s="33" t="s">
         <v>163</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="77" t="s">
+      <c r="D11" s="34" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B12" s="76" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="77" t="s">
+      <c r="D12" s="34" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B13" s="76" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="D13" s="77" t="s">
+      <c r="D13" s="34" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B14" s="76" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="33" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="D14" s="77" t="s">
+      <c r="D14" s="34" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B15" s="76" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="D15" s="77" t="s">
+      <c r="D15" s="34" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B16" s="76" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="33" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D16" s="77" t="s">
+      <c r="D16" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B17" s="76" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="33" t="s">
         <v>176</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D17" s="77" t="s">
+      <c r="D17" s="34" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B18" s="76" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="33" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D18" s="77" t="s">
+      <c r="D18" s="34" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B19" s="76" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="33" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D19" s="77" t="s">
+      <c r="D19" s="34" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B20" s="76" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="77" t="s">
+      <c r="D20" s="34" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="78" t="s">
+      <c r="C21" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="D21" s="79" t="s">
+      <c r="D21" s="36" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" s="68" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
         <v>135</v>
       </c>
       <c r="B23" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="25" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B25" s="83" t="s">
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="C25" s="84" t="s">
+      <c r="C25" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="D25" s="85"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B26" s="80" t="s">
+      <c r="D25" s="42"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="81" t="s">
+      <c r="C26" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="D26" s="82"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B27" s="76" t="s">
+      <c r="D26" s="39"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="33" t="s">
         <v>19</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="D27" s="77"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B28" s="76" t="s">
+      <c r="D27" s="34"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="33" t="s">
         <v>157</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="D28" s="77"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B29" s="76" t="s">
+      <c r="D28" s="34"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="33" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="D29" s="77"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B30" s="76" t="s">
+      <c r="D29" s="34"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="33" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="D30" s="77"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B31" s="76" t="s">
+      <c r="D30" s="34"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="33" t="s">
         <v>163</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="D31" s="77"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B32" s="76" t="s">
+      <c r="D31" s="34"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="D32" s="77"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B33" s="76" t="s">
+      <c r="D32" s="34"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="D33" s="77"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B34" s="76" t="s">
+      <c r="D33" s="34"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="33" t="s">
         <v>39</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="D34" s="77"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B35" s="76" t="s">
+      <c r="D34" s="34"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="D35" s="77"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B36" s="76" t="s">
+      <c r="D35" s="34"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="33" t="s">
         <v>48</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="D36" s="77"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B37" s="76" t="s">
+      <c r="D36" s="34"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="33" t="s">
         <v>176</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="D37" s="77"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B38" s="76" t="s">
+      <c r="D37" s="34"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="33" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="D38" s="77"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B39" s="76" t="s">
+      <c r="D38" s="34"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="33" t="s">
         <v>14</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D39" s="77"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B40" s="76" t="s">
+      <c r="D39" s="34"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="D40" s="77"/>
-    </row>
-    <row r="41" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D40" s="34"/>
+    </row>
+    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="78" t="s">
+      <c r="C41" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="D41" s="79"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A44" s="68" t="s">
+      <c r="D41" s="36"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="27" t="s">
         <v>232</v>
       </c>
       <c r="B44" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="68"/>
-    </row>
-    <row r="46" spans="1:4" s="68" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B46" s="72" t="s">
+    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="27"/>
+    </row>
+    <row r="46" spans="1:4" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="C46" s="73" t="s">
+      <c r="C46" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="D46" s="74" t="s">
+      <c r="D46" s="31" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="87" t="s">
+      <c r="C47" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="D47" s="75" t="s">
+      <c r="D47" s="32" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B48" s="76" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="33" t="s">
         <v>19</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="D48" s="77" t="s">
+      <c r="D48" s="34" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B49" s="76" t="s">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B49" s="33" t="s">
         <v>157</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="D49" s="77" t="s">
+      <c r="D49" s="34" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B50" s="76" t="s">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B50" s="33" t="s">
         <v>22</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="D50" s="77" t="s">
+      <c r="D50" s="34" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B51" s="76" t="s">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B51" s="33" t="s">
         <v>29</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="D51" s="77" t="s">
+      <c r="D51" s="34" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B52" s="76" t="s">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B52" s="33" t="s">
         <v>163</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="D52" s="77" t="s">
+      <c r="D52" s="34" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B53" s="76" t="s">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B53" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="D53" s="77" t="s">
+      <c r="D53" s="34" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B54" s="76" t="s">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B54" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="D54" s="77" t="s">
+      <c r="D54" s="34" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B55" s="76" t="s">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B55" s="33" t="s">
         <v>39</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="D55" s="77" t="s">
+      <c r="D55" s="34" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B56" s="76" t="s">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B56" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="D56" s="77" t="s">
+      <c r="D56" s="34" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B57" s="76" t="s">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B57" s="33" t="s">
         <v>48</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="D57" s="77" t="s">
+      <c r="D57" s="34" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="B58" s="76" t="s">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B58" s="33" t="s">
         <v>176</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="D58" s="77" t="s">
+      <c r="D58" s="34" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B59" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="C59" s="78" t="s">
+      <c r="C59" s="35" t="s">
         <v>230</v>
       </c>
-      <c r="D59" s="79"/>
-    </row>
-    <row r="61" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="68" t="s">
+      <c r="D59" s="36"/>
+    </row>
+    <row r="61" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="27" t="s">
         <v>233</v>
       </c>
       <c r="B61" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B62" s="88" t="s">
+    <row r="62" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="C62" s="89" t="s">
+      <c r="C62" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="D62" s="85" t="s">
+      <c r="D62" s="42" t="s">
         <v>153</v>
       </c>
       <c r="G62" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H62" s="25">
+      <c r="H62" s="52">
         <v>0</v>
       </c>
-      <c r="I62" s="25"/>
-      <c r="J62" s="25"/>
-      <c r="K62" s="91"/>
-      <c r="L62" s="92"/>
-      <c r="M62" s="60"/>
-      <c r="N62" s="60"/>
-      <c r="O62" s="60"/>
-    </row>
-    <row r="63" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B63" s="80" t="s">
+      <c r="I62" s="52"/>
+      <c r="J62" s="52"/>
+      <c r="K62" s="56"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="58"/>
+      <c r="N62" s="58"/>
+      <c r="O62" s="58"/>
+    </row>
+    <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C63" s="81" t="s">
+      <c r="C63" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="D63" s="82" t="s">
+      <c r="D63" s="39" t="s">
         <v>236</v>
       </c>
       <c r="G63" s="10" t="s">
@@ -2918,72 +2893,72 @@
       <c r="J63" s="5">
         <v>2</v>
       </c>
-      <c r="K63" s="93">
+      <c r="K63" s="48">
         <v>3</v>
       </c>
-      <c r="L63" s="94"/>
-      <c r="M63" s="90"/>
-      <c r="N63" s="90"/>
-      <c r="O63" s="90"/>
-    </row>
-    <row r="64" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L63" s="47"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+    </row>
+    <row r="64" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C64" s="78" t="s">
+      <c r="C64" s="35" t="s">
         <v>237</v>
       </c>
-      <c r="D64" s="79" t="s">
+      <c r="D64" s="36" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="66" spans="7:11" x14ac:dyDescent="0.45">
-      <c r="G66" s="68" t="s">
+    <row r="66" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G66" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="H66" s="71" t="s">
+      <c r="H66" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="I66" s="71" t="s">
+      <c r="I66" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="J66" s="22" t="s">
+      <c r="J66" s="53" t="s">
         <v>243</v>
       </c>
-      <c r="K66" s="22"/>
-    </row>
-    <row r="67" spans="7:11" x14ac:dyDescent="0.45">
-      <c r="G67" s="95" t="s">
+      <c r="K66" s="53"/>
+    </row>
+    <row r="67" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="G67" s="28" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="68" spans="7:11" x14ac:dyDescent="0.45">
-      <c r="H68" s="71" t="s">
+    <row r="68" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="H68" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="I68" s="96" t="s">
+      <c r="I68" s="49" t="s">
         <v>181</v>
       </c>
       <c r="J68" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="69" spans="7:11" x14ac:dyDescent="0.45">
-      <c r="H69" s="71" t="s">
+    <row r="69" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="H69" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="I69" s="96" t="s">
+      <c r="I69" s="49" t="s">
         <v>181</v>
       </c>
       <c r="J69" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="70" spans="7:11" x14ac:dyDescent="0.45">
-      <c r="H70" s="71" t="s">
+    <row r="70" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="H70" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="I70" s="97" t="s">
+      <c r="I70" s="50" t="s">
         <v>245</v>
       </c>
       <c r="J70" t="s">
@@ -3006,81 +2981,81 @@
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.19921875" customWidth="1"/>
-    <col min="4" max="6" width="4.796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.796875" style="15" customWidth="1"/>
-    <col min="8" max="10" width="4.796875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="4.796875" style="15" customWidth="1"/>
-    <col min="12" max="19" width="4.796875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="2.1328125" customWidth="1"/>
-    <col min="28" max="28" width="11.53125" customWidth="1"/>
-    <col min="29" max="29" width="10.53125" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" customWidth="1"/>
+    <col min="4" max="6" width="4.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.77734375" style="15" customWidth="1"/>
+    <col min="8" max="10" width="4.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="4.77734375" style="15" customWidth="1"/>
+    <col min="12" max="19" width="4.77734375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="2.109375" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" customWidth="1"/>
+    <col min="29" max="29" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="55">
         <v>0</v>
       </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25">
+      <c r="E7" s="52"/>
+      <c r="F7" s="52">
         <v>1</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25">
+      <c r="G7" s="52"/>
+      <c r="H7" s="52">
         <v>2</v>
       </c>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25">
+      <c r="I7" s="52"/>
+      <c r="J7" s="52">
         <v>3</v>
       </c>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25">
+      <c r="K7" s="52"/>
+      <c r="L7" s="52">
         <v>4</v>
       </c>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25">
+      <c r="M7" s="52"/>
+      <c r="N7" s="52">
         <v>5</v>
       </c>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25">
+      <c r="O7" s="52"/>
+      <c r="P7" s="52">
         <v>6</v>
       </c>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25">
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52">
         <v>7</v>
       </c>
-      <c r="S7" s="26"/>
-    </row>
-    <row r="8" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="S7" s="85"/>
+    </row>
+    <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="87"/>
       <c r="D8" s="4">
         <v>0</v>
       </c>
@@ -3130,15 +3105,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>94</v>
       </c>
@@ -3149,7 +3124,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>95</v>
       </c>
@@ -3160,7 +3135,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>96</v>
       </c>
@@ -3171,10 +3146,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -3187,17 +3162,17 @@
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="31" t="s">
+      <c r="U15" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
-      <c r="X15" s="31"/>
+      <c r="V15" s="54"/>
+      <c r="W15" s="54"/>
+      <c r="X15" s="54"/>
       <c r="AA15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="C16" s="7">
         <v>2</v>
       </c>
@@ -3213,15 +3188,15 @@
       <c r="G16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U16" s="31"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="31"/>
-      <c r="X16" s="31"/>
+      <c r="U16" s="54"/>
+      <c r="V16" s="54"/>
+      <c r="W16" s="54"/>
+      <c r="X16" s="54"/>
       <c r="AA16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C17" s="7">
         <v>4</v>
       </c>
@@ -3249,15 +3224,15 @@
       <c r="K17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="31"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="31"/>
+      <c r="U17" s="54"/>
+      <c r="V17" s="54"/>
+      <c r="W17" s="54"/>
+      <c r="X17" s="54"/>
       <c r="AA17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C18" s="7">
         <v>8</v>
       </c>
@@ -3309,17 +3284,17 @@
       <c r="S18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="31"/>
-    </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="U18" s="54"/>
+      <c r="V18" s="54"/>
+      <c r="W18" s="54"/>
+      <c r="X18" s="54"/>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -3332,14 +3307,14 @@
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U21" s="31" t="s">
+      <c r="U21" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="V21" s="31"/>
-      <c r="W21" s="31"/>
-      <c r="X21" s="31"/>
-    </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V21" s="54"/>
+      <c r="W21" s="54"/>
+      <c r="X21" s="54"/>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C22" s="7">
         <v>2</v>
       </c>
@@ -3355,26 +3330,26 @@
       <c r="G22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="31"/>
-    </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="I22" s="68"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="68"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="68"/>
+      <c r="P22" s="68"/>
+      <c r="Q22" s="68"/>
+      <c r="R22" s="68"/>
+      <c r="S22" s="68"/>
+      <c r="U22" s="54"/>
+      <c r="V22" s="54"/>
+      <c r="W22" s="54"/>
+      <c r="X22" s="54"/>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C23" s="7">
         <v>4</v>
       </c>
@@ -3387,19 +3362,19 @@
       <c r="F23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="21"/>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="31"/>
-      <c r="X23" s="31"/>
-    </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="H23" s="88"/>
+      <c r="I23" s="88"/>
+      <c r="J23" s="88"/>
+      <c r="K23" s="60"/>
+      <c r="U23" s="54"/>
+      <c r="V23" s="54"/>
+      <c r="W23" s="54"/>
+      <c r="X23" s="54"/>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C24" s="7">
         <v>8</v>
       </c>
@@ -3412,13 +3387,13 @@
       <c r="F24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="G24" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="21"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="60"/>
       <c r="L24" s="3" t="s">
         <v>16</v>
       </c>
@@ -3443,42 +3418,42 @@
       <c r="S24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U24" s="31"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="31"/>
-    </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="U24" s="54"/>
+      <c r="V24" s="54"/>
+      <c r="W24" s="54"/>
+      <c r="X24" s="54"/>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
-      <c r="U26" s="30" t="s">
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="68"/>
+      <c r="M26" s="68"/>
+      <c r="N26" s="68"/>
+      <c r="O26" s="68"/>
+      <c r="P26" s="68"/>
+      <c r="Q26" s="68"/>
+      <c r="R26" s="68"/>
+      <c r="S26" s="68"/>
+      <c r="U26" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="V26" s="30"/>
-      <c r="W26" s="30"/>
-      <c r="X26" s="30"/>
-    </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V26" s="58"/>
+      <c r="W26" s="58"/>
+      <c r="X26" s="58"/>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>21</v>
       </c>
@@ -3491,18 +3466,18 @@
       <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U28" s="32" t="s">
+      <c r="U28" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="V28" s="33"/>
-      <c r="W28" s="33"/>
-      <c r="X28" s="33"/>
-      <c r="Y28" s="34"/>
-      <c r="Z28" s="34"/>
-      <c r="AA28" s="34"/>
-      <c r="AB28" s="35"/>
-    </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V28" s="65"/>
+      <c r="W28" s="65"/>
+      <c r="X28" s="65"/>
+      <c r="Y28" s="18"/>
+      <c r="Z28" s="18"/>
+      <c r="AA28" s="18"/>
+      <c r="AB28" s="19"/>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C29" s="7">
         <v>2</v>
       </c>
@@ -3518,18 +3493,15 @@
       <c r="G29" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="24" t="s">
+      <c r="U29" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="V29" s="36"/>
-      <c r="W29" s="36"/>
-      <c r="X29" s="36"/>
-      <c r="Y29" s="37"/>
-      <c r="Z29" s="37"/>
-      <c r="AA29" s="37"/>
-      <c r="AB29" s="38"/>
-    </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V29" s="68"/>
+      <c r="W29" s="68"/>
+      <c r="X29" s="68"/>
+      <c r="AB29" s="20"/>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C30" s="7">
         <v>4</v>
       </c>
@@ -3542,27 +3514,27 @@
       <c r="F30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="G30" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="23" t="s">
+      <c r="H30" s="53"/>
+      <c r="I30" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="U30" s="24" t="s">
+      <c r="J30" s="89"/>
+      <c r="K30" s="89"/>
+      <c r="U30" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="V30" s="36"/>
-      <c r="W30" s="36"/>
-      <c r="X30" s="36"/>
-      <c r="Y30" s="36"/>
-      <c r="Z30" s="36"/>
-      <c r="AA30" s="36"/>
-      <c r="AB30" s="39"/>
-    </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V30" s="68"/>
+      <c r="W30" s="68"/>
+      <c r="X30" s="68"/>
+      <c r="Y30" s="68"/>
+      <c r="Z30" s="68"/>
+      <c r="AA30" s="68"/>
+      <c r="AB30" s="69"/>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C31" s="7">
         <v>8</v>
       </c>
@@ -3575,65 +3547,65 @@
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22" t="s">
+      <c r="H31" s="53"/>
+      <c r="I31" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="22"/>
-      <c r="Q31" s="22"/>
-      <c r="R31" s="22"/>
-      <c r="S31" s="22"/>
-      <c r="U31" s="40" t="s">
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="53"/>
+      <c r="O31" s="53"/>
+      <c r="P31" s="53"/>
+      <c r="Q31" s="53"/>
+      <c r="R31" s="53"/>
+      <c r="S31" s="53"/>
+      <c r="U31" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="V31" s="41"/>
-      <c r="W31" s="41"/>
-      <c r="X31" s="41"/>
-      <c r="Y31" s="41"/>
-      <c r="Z31" s="41"/>
-      <c r="AA31" s="41"/>
-      <c r="AB31" s="42"/>
-    </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V31" s="62"/>
+      <c r="W31" s="62"/>
+      <c r="X31" s="62"/>
+      <c r="Y31" s="62"/>
+      <c r="Z31" s="62"/>
+      <c r="AA31" s="62"/>
+      <c r="AB31" s="63"/>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
-      <c r="P33" s="18"/>
-      <c r="Q33" s="18"/>
-      <c r="R33" s="18"/>
-      <c r="S33" s="18"/>
-      <c r="U33" s="43" t="s">
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="68"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
+      <c r="Q33" s="68"/>
+      <c r="R33" s="68"/>
+      <c r="S33" s="68"/>
+      <c r="U33" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="V33" s="44"/>
-      <c r="W33" s="44"/>
-      <c r="X33" s="45"/>
-    </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V33" s="77"/>
+      <c r="W33" s="77"/>
+      <c r="X33" s="78"/>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>27</v>
       </c>
@@ -3646,18 +3618,18 @@
       <c r="E35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U35" s="32" t="s">
+      <c r="U35" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="V35" s="33"/>
-      <c r="W35" s="33"/>
-      <c r="X35" s="33"/>
-      <c r="Y35" s="34"/>
-      <c r="Z35" s="34"/>
-      <c r="AA35" s="34"/>
-      <c r="AB35" s="35"/>
-    </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V35" s="65"/>
+      <c r="W35" s="65"/>
+      <c r="X35" s="65"/>
+      <c r="Y35" s="18"/>
+      <c r="Z35" s="18"/>
+      <c r="AA35" s="18"/>
+      <c r="AB35" s="19"/>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C36" s="7">
         <v>2</v>
       </c>
@@ -3673,18 +3645,15 @@
       <c r="G36" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U36" s="24" t="s">
+      <c r="U36" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="V36" s="36"/>
-      <c r="W36" s="36"/>
-      <c r="X36" s="36"/>
-      <c r="Y36" s="37"/>
-      <c r="Z36" s="37"/>
-      <c r="AA36" s="37"/>
-      <c r="AB36" s="38"/>
-    </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V36" s="68"/>
+      <c r="W36" s="68"/>
+      <c r="X36" s="68"/>
+      <c r="AB36" s="20"/>
+    </row>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C37" s="7">
         <v>4</v>
       </c>
@@ -3697,27 +3666,27 @@
       <c r="F37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="23" t="s">
+      <c r="H37" s="53"/>
+      <c r="I37" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="23"/>
-      <c r="K37" s="23"/>
-      <c r="U37" s="24" t="s">
+      <c r="J37" s="89"/>
+      <c r="K37" s="89"/>
+      <c r="U37" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="V37" s="36"/>
-      <c r="W37" s="36"/>
-      <c r="X37" s="36"/>
-      <c r="Y37" s="36"/>
-      <c r="Z37" s="36"/>
-      <c r="AA37" s="36"/>
-      <c r="AB37" s="39"/>
-    </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V37" s="68"/>
+      <c r="W37" s="68"/>
+      <c r="X37" s="68"/>
+      <c r="Y37" s="68"/>
+      <c r="Z37" s="68"/>
+      <c r="AA37" s="68"/>
+      <c r="AB37" s="69"/>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C38" s="7">
         <v>8</v>
       </c>
@@ -3730,15 +3699,15 @@
       <c r="F38" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="G38" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="19" t="s">
+      <c r="H38" s="53"/>
+      <c r="I38" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="J38" s="20"/>
-      <c r="K38" s="21"/>
+      <c r="J38" s="88"/>
+      <c r="K38" s="60"/>
       <c r="L38" s="3" t="s">
         <v>16</v>
       </c>
@@ -3763,18 +3732,18 @@
       <c r="S38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U38" s="40" t="s">
+      <c r="U38" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="V38" s="41"/>
-      <c r="W38" s="41"/>
-      <c r="X38" s="41"/>
-      <c r="Y38" s="41"/>
-      <c r="Z38" s="41"/>
-      <c r="AA38" s="41"/>
-      <c r="AB38" s="42"/>
-    </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V38" s="62"/>
+      <c r="W38" s="62"/>
+      <c r="X38" s="62"/>
+      <c r="Y38" s="62"/>
+      <c r="Z38" s="62"/>
+      <c r="AA38" s="62"/>
+      <c r="AB38" s="63"/>
+    </row>
+    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>30</v>
       </c>
@@ -3787,14 +3756,14 @@
       <c r="E40" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U40" s="46" t="s">
+      <c r="U40" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="V40" s="47"/>
-      <c r="W40" s="47"/>
-      <c r="X40" s="48"/>
-    </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V40" s="80"/>
+      <c r="W40" s="80"/>
+      <c r="X40" s="81"/>
+    </row>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C41" s="7">
         <v>2</v>
       </c>
@@ -3804,49 +3773,49 @@
       <c r="E41" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="19" t="s">
+      <c r="F41" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="21"/>
-      <c r="U41" s="49"/>
-      <c r="V41" s="50"/>
-      <c r="W41" s="50"/>
-      <c r="X41" s="51"/>
-    </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="G41" s="60"/>
+      <c r="U41" s="82"/>
+      <c r="V41" s="83"/>
+      <c r="W41" s="83"/>
+      <c r="X41" s="84"/>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="U43" s="43" t="s">
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="68"/>
+      <c r="I43" s="68"/>
+      <c r="J43" s="68"/>
+      <c r="K43" s="68"/>
+      <c r="L43" s="68"/>
+      <c r="M43" s="68"/>
+      <c r="N43" s="68"/>
+      <c r="O43" s="68"/>
+      <c r="P43" s="68"/>
+      <c r="Q43" s="68"/>
+      <c r="R43" s="68"/>
+      <c r="S43" s="68"/>
+      <c r="U43" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="V43" s="44"/>
-      <c r="W43" s="44"/>
-      <c r="X43" s="45"/>
-    </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V43" s="77"/>
+      <c r="W43" s="77"/>
+      <c r="X43" s="78"/>
+    </row>
+    <row r="44" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C44" s="12"/>
     </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>33</v>
       </c>
@@ -3859,18 +3828,18 @@
       <c r="E45" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U45" s="52" t="s">
+      <c r="U45" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="V45" s="34"/>
-      <c r="W45" s="34"/>
-      <c r="X45" s="34"/>
-      <c r="Y45" s="34"/>
-      <c r="Z45" s="34"/>
-      <c r="AA45" s="34"/>
-      <c r="AB45" s="35"/>
-    </row>
-    <row r="46" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="V45" s="18"/>
+      <c r="W45" s="18"/>
+      <c r="X45" s="18"/>
+      <c r="Y45" s="18"/>
+      <c r="Z45" s="18"/>
+      <c r="AA45" s="18"/>
+      <c r="AB45" s="19"/>
+    </row>
+    <row r="46" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C46" s="7">
         <v>2</v>
       </c>
@@ -3886,18 +3855,12 @@
       <c r="G46" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U46" s="53" t="s">
+      <c r="U46" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="V46" s="54"/>
-      <c r="W46" s="54"/>
-      <c r="X46" s="54"/>
-      <c r="Y46" s="54"/>
-      <c r="Z46" s="54"/>
-      <c r="AA46" s="54"/>
-      <c r="AB46" s="55"/>
-    </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="AB46" s="20"/>
+    </row>
+    <row r="47" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C47" s="7">
         <v>4</v>
       </c>
@@ -3907,28 +3870,22 @@
       <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="22" t="s">
+      <c r="F47" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="22"/>
-      <c r="H47" s="23" t="s">
+      <c r="G47" s="53"/>
+      <c r="H47" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="23"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="23"/>
-      <c r="U47" s="53" t="s">
+      <c r="I47" s="89"/>
+      <c r="J47" s="89"/>
+      <c r="K47" s="89"/>
+      <c r="U47" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="V47" s="54"/>
-      <c r="W47" s="54"/>
-      <c r="X47" s="54"/>
-      <c r="Y47" s="54"/>
-      <c r="Z47" s="54"/>
-      <c r="AA47" s="54"/>
-      <c r="AB47" s="55"/>
-    </row>
-    <row r="48" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="AB47" s="20"/>
+    </row>
+    <row r="48" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C48" s="11">
         <v>8</v>
       </c>
@@ -3938,36 +3895,36 @@
       <c r="E48" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F48" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="G48" s="22"/>
-      <c r="H48" s="22" t="s">
+      <c r="G48" s="53"/>
+      <c r="H48" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="I48" s="22"/>
-      <c r="J48" s="22"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="22"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="22"/>
-      <c r="Q48" s="22"/>
-      <c r="R48" s="22"/>
-      <c r="S48" s="22"/>
-      <c r="U48" s="56" t="s">
+      <c r="I48" s="53"/>
+      <c r="J48" s="53"/>
+      <c r="K48" s="53"/>
+      <c r="L48" s="53"/>
+      <c r="M48" s="53"/>
+      <c r="N48" s="53"/>
+      <c r="O48" s="53"/>
+      <c r="P48" s="53"/>
+      <c r="Q48" s="53"/>
+      <c r="R48" s="53"/>
+      <c r="S48" s="53"/>
+      <c r="U48" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="V48" s="57"/>
-      <c r="W48" s="57"/>
-      <c r="X48" s="57"/>
-      <c r="Y48" s="57"/>
-      <c r="Z48" s="57"/>
-      <c r="AA48" s="57"/>
-      <c r="AB48" s="58"/>
-    </row>
-    <row r="50" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="V48" s="24"/>
+      <c r="W48" s="24"/>
+      <c r="X48" s="24"/>
+      <c r="Y48" s="24"/>
+      <c r="Z48" s="24"/>
+      <c r="AA48" s="24"/>
+      <c r="AB48" s="25"/>
+    </row>
+    <row r="50" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>34</v>
       </c>
@@ -3980,19 +3937,19 @@
       <c r="E50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U50" s="32" t="s">
+      <c r="U50" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="V50" s="33"/>
-      <c r="W50" s="33"/>
-      <c r="X50" s="33"/>
-      <c r="Y50" s="33"/>
-      <c r="Z50" s="33"/>
-      <c r="AA50" s="33"/>
-      <c r="AB50" s="33"/>
-      <c r="AC50" s="59"/>
-    </row>
-    <row r="51" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="V50" s="65"/>
+      <c r="W50" s="65"/>
+      <c r="X50" s="65"/>
+      <c r="Y50" s="65"/>
+      <c r="Z50" s="65"/>
+      <c r="AA50" s="65"/>
+      <c r="AB50" s="65"/>
+      <c r="AC50" s="66"/>
+    </row>
+    <row r="51" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C51" s="7">
         <v>2</v>
       </c>
@@ -4008,19 +3965,19 @@
       <c r="G51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U51" s="24" t="s">
+      <c r="U51" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="V51" s="36"/>
-      <c r="W51" s="36"/>
-      <c r="X51" s="36"/>
-      <c r="Y51" s="36"/>
-      <c r="Z51" s="36"/>
-      <c r="AA51" s="36"/>
-      <c r="AB51" s="36"/>
-      <c r="AC51" s="39"/>
-    </row>
-    <row r="52" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="V51" s="68"/>
+      <c r="W51" s="68"/>
+      <c r="X51" s="68"/>
+      <c r="Y51" s="68"/>
+      <c r="Z51" s="68"/>
+      <c r="AA51" s="68"/>
+      <c r="AB51" s="68"/>
+      <c r="AC51" s="69"/>
+    </row>
+    <row r="52" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C52" s="7">
         <v>4</v>
       </c>
@@ -4030,29 +3987,29 @@
       <c r="E52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="22" t="s">
+      <c r="F52" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="22"/>
-      <c r="H52" s="23" t="s">
+      <c r="G52" s="53"/>
+      <c r="H52" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="23"/>
-      <c r="J52" s="23"/>
-      <c r="K52" s="23"/>
-      <c r="U52" s="24" t="s">
+      <c r="I52" s="89"/>
+      <c r="J52" s="89"/>
+      <c r="K52" s="89"/>
+      <c r="U52" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="V52" s="36"/>
-      <c r="W52" s="36"/>
-      <c r="X52" s="36"/>
-      <c r="Y52" s="36"/>
-      <c r="Z52" s="36"/>
-      <c r="AA52" s="36"/>
-      <c r="AB52" s="36"/>
-      <c r="AC52" s="39"/>
-    </row>
-    <row r="53" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="V52" s="68"/>
+      <c r="W52" s="68"/>
+      <c r="X52" s="68"/>
+      <c r="Y52" s="68"/>
+      <c r="Z52" s="68"/>
+      <c r="AA52" s="68"/>
+      <c r="AB52" s="68"/>
+      <c r="AC52" s="69"/>
+    </row>
+    <row r="53" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C53" s="11">
         <v>8</v>
       </c>
@@ -4062,72 +4019,72 @@
       <c r="E53" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F53" s="22" t="s">
+      <c r="F53" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="G53" s="22"/>
-      <c r="H53" s="22" t="s">
+      <c r="G53" s="53"/>
+      <c r="H53" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="22"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="22"/>
-      <c r="M53" s="22"/>
-      <c r="N53" s="22"/>
-      <c r="O53" s="22"/>
-      <c r="P53" s="22"/>
-      <c r="Q53" s="22"/>
-      <c r="R53" s="22"/>
-      <c r="S53" s="22"/>
-      <c r="U53" s="40" t="s">
+      <c r="I53" s="53"/>
+      <c r="J53" s="53"/>
+      <c r="K53" s="53"/>
+      <c r="L53" s="53"/>
+      <c r="M53" s="53"/>
+      <c r="N53" s="53"/>
+      <c r="O53" s="53"/>
+      <c r="P53" s="53"/>
+      <c r="Q53" s="53"/>
+      <c r="R53" s="53"/>
+      <c r="S53" s="53"/>
+      <c r="U53" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="V53" s="41"/>
-      <c r="W53" s="41"/>
-      <c r="X53" s="41"/>
-      <c r="Y53" s="41"/>
-      <c r="Z53" s="41"/>
-      <c r="AA53" s="41"/>
-      <c r="AB53" s="41"/>
-      <c r="AC53" s="42"/>
-    </row>
-    <row r="55" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="V53" s="62"/>
+      <c r="W53" s="62"/>
+      <c r="X53" s="62"/>
+      <c r="Y53" s="62"/>
+      <c r="Z53" s="62"/>
+      <c r="AA53" s="62"/>
+      <c r="AB53" s="62"/>
+      <c r="AC53" s="63"/>
+    </row>
+    <row r="55" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>36</v>
       </c>
-      <c r="C55" s="18" t="s">
+      <c r="C55" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18"/>
-      <c r="M55" s="18"/>
-      <c r="N55" s="18"/>
-      <c r="O55" s="18"/>
-      <c r="P55" s="18"/>
-      <c r="Q55" s="18"/>
-      <c r="R55" s="18"/>
-      <c r="S55" s="18"/>
-      <c r="U55" s="43" t="s">
+      <c r="D55" s="68"/>
+      <c r="E55" s="68"/>
+      <c r="F55" s="68"/>
+      <c r="G55" s="68"/>
+      <c r="H55" s="68"/>
+      <c r="I55" s="68"/>
+      <c r="J55" s="68"/>
+      <c r="K55" s="68"/>
+      <c r="L55" s="68"/>
+      <c r="M55" s="68"/>
+      <c r="N55" s="68"/>
+      <c r="O55" s="68"/>
+      <c r="P55" s="68"/>
+      <c r="Q55" s="68"/>
+      <c r="R55" s="68"/>
+      <c r="S55" s="68"/>
+      <c r="U55" s="76" t="s">
         <v>78</v>
       </c>
-      <c r="V55" s="44"/>
-      <c r="W55" s="44"/>
-      <c r="X55" s="44"/>
-      <c r="Y55" s="44"/>
-      <c r="Z55" s="44"/>
-      <c r="AA55" s="44"/>
-      <c r="AB55" s="44"/>
-      <c r="AC55" s="45"/>
-    </row>
-    <row r="57" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="V55" s="77"/>
+      <c r="W55" s="77"/>
+      <c r="X55" s="77"/>
+      <c r="Y55" s="77"/>
+      <c r="Z55" s="77"/>
+      <c r="AA55" s="77"/>
+      <c r="AB55" s="77"/>
+      <c r="AC55" s="78"/>
+    </row>
+    <row r="57" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>8</v>
       </c>
@@ -4140,19 +4097,19 @@
       <c r="E57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U57" s="32" t="s">
+      <c r="U57" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="V57" s="33"/>
-      <c r="W57" s="33"/>
-      <c r="X57" s="33"/>
-      <c r="Y57" s="33"/>
-      <c r="Z57" s="33"/>
-      <c r="AA57" s="33"/>
-      <c r="AB57" s="33"/>
-      <c r="AC57" s="59"/>
-    </row>
-    <row r="58" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="V57" s="65"/>
+      <c r="W57" s="65"/>
+      <c r="X57" s="65"/>
+      <c r="Y57" s="65"/>
+      <c r="Z57" s="65"/>
+      <c r="AA57" s="65"/>
+      <c r="AB57" s="65"/>
+      <c r="AC57" s="66"/>
+    </row>
+    <row r="58" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C58" s="7">
         <v>2</v>
       </c>
@@ -4162,23 +4119,23 @@
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="19" t="s">
+      <c r="F58" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="G58" s="21"/>
-      <c r="U58" s="24" t="s">
+      <c r="G58" s="60"/>
+      <c r="U58" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="V58" s="36"/>
-      <c r="W58" s="36"/>
-      <c r="X58" s="36"/>
-      <c r="Y58" s="36"/>
-      <c r="Z58" s="36"/>
-      <c r="AA58" s="36"/>
-      <c r="AB58" s="36"/>
-      <c r="AC58" s="39"/>
-    </row>
-    <row r="59" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="V58" s="68"/>
+      <c r="W58" s="68"/>
+      <c r="X58" s="68"/>
+      <c r="Y58" s="68"/>
+      <c r="Z58" s="68"/>
+      <c r="AA58" s="68"/>
+      <c r="AB58" s="68"/>
+      <c r="AC58" s="69"/>
+    </row>
+    <row r="59" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C59" s="7">
         <v>4</v>
       </c>
@@ -4188,27 +4145,27 @@
       <c r="E59" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F59" s="22" t="s">
+      <c r="F59" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22" t="s">
+      <c r="G59" s="53"/>
+      <c r="H59" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="I59" s="22"/>
-      <c r="U59" s="40" t="s">
+      <c r="I59" s="53"/>
+      <c r="U59" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="V59" s="41"/>
-      <c r="W59" s="41"/>
-      <c r="X59" s="41"/>
-      <c r="Y59" s="41"/>
-      <c r="Z59" s="41"/>
-      <c r="AA59" s="41"/>
-      <c r="AB59" s="41"/>
-      <c r="AC59" s="42"/>
-    </row>
-    <row r="61" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="V59" s="62"/>
+      <c r="W59" s="62"/>
+      <c r="X59" s="62"/>
+      <c r="Y59" s="62"/>
+      <c r="Z59" s="62"/>
+      <c r="AA59" s="62"/>
+      <c r="AB59" s="62"/>
+      <c r="AC59" s="63"/>
+    </row>
+    <row r="61" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>0</v>
       </c>
@@ -4221,19 +4178,19 @@
       <c r="E61" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U61" s="52" t="s">
+      <c r="U61" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="V61" s="34"/>
-      <c r="W61" s="34"/>
-      <c r="X61" s="34"/>
-      <c r="Y61" s="34"/>
-      <c r="Z61" s="34"/>
-      <c r="AA61" s="34"/>
-      <c r="AB61" s="34"/>
-      <c r="AC61" s="35"/>
-    </row>
-    <row r="62" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="V61" s="18"/>
+      <c r="W61" s="18"/>
+      <c r="X61" s="18"/>
+      <c r="Y61" s="18"/>
+      <c r="Z61" s="18"/>
+      <c r="AA61" s="18"/>
+      <c r="AB61" s="18"/>
+      <c r="AC61" s="19"/>
+    </row>
+    <row r="62" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C62" s="7">
         <v>2</v>
       </c>
@@ -4243,23 +4200,23 @@
       <c r="E62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="19" t="s">
+      <c r="F62" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="21"/>
-      <c r="U62" s="24" t="s">
+      <c r="G62" s="60"/>
+      <c r="U62" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="V62" s="36"/>
-      <c r="W62" s="36"/>
-      <c r="X62" s="36"/>
-      <c r="Y62" s="36"/>
-      <c r="Z62" s="36"/>
-      <c r="AA62" s="36"/>
-      <c r="AB62" s="36"/>
-      <c r="AC62" s="39"/>
-    </row>
-    <row r="63" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="V62" s="68"/>
+      <c r="W62" s="68"/>
+      <c r="X62" s="68"/>
+      <c r="Y62" s="68"/>
+      <c r="Z62" s="68"/>
+      <c r="AA62" s="68"/>
+      <c r="AB62" s="68"/>
+      <c r="AC62" s="69"/>
+    </row>
+    <row r="63" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C63" s="7">
         <v>4</v>
       </c>
@@ -4269,64 +4226,64 @@
       <c r="E63" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="22" t="s">
+      <c r="F63" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="G63" s="22"/>
-      <c r="H63" s="22" t="s">
+      <c r="G63" s="53"/>
+      <c r="H63" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="I63" s="22"/>
-      <c r="J63" s="22" t="s">
+      <c r="I63" s="53"/>
+      <c r="J63" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="K63" s="22"/>
-      <c r="U63" s="63" t="s">
+      <c r="K63" s="53"/>
+      <c r="U63" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="V63" s="61"/>
-      <c r="W63" s="61"/>
-      <c r="X63" s="61"/>
-      <c r="Y63" s="61"/>
-      <c r="Z63" s="61"/>
-      <c r="AA63" s="61"/>
-      <c r="AB63" s="61"/>
-      <c r="AC63" s="64"/>
-    </row>
-    <row r="64" spans="2:29" x14ac:dyDescent="0.45">
-      <c r="U64" s="63"/>
-      <c r="V64" s="61"/>
-      <c r="W64" s="61"/>
-      <c r="X64" s="61"/>
-      <c r="Y64" s="61"/>
-      <c r="Z64" s="61"/>
-      <c r="AA64" s="61"/>
-      <c r="AB64" s="61"/>
-      <c r="AC64" s="64"/>
-    </row>
-    <row r="65" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="U65" s="65"/>
-      <c r="V65" s="66"/>
-      <c r="W65" s="66"/>
-      <c r="X65" s="66"/>
-      <c r="Y65" s="66"/>
-      <c r="Z65" s="66"/>
-      <c r="AA65" s="66"/>
-      <c r="AB65" s="66"/>
-      <c r="AC65" s="67"/>
-    </row>
-    <row r="66" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="U66" s="62"/>
-      <c r="V66" s="62"/>
-      <c r="W66" s="62"/>
-      <c r="X66" s="62"/>
-      <c r="Y66" s="62"/>
-      <c r="Z66" s="62"/>
-      <c r="AA66" s="62"/>
-      <c r="AB66" s="62"/>
-      <c r="AC66" s="62"/>
-    </row>
-    <row r="67" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="V63" s="71"/>
+      <c r="W63" s="71"/>
+      <c r="X63" s="71"/>
+      <c r="Y63" s="71"/>
+      <c r="Z63" s="71"/>
+      <c r="AA63" s="71"/>
+      <c r="AB63" s="71"/>
+      <c r="AC63" s="72"/>
+    </row>
+    <row r="64" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="U64" s="70"/>
+      <c r="V64" s="71"/>
+      <c r="W64" s="71"/>
+      <c r="X64" s="71"/>
+      <c r="Y64" s="71"/>
+      <c r="Z64" s="71"/>
+      <c r="AA64" s="71"/>
+      <c r="AB64" s="71"/>
+      <c r="AC64" s="72"/>
+    </row>
+    <row r="65" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="U65" s="73"/>
+      <c r="V65" s="74"/>
+      <c r="W65" s="74"/>
+      <c r="X65" s="74"/>
+      <c r="Y65" s="74"/>
+      <c r="Z65" s="74"/>
+      <c r="AA65" s="74"/>
+      <c r="AB65" s="74"/>
+      <c r="AC65" s="75"/>
+    </row>
+    <row r="66" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="U66" s="26"/>
+      <c r="V66" s="26"/>
+      <c r="W66" s="26"/>
+      <c r="X66" s="26"/>
+      <c r="Y66" s="26"/>
+      <c r="Z66" s="26"/>
+      <c r="AA66" s="26"/>
+      <c r="AB66" s="26"/>
+      <c r="AC66" s="26"/>
+    </row>
+    <row r="67" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>38</v>
       </c>
@@ -4339,20 +4296,20 @@
       <c r="E67" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U67" s="32" t="s">
+      <c r="U67" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="V67" s="33"/>
-      <c r="W67" s="33"/>
-      <c r="X67" s="33"/>
-      <c r="Y67" s="33"/>
-      <c r="Z67" s="33"/>
-      <c r="AA67" s="33"/>
-      <c r="AB67" s="33"/>
-      <c r="AC67" s="33"/>
-      <c r="AD67" s="59"/>
-    </row>
-    <row r="68" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="V67" s="65"/>
+      <c r="W67" s="65"/>
+      <c r="X67" s="65"/>
+      <c r="Y67" s="65"/>
+      <c r="Z67" s="65"/>
+      <c r="AA67" s="65"/>
+      <c r="AB67" s="65"/>
+      <c r="AC67" s="65"/>
+      <c r="AD67" s="66"/>
+    </row>
+    <row r="68" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C68" s="7">
         <v>2</v>
       </c>
@@ -4368,20 +4325,20 @@
       <c r="G68" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U68" s="24" t="s">
+      <c r="U68" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="V68" s="36"/>
-      <c r="W68" s="36"/>
-      <c r="X68" s="36"/>
-      <c r="Y68" s="36"/>
-      <c r="Z68" s="36"/>
-      <c r="AA68" s="36"/>
-      <c r="AB68" s="36"/>
-      <c r="AC68" s="36"/>
-      <c r="AD68" s="39"/>
-    </row>
-    <row r="69" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="V68" s="68"/>
+      <c r="W68" s="68"/>
+      <c r="X68" s="68"/>
+      <c r="Y68" s="68"/>
+      <c r="Z68" s="68"/>
+      <c r="AA68" s="68"/>
+      <c r="AB68" s="68"/>
+      <c r="AC68" s="68"/>
+      <c r="AD68" s="69"/>
+    </row>
+    <row r="69" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C69" s="7">
         <v>4</v>
       </c>
@@ -4403,24 +4360,24 @@
       <c r="I69" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J69" s="19" t="s">
+      <c r="J69" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="K69" s="21"/>
-      <c r="U69" s="24" t="s">
+      <c r="K69" s="60"/>
+      <c r="U69" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="V69" s="36"/>
-      <c r="W69" s="36"/>
-      <c r="X69" s="36"/>
-      <c r="Y69" s="36"/>
-      <c r="Z69" s="36"/>
-      <c r="AA69" s="36"/>
-      <c r="AB69" s="36"/>
-      <c r="AC69" s="36"/>
-      <c r="AD69" s="39"/>
-    </row>
-    <row r="70" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="V69" s="68"/>
+      <c r="W69" s="68"/>
+      <c r="X69" s="68"/>
+      <c r="Y69" s="68"/>
+      <c r="Z69" s="68"/>
+      <c r="AA69" s="68"/>
+      <c r="AB69" s="68"/>
+      <c r="AC69" s="68"/>
+      <c r="AD69" s="69"/>
+    </row>
+    <row r="70" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C70" s="11">
         <v>8</v>
       </c>
@@ -4430,46 +4387,46 @@
       <c r="E70" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F70" s="22" t="s">
+      <c r="F70" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="22"/>
-      <c r="H70" s="19" t="s">
+      <c r="G70" s="53"/>
+      <c r="H70" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="I70" s="21"/>
-      <c r="J70" s="19" t="s">
+      <c r="I70" s="60"/>
+      <c r="J70" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="K70" s="21"/>
-      <c r="L70" s="19" t="s">
+      <c r="K70" s="60"/>
+      <c r="L70" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="M70" s="21"/>
-      <c r="N70" s="19" t="s">
+      <c r="M70" s="60"/>
+      <c r="N70" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="O70" s="21"/>
-      <c r="P70" s="19" t="s">
+      <c r="O70" s="60"/>
+      <c r="P70" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="Q70" s="20"/>
-      <c r="R70" s="20"/>
-      <c r="S70" s="21"/>
-      <c r="U70" s="40" t="s">
+      <c r="Q70" s="88"/>
+      <c r="R70" s="88"/>
+      <c r="S70" s="60"/>
+      <c r="U70" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="V70" s="41"/>
-      <c r="W70" s="41"/>
-      <c r="X70" s="41"/>
-      <c r="Y70" s="41"/>
-      <c r="Z70" s="41"/>
-      <c r="AA70" s="41"/>
-      <c r="AB70" s="41"/>
-      <c r="AC70" s="41"/>
-      <c r="AD70" s="42"/>
-    </row>
-    <row r="72" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="V70" s="62"/>
+      <c r="W70" s="62"/>
+      <c r="X70" s="62"/>
+      <c r="Y70" s="62"/>
+      <c r="Z70" s="62"/>
+      <c r="AA70" s="62"/>
+      <c r="AB70" s="62"/>
+      <c r="AC70" s="62"/>
+      <c r="AD70" s="63"/>
+    </row>
+    <row r="72" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>45</v>
       </c>
@@ -4482,15 +4439,15 @@
       <c r="E72" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U72" s="32" t="s">
+      <c r="U72" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="V72" s="33"/>
-      <c r="W72" s="33"/>
-      <c r="X72" s="33"/>
-      <c r="Y72" s="59"/>
-    </row>
-    <row r="73" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="V72" s="65"/>
+      <c r="W72" s="65"/>
+      <c r="X72" s="65"/>
+      <c r="Y72" s="66"/>
+    </row>
+    <row r="73" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C73" s="7">
         <v>2</v>
       </c>
@@ -4500,19 +4457,19 @@
       <c r="E73" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F73" s="19" t="s">
+      <c r="F73" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="G73" s="21"/>
-      <c r="U73" s="40" t="s">
+      <c r="G73" s="60"/>
+      <c r="U73" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="V73" s="41"/>
-      <c r="W73" s="41"/>
-      <c r="X73" s="41"/>
-      <c r="Y73" s="42"/>
-    </row>
-    <row r="75" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="V73" s="62"/>
+      <c r="W73" s="62"/>
+      <c r="X73" s="62"/>
+      <c r="Y73" s="63"/>
+    </row>
+    <row r="75" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>47</v>
       </c>
@@ -4525,20 +4482,20 @@
       <c r="E75" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U75" s="32" t="s">
+      <c r="U75" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="V75" s="33"/>
-      <c r="W75" s="33"/>
-      <c r="X75" s="33"/>
-      <c r="Y75" s="33"/>
-      <c r="Z75" s="33"/>
-      <c r="AA75" s="33"/>
-      <c r="AB75" s="33"/>
-      <c r="AC75" s="33"/>
-      <c r="AD75" s="59"/>
-    </row>
-    <row r="76" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="V75" s="65"/>
+      <c r="W75" s="65"/>
+      <c r="X75" s="65"/>
+      <c r="Y75" s="65"/>
+      <c r="Z75" s="65"/>
+      <c r="AA75" s="65"/>
+      <c r="AB75" s="65"/>
+      <c r="AC75" s="65"/>
+      <c r="AD75" s="66"/>
+    </row>
+    <row r="76" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C76" s="7">
         <v>2</v>
       </c>
@@ -4548,24 +4505,24 @@
       <c r="E76" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F76" s="19" t="s">
+      <c r="F76" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="G76" s="21"/>
-      <c r="U76" s="24" t="s">
+      <c r="G76" s="60"/>
+      <c r="U76" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="V76" s="36"/>
-      <c r="W76" s="36"/>
-      <c r="X76" s="36"/>
-      <c r="Y76" s="36"/>
-      <c r="Z76" s="36"/>
-      <c r="AA76" s="36"/>
-      <c r="AB76" s="36"/>
-      <c r="AC76" s="36"/>
-      <c r="AD76" s="39"/>
-    </row>
-    <row r="77" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="V76" s="68"/>
+      <c r="W76" s="68"/>
+      <c r="X76" s="68"/>
+      <c r="Y76" s="68"/>
+      <c r="Z76" s="68"/>
+      <c r="AA76" s="68"/>
+      <c r="AB76" s="68"/>
+      <c r="AC76" s="68"/>
+      <c r="AD76" s="69"/>
+    </row>
+    <row r="77" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C77" s="7">
         <v>4</v>
       </c>
@@ -4575,58 +4532,58 @@
       <c r="E77" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F77" s="22" t="s">
+      <c r="F77" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="G77" s="22"/>
-      <c r="H77" s="22" t="s">
+      <c r="G77" s="53"/>
+      <c r="H77" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="I77" s="22"/>
+      <c r="I77" s="53"/>
       <c r="J77" s="7" t="s">
         <v>41</v>
       </c>
       <c r="K77" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U77" s="40" t="s">
+      <c r="U77" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="V77" s="41"/>
-      <c r="W77" s="41"/>
-      <c r="X77" s="41"/>
-      <c r="Y77" s="41"/>
-      <c r="Z77" s="41"/>
-      <c r="AA77" s="41"/>
-      <c r="AB77" s="41"/>
-      <c r="AC77" s="41"/>
-      <c r="AD77" s="42"/>
-    </row>
-    <row r="79" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="V77" s="62"/>
+      <c r="W77" s="62"/>
+      <c r="X77" s="62"/>
+      <c r="Y77" s="62"/>
+      <c r="Z77" s="62"/>
+      <c r="AA77" s="62"/>
+      <c r="AB77" s="62"/>
+      <c r="AC77" s="62"/>
+      <c r="AD77" s="63"/>
+    </row>
+    <row r="79" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>51</v>
       </c>
-      <c r="C79" s="18" t="s">
+      <c r="C79" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="D79" s="18"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="18"/>
-      <c r="G79" s="18"/>
-      <c r="H79" s="18"/>
-      <c r="I79" s="18"/>
-      <c r="J79" s="18"/>
-      <c r="K79" s="18"/>
-      <c r="L79" s="18"/>
-      <c r="M79" s="18"/>
-      <c r="N79" s="18"/>
-      <c r="O79" s="18"/>
-      <c r="P79" s="18"/>
-      <c r="Q79" s="18"/>
-      <c r="R79" s="18"/>
-      <c r="S79" s="18"/>
-    </row>
-    <row r="81" spans="2:21" x14ac:dyDescent="0.45">
+      <c r="D79" s="68"/>
+      <c r="E79" s="68"/>
+      <c r="F79" s="68"/>
+      <c r="G79" s="68"/>
+      <c r="H79" s="68"/>
+      <c r="I79" s="68"/>
+      <c r="J79" s="68"/>
+      <c r="K79" s="68"/>
+      <c r="L79" s="68"/>
+      <c r="M79" s="68"/>
+      <c r="N79" s="68"/>
+      <c r="O79" s="68"/>
+      <c r="P79" s="68"/>
+      <c r="Q79" s="68"/>
+      <c r="R79" s="68"/>
+      <c r="S79" s="68"/>
+    </row>
+    <row r="81" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>100</v>
       </c>
@@ -4643,7 +4600,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="82" spans="2:21" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C82" s="7">
         <v>2</v>
       </c>
@@ -4653,80 +4610,13 @@
       <c r="E82" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F82" s="19" t="s">
+      <c r="F82" s="59" t="s">
         <v>251</v>
       </c>
-      <c r="G82" s="21"/>
+      <c r="G82" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="86">
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="U73:Y73"/>
-    <mergeCell ref="U75:AD75"/>
-    <mergeCell ref="U76:AD76"/>
-    <mergeCell ref="U77:AD77"/>
-    <mergeCell ref="U67:AD67"/>
-    <mergeCell ref="U68:AD68"/>
-    <mergeCell ref="U69:AD69"/>
-    <mergeCell ref="U70:AD70"/>
-    <mergeCell ref="U72:Y72"/>
-    <mergeCell ref="U57:AC57"/>
-    <mergeCell ref="U58:AC58"/>
-    <mergeCell ref="U59:AC59"/>
-    <mergeCell ref="U62:AC62"/>
-    <mergeCell ref="U63:AC65"/>
-    <mergeCell ref="U50:AC50"/>
-    <mergeCell ref="U51:AC51"/>
-    <mergeCell ref="U52:AC52"/>
-    <mergeCell ref="U53:AC53"/>
-    <mergeCell ref="U55:AC55"/>
-    <mergeCell ref="U40:X41"/>
-    <mergeCell ref="U43:X43"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="U35:X35"/>
-    <mergeCell ref="U36:X36"/>
-    <mergeCell ref="U37:AB37"/>
-    <mergeCell ref="U38:AB38"/>
-    <mergeCell ref="U15:X18"/>
-    <mergeCell ref="U21:X24"/>
-    <mergeCell ref="U26:X26"/>
-    <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U29:X29"/>
-    <mergeCell ref="U30:AB30"/>
-    <mergeCell ref="U31:AB31"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="C26:S26"/>
-    <mergeCell ref="H22:S22"/>
-    <mergeCell ref="C33:S33"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="C43:S43"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:K47"/>
-    <mergeCell ref="I31:S31"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="H48:S48"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:S53"/>
     <mergeCell ref="C55:S55"/>
     <mergeCell ref="F70:G70"/>
     <mergeCell ref="J69:K69"/>
@@ -4740,8 +4630,75 @@
     <mergeCell ref="H59:I59"/>
     <mergeCell ref="H63:I63"/>
     <mergeCell ref="J63:K63"/>
+    <mergeCell ref="P70:S70"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="H48:S48"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:S53"/>
+    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="I31:S31"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="C26:S26"/>
+    <mergeCell ref="H22:S22"/>
+    <mergeCell ref="C33:S33"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="C43:S43"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="U30:AB30"/>
+    <mergeCell ref="U31:AB31"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="U15:X18"/>
+    <mergeCell ref="U21:X24"/>
+    <mergeCell ref="U26:X26"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="U40:X41"/>
+    <mergeCell ref="U43:X43"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="U36:X36"/>
+    <mergeCell ref="U37:AB37"/>
+    <mergeCell ref="U38:AB38"/>
+    <mergeCell ref="U50:AC50"/>
+    <mergeCell ref="U51:AC51"/>
+    <mergeCell ref="U52:AC52"/>
+    <mergeCell ref="U53:AC53"/>
+    <mergeCell ref="U55:AC55"/>
+    <mergeCell ref="U57:AC57"/>
+    <mergeCell ref="U58:AC58"/>
+    <mergeCell ref="U59:AC59"/>
+    <mergeCell ref="U62:AC62"/>
+    <mergeCell ref="U63:AC65"/>
+    <mergeCell ref="U67:AD67"/>
+    <mergeCell ref="U68:AD68"/>
+    <mergeCell ref="U69:AD69"/>
+    <mergeCell ref="U70:AD70"/>
+    <mergeCell ref="U72:Y72"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="U73:Y73"/>
+    <mergeCell ref="U75:AD75"/>
+    <mergeCell ref="U76:AD76"/>
+    <mergeCell ref="U77:AD77"/>
     <mergeCell ref="C79:S79"/>
-    <mergeCell ref="P70:S70"/>
     <mergeCell ref="F73:G73"/>
     <mergeCell ref="F76:G76"/>
     <mergeCell ref="F77:G77"/>
@@ -4760,15 +4717,15 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B4" s="98"/>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
vm boiler plate ready
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aroma\Desktop\vcda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar\Documents\Work\AI\CPU\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FA8F48-84F3-44A6-B9DB-2D3018C6A2F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72131D51-20AF-47DC-AFFF-CB1ACB76AB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
+    <workbookView xWindow="19118" yWindow="0" windowWidth="19365" windowHeight="20963" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="258">
   <si>
     <t>POP</t>
   </si>
@@ -823,6 +823,9 @@
   </si>
   <si>
     <t>4-bit unsigned int type</t>
+  </si>
+  <si>
+    <t>bit</t>
   </si>
 </sst>
 </file>
@@ -1436,15 +1439,15 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1457,12 +1460,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1472,25 +1490,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1507,48 +1552,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1884,207 +1887,214 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CDEC23-057C-4C1E-AB18-5AC9130DB945}">
-  <dimension ref="B3:R31"/>
+  <dimension ref="B3:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="6.109375" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" customWidth="1"/>
-    <col min="5" max="5" width="2.21875" customWidth="1"/>
+    <col min="3" max="3" width="6.1328125" customWidth="1"/>
+    <col min="4" max="4" width="4.86328125" customWidth="1"/>
+    <col min="5" max="5" width="3.1328125" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="8" width="16.21875" customWidth="1"/>
-    <col min="10" max="10" width="14.21875" customWidth="1"/>
-    <col min="11" max="18" width="4.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.19921875" customWidth="1"/>
+    <col min="8" max="8" width="5.9296875" customWidth="1"/>
+    <col min="9" max="9" width="14.19921875" customWidth="1"/>
+    <col min="10" max="17" width="4.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="27" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C4" s="27" t="s">
         <v>103</v>
       </c>
       <c r="D4">
         <v>32</v>
       </c>
+      <c r="E4" t="s">
+        <v>257</v>
+      </c>
       <c r="F4" t="s">
         <v>105</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="55">
+      <c r="J4" s="55">
         <v>0</v>
       </c>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52">
+      <c r="K4" s="54"/>
+      <c r="L4" s="54">
         <v>1</v>
       </c>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52">
+      <c r="M4" s="54"/>
+      <c r="N4" s="54">
         <v>2</v>
       </c>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52">
+      <c r="O4" s="54"/>
+      <c r="P4" s="54">
         <v>3</v>
       </c>
-      <c r="R4" s="52"/>
-    </row>
-    <row r="5" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q4" s="54"/>
+    </row>
+    <row r="5" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C5" s="27" t="s">
         <v>104</v>
       </c>
       <c r="D5">
         <v>16</v>
       </c>
+      <c r="E5" t="s">
+        <v>257</v>
+      </c>
       <c r="F5" t="s">
         <v>106</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="4">
+      <c r="J5" s="4">
         <v>0</v>
       </c>
+      <c r="K5" s="5">
+        <v>1</v>
+      </c>
       <c r="L5" s="5">
-        <v>1</v>
-      </c>
-      <c r="M5" s="5">
         <v>2</v>
       </c>
-      <c r="N5" s="16">
+      <c r="M5" s="16">
         <v>3</v>
       </c>
-      <c r="O5" s="4">
+      <c r="N5" s="4">
         <v>4</v>
       </c>
+      <c r="O5" s="5">
+        <v>5</v>
+      </c>
       <c r="P5" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="5">
         <v>6</v>
       </c>
-      <c r="R5" s="16">
+      <c r="Q5" s="16">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B8" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="K8" s="53" t="s">
+      <c r="J8" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53" t="s">
+      <c r="K8" s="52"/>
+      <c r="L8" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="N8" s="53"/>
-      <c r="O8" s="53" t="s">
+      <c r="M8" s="52"/>
+      <c r="N8" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="P8" s="53"/>
-      <c r="Q8" s="53" t="s">
+      <c r="O8" s="52"/>
+      <c r="P8" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="R8" s="53"/>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="Q8" s="52"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
         <v>108</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="54"/>
+      <c r="G9" s="53"/>
       <c r="H9" s="8"/>
-      <c r="J9" s="28" t="s">
+      <c r="I9" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>109</v>
       </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="8"/>
+      <c r="J10" t="s">
+        <v>30</v>
+      </c>
       <c r="K10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" t="s">
         <v>138</v>
       </c>
-      <c r="N10" t="s">
+      <c r="M10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>119</v>
       </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
       <c r="H11" s="8"/>
+      <c r="J11" t="s">
+        <v>128</v>
+      </c>
       <c r="K11" t="s">
-        <v>128</v>
-      </c>
-      <c r="L11" t="s">
         <v>138</v>
       </c>
-      <c r="N11" t="s">
+      <c r="M11" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="J12" t="s">
+        <v>129</v>
+      </c>
       <c r="K12" t="s">
-        <v>129</v>
-      </c>
-      <c r="L12" t="s">
         <v>138</v>
       </c>
-      <c r="N12" t="s">
+      <c r="M12" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>118</v>
       </c>
       <c r="F13" t="s">
         <v>111</v>
       </c>
+      <c r="J13" t="s">
+        <v>31</v>
+      </c>
       <c r="K13" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" t="s">
         <v>138</v>
       </c>
-      <c r="N13" t="s">
+      <c r="M13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>117</v>
       </c>
       <c r="F14" t="s">
         <v>112</v>
       </c>
-      <c r="O14" t="s">
+      <c r="N14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
         <v>116</v>
       </c>
@@ -2092,208 +2102,208 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>115</v>
       </c>
       <c r="F16" t="s">
         <v>114</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="I16" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="K16" s="53" t="s">
+      <c r="J16" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="L16" s="53"/>
-      <c r="M16" s="53" t="s">
+      <c r="K16" s="52"/>
+      <c r="L16" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="N16" s="53"/>
-      <c r="O16" s="53" t="s">
+      <c r="M16" s="52"/>
+      <c r="N16" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="P16" s="53"/>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="53"/>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="J17" s="28" t="s">
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="I17" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
         <v>120</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="F18" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="G18" s="54"/>
+      <c r="G18" s="53"/>
       <c r="H18" s="8"/>
-      <c r="K18" t="s">
+      <c r="J18" t="s">
         <v>131</v>
       </c>
+      <c r="L18" t="s">
+        <v>138</v>
+      </c>
       <c r="M18" t="s">
-        <v>138</v>
-      </c>
-      <c r="N18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>109</v>
       </c>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
       <c r="H19" s="8"/>
-      <c r="K19" t="s">
+      <c r="J19" t="s">
         <v>130</v>
       </c>
+      <c r="L19" t="s">
+        <v>138</v>
+      </c>
       <c r="M19" t="s">
-        <v>138</v>
-      </c>
-      <c r="N19" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
         <v>127</v>
       </c>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
       <c r="H20" s="8"/>
-      <c r="K20" t="s">
+      <c r="J20" t="s">
         <v>133</v>
       </c>
+      <c r="L20" t="s">
+        <v>144</v>
+      </c>
       <c r="M20" t="s">
-        <v>144</v>
-      </c>
-      <c r="N20" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
         <v>126</v>
       </c>
       <c r="F22" t="s">
         <v>121</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="I22" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="K22" s="53" t="s">
+      <c r="J22" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="L22" s="53"/>
-      <c r="M22" s="53"/>
-      <c r="N22" s="53"/>
-      <c r="O22" s="53" t="s">
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="P22" s="53"/>
-      <c r="Q22" s="53"/>
-      <c r="R22" s="53"/>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.3">
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="52"/>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
         <v>125</v>
       </c>
       <c r="F23" t="s">
         <v>122</v>
       </c>
-      <c r="J23" s="28" t="s">
+      <c r="I23" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
         <v>124</v>
       </c>
       <c r="F24" t="s">
         <v>123</v>
       </c>
-      <c r="K24" t="s">
+      <c r="J24" t="s">
         <v>132</v>
       </c>
+      <c r="L24" t="s">
+        <v>144</v>
+      </c>
       <c r="M24" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="J25" t="s">
+        <v>134</v>
+      </c>
+      <c r="L25" t="s">
         <v>144</v>
       </c>
-      <c r="N24" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="K25" t="s">
-        <v>134</v>
-      </c>
       <c r="M25" t="s">
-        <v>144</v>
-      </c>
-      <c r="N25" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="J28" s="7" t="s">
+    <row r="28" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="I28" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="K28" s="53" t="s">
+      <c r="J28" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53" t="s">
+      <c r="K28" s="52"/>
+      <c r="L28" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="N28" s="53"/>
-      <c r="O28" s="53"/>
-      <c r="P28" s="53"/>
-      <c r="Q28" s="53"/>
-      <c r="R28" s="53"/>
-    </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="J29" s="28" t="s">
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="52"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="I29" s="28" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="K30" t="s">
+    <row r="30" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="J30" t="s">
         <v>135</v>
       </c>
-      <c r="M30" t="s">
+      <c r="L30" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.3">
-      <c r="K31" t="s">
+    <row r="31" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="J31" t="s">
         <v>136</v>
       </c>
-      <c r="M31" t="s">
+      <c r="L31" t="s">
         <v>150</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="O22:R22"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="M28:R28"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="O16:R16"/>
     <mergeCell ref="F9:G11"/>
     <mergeCell ref="F18:G20"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:Q28"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2303,20 +2313,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A222D11D-FBDB-42C8-93C4-B5D16645D996}">
   <dimension ref="A3:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.88671875" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="34.86328125" customWidth="1"/>
+    <col min="7" max="7" width="7.46484375" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
         <v>131</v>
       </c>
@@ -2324,10 +2334,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="27"/>
     </row>
-    <row r="5" spans="1:4" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" s="27" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="40" t="s">
         <v>151</v>
       </c>
@@ -2338,7 +2348,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" s="37" t="s">
         <v>13</v>
       </c>
@@ -2349,7 +2359,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
@@ -2360,7 +2370,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="33" t="s">
         <v>157</v>
       </c>
@@ -2371,7 +2381,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" s="33" t="s">
         <v>22</v>
       </c>
@@ -2382,7 +2392,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B10" s="33" t="s">
         <v>29</v>
       </c>
@@ -2393,7 +2403,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B11" s="33" t="s">
         <v>163</v>
       </c>
@@ -2404,7 +2414,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B12" s="33" t="s">
         <v>9</v>
       </c>
@@ -2415,7 +2425,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
@@ -2426,7 +2436,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B14" s="33" t="s">
         <v>39</v>
       </c>
@@ -2437,7 +2447,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B15" s="33" t="s">
         <v>46</v>
       </c>
@@ -2448,7 +2458,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B16" s="33" t="s">
         <v>48</v>
       </c>
@@ -2459,7 +2469,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B17" s="33" t="s">
         <v>176</v>
       </c>
@@ -2470,7 +2480,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B18" s="33" t="s">
         <v>4</v>
       </c>
@@ -2481,7 +2491,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B19" s="33" t="s">
         <v>14</v>
       </c>
@@ -2492,7 +2502,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B20" s="33" t="s">
         <v>15</v>
       </c>
@@ -2503,7 +2513,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B21" s="10" t="s">
         <v>101</v>
       </c>
@@ -2514,7 +2524,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="27" t="s">
         <v>135</v>
       </c>
@@ -2522,8 +2532,8 @@
         <v>186</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="25" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B25" s="40" t="s">
         <v>151</v>
       </c>
@@ -2532,7 +2542,7 @@
       </c>
       <c r="D25" s="42"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B26" s="37" t="s">
         <v>13</v>
       </c>
@@ -2541,7 +2551,7 @@
       </c>
       <c r="D26" s="39"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B27" s="33" t="s">
         <v>19</v>
       </c>
@@ -2550,7 +2560,7 @@
       </c>
       <c r="D27" s="34"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B28" s="33" t="s">
         <v>157</v>
       </c>
@@ -2559,7 +2569,7 @@
       </c>
       <c r="D28" s="34"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B29" s="33" t="s">
         <v>22</v>
       </c>
@@ -2568,7 +2578,7 @@
       </c>
       <c r="D29" s="34"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B30" s="33" t="s">
         <v>29</v>
       </c>
@@ -2577,7 +2587,7 @@
       </c>
       <c r="D30" s="34"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B31" s="33" t="s">
         <v>163</v>
       </c>
@@ -2586,7 +2596,7 @@
       </c>
       <c r="D31" s="34"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B32" s="33" t="s">
         <v>9</v>
       </c>
@@ -2595,7 +2605,7 @@
       </c>
       <c r="D32" s="34"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B33" s="33" t="s">
         <v>2</v>
       </c>
@@ -2604,7 +2614,7 @@
       </c>
       <c r="D33" s="34"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B34" s="33" t="s">
         <v>39</v>
       </c>
@@ -2613,7 +2623,7 @@
       </c>
       <c r="D34" s="34"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B35" s="33" t="s">
         <v>46</v>
       </c>
@@ -2622,7 +2632,7 @@
       </c>
       <c r="D35" s="34"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B36" s="33" t="s">
         <v>48</v>
       </c>
@@ -2631,7 +2641,7 @@
       </c>
       <c r="D36" s="34"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B37" s="33" t="s">
         <v>176</v>
       </c>
@@ -2640,7 +2650,7 @@
       </c>
       <c r="D37" s="34"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B38" s="33" t="s">
         <v>4</v>
       </c>
@@ -2649,7 +2659,7 @@
       </c>
       <c r="D38" s="34"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B39" s="33" t="s">
         <v>14</v>
       </c>
@@ -2658,7 +2668,7 @@
       </c>
       <c r="D39" s="34"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B40" s="33" t="s">
         <v>15</v>
       </c>
@@ -2667,7 +2677,7 @@
       </c>
       <c r="D40" s="34"/>
     </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B41" s="10" t="s">
         <v>101</v>
       </c>
@@ -2676,7 +2686,7 @@
       </c>
       <c r="D41" s="36"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="27" t="s">
         <v>232</v>
       </c>
@@ -2684,10 +2694,10 @@
         <v>231</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A45" s="27"/>
     </row>
-    <row r="46" spans="1:4" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" s="27" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B46" s="29" t="s">
         <v>151</v>
       </c>
@@ -2698,7 +2708,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B47" s="9" t="s">
         <v>13</v>
       </c>
@@ -2709,7 +2719,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B48" s="33" t="s">
         <v>19</v>
       </c>
@@ -2720,7 +2730,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B49" s="33" t="s">
         <v>157</v>
       </c>
@@ -2731,7 +2741,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B50" s="33" t="s">
         <v>22</v>
       </c>
@@ -2742,7 +2752,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B51" s="33" t="s">
         <v>29</v>
       </c>
@@ -2753,7 +2763,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B52" s="33" t="s">
         <v>163</v>
       </c>
@@ -2764,7 +2774,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B53" s="33" t="s">
         <v>9</v>
       </c>
@@ -2775,7 +2785,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B54" s="33" t="s">
         <v>2</v>
       </c>
@@ -2786,7 +2796,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B55" s="33" t="s">
         <v>39</v>
       </c>
@@ -2797,7 +2807,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B56" s="33" t="s">
         <v>46</v>
       </c>
@@ -2808,7 +2818,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B57" s="33" t="s">
         <v>48</v>
       </c>
@@ -2819,7 +2829,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B58" s="33" t="s">
         <v>176</v>
       </c>
@@ -2830,7 +2840,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B59" s="10" t="s">
         <v>229</v>
       </c>
@@ -2839,7 +2849,7 @@
       </c>
       <c r="D59" s="36"/>
     </row>
-    <row r="61" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A61" s="27" t="s">
         <v>233</v>
       </c>
@@ -2847,7 +2857,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B62" s="45" t="s">
         <v>151</v>
       </c>
@@ -2860,18 +2870,18 @@
       <c r="G62" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H62" s="52">
+      <c r="H62" s="54">
         <v>0</v>
       </c>
-      <c r="I62" s="52"/>
-      <c r="J62" s="52"/>
+      <c r="I62" s="54"/>
+      <c r="J62" s="54"/>
       <c r="K62" s="56"/>
       <c r="L62" s="57"/>
       <c r="M62" s="58"/>
       <c r="N62" s="58"/>
       <c r="O62" s="58"/>
     </row>
-    <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B63" s="37" t="s">
         <v>13</v>
       </c>
@@ -2901,7 +2911,7 @@
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
     </row>
-    <row r="64" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B64" s="10" t="s">
         <v>19</v>
       </c>
@@ -2912,7 +2922,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="66" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G66" s="27" t="s">
         <v>240</v>
       </c>
@@ -2922,17 +2932,17 @@
       <c r="I66" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="J66" s="53" t="s">
+      <c r="J66" s="52" t="s">
         <v>243</v>
       </c>
-      <c r="K66" s="53"/>
-    </row>
-    <row r="67" spans="7:11" x14ac:dyDescent="0.3">
+      <c r="K66" s="52"/>
+    </row>
+    <row r="67" spans="7:11" x14ac:dyDescent="0.45">
       <c r="G67" s="28" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="68" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="7:11" x14ac:dyDescent="0.45">
       <c r="H68" s="7" t="s">
         <v>242</v>
       </c>
@@ -2943,7 +2953,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="69" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:11" x14ac:dyDescent="0.45">
       <c r="H69" s="7" t="s">
         <v>241</v>
       </c>
@@ -2954,7 +2964,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="70" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="7:11" x14ac:dyDescent="0.45">
       <c r="H70" s="7" t="s">
         <v>243</v>
       </c>
@@ -2979,83 +2989,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43404EB-A4C0-4EEB-BCD6-93EC84295AA2}">
   <dimension ref="A2:AD82"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.21875" customWidth="1"/>
-    <col min="4" max="6" width="4.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.77734375" style="15" customWidth="1"/>
-    <col min="8" max="10" width="4.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="4.77734375" style="15" customWidth="1"/>
-    <col min="12" max="19" width="4.77734375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="2.109375" customWidth="1"/>
-    <col min="28" max="28" width="11.5546875" customWidth="1"/>
-    <col min="29" max="29" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="5.19921875" customWidth="1"/>
+    <col min="4" max="6" width="4.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.796875" style="15" customWidth="1"/>
+    <col min="8" max="10" width="4.796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="4.796875" style="15" customWidth="1"/>
+    <col min="12" max="19" width="4.796875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="2.1328125" customWidth="1"/>
+    <col min="28" max="28" width="11.53125" customWidth="1"/>
+    <col min="29" max="29" width="10.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="70" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="55">
         <v>0</v>
       </c>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52">
+      <c r="E7" s="54"/>
+      <c r="F7" s="54">
         <v>1</v>
       </c>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52">
+      <c r="G7" s="54"/>
+      <c r="H7" s="54">
         <v>2</v>
       </c>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52">
+      <c r="I7" s="54"/>
+      <c r="J7" s="54">
         <v>3</v>
       </c>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52">
+      <c r="K7" s="54"/>
+      <c r="L7" s="54">
         <v>4</v>
       </c>
-      <c r="M7" s="52"/>
-      <c r="N7" s="52">
+      <c r="M7" s="54"/>
+      <c r="N7" s="54">
         <v>5</v>
       </c>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52">
+      <c r="O7" s="54"/>
+      <c r="P7" s="54">
         <v>6</v>
       </c>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52">
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54">
         <v>7</v>
       </c>
-      <c r="S7" s="85"/>
-    </row>
-    <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S7" s="69"/>
+    </row>
+    <row r="8" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="87"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="4">
         <v>0</v>
       </c>
@@ -3105,15 +3115,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>94</v>
       </c>
@@ -3124,7 +3134,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>95</v>
       </c>
@@ -3135,7 +3145,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>96</v>
       </c>
@@ -3146,10 +3156,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -3162,17 +3172,17 @@
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="54" t="s">
+      <c r="U15" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="V15" s="54"/>
-      <c r="W15" s="54"/>
-      <c r="X15" s="54"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="53"/>
       <c r="AA15" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="C16" s="7">
         <v>2</v>
       </c>
@@ -3188,15 +3198,15 @@
       <c r="G16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U16" s="54"/>
-      <c r="V16" s="54"/>
-      <c r="W16" s="54"/>
-      <c r="X16" s="54"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="53"/>
+      <c r="W16" s="53"/>
+      <c r="X16" s="53"/>
       <c r="AA16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C17" s="7">
         <v>4</v>
       </c>
@@ -3224,15 +3234,15 @@
       <c r="K17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="54"/>
-      <c r="V17" s="54"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="54"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
       <c r="AA17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C18" s="7">
         <v>8</v>
       </c>
@@ -3284,17 +3294,17 @@
       <c r="S18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="54"/>
-      <c r="V18" s="54"/>
-      <c r="W18" s="54"/>
-      <c r="X18" s="54"/>
-    </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -3307,14 +3317,14 @@
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U21" s="54" t="s">
+      <c r="U21" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="V21" s="54"/>
-      <c r="W21" s="54"/>
-      <c r="X21" s="54"/>
-    </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V21" s="53"/>
+      <c r="W21" s="53"/>
+      <c r="X21" s="53"/>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C22" s="7">
         <v>2</v>
       </c>
@@ -3330,26 +3340,26 @@
       <c r="G22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="67" t="s">
+      <c r="H22" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="68"/>
-      <c r="O22" s="68"/>
-      <c r="P22" s="68"/>
-      <c r="Q22" s="68"/>
-      <c r="R22" s="68"/>
-      <c r="S22" s="68"/>
-      <c r="U22" s="54"/>
-      <c r="V22" s="54"/>
-      <c r="W22" s="54"/>
-      <c r="X22" s="54"/>
-    </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="59"/>
+      <c r="U22" s="53"/>
+      <c r="V22" s="53"/>
+      <c r="W22" s="53"/>
+      <c r="X22" s="53"/>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C23" s="7">
         <v>4</v>
       </c>
@@ -3362,19 +3372,19 @@
       <c r="F23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="59" t="s">
+      <c r="G23" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="88"/>
-      <c r="I23" s="88"/>
-      <c r="J23" s="88"/>
-      <c r="K23" s="60"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="54"/>
-      <c r="W23" s="54"/>
-      <c r="X23" s="54"/>
-    </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="61"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="53"/>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C24" s="7">
         <v>8</v>
       </c>
@@ -3387,13 +3397,13 @@
       <c r="F24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="59" t="s">
+      <c r="G24" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="88"/>
-      <c r="K24" s="60"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="61"/>
       <c r="L24" s="3" t="s">
         <v>16</v>
       </c>
@@ -3418,34 +3428,34 @@
       <c r="S24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U24" s="54"/>
-      <c r="V24" s="54"/>
-      <c r="W24" s="54"/>
-      <c r="X24" s="54"/>
-    </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="U24" s="53"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
+      <c r="X24" s="53"/>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
-      <c r="M26" s="68"/>
-      <c r="N26" s="68"/>
-      <c r="O26" s="68"/>
-      <c r="P26" s="68"/>
-      <c r="Q26" s="68"/>
-      <c r="R26" s="68"/>
-      <c r="S26" s="68"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
       <c r="U26" s="58" t="s">
         <v>55</v>
       </c>
@@ -3453,7 +3463,7 @@
       <c r="W26" s="58"/>
       <c r="X26" s="58"/>
     </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>21</v>
       </c>
@@ -3466,18 +3476,18 @@
       <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U28" s="64" t="s">
+      <c r="U28" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="V28" s="65"/>
-      <c r="W28" s="65"/>
-      <c r="X28" s="65"/>
+      <c r="V28" s="73"/>
+      <c r="W28" s="73"/>
+      <c r="X28" s="73"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
       <c r="AB28" s="19"/>
     </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C29" s="7">
         <v>2</v>
       </c>
@@ -3493,15 +3503,15 @@
       <c r="G29" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="67" t="s">
+      <c r="U29" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="V29" s="68"/>
-      <c r="W29" s="68"/>
-      <c r="X29" s="68"/>
+      <c r="V29" s="59"/>
+      <c r="W29" s="59"/>
+      <c r="X29" s="59"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C30" s="7">
         <v>4</v>
       </c>
@@ -3514,27 +3524,27 @@
       <c r="F30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="53" t="s">
+      <c r="G30" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="53"/>
-      <c r="I30" s="89" t="s">
+      <c r="H30" s="52"/>
+      <c r="I30" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="89"/>
-      <c r="K30" s="89"/>
-      <c r="U30" s="67" t="s">
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="U30" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="V30" s="68"/>
-      <c r="W30" s="68"/>
-      <c r="X30" s="68"/>
-      <c r="Y30" s="68"/>
-      <c r="Z30" s="68"/>
-      <c r="AA30" s="68"/>
-      <c r="AB30" s="69"/>
-    </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V30" s="59"/>
+      <c r="W30" s="59"/>
+      <c r="X30" s="59"/>
+      <c r="Y30" s="59"/>
+      <c r="Z30" s="59"/>
+      <c r="AA30" s="59"/>
+      <c r="AB30" s="65"/>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C31" s="7">
         <v>8</v>
       </c>
@@ -3547,65 +3557,65 @@
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="53" t="s">
+      <c r="G31" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53" t="s">
+      <c r="H31" s="52"/>
+      <c r="I31" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="53"/>
-      <c r="K31" s="53"/>
-      <c r="L31" s="53"/>
-      <c r="M31" s="53"/>
-      <c r="N31" s="53"/>
-      <c r="O31" s="53"/>
-      <c r="P31" s="53"/>
-      <c r="Q31" s="53"/>
-      <c r="R31" s="53"/>
-      <c r="S31" s="53"/>
-      <c r="U31" s="61" t="s">
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="52"/>
+      <c r="O31" s="52"/>
+      <c r="P31" s="52"/>
+      <c r="Q31" s="52"/>
+      <c r="R31" s="52"/>
+      <c r="S31" s="52"/>
+      <c r="U31" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="V31" s="62"/>
-      <c r="W31" s="62"/>
-      <c r="X31" s="62"/>
-      <c r="Y31" s="62"/>
-      <c r="Z31" s="62"/>
-      <c r="AA31" s="62"/>
-      <c r="AB31" s="63"/>
-    </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V31" s="67"/>
+      <c r="W31" s="67"/>
+      <c r="X31" s="67"/>
+      <c r="Y31" s="67"/>
+      <c r="Z31" s="67"/>
+      <c r="AA31" s="67"/>
+      <c r="AB31" s="68"/>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="68" t="s">
+      <c r="C33" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="68"/>
-      <c r="M33" s="68"/>
-      <c r="N33" s="68"/>
-      <c r="O33" s="68"/>
-      <c r="P33" s="68"/>
-      <c r="Q33" s="68"/>
-      <c r="R33" s="68"/>
-      <c r="S33" s="68"/>
-      <c r="U33" s="76" t="s">
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="59"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="59"/>
+      <c r="P33" s="59"/>
+      <c r="Q33" s="59"/>
+      <c r="R33" s="59"/>
+      <c r="S33" s="59"/>
+      <c r="U33" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="V33" s="77"/>
-      <c r="W33" s="77"/>
-      <c r="X33" s="78"/>
-    </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V33" s="81"/>
+      <c r="W33" s="81"/>
+      <c r="X33" s="82"/>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>27</v>
       </c>
@@ -3618,18 +3628,18 @@
       <c r="E35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="U35" s="64" t="s">
+      <c r="U35" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="V35" s="65"/>
-      <c r="W35" s="65"/>
-      <c r="X35" s="65"/>
+      <c r="V35" s="73"/>
+      <c r="W35" s="73"/>
+      <c r="X35" s="73"/>
       <c r="Y35" s="18"/>
       <c r="Z35" s="18"/>
       <c r="AA35" s="18"/>
       <c r="AB35" s="19"/>
     </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C36" s="7">
         <v>2</v>
       </c>
@@ -3645,15 +3655,15 @@
       <c r="G36" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U36" s="67" t="s">
+      <c r="U36" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="V36" s="68"/>
-      <c r="W36" s="68"/>
-      <c r="X36" s="68"/>
+      <c r="V36" s="59"/>
+      <c r="W36" s="59"/>
+      <c r="X36" s="59"/>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C37" s="7">
         <v>4</v>
       </c>
@@ -3666,27 +3676,27 @@
       <c r="F37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="53" t="s">
+      <c r="G37" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H37" s="53"/>
-      <c r="I37" s="89" t="s">
+      <c r="H37" s="52"/>
+      <c r="I37" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="89"/>
-      <c r="K37" s="89"/>
-      <c r="U37" s="67" t="s">
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
+      <c r="U37" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="V37" s="68"/>
-      <c r="W37" s="68"/>
-      <c r="X37" s="68"/>
-      <c r="Y37" s="68"/>
-      <c r="Z37" s="68"/>
-      <c r="AA37" s="68"/>
-      <c r="AB37" s="69"/>
-    </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V37" s="59"/>
+      <c r="W37" s="59"/>
+      <c r="X37" s="59"/>
+      <c r="Y37" s="59"/>
+      <c r="Z37" s="59"/>
+      <c r="AA37" s="59"/>
+      <c r="AB37" s="65"/>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C38" s="7">
         <v>8</v>
       </c>
@@ -3699,15 +3709,15 @@
       <c r="F38" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G38" s="53" t="s">
+      <c r="G38" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H38" s="53"/>
-      <c r="I38" s="59" t="s">
+      <c r="H38" s="52"/>
+      <c r="I38" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="J38" s="88"/>
-      <c r="K38" s="60"/>
+      <c r="J38" s="62"/>
+      <c r="K38" s="61"/>
       <c r="L38" s="3" t="s">
         <v>16</v>
       </c>
@@ -3732,18 +3742,18 @@
       <c r="S38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U38" s="61" t="s">
+      <c r="U38" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="V38" s="62"/>
-      <c r="W38" s="62"/>
-      <c r="X38" s="62"/>
-      <c r="Y38" s="62"/>
-      <c r="Z38" s="62"/>
-      <c r="AA38" s="62"/>
-      <c r="AB38" s="63"/>
-    </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V38" s="67"/>
+      <c r="W38" s="67"/>
+      <c r="X38" s="67"/>
+      <c r="Y38" s="67"/>
+      <c r="Z38" s="67"/>
+      <c r="AA38" s="67"/>
+      <c r="AB38" s="68"/>
+    </row>
+    <row r="40" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>30</v>
       </c>
@@ -3756,14 +3766,14 @@
       <c r="E40" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U40" s="79" t="s">
+      <c r="U40" s="74" t="s">
         <v>68</v>
       </c>
-      <c r="V40" s="80"/>
-      <c r="W40" s="80"/>
-      <c r="X40" s="81"/>
-    </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V40" s="75"/>
+      <c r="W40" s="75"/>
+      <c r="X40" s="76"/>
+    </row>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C41" s="7">
         <v>2</v>
       </c>
@@ -3773,49 +3783,49 @@
       <c r="E41" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F41" s="59" t="s">
+      <c r="F41" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="G41" s="60"/>
-      <c r="U41" s="82"/>
-      <c r="V41" s="83"/>
-      <c r="W41" s="83"/>
-      <c r="X41" s="84"/>
-    </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="G41" s="61"/>
+      <c r="U41" s="77"/>
+      <c r="V41" s="78"/>
+      <c r="W41" s="78"/>
+      <c r="X41" s="79"/>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="68" t="s">
+      <c r="C43" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="68"/>
-      <c r="J43" s="68"/>
-      <c r="K43" s="68"/>
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="68"/>
-      <c r="O43" s="68"/>
-      <c r="P43" s="68"/>
-      <c r="Q43" s="68"/>
-      <c r="R43" s="68"/>
-      <c r="S43" s="68"/>
-      <c r="U43" s="76" t="s">
+      <c r="D43" s="59"/>
+      <c r="E43" s="59"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="59"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="59"/>
+      <c r="J43" s="59"/>
+      <c r="K43" s="59"/>
+      <c r="L43" s="59"/>
+      <c r="M43" s="59"/>
+      <c r="N43" s="59"/>
+      <c r="O43" s="59"/>
+      <c r="P43" s="59"/>
+      <c r="Q43" s="59"/>
+      <c r="R43" s="59"/>
+      <c r="S43" s="59"/>
+      <c r="U43" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="V43" s="77"/>
-      <c r="W43" s="77"/>
-      <c r="X43" s="78"/>
-    </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V43" s="81"/>
+      <c r="W43" s="81"/>
+      <c r="X43" s="82"/>
+    </row>
+    <row r="44" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C44" s="12"/>
     </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B45" t="s">
         <v>33</v>
       </c>
@@ -3839,7 +3849,7 @@
       <c r="AA45" s="18"/>
       <c r="AB45" s="19"/>
     </row>
-    <row r="46" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C46" s="7">
         <v>2</v>
       </c>
@@ -3860,7 +3870,7 @@
       </c>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C47" s="7">
         <v>4</v>
       </c>
@@ -3870,22 +3880,22 @@
       <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="53" t="s">
+      <c r="F47" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="53"/>
-      <c r="H47" s="89" t="s">
+      <c r="G47" s="52"/>
+      <c r="H47" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="89"/>
-      <c r="J47" s="89"/>
-      <c r="K47" s="89"/>
+      <c r="I47" s="63"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
       <c r="U47" s="22" t="s">
         <v>70</v>
       </c>
       <c r="AB47" s="20"/>
     </row>
-    <row r="48" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C48" s="11">
         <v>8</v>
       </c>
@@ -3895,24 +3905,24 @@
       <c r="E48" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F48" s="53" t="s">
+      <c r="F48" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G48" s="53"/>
-      <c r="H48" s="53" t="s">
+      <c r="G48" s="52"/>
+      <c r="H48" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="I48" s="53"/>
-      <c r="J48" s="53"/>
-      <c r="K48" s="53"/>
-      <c r="L48" s="53"/>
-      <c r="M48" s="53"/>
-      <c r="N48" s="53"/>
-      <c r="O48" s="53"/>
-      <c r="P48" s="53"/>
-      <c r="Q48" s="53"/>
-      <c r="R48" s="53"/>
-      <c r="S48" s="53"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+      <c r="K48" s="52"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="52"/>
+      <c r="P48" s="52"/>
+      <c r="Q48" s="52"/>
+      <c r="R48" s="52"/>
+      <c r="S48" s="52"/>
       <c r="U48" s="23" t="s">
         <v>69</v>
       </c>
@@ -3924,7 +3934,7 @@
       <c r="AA48" s="24"/>
       <c r="AB48" s="25"/>
     </row>
-    <row r="50" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
         <v>34</v>
       </c>
@@ -3937,19 +3947,19 @@
       <c r="E50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U50" s="64" t="s">
+      <c r="U50" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="V50" s="65"/>
-      <c r="W50" s="65"/>
-      <c r="X50" s="65"/>
-      <c r="Y50" s="65"/>
-      <c r="Z50" s="65"/>
-      <c r="AA50" s="65"/>
-      <c r="AB50" s="65"/>
-      <c r="AC50" s="66"/>
-    </row>
-    <row r="51" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V50" s="73"/>
+      <c r="W50" s="73"/>
+      <c r="X50" s="73"/>
+      <c r="Y50" s="73"/>
+      <c r="Z50" s="73"/>
+      <c r="AA50" s="73"/>
+      <c r="AB50" s="73"/>
+      <c r="AC50" s="83"/>
+    </row>
+    <row r="51" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C51" s="7">
         <v>2</v>
       </c>
@@ -3965,19 +3975,19 @@
       <c r="G51" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U51" s="67" t="s">
+      <c r="U51" s="64" t="s">
         <v>74</v>
       </c>
-      <c r="V51" s="68"/>
-      <c r="W51" s="68"/>
-      <c r="X51" s="68"/>
-      <c r="Y51" s="68"/>
-      <c r="Z51" s="68"/>
-      <c r="AA51" s="68"/>
-      <c r="AB51" s="68"/>
-      <c r="AC51" s="69"/>
-    </row>
-    <row r="52" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V51" s="59"/>
+      <c r="W51" s="59"/>
+      <c r="X51" s="59"/>
+      <c r="Y51" s="59"/>
+      <c r="Z51" s="59"/>
+      <c r="AA51" s="59"/>
+      <c r="AB51" s="59"/>
+      <c r="AC51" s="65"/>
+    </row>
+    <row r="52" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C52" s="7">
         <v>4</v>
       </c>
@@ -3987,29 +3997,29 @@
       <c r="E52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="53" t="s">
+      <c r="F52" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="53"/>
-      <c r="H52" s="89" t="s">
+      <c r="G52" s="52"/>
+      <c r="H52" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="89"/>
-      <c r="J52" s="89"/>
-      <c r="K52" s="89"/>
-      <c r="U52" s="67" t="s">
+      <c r="I52" s="63"/>
+      <c r="J52" s="63"/>
+      <c r="K52" s="63"/>
+      <c r="U52" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="V52" s="68"/>
-      <c r="W52" s="68"/>
-      <c r="X52" s="68"/>
-      <c r="Y52" s="68"/>
-      <c r="Z52" s="68"/>
-      <c r="AA52" s="68"/>
-      <c r="AB52" s="68"/>
-      <c r="AC52" s="69"/>
-    </row>
-    <row r="53" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V52" s="59"/>
+      <c r="W52" s="59"/>
+      <c r="X52" s="59"/>
+      <c r="Y52" s="59"/>
+      <c r="Z52" s="59"/>
+      <c r="AA52" s="59"/>
+      <c r="AB52" s="59"/>
+      <c r="AC52" s="65"/>
+    </row>
+    <row r="53" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C53" s="11">
         <v>8</v>
       </c>
@@ -4019,72 +4029,72 @@
       <c r="E53" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F53" s="53" t="s">
+      <c r="F53" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="G53" s="53"/>
-      <c r="H53" s="53" t="s">
+      <c r="G53" s="52"/>
+      <c r="H53" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="53"/>
-      <c r="J53" s="53"/>
-      <c r="K53" s="53"/>
-      <c r="L53" s="53"/>
-      <c r="M53" s="53"/>
-      <c r="N53" s="53"/>
-      <c r="O53" s="53"/>
-      <c r="P53" s="53"/>
-      <c r="Q53" s="53"/>
-      <c r="R53" s="53"/>
-      <c r="S53" s="53"/>
-      <c r="U53" s="61" t="s">
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="K53" s="52"/>
+      <c r="L53" s="52"/>
+      <c r="M53" s="52"/>
+      <c r="N53" s="52"/>
+      <c r="O53" s="52"/>
+      <c r="P53" s="52"/>
+      <c r="Q53" s="52"/>
+      <c r="R53" s="52"/>
+      <c r="S53" s="52"/>
+      <c r="U53" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="V53" s="62"/>
-      <c r="W53" s="62"/>
-      <c r="X53" s="62"/>
-      <c r="Y53" s="62"/>
-      <c r="Z53" s="62"/>
-      <c r="AA53" s="62"/>
-      <c r="AB53" s="62"/>
-      <c r="AC53" s="63"/>
-    </row>
-    <row r="55" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V53" s="67"/>
+      <c r="W53" s="67"/>
+      <c r="X53" s="67"/>
+      <c r="Y53" s="67"/>
+      <c r="Z53" s="67"/>
+      <c r="AA53" s="67"/>
+      <c r="AB53" s="67"/>
+      <c r="AC53" s="68"/>
+    </row>
+    <row r="55" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
         <v>36</v>
       </c>
-      <c r="C55" s="68" t="s">
+      <c r="C55" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="D55" s="68"/>
-      <c r="E55" s="68"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="68"/>
-      <c r="J55" s="68"/>
-      <c r="K55" s="68"/>
-      <c r="L55" s="68"/>
-      <c r="M55" s="68"/>
-      <c r="N55" s="68"/>
-      <c r="O55" s="68"/>
-      <c r="P55" s="68"/>
-      <c r="Q55" s="68"/>
-      <c r="R55" s="68"/>
-      <c r="S55" s="68"/>
-      <c r="U55" s="76" t="s">
+      <c r="D55" s="59"/>
+      <c r="E55" s="59"/>
+      <c r="F55" s="59"/>
+      <c r="G55" s="59"/>
+      <c r="H55" s="59"/>
+      <c r="I55" s="59"/>
+      <c r="J55" s="59"/>
+      <c r="K55" s="59"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="59"/>
+      <c r="N55" s="59"/>
+      <c r="O55" s="59"/>
+      <c r="P55" s="59"/>
+      <c r="Q55" s="59"/>
+      <c r="R55" s="59"/>
+      <c r="S55" s="59"/>
+      <c r="U55" s="80" t="s">
         <v>78</v>
       </c>
-      <c r="V55" s="77"/>
-      <c r="W55" s="77"/>
-      <c r="X55" s="77"/>
-      <c r="Y55" s="77"/>
-      <c r="Z55" s="77"/>
-      <c r="AA55" s="77"/>
-      <c r="AB55" s="77"/>
-      <c r="AC55" s="78"/>
-    </row>
-    <row r="57" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V55" s="81"/>
+      <c r="W55" s="81"/>
+      <c r="X55" s="81"/>
+      <c r="Y55" s="81"/>
+      <c r="Z55" s="81"/>
+      <c r="AA55" s="81"/>
+      <c r="AB55" s="81"/>
+      <c r="AC55" s="82"/>
+    </row>
+    <row r="57" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
         <v>8</v>
       </c>
@@ -4097,19 +4107,19 @@
       <c r="E57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U57" s="64" t="s">
+      <c r="U57" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="V57" s="65"/>
-      <c r="W57" s="65"/>
-      <c r="X57" s="65"/>
-      <c r="Y57" s="65"/>
-      <c r="Z57" s="65"/>
-      <c r="AA57" s="65"/>
-      <c r="AB57" s="65"/>
-      <c r="AC57" s="66"/>
-    </row>
-    <row r="58" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V57" s="73"/>
+      <c r="W57" s="73"/>
+      <c r="X57" s="73"/>
+      <c r="Y57" s="73"/>
+      <c r="Z57" s="73"/>
+      <c r="AA57" s="73"/>
+      <c r="AB57" s="73"/>
+      <c r="AC57" s="83"/>
+    </row>
+    <row r="58" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C58" s="7">
         <v>2</v>
       </c>
@@ -4119,23 +4129,23 @@
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="59" t="s">
+      <c r="F58" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="G58" s="60"/>
-      <c r="U58" s="67" t="s">
+      <c r="G58" s="61"/>
+      <c r="U58" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="V58" s="68"/>
-      <c r="W58" s="68"/>
-      <c r="X58" s="68"/>
-      <c r="Y58" s="68"/>
-      <c r="Z58" s="68"/>
-      <c r="AA58" s="68"/>
-      <c r="AB58" s="68"/>
-      <c r="AC58" s="69"/>
-    </row>
-    <row r="59" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V58" s="59"/>
+      <c r="W58" s="59"/>
+      <c r="X58" s="59"/>
+      <c r="Y58" s="59"/>
+      <c r="Z58" s="59"/>
+      <c r="AA58" s="59"/>
+      <c r="AB58" s="59"/>
+      <c r="AC58" s="65"/>
+    </row>
+    <row r="59" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C59" s="7">
         <v>4</v>
       </c>
@@ -4145,27 +4155,27 @@
       <c r="E59" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F59" s="53" t="s">
+      <c r="F59" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G59" s="53"/>
-      <c r="H59" s="53" t="s">
+      <c r="G59" s="52"/>
+      <c r="H59" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="I59" s="53"/>
-      <c r="U59" s="61" t="s">
+      <c r="I59" s="52"/>
+      <c r="U59" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="V59" s="62"/>
-      <c r="W59" s="62"/>
-      <c r="X59" s="62"/>
-      <c r="Y59" s="62"/>
-      <c r="Z59" s="62"/>
-      <c r="AA59" s="62"/>
-      <c r="AB59" s="62"/>
-      <c r="AC59" s="63"/>
-    </row>
-    <row r="61" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V59" s="67"/>
+      <c r="W59" s="67"/>
+      <c r="X59" s="67"/>
+      <c r="Y59" s="67"/>
+      <c r="Z59" s="67"/>
+      <c r="AA59" s="67"/>
+      <c r="AB59" s="67"/>
+      <c r="AC59" s="68"/>
+    </row>
+    <row r="61" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B61" t="s">
         <v>0</v>
       </c>
@@ -4190,7 +4200,7 @@
       <c r="AB61" s="18"/>
       <c r="AC61" s="19"/>
     </row>
-    <row r="62" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C62" s="7">
         <v>2</v>
       </c>
@@ -4200,23 +4210,23 @@
       <c r="E62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="59" t="s">
+      <c r="F62" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="60"/>
-      <c r="U62" s="67" t="s">
+      <c r="G62" s="61"/>
+      <c r="U62" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="V62" s="68"/>
-      <c r="W62" s="68"/>
-      <c r="X62" s="68"/>
-      <c r="Y62" s="68"/>
-      <c r="Z62" s="68"/>
-      <c r="AA62" s="68"/>
-      <c r="AB62" s="68"/>
-      <c r="AC62" s="69"/>
-    </row>
-    <row r="63" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V62" s="59"/>
+      <c r="W62" s="59"/>
+      <c r="X62" s="59"/>
+      <c r="Y62" s="59"/>
+      <c r="Z62" s="59"/>
+      <c r="AA62" s="59"/>
+      <c r="AB62" s="59"/>
+      <c r="AC62" s="65"/>
+    </row>
+    <row r="63" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C63" s="7">
         <v>4</v>
       </c>
@@ -4226,53 +4236,53 @@
       <c r="E63" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="53" t="s">
+      <c r="F63" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G63" s="53"/>
-      <c r="H63" s="53" t="s">
+      <c r="G63" s="52"/>
+      <c r="H63" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="I63" s="53"/>
-      <c r="J63" s="53" t="s">
+      <c r="I63" s="52"/>
+      <c r="J63" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="K63" s="53"/>
-      <c r="U63" s="70" t="s">
+      <c r="K63" s="52"/>
+      <c r="U63" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="V63" s="71"/>
-      <c r="W63" s="71"/>
-      <c r="X63" s="71"/>
-      <c r="Y63" s="71"/>
-      <c r="Z63" s="71"/>
-      <c r="AA63" s="71"/>
-      <c r="AB63" s="71"/>
-      <c r="AC63" s="72"/>
-    </row>
-    <row r="64" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="U64" s="70"/>
-      <c r="V64" s="71"/>
-      <c r="W64" s="71"/>
-      <c r="X64" s="71"/>
-      <c r="Y64" s="71"/>
-      <c r="Z64" s="71"/>
-      <c r="AA64" s="71"/>
-      <c r="AB64" s="71"/>
-      <c r="AC64" s="72"/>
-    </row>
-    <row r="65" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="U65" s="73"/>
-      <c r="V65" s="74"/>
-      <c r="W65" s="74"/>
-      <c r="X65" s="74"/>
-      <c r="Y65" s="74"/>
-      <c r="Z65" s="74"/>
-      <c r="AA65" s="74"/>
-      <c r="AB65" s="74"/>
-      <c r="AC65" s="75"/>
-    </row>
-    <row r="66" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="V63" s="85"/>
+      <c r="W63" s="85"/>
+      <c r="X63" s="85"/>
+      <c r="Y63" s="85"/>
+      <c r="Z63" s="85"/>
+      <c r="AA63" s="85"/>
+      <c r="AB63" s="85"/>
+      <c r="AC63" s="86"/>
+    </row>
+    <row r="64" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="U64" s="84"/>
+      <c r="V64" s="85"/>
+      <c r="W64" s="85"/>
+      <c r="X64" s="85"/>
+      <c r="Y64" s="85"/>
+      <c r="Z64" s="85"/>
+      <c r="AA64" s="85"/>
+      <c r="AB64" s="85"/>
+      <c r="AC64" s="86"/>
+    </row>
+    <row r="65" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="U65" s="87"/>
+      <c r="V65" s="88"/>
+      <c r="W65" s="88"/>
+      <c r="X65" s="88"/>
+      <c r="Y65" s="88"/>
+      <c r="Z65" s="88"/>
+      <c r="AA65" s="88"/>
+      <c r="AB65" s="88"/>
+      <c r="AC65" s="89"/>
+    </row>
+    <row r="66" spans="2:30" x14ac:dyDescent="0.45">
       <c r="U66" s="26"/>
       <c r="V66" s="26"/>
       <c r="W66" s="26"/>
@@ -4283,7 +4293,7 @@
       <c r="AB66" s="26"/>
       <c r="AC66" s="26"/>
     </row>
-    <row r="67" spans="2:30" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:30" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
         <v>38</v>
       </c>
@@ -4296,20 +4306,20 @@
       <c r="E67" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U67" s="64" t="s">
+      <c r="U67" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="V67" s="65"/>
-      <c r="W67" s="65"/>
-      <c r="X67" s="65"/>
-      <c r="Y67" s="65"/>
-      <c r="Z67" s="65"/>
-      <c r="AA67" s="65"/>
-      <c r="AB67" s="65"/>
-      <c r="AC67" s="65"/>
-      <c r="AD67" s="66"/>
-    </row>
-    <row r="68" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="V67" s="73"/>
+      <c r="W67" s="73"/>
+      <c r="X67" s="73"/>
+      <c r="Y67" s="73"/>
+      <c r="Z67" s="73"/>
+      <c r="AA67" s="73"/>
+      <c r="AB67" s="73"/>
+      <c r="AC67" s="73"/>
+      <c r="AD67" s="83"/>
+    </row>
+    <row r="68" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C68" s="7">
         <v>2</v>
       </c>
@@ -4325,20 +4335,20 @@
       <c r="G68" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U68" s="67" t="s">
+      <c r="U68" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="V68" s="68"/>
-      <c r="W68" s="68"/>
-      <c r="X68" s="68"/>
-      <c r="Y68" s="68"/>
-      <c r="Z68" s="68"/>
-      <c r="AA68" s="68"/>
-      <c r="AB68" s="68"/>
-      <c r="AC68" s="68"/>
-      <c r="AD68" s="69"/>
-    </row>
-    <row r="69" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="V68" s="59"/>
+      <c r="W68" s="59"/>
+      <c r="X68" s="59"/>
+      <c r="Y68" s="59"/>
+      <c r="Z68" s="59"/>
+      <c r="AA68" s="59"/>
+      <c r="AB68" s="59"/>
+      <c r="AC68" s="59"/>
+      <c r="AD68" s="65"/>
+    </row>
+    <row r="69" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C69" s="7">
         <v>4</v>
       </c>
@@ -4360,24 +4370,24 @@
       <c r="I69" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J69" s="59" t="s">
+      <c r="J69" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="K69" s="60"/>
-      <c r="U69" s="67" t="s">
+      <c r="K69" s="61"/>
+      <c r="U69" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="V69" s="68"/>
-      <c r="W69" s="68"/>
-      <c r="X69" s="68"/>
-      <c r="Y69" s="68"/>
-      <c r="Z69" s="68"/>
-      <c r="AA69" s="68"/>
-      <c r="AB69" s="68"/>
-      <c r="AC69" s="68"/>
-      <c r="AD69" s="69"/>
-    </row>
-    <row r="70" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="V69" s="59"/>
+      <c r="W69" s="59"/>
+      <c r="X69" s="59"/>
+      <c r="Y69" s="59"/>
+      <c r="Z69" s="59"/>
+      <c r="AA69" s="59"/>
+      <c r="AB69" s="59"/>
+      <c r="AC69" s="59"/>
+      <c r="AD69" s="65"/>
+    </row>
+    <row r="70" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C70" s="11">
         <v>8</v>
       </c>
@@ -4387,46 +4397,46 @@
       <c r="E70" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F70" s="53" t="s">
+      <c r="F70" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="53"/>
-      <c r="H70" s="59" t="s">
+      <c r="G70" s="52"/>
+      <c r="H70" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="I70" s="60"/>
-      <c r="J70" s="59" t="s">
+      <c r="I70" s="61"/>
+      <c r="J70" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="K70" s="60"/>
-      <c r="L70" s="59" t="s">
+      <c r="K70" s="61"/>
+      <c r="L70" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M70" s="60"/>
-      <c r="N70" s="59" t="s">
+      <c r="M70" s="61"/>
+      <c r="N70" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="O70" s="60"/>
-      <c r="P70" s="59" t="s">
+      <c r="O70" s="61"/>
+      <c r="P70" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="Q70" s="88"/>
-      <c r="R70" s="88"/>
-      <c r="S70" s="60"/>
-      <c r="U70" s="61" t="s">
+      <c r="Q70" s="62"/>
+      <c r="R70" s="62"/>
+      <c r="S70" s="61"/>
+      <c r="U70" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="V70" s="62"/>
-      <c r="W70" s="62"/>
-      <c r="X70" s="62"/>
-      <c r="Y70" s="62"/>
-      <c r="Z70" s="62"/>
-      <c r="AA70" s="62"/>
-      <c r="AB70" s="62"/>
-      <c r="AC70" s="62"/>
-      <c r="AD70" s="63"/>
-    </row>
-    <row r="72" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="V70" s="67"/>
+      <c r="W70" s="67"/>
+      <c r="X70" s="67"/>
+      <c r="Y70" s="67"/>
+      <c r="Z70" s="67"/>
+      <c r="AA70" s="67"/>
+      <c r="AB70" s="67"/>
+      <c r="AC70" s="67"/>
+      <c r="AD70" s="68"/>
+    </row>
+    <row r="72" spans="2:30" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
         <v>45</v>
       </c>
@@ -4439,15 +4449,15 @@
       <c r="E72" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U72" s="64" t="s">
+      <c r="U72" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="V72" s="65"/>
-      <c r="W72" s="65"/>
-      <c r="X72" s="65"/>
-      <c r="Y72" s="66"/>
-    </row>
-    <row r="73" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="V72" s="73"/>
+      <c r="W72" s="73"/>
+      <c r="X72" s="73"/>
+      <c r="Y72" s="83"/>
+    </row>
+    <row r="73" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C73" s="7">
         <v>2</v>
       </c>
@@ -4457,19 +4467,19 @@
       <c r="E73" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F73" s="59" t="s">
+      <c r="F73" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="G73" s="60"/>
-      <c r="U73" s="61" t="s">
+      <c r="G73" s="61"/>
+      <c r="U73" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="V73" s="62"/>
-      <c r="W73" s="62"/>
-      <c r="X73" s="62"/>
-      <c r="Y73" s="63"/>
-    </row>
-    <row r="75" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="V73" s="67"/>
+      <c r="W73" s="67"/>
+      <c r="X73" s="67"/>
+      <c r="Y73" s="68"/>
+    </row>
+    <row r="75" spans="2:30" x14ac:dyDescent="0.45">
       <c r="B75" t="s">
         <v>47</v>
       </c>
@@ -4482,20 +4492,20 @@
       <c r="E75" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U75" s="64" t="s">
+      <c r="U75" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="V75" s="65"/>
-      <c r="W75" s="65"/>
-      <c r="X75" s="65"/>
-      <c r="Y75" s="65"/>
-      <c r="Z75" s="65"/>
-      <c r="AA75" s="65"/>
-      <c r="AB75" s="65"/>
-      <c r="AC75" s="65"/>
-      <c r="AD75" s="66"/>
-    </row>
-    <row r="76" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="V75" s="73"/>
+      <c r="W75" s="73"/>
+      <c r="X75" s="73"/>
+      <c r="Y75" s="73"/>
+      <c r="Z75" s="73"/>
+      <c r="AA75" s="73"/>
+      <c r="AB75" s="73"/>
+      <c r="AC75" s="73"/>
+      <c r="AD75" s="83"/>
+    </row>
+    <row r="76" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C76" s="7">
         <v>2</v>
       </c>
@@ -4505,24 +4515,24 @@
       <c r="E76" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F76" s="59" t="s">
+      <c r="F76" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="G76" s="60"/>
-      <c r="U76" s="67" t="s">
+      <c r="G76" s="61"/>
+      <c r="U76" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="V76" s="68"/>
-      <c r="W76" s="68"/>
-      <c r="X76" s="68"/>
-      <c r="Y76" s="68"/>
-      <c r="Z76" s="68"/>
-      <c r="AA76" s="68"/>
-      <c r="AB76" s="68"/>
-      <c r="AC76" s="68"/>
-      <c r="AD76" s="69"/>
-    </row>
-    <row r="77" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="V76" s="59"/>
+      <c r="W76" s="59"/>
+      <c r="X76" s="59"/>
+      <c r="Y76" s="59"/>
+      <c r="Z76" s="59"/>
+      <c r="AA76" s="59"/>
+      <c r="AB76" s="59"/>
+      <c r="AC76" s="59"/>
+      <c r="AD76" s="65"/>
+    </row>
+    <row r="77" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C77" s="7">
         <v>4</v>
       </c>
@@ -4532,58 +4542,58 @@
       <c r="E77" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F77" s="53" t="s">
+      <c r="F77" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="G77" s="53"/>
-      <c r="H77" s="53" t="s">
+      <c r="G77" s="52"/>
+      <c r="H77" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="I77" s="53"/>
+      <c r="I77" s="52"/>
       <c r="J77" s="7" t="s">
         <v>41</v>
       </c>
       <c r="K77" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U77" s="61" t="s">
+      <c r="U77" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="V77" s="62"/>
-      <c r="W77" s="62"/>
-      <c r="X77" s="62"/>
-      <c r="Y77" s="62"/>
-      <c r="Z77" s="62"/>
-      <c r="AA77" s="62"/>
-      <c r="AB77" s="62"/>
-      <c r="AC77" s="62"/>
-      <c r="AD77" s="63"/>
-    </row>
-    <row r="79" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="V77" s="67"/>
+      <c r="W77" s="67"/>
+      <c r="X77" s="67"/>
+      <c r="Y77" s="67"/>
+      <c r="Z77" s="67"/>
+      <c r="AA77" s="67"/>
+      <c r="AB77" s="67"/>
+      <c r="AC77" s="67"/>
+      <c r="AD77" s="68"/>
+    </row>
+    <row r="79" spans="2:30" x14ac:dyDescent="0.45">
       <c r="B79" t="s">
         <v>51</v>
       </c>
-      <c r="C79" s="68" t="s">
+      <c r="C79" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D79" s="68"/>
-      <c r="E79" s="68"/>
-      <c r="F79" s="68"/>
-      <c r="G79" s="68"/>
-      <c r="H79" s="68"/>
-      <c r="I79" s="68"/>
-      <c r="J79" s="68"/>
-      <c r="K79" s="68"/>
-      <c r="L79" s="68"/>
-      <c r="M79" s="68"/>
-      <c r="N79" s="68"/>
-      <c r="O79" s="68"/>
-      <c r="P79" s="68"/>
-      <c r="Q79" s="68"/>
-      <c r="R79" s="68"/>
-      <c r="S79" s="68"/>
-    </row>
-    <row r="81" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="D79" s="59"/>
+      <c r="E79" s="59"/>
+      <c r="F79" s="59"/>
+      <c r="G79" s="59"/>
+      <c r="H79" s="59"/>
+      <c r="I79" s="59"/>
+      <c r="J79" s="59"/>
+      <c r="K79" s="59"/>
+      <c r="L79" s="59"/>
+      <c r="M79" s="59"/>
+      <c r="N79" s="59"/>
+      <c r="O79" s="59"/>
+      <c r="P79" s="59"/>
+      <c r="Q79" s="59"/>
+      <c r="R79" s="59"/>
+      <c r="S79" s="59"/>
+    </row>
+    <row r="81" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B81" t="s">
         <v>100</v>
       </c>
@@ -4600,7 +4610,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="82" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:21" x14ac:dyDescent="0.45">
       <c r="C82" s="7">
         <v>2</v>
       </c>
@@ -4610,13 +4620,84 @@
       <c r="E82" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F82" s="59" t="s">
+      <c r="F82" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="G82" s="60"/>
+      <c r="G82" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="86">
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="U73:Y73"/>
+    <mergeCell ref="U75:AD75"/>
+    <mergeCell ref="U76:AD76"/>
+    <mergeCell ref="U77:AD77"/>
+    <mergeCell ref="C79:S79"/>
+    <mergeCell ref="F73:G73"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="U67:AD67"/>
+    <mergeCell ref="U68:AD68"/>
+    <mergeCell ref="U69:AD69"/>
+    <mergeCell ref="U70:AD70"/>
+    <mergeCell ref="U72:Y72"/>
+    <mergeCell ref="U57:AC57"/>
+    <mergeCell ref="U58:AC58"/>
+    <mergeCell ref="U59:AC59"/>
+    <mergeCell ref="U62:AC62"/>
+    <mergeCell ref="U63:AC65"/>
+    <mergeCell ref="U50:AC50"/>
+    <mergeCell ref="U51:AC51"/>
+    <mergeCell ref="U52:AC52"/>
+    <mergeCell ref="U53:AC53"/>
+    <mergeCell ref="U55:AC55"/>
+    <mergeCell ref="U40:X41"/>
+    <mergeCell ref="U43:X43"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="U36:X36"/>
+    <mergeCell ref="U37:AB37"/>
+    <mergeCell ref="U38:AB38"/>
+    <mergeCell ref="U30:AB30"/>
+    <mergeCell ref="U31:AB31"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="U15:X18"/>
+    <mergeCell ref="U21:X24"/>
+    <mergeCell ref="U26:X26"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="C26:S26"/>
+    <mergeCell ref="H22:S22"/>
+    <mergeCell ref="C33:S33"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="I31:S31"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="C43:S43"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="H48:S48"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="H53:S53"/>
     <mergeCell ref="C55:S55"/>
     <mergeCell ref="F70:G70"/>
     <mergeCell ref="J69:K69"/>
@@ -4631,78 +4712,7 @@
     <mergeCell ref="H63:I63"/>
     <mergeCell ref="J63:K63"/>
     <mergeCell ref="P70:S70"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="H48:S48"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:S53"/>
-    <mergeCell ref="H47:K47"/>
-    <mergeCell ref="I31:S31"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:K38"/>
     <mergeCell ref="F62:G62"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="C26:S26"/>
-    <mergeCell ref="H22:S22"/>
-    <mergeCell ref="C33:S33"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="C43:S43"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="U30:AB30"/>
-    <mergeCell ref="U31:AB31"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="U15:X18"/>
-    <mergeCell ref="U21:X24"/>
-    <mergeCell ref="U26:X26"/>
-    <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U29:X29"/>
-    <mergeCell ref="U40:X41"/>
-    <mergeCell ref="U43:X43"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="U35:X35"/>
-    <mergeCell ref="U36:X36"/>
-    <mergeCell ref="U37:AB37"/>
-    <mergeCell ref="U38:AB38"/>
-    <mergeCell ref="U50:AC50"/>
-    <mergeCell ref="U51:AC51"/>
-    <mergeCell ref="U52:AC52"/>
-    <mergeCell ref="U53:AC53"/>
-    <mergeCell ref="U55:AC55"/>
-    <mergeCell ref="U57:AC57"/>
-    <mergeCell ref="U58:AC58"/>
-    <mergeCell ref="U59:AC59"/>
-    <mergeCell ref="U62:AC62"/>
-    <mergeCell ref="U63:AC65"/>
-    <mergeCell ref="U67:AD67"/>
-    <mergeCell ref="U68:AD68"/>
-    <mergeCell ref="U69:AD69"/>
-    <mergeCell ref="U70:AD70"/>
-    <mergeCell ref="U72:Y72"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="U73:Y73"/>
-    <mergeCell ref="U75:AD75"/>
-    <mergeCell ref="U76:AD76"/>
-    <mergeCell ref="U77:AD77"/>
-    <mergeCell ref="C79:S79"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4717,14 +4727,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B4" s="51"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ALU instructions, fixed ISA
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aroma\Desktop\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2A2750-1674-424F-809B-6FF861E06D7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00AFC288-A2C4-4B75-B103-78D3171401DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="258">
   <si>
     <t>POP</t>
   </si>
@@ -228,9 +228,6 @@
   </si>
   <si>
     <t>two byte form: Inverts range of registers from R[reg] to R[reg+cnt], where reg is u8 and cnt is u12</t>
-  </si>
-  <si>
-    <t>eight byte form: same as above</t>
   </si>
   <si>
     <t>Nibble Select, sets n.NS = val</t>
@@ -826,6 +823,9 @@
   </si>
   <si>
     <t>Return from function, SP += cnt, POP IP</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -865,7 +865,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1344,11 +1344,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashDotDot">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1440,14 +1453,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1460,12 +1473,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1475,25 +1503,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1511,55 +1566,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1914,21 +1928,21 @@
   <sheetData>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C4" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4">
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>10</v>
@@ -1936,32 +1950,32 @@
       <c r="J4" s="55">
         <v>0</v>
       </c>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53">
+      <c r="K4" s="54"/>
+      <c r="L4" s="54">
         <v>1</v>
       </c>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53">
+      <c r="M4" s="54"/>
+      <c r="N4" s="54">
         <v>2</v>
       </c>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53">
+      <c r="O4" s="54"/>
+      <c r="P4" s="54">
         <v>3</v>
       </c>
-      <c r="Q4" s="53"/>
+      <c r="Q4" s="54"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>11</v>
@@ -1993,314 +2007,307 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J8" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="J8" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54" t="s">
+      <c r="K8" s="52"/>
+      <c r="L8" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54" t="s">
-        <v>128</v>
-      </c>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54" t="s">
+      <c r="O8" s="52"/>
+      <c r="P8" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="54"/>
+      <c r="Q8" s="52"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F9" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="G9" s="52"/>
+        <v>106</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="53"/>
       <c r="H9" s="8"/>
       <c r="I9" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
+        <v>107</v>
+      </c>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="8"/>
       <c r="J10" t="s">
         <v>30</v>
       </c>
       <c r="K10" t="s">
+        <v>136</v>
+      </c>
+      <c r="M10" t="s">
         <v>137</v>
-      </c>
-      <c r="M10" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>118</v>
-      </c>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
+        <v>117</v>
+      </c>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
       <c r="H11" s="8"/>
       <c r="J11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J13" t="s">
         <v>31</v>
       </c>
       <c r="K13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="J16" s="54" t="s">
-        <v>130</v>
-      </c>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="J16" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54" t="s">
-        <v>132</v>
-      </c>
-      <c r="O16" s="54"/>
-      <c r="P16" s="54"/>
-      <c r="Q16" s="54"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I17" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>119</v>
-      </c>
-      <c r="F18" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="G18" s="52"/>
+        <v>118</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="53"/>
       <c r="H18" s="8"/>
       <c r="J18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
+        <v>107</v>
+      </c>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
       <c r="H19" s="8"/>
       <c r="J19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>126</v>
-      </c>
-      <c r="F20" s="52"/>
-      <c r="G20" s="52"/>
+        <v>125</v>
+      </c>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
       <c r="H20" s="8"/>
       <c r="J20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="J22" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54" t="s">
-        <v>133</v>
-      </c>
-      <c r="O22" s="54"/>
-      <c r="P22" s="54"/>
-      <c r="Q22" s="54"/>
+        <v>111</v>
+      </c>
+      <c r="J22" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="52"/>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I23" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="3:17" x14ac:dyDescent="0.3">
       <c r="J25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I28" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="J28" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="J28" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="K28" s="54"/>
-      <c r="L28" s="54" t="s">
-        <v>135</v>
-      </c>
-      <c r="M28" s="54"/>
-      <c r="N28" s="54"/>
-      <c r="O28" s="54"/>
-      <c r="P28" s="54"/>
-      <c r="Q28" s="54"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="52"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I29" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="3:17" x14ac:dyDescent="0.3">
       <c r="J30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="3:17" x14ac:dyDescent="0.3">
       <c r="J31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:Q28"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:Q16"/>
     <mergeCell ref="F9:G11"/>
     <mergeCell ref="F18:G20"/>
     <mergeCell ref="P4:Q4"/>
@@ -2311,6 +2318,13 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:Q28"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2320,7 +2334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A222D11D-FBDB-42C8-93C4-B5D16645D996}">
   <dimension ref="A3:O70"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
@@ -2335,10 +2349,10 @@
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2346,13 +2360,13 @@
     </row>
     <row r="5" spans="1:4" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="41" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="D5" s="43" t="s">
         <v>151</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -2360,10 +2374,10 @@
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="34" t="s">
         <v>180</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2371,21 +2385,21 @@
         <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>254</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D8" s="34" t="s">
         <v>182</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2393,10 +2407,10 @@
         <v>22</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -2404,21 +2418,21 @@
         <v>29</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="34" t="s">
         <v>154</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2426,10 +2440,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="34" t="s">
         <v>158</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2437,10 +2451,10 @@
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="34" t="s">
         <v>160</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2448,10 +2462,10 @@
         <v>39</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D14" s="34" t="s">
         <v>163</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -2459,10 +2473,10 @@
         <v>46</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" s="34" t="s">
         <v>165</v>
-      </c>
-      <c r="D15" s="34" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2470,21 +2484,21 @@
         <v>48</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D16" s="34" t="s">
         <v>173</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="34" t="s">
         <v>176</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -2492,10 +2506,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D18" s="34" t="s">
         <v>178</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -2503,10 +2517,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="34" t="s">
         <v>167</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -2514,38 +2528,38 @@
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="34" t="s">
         <v>169</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C21" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="36" t="s">
         <v>171</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D25" s="42"/>
     </row>
@@ -2554,7 +2568,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" s="39"/>
     </row>
@@ -2563,16 +2577,16 @@
         <v>19</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D27" s="34"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D28" s="34"/>
     </row>
@@ -2581,7 +2595,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D29" s="34"/>
     </row>
@@ -2590,16 +2604,16 @@
         <v>29</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D30" s="34"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" s="33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D31" s="34"/>
     </row>
@@ -2608,7 +2622,7 @@
         <v>9</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" s="34"/>
     </row>
@@ -2617,7 +2631,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D33" s="34"/>
     </row>
@@ -2626,7 +2640,7 @@
         <v>39</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D34" s="34"/>
     </row>
@@ -2635,7 +2649,7 @@
         <v>46</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D35" s="34"/>
     </row>
@@ -2644,16 +2658,16 @@
         <v>48</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D36" s="34"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D37" s="34"/>
     </row>
@@ -2662,7 +2676,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D38" s="34"/>
     </row>
@@ -2671,7 +2685,7 @@
         <v>14</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D39" s="34"/>
     </row>
@@ -2680,25 +2694,25 @@
         <v>15</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D40" s="34"/>
     </row>
     <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D41" s="36"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B44" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2706,13 +2720,13 @@
     </row>
     <row r="46" spans="1:4" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -2720,10 +2734,10 @@
         <v>13</v>
       </c>
       <c r="C47" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="D47" s="32" t="s">
         <v>204</v>
-      </c>
-      <c r="D47" s="32" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -2731,21 +2745,21 @@
         <v>19</v>
       </c>
       <c r="C48" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D48" s="34" t="s">
         <v>206</v>
-      </c>
-      <c r="D48" s="34" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B49" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C49" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D49" s="34" t="s">
         <v>208</v>
-      </c>
-      <c r="D49" s="34" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -2753,10 +2767,10 @@
         <v>22</v>
       </c>
       <c r="C50" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D50" s="34" t="s">
         <v>210</v>
-      </c>
-      <c r="D50" s="34" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -2764,21 +2778,21 @@
         <v>29</v>
       </c>
       <c r="C51" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D51" s="34" t="s">
         <v>212</v>
-      </c>
-      <c r="D51" s="34" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B52" s="33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C52" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D52" s="34" t="s">
         <v>214</v>
-      </c>
-      <c r="D52" s="34" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -2786,10 +2800,10 @@
         <v>9</v>
       </c>
       <c r="C53" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D53" s="34" t="s">
         <v>216</v>
-      </c>
-      <c r="D53" s="34" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
@@ -2797,10 +2811,10 @@
         <v>2</v>
       </c>
       <c r="C54" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D54" s="34" t="s">
         <v>218</v>
-      </c>
-      <c r="D54" s="34" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -2808,10 +2822,10 @@
         <v>39</v>
       </c>
       <c r="C55" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="D55" s="34" t="s">
         <v>220</v>
-      </c>
-      <c r="D55" s="34" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
@@ -2819,10 +2833,10 @@
         <v>46</v>
       </c>
       <c r="C56" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D56" s="34" t="s">
         <v>222</v>
-      </c>
-      <c r="D56" s="34" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
@@ -2830,58 +2844,58 @@
         <v>48</v>
       </c>
       <c r="C57" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D57" s="34" t="s">
         <v>224</v>
-      </c>
-      <c r="D57" s="34" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B58" s="33" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C58" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D58" s="34" t="s">
         <v>226</v>
-      </c>
-      <c r="D58" s="34" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B59" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C59" s="35" t="s">
         <v>228</v>
-      </c>
-      <c r="C59" s="35" t="s">
-        <v>229</v>
       </c>
       <c r="D59" s="36"/>
     </row>
     <row r="61" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="B61" t="s">
         <v>232</v>
-      </c>
-      <c r="B61" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B62" s="45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C62" s="46" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D62" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G62" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H62" s="53">
+      <c r="H62" s="54">
         <v>0</v>
       </c>
-      <c r="I62" s="53"/>
-      <c r="J62" s="53"/>
+      <c r="I62" s="54"/>
+      <c r="J62" s="54"/>
       <c r="K62" s="56"/>
       <c r="L62" s="57"/>
       <c r="M62" s="58"/>
@@ -2893,13 +2907,13 @@
         <v>13</v>
       </c>
       <c r="C63" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="D63" s="39" t="s">
         <v>234</v>
       </c>
-      <c r="D63" s="39" t="s">
-        <v>235</v>
-      </c>
       <c r="G63" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H63" s="5">
         <v>0</v>
@@ -2923,63 +2937,63 @@
         <v>19</v>
       </c>
       <c r="C64" s="35" t="s">
+        <v>235</v>
+      </c>
+      <c r="D64" s="36" t="s">
         <v>236</v>
-      </c>
-      <c r="D64" s="36" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="66" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G66" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="I66" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="H66" s="7" t="s">
+      <c r="J66" s="52" t="s">
         <v>241</v>
       </c>
-      <c r="I66" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="J66" s="54" t="s">
-        <v>242</v>
-      </c>
-      <c r="K66" s="54"/>
+      <c r="K66" s="52"/>
     </row>
     <row r="67" spans="7:11" x14ac:dyDescent="0.3">
       <c r="G67" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="68" spans="7:11" x14ac:dyDescent="0.3">
       <c r="H68" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I68" s="49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J68" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="7:11" x14ac:dyDescent="0.3">
       <c r="H69" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I69" s="49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J69" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="7:11" x14ac:dyDescent="0.3">
       <c r="H70" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I70" s="50" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J70" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2994,10 +3008,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43404EB-A4C0-4EEB-BCD6-93EC84295AA2}">
-  <dimension ref="A2:AD82"/>
+  <dimension ref="A2:AD81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="AA36" sqref="AA36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3016,17 +3030,17 @@
   <sheetData>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -3034,47 +3048,47 @@
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="70" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="55">
         <v>0</v>
       </c>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53">
+      <c r="E7" s="54"/>
+      <c r="F7" s="54">
         <v>1</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53">
+      <c r="G7" s="54"/>
+      <c r="H7" s="54">
         <v>2</v>
       </c>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53">
+      <c r="I7" s="54"/>
+      <c r="J7" s="54">
         <v>3</v>
       </c>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53">
+      <c r="K7" s="54"/>
+      <c r="L7" s="54">
         <v>4</v>
       </c>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53">
+      <c r="M7" s="54"/>
+      <c r="N7" s="54">
         <v>5</v>
       </c>
-      <c r="O7" s="53"/>
-      <c r="P7" s="53">
+      <c r="O7" s="54"/>
+      <c r="P7" s="54">
         <v>6</v>
       </c>
-      <c r="Q7" s="53"/>
-      <c r="R7" s="53">
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54">
         <v>7</v>
       </c>
-      <c r="S7" s="85"/>
+      <c r="S7" s="69"/>
     </row>
     <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="87"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="4">
         <v>0</v>
       </c>
@@ -3129,40 +3143,40 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
@@ -3181,14 +3195,14 @@
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="52" t="s">
+      <c r="U15" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="V15" s="52"/>
-      <c r="W15" s="52"/>
-      <c r="X15" s="52"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="53"/>
       <c r="AA15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
@@ -3207,12 +3221,12 @@
       <c r="G16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U16" s="52"/>
-      <c r="V16" s="52"/>
-      <c r="W16" s="52"/>
-      <c r="X16" s="52"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="53"/>
+      <c r="W16" s="53"/>
+      <c r="X16" s="53"/>
       <c r="AA16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.3">
@@ -3243,12 +3257,12 @@
       <c r="K17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="52"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="52"/>
-      <c r="X17" s="52"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
       <c r="AA17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.3">
@@ -3303,10 +3317,10 @@
       <c r="S18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="52"/>
-      <c r="V18" s="52"/>
-      <c r="W18" s="52"/>
-      <c r="X18" s="52"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -3326,12 +3340,12 @@
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U21" s="52" t="s">
-        <v>257</v>
-      </c>
-      <c r="V21" s="52"/>
-      <c r="W21" s="52"/>
-      <c r="X21" s="52"/>
+      <c r="U21" s="53" t="s">
+        <v>256</v>
+      </c>
+      <c r="V21" s="53"/>
+      <c r="W21" s="53"/>
+      <c r="X21" s="53"/>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C22" s="7">
@@ -3349,24 +3363,24 @@
       <c r="G22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="67" t="s">
+      <c r="H22" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="68"/>
-      <c r="O22" s="68"/>
-      <c r="P22" s="68"/>
-      <c r="Q22" s="68"/>
-      <c r="R22" s="68"/>
-      <c r="S22" s="68"/>
-      <c r="U22" s="52"/>
-      <c r="V22" s="52"/>
-      <c r="W22" s="52"/>
-      <c r="X22" s="52"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="59"/>
+      <c r="U22" s="53"/>
+      <c r="V22" s="53"/>
+      <c r="W22" s="53"/>
+      <c r="X22" s="53"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C23" s="7">
@@ -3381,64 +3395,52 @@
       <c r="F23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="59" t="s">
+      <c r="G23" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="89"/>
-      <c r="I23" s="89"/>
-      <c r="J23" s="89"/>
-      <c r="K23" s="60"/>
-      <c r="U23" s="52"/>
-      <c r="V23" s="52"/>
-      <c r="W23" s="52"/>
-      <c r="X23" s="52"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="61"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="53"/>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="C24" s="90"/>
-      <c r="D24" s="91"/>
-      <c r="E24" s="91"/>
-      <c r="F24" s="91"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-      <c r="L24" s="91"/>
-      <c r="M24" s="91"/>
-      <c r="N24" s="91"/>
-      <c r="O24" s="91"/>
-      <c r="P24" s="91"/>
-      <c r="Q24" s="91"/>
-      <c r="R24" s="91"/>
-      <c r="S24" s="91"/>
-      <c r="U24" s="52"/>
-      <c r="V24" s="52"/>
-      <c r="W24" s="52"/>
-      <c r="X24" s="52"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="U24" s="53"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
+      <c r="X24" s="53"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
-      <c r="M26" s="68"/>
-      <c r="N26" s="68"/>
-      <c r="O26" s="68"/>
-      <c r="P26" s="68"/>
-      <c r="Q26" s="68"/>
-      <c r="R26" s="68"/>
-      <c r="S26" s="68"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
       <c r="U26" s="58" t="s">
         <v>54</v>
       </c>
@@ -3459,12 +3461,12 @@
       <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U28" s="64" t="s">
+      <c r="U28" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="V28" s="65"/>
-      <c r="W28" s="65"/>
-      <c r="X28" s="65"/>
+      <c r="V28" s="73"/>
+      <c r="W28" s="73"/>
+      <c r="X28" s="73"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
@@ -3486,12 +3488,12 @@
       <c r="G29" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="67" t="s">
+      <c r="U29" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="V29" s="68"/>
-      <c r="W29" s="68"/>
-      <c r="X29" s="68"/>
+      <c r="V29" s="59"/>
+      <c r="W29" s="59"/>
+      <c r="X29" s="59"/>
       <c r="AB29" s="20"/>
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.3">
@@ -3507,25 +3509,25 @@
       <c r="F30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="54" t="s">
+      <c r="G30" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="54"/>
-      <c r="I30" s="88" t="s">
+      <c r="H30" s="52"/>
+      <c r="I30" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="88"/>
-      <c r="K30" s="88"/>
-      <c r="U30" s="67" t="s">
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="U30" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="V30" s="68"/>
-      <c r="W30" s="68"/>
-      <c r="X30" s="68"/>
-      <c r="Y30" s="68"/>
-      <c r="Z30" s="68"/>
-      <c r="AA30" s="68"/>
-      <c r="AB30" s="69"/>
+      <c r="V30" s="59"/>
+      <c r="W30" s="59"/>
+      <c r="X30" s="59"/>
+      <c r="Y30" s="59"/>
+      <c r="Z30" s="59"/>
+      <c r="AA30" s="59"/>
+      <c r="AB30" s="65"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C31" s="7">
@@ -3540,63 +3542,63 @@
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="54" t="s">
+      <c r="G31" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54" t="s">
+      <c r="H31" s="52"/>
+      <c r="I31" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="54"/>
-      <c r="O31" s="54"/>
-      <c r="P31" s="54"/>
-      <c r="Q31" s="54"/>
-      <c r="R31" s="54"/>
-      <c r="S31" s="54"/>
-      <c r="U31" s="61" t="s">
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="52"/>
+      <c r="O31" s="52"/>
+      <c r="P31" s="52"/>
+      <c r="Q31" s="52"/>
+      <c r="R31" s="52"/>
+      <c r="S31" s="52"/>
+      <c r="U31" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="V31" s="62"/>
-      <c r="W31" s="62"/>
-      <c r="X31" s="62"/>
-      <c r="Y31" s="62"/>
-      <c r="Z31" s="62"/>
-      <c r="AA31" s="62"/>
-      <c r="AB31" s="63"/>
+      <c r="V31" s="67"/>
+      <c r="W31" s="67"/>
+      <c r="X31" s="67"/>
+      <c r="Y31" s="67"/>
+      <c r="Z31" s="67"/>
+      <c r="AA31" s="67"/>
+      <c r="AB31" s="68"/>
     </row>
     <row r="33" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="68" t="s">
+      <c r="C33" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="68"/>
-      <c r="M33" s="68"/>
-      <c r="N33" s="68"/>
-      <c r="O33" s="68"/>
-      <c r="P33" s="68"/>
-      <c r="Q33" s="68"/>
-      <c r="R33" s="68"/>
-      <c r="S33" s="68"/>
-      <c r="U33" s="76" t="s">
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="59"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="59"/>
+      <c r="P33" s="59"/>
+      <c r="Q33" s="59"/>
+      <c r="R33" s="59"/>
+      <c r="S33" s="59"/>
+      <c r="U33" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="V33" s="77"/>
-      <c r="W33" s="77"/>
-      <c r="X33" s="78"/>
+      <c r="V33" s="81"/>
+      <c r="W33" s="81"/>
+      <c r="X33" s="82"/>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
@@ -3609,14 +3611,14 @@
         <v>13</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U35" s="64" t="s">
+        <v>161</v>
+      </c>
+      <c r="U35" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="V35" s="65"/>
-      <c r="W35" s="65"/>
-      <c r="X35" s="65"/>
+      <c r="V35" s="73"/>
+      <c r="W35" s="73"/>
+      <c r="X35" s="73"/>
       <c r="Y35" s="18"/>
       <c r="Z35" s="18"/>
       <c r="AA35" s="18"/>
@@ -3633,17 +3635,17 @@
         <v>13</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="G36" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="U36" s="67" t="s">
+      <c r="U36" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="V36" s="68"/>
-      <c r="W36" s="68"/>
-      <c r="X36" s="68"/>
+      <c r="V36" s="93"/>
+      <c r="W36" s="93"/>
+      <c r="X36" s="93"/>
       <c r="AB36" s="20"/>
     </row>
     <row r="37" spans="2:28" x14ac:dyDescent="0.3">
@@ -3656,658 +3658,632 @@
       <c r="E37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G37" s="54" t="s">
+      <c r="F37" s="90" t="s">
+        <v>161</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H37" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H37" s="54"/>
-      <c r="I37" s="88" t="s">
+      <c r="I37" s="52"/>
+      <c r="J37" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="88"/>
-      <c r="K37" s="88"/>
-      <c r="U37" s="67" t="s">
+      <c r="K37" s="52"/>
+      <c r="U37" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="V37" s="68"/>
-      <c r="W37" s="68"/>
-      <c r="X37" s="68"/>
-      <c r="Y37" s="68"/>
-      <c r="Z37" s="68"/>
-      <c r="AA37" s="68"/>
-      <c r="AB37" s="69"/>
-    </row>
-    <row r="38" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="C38" s="7">
-        <v>8</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G38" s="54" t="s">
+      <c r="V37" s="59"/>
+      <c r="W37" s="59"/>
+      <c r="X37" s="59"/>
+      <c r="Y37" s="59"/>
+      <c r="Z37" s="59"/>
+      <c r="AA37" s="59"/>
+      <c r="AB37" s="65"/>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="7">
+        <v>1</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H38" s="54"/>
-      <c r="I38" s="59" t="s">
-        <v>6</v>
-      </c>
-      <c r="J38" s="89"/>
-      <c r="K38" s="60"/>
-      <c r="L38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="U38" s="61" t="s">
+      <c r="U39" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="V39" s="75"/>
+      <c r="W39" s="75"/>
+      <c r="X39" s="76"/>
+    </row>
+    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C40" s="7">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="61"/>
+      <c r="U40" s="77"/>
+      <c r="V40" s="78"/>
+      <c r="W40" s="78"/>
+      <c r="X40" s="79"/>
+    </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="59"/>
+      <c r="P42" s="59"/>
+      <c r="Q42" s="59"/>
+      <c r="R42" s="59"/>
+      <c r="S42" s="59"/>
+      <c r="U42" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="V38" s="62"/>
-      <c r="W38" s="62"/>
-      <c r="X38" s="62"/>
-      <c r="Y38" s="62"/>
-      <c r="Z38" s="62"/>
-      <c r="AA38" s="62"/>
-      <c r="AB38" s="63"/>
-    </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C40" s="7">
+      <c r="V42" s="81"/>
+      <c r="W42" s="81"/>
+      <c r="X42" s="82"/>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C43" s="12"/>
+    </row>
+    <row r="44" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="7">
         <v>1</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="D44" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U44" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="V44" s="18"/>
+      <c r="W44" s="18"/>
+      <c r="X44" s="18"/>
+      <c r="Y44" s="18"/>
+      <c r="Z44" s="18"/>
+      <c r="AA44" s="18"/>
+      <c r="AB44" s="19"/>
+    </row>
+    <row r="45" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C45" s="7">
+        <v>2</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U40" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="V40" s="80"/>
-      <c r="W40" s="80"/>
-      <c r="X40" s="81"/>
-    </row>
-    <row r="41" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="C41" s="7">
-        <v>2</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="G41" s="60"/>
-      <c r="U41" s="82"/>
-      <c r="V41" s="83"/>
-      <c r="W41" s="83"/>
-      <c r="X41" s="84"/>
-    </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C43" s="68" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="68"/>
-      <c r="E43" s="68"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="68"/>
-      <c r="I43" s="68"/>
-      <c r="J43" s="68"/>
-      <c r="K43" s="68"/>
-      <c r="L43" s="68"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="68"/>
-      <c r="O43" s="68"/>
-      <c r="P43" s="68"/>
-      <c r="Q43" s="68"/>
-      <c r="R43" s="68"/>
-      <c r="S43" s="68"/>
-      <c r="U43" s="76" t="s">
-        <v>64</v>
-      </c>
-      <c r="V43" s="77"/>
-      <c r="W43" s="77"/>
-      <c r="X43" s="78"/>
-    </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="C44" s="12"/>
-    </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="7">
-        <v>1</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E45" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U45" s="21" t="s">
+      <c r="U45" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="V45" s="18"/>
-      <c r="W45" s="18"/>
-      <c r="X45" s="18"/>
-      <c r="Y45" s="18"/>
-      <c r="Z45" s="18"/>
-      <c r="AA45" s="18"/>
-      <c r="AB45" s="19"/>
+      <c r="AB45" s="20"/>
     </row>
     <row r="46" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C46" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G46" s="52"/>
+      <c r="H46" s="63" t="s">
         <v>28</v>
       </c>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
       <c r="U46" s="22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AB46" s="20"/>
     </row>
     <row r="47" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="C47" s="7">
-        <v>4</v>
+      <c r="C47" s="11">
+        <v>8</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="54" t="s">
+      <c r="F47" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="54"/>
-      <c r="H47" s="88" t="s">
+      <c r="G47" s="52"/>
+      <c r="H47" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="88"/>
-      <c r="J47" s="88"/>
-      <c r="K47" s="88"/>
-      <c r="U47" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB47" s="20"/>
-    </row>
-    <row r="48" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="C48" s="11">
-        <v>8</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F48" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="G48" s="54"/>
-      <c r="H48" s="54" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="54"/>
-      <c r="J48" s="54"/>
-      <c r="K48" s="54"/>
-      <c r="L48" s="54"/>
-      <c r="M48" s="54"/>
-      <c r="N48" s="54"/>
-      <c r="O48" s="54"/>
-      <c r="P48" s="54"/>
-      <c r="Q48" s="54"/>
-      <c r="R48" s="54"/>
-      <c r="S48" s="54"/>
-      <c r="U48" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="V48" s="24"/>
-      <c r="W48" s="24"/>
-      <c r="X48" s="24"/>
-      <c r="Y48" s="24"/>
-      <c r="Z48" s="24"/>
-      <c r="AA48" s="24"/>
-      <c r="AB48" s="25"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="52"/>
+      <c r="L47" s="52"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="52"/>
+      <c r="P47" s="52"/>
+      <c r="Q47" s="52"/>
+      <c r="R47" s="52"/>
+      <c r="S47" s="52"/>
+      <c r="U47" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="V47" s="24"/>
+      <c r="W47" s="24"/>
+      <c r="X47" s="24"/>
+      <c r="Y47" s="24"/>
+      <c r="Z47" s="24"/>
+      <c r="AA47" s="24"/>
+      <c r="AB47" s="25"/>
+    </row>
+    <row r="49" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="7">
+        <v>1</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U49" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="V49" s="73"/>
+      <c r="W49" s="73"/>
+      <c r="X49" s="73"/>
+      <c r="Y49" s="73"/>
+      <c r="Z49" s="73"/>
+      <c r="AA49" s="73"/>
+      <c r="AB49" s="73"/>
+      <c r="AC49" s="83"/>
     </row>
     <row r="50" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>34</v>
-      </c>
       <c r="C50" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D50" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="U50" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="V50" s="65"/>
-      <c r="W50" s="65"/>
-      <c r="X50" s="65"/>
-      <c r="Y50" s="65"/>
-      <c r="Z50" s="65"/>
-      <c r="AA50" s="65"/>
-      <c r="AB50" s="65"/>
-      <c r="AC50" s="66"/>
+        <v>72</v>
+      </c>
+      <c r="V50" s="59"/>
+      <c r="W50" s="59"/>
+      <c r="X50" s="59"/>
+      <c r="Y50" s="59"/>
+      <c r="Z50" s="59"/>
+      <c r="AA50" s="59"/>
+      <c r="AB50" s="59"/>
+      <c r="AC50" s="65"/>
     </row>
     <row r="51" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C51" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G51" s="52"/>
+      <c r="H51" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="U51" s="67" t="s">
+      <c r="I51" s="63"/>
+      <c r="J51" s="63"/>
+      <c r="K51" s="63"/>
+      <c r="U51" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="V51" s="68"/>
-      <c r="W51" s="68"/>
-      <c r="X51" s="68"/>
-      <c r="Y51" s="68"/>
-      <c r="Z51" s="68"/>
-      <c r="AA51" s="68"/>
-      <c r="AB51" s="68"/>
-      <c r="AC51" s="69"/>
+      <c r="V51" s="59"/>
+      <c r="W51" s="59"/>
+      <c r="X51" s="59"/>
+      <c r="Y51" s="59"/>
+      <c r="Z51" s="59"/>
+      <c r="AA51" s="59"/>
+      <c r="AB51" s="59"/>
+      <c r="AC51" s="65"/>
     </row>
     <row r="52" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C52" s="7">
-        <v>4</v>
+      <c r="C52" s="11">
+        <v>8</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="54" t="s">
+      <c r="F52" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="54"/>
-      <c r="H52" s="88" t="s">
+      <c r="G52" s="52"/>
+      <c r="H52" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="88"/>
-      <c r="J52" s="88"/>
-      <c r="K52" s="88"/>
-      <c r="U52" s="67" t="s">
+      <c r="I52" s="52"/>
+      <c r="J52" s="52"/>
+      <c r="K52" s="52"/>
+      <c r="L52" s="52"/>
+      <c r="M52" s="52"/>
+      <c r="N52" s="52"/>
+      <c r="O52" s="52"/>
+      <c r="P52" s="52"/>
+      <c r="Q52" s="52"/>
+      <c r="R52" s="52"/>
+      <c r="S52" s="52"/>
+      <c r="U52" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="V52" s="68"/>
-      <c r="W52" s="68"/>
-      <c r="X52" s="68"/>
-      <c r="Y52" s="68"/>
-      <c r="Z52" s="68"/>
-      <c r="AA52" s="68"/>
-      <c r="AB52" s="68"/>
-      <c r="AC52" s="69"/>
-    </row>
-    <row r="53" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C53" s="11">
+      <c r="V52" s="67"/>
+      <c r="W52" s="67"/>
+      <c r="X52" s="67"/>
+      <c r="Y52" s="67"/>
+      <c r="Z52" s="67"/>
+      <c r="AA52" s="67"/>
+      <c r="AB52" s="67"/>
+      <c r="AC52" s="68"/>
+    </row>
+    <row r="54" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" s="59"/>
+      <c r="E54" s="59"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="59"/>
+      <c r="J54" s="59"/>
+      <c r="K54" s="59"/>
+      <c r="L54" s="59"/>
+      <c r="M54" s="59"/>
+      <c r="N54" s="59"/>
+      <c r="O54" s="59"/>
+      <c r="P54" s="59"/>
+      <c r="Q54" s="59"/>
+      <c r="R54" s="59"/>
+      <c r="S54" s="59"/>
+      <c r="U54" s="80" t="s">
+        <v>76</v>
+      </c>
+      <c r="V54" s="81"/>
+      <c r="W54" s="81"/>
+      <c r="X54" s="81"/>
+      <c r="Y54" s="81"/>
+      <c r="Z54" s="81"/>
+      <c r="AA54" s="81"/>
+      <c r="AB54" s="81"/>
+      <c r="AC54" s="82"/>
+    </row>
+    <row r="56" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F53" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="G53" s="54"/>
-      <c r="H53" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="I53" s="54"/>
-      <c r="J53" s="54"/>
-      <c r="K53" s="54"/>
-      <c r="L53" s="54"/>
-      <c r="M53" s="54"/>
-      <c r="N53" s="54"/>
-      <c r="O53" s="54"/>
-      <c r="P53" s="54"/>
-      <c r="Q53" s="54"/>
-      <c r="R53" s="54"/>
-      <c r="S53" s="54"/>
-      <c r="U53" s="61" t="s">
-        <v>75</v>
-      </c>
-      <c r="V53" s="62"/>
-      <c r="W53" s="62"/>
-      <c r="X53" s="62"/>
-      <c r="Y53" s="62"/>
-      <c r="Z53" s="62"/>
-      <c r="AA53" s="62"/>
-      <c r="AB53" s="62"/>
-      <c r="AC53" s="63"/>
-    </row>
-    <row r="55" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
-        <v>36</v>
-      </c>
-      <c r="C55" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="D55" s="68"/>
-      <c r="E55" s="68"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="68"/>
-      <c r="J55" s="68"/>
-      <c r="K55" s="68"/>
-      <c r="L55" s="68"/>
-      <c r="M55" s="68"/>
-      <c r="N55" s="68"/>
-      <c r="O55" s="68"/>
-      <c r="P55" s="68"/>
-      <c r="Q55" s="68"/>
-      <c r="R55" s="68"/>
-      <c r="S55" s="68"/>
-      <c r="U55" s="76" t="s">
+      <c r="C56" s="7">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U56" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="V55" s="77"/>
-      <c r="W55" s="77"/>
-      <c r="X55" s="77"/>
-      <c r="Y55" s="77"/>
-      <c r="Z55" s="77"/>
-      <c r="AA55" s="77"/>
-      <c r="AB55" s="77"/>
-      <c r="AC55" s="78"/>
+      <c r="V56" s="73"/>
+      <c r="W56" s="73"/>
+      <c r="X56" s="73"/>
+      <c r="Y56" s="73"/>
+      <c r="Z56" s="73"/>
+      <c r="AA56" s="73"/>
+      <c r="AB56" s="73"/>
+      <c r="AC56" s="83"/>
     </row>
     <row r="57" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B57" t="s">
-        <v>8</v>
-      </c>
       <c r="C57" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E57" s="2" t="s">
+      <c r="F57" s="60" t="s">
         <v>3</v>
       </c>
+      <c r="G57" s="61"/>
       <c r="U57" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="V57" s="65"/>
-      <c r="W57" s="65"/>
-      <c r="X57" s="65"/>
-      <c r="Y57" s="65"/>
-      <c r="Z57" s="65"/>
-      <c r="AA57" s="65"/>
-      <c r="AB57" s="65"/>
-      <c r="AC57" s="66"/>
+        <v>79</v>
+      </c>
+      <c r="V57" s="59"/>
+      <c r="W57" s="59"/>
+      <c r="X57" s="59"/>
+      <c r="Y57" s="59"/>
+      <c r="Z57" s="59"/>
+      <c r="AA57" s="59"/>
+      <c r="AB57" s="59"/>
+      <c r="AC57" s="65"/>
     </row>
     <row r="58" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C58" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="59" t="s">
+      <c r="F58" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G58" s="60"/>
-      <c r="U58" s="67" t="s">
+      <c r="G58" s="52"/>
+      <c r="H58" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="I58" s="52"/>
+      <c r="U58" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="V58" s="68"/>
-      <c r="W58" s="68"/>
-      <c r="X58" s="68"/>
-      <c r="Y58" s="68"/>
-      <c r="Z58" s="68"/>
-      <c r="AA58" s="68"/>
-      <c r="AB58" s="68"/>
-      <c r="AC58" s="69"/>
-    </row>
-    <row r="59" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C59" s="7">
+      <c r="V58" s="67"/>
+      <c r="W58" s="67"/>
+      <c r="X58" s="67"/>
+      <c r="Y58" s="67"/>
+      <c r="Z58" s="67"/>
+      <c r="AA58" s="67"/>
+      <c r="AB58" s="67"/>
+      <c r="AC58" s="68"/>
+    </row>
+    <row r="60" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="7">
+        <v>1</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U60" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="V60" s="18"/>
+      <c r="W60" s="18"/>
+      <c r="X60" s="18"/>
+      <c r="Y60" s="18"/>
+      <c r="Z60" s="18"/>
+      <c r="AA60" s="18"/>
+      <c r="AB60" s="18"/>
+      <c r="AC60" s="19"/>
+    </row>
+    <row r="61" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="C61" s="7">
+        <v>2</v>
+      </c>
+      <c r="D61" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E61" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="G61" s="61"/>
+      <c r="U61" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="V61" s="59"/>
+      <c r="W61" s="59"/>
+      <c r="X61" s="59"/>
+      <c r="Y61" s="59"/>
+      <c r="Z61" s="59"/>
+      <c r="AA61" s="59"/>
+      <c r="AB61" s="59"/>
+      <c r="AC61" s="65"/>
+    </row>
+    <row r="62" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C62" s="7">
+        <v>4</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="G59" s="54"/>
-      <c r="H59" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="I59" s="54"/>
-      <c r="U59" s="61" t="s">
-        <v>81</v>
-      </c>
-      <c r="V59" s="62"/>
-      <c r="W59" s="62"/>
-      <c r="X59" s="62"/>
-      <c r="Y59" s="62"/>
-      <c r="Z59" s="62"/>
-      <c r="AA59" s="62"/>
-      <c r="AB59" s="62"/>
-      <c r="AC59" s="63"/>
-    </row>
-    <row r="61" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="B61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" s="7">
-        <v>1</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="U61" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="V61" s="18"/>
-      <c r="W61" s="18"/>
-      <c r="X61" s="18"/>
-      <c r="Y61" s="18"/>
-      <c r="Z61" s="18"/>
-      <c r="AA61" s="18"/>
-      <c r="AB61" s="18"/>
-      <c r="AC61" s="19"/>
-    </row>
-    <row r="62" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="C62" s="7">
-        <v>2</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="59" t="s">
+      <c r="F62" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="60"/>
-      <c r="U62" s="67" t="s">
-        <v>80</v>
-      </c>
-      <c r="V62" s="68"/>
-      <c r="W62" s="68"/>
-      <c r="X62" s="68"/>
-      <c r="Y62" s="68"/>
-      <c r="Z62" s="68"/>
-      <c r="AA62" s="68"/>
-      <c r="AB62" s="68"/>
-      <c r="AC62" s="69"/>
-    </row>
-    <row r="63" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C63" s="7">
+      <c r="G62" s="52"/>
+      <c r="H62" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="I62" s="52"/>
+      <c r="J62" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="K62" s="52"/>
+      <c r="U62" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="V62" s="85"/>
+      <c r="W62" s="85"/>
+      <c r="X62" s="85"/>
+      <c r="Y62" s="85"/>
+      <c r="Z62" s="85"/>
+      <c r="AA62" s="85"/>
+      <c r="AB62" s="85"/>
+      <c r="AC62" s="86"/>
+    </row>
+    <row r="63" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="U63" s="84"/>
+      <c r="V63" s="85"/>
+      <c r="W63" s="85"/>
+      <c r="X63" s="85"/>
+      <c r="Y63" s="85"/>
+      <c r="Z63" s="85"/>
+      <c r="AA63" s="85"/>
+      <c r="AB63" s="85"/>
+      <c r="AC63" s="86"/>
+    </row>
+    <row r="64" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="U64" s="87"/>
+      <c r="V64" s="88"/>
+      <c r="W64" s="88"/>
+      <c r="X64" s="88"/>
+      <c r="Y64" s="88"/>
+      <c r="Z64" s="88"/>
+      <c r="AA64" s="88"/>
+      <c r="AB64" s="88"/>
+      <c r="AC64" s="89"/>
+    </row>
+    <row r="65" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="U65" s="26"/>
+      <c r="V65" s="26"/>
+      <c r="W65" s="26"/>
+      <c r="X65" s="26"/>
+      <c r="Y65" s="26"/>
+      <c r="Z65" s="26"/>
+      <c r="AA65" s="26"/>
+      <c r="AB65" s="26"/>
+      <c r="AC65" s="26"/>
+    </row>
+    <row r="66" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>38</v>
+      </c>
+      <c r="C66" s="7">
+        <v>1</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U66" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="V66" s="73"/>
+      <c r="W66" s="73"/>
+      <c r="X66" s="73"/>
+      <c r="Y66" s="73"/>
+      <c r="Z66" s="73"/>
+      <c r="AA66" s="73"/>
+      <c r="AB66" s="73"/>
+      <c r="AC66" s="73"/>
+      <c r="AD66" s="83"/>
+    </row>
+    <row r="67" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C67" s="7">
+        <v>2</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F63" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="I63" s="54"/>
-      <c r="J63" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="K63" s="54"/>
-      <c r="U63" s="70" t="s">
+      <c r="E67" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U67" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="V63" s="71"/>
-      <c r="W63" s="71"/>
-      <c r="X63" s="71"/>
-      <c r="Y63" s="71"/>
-      <c r="Z63" s="71"/>
-      <c r="AA63" s="71"/>
-      <c r="AB63" s="71"/>
-      <c r="AC63" s="72"/>
-    </row>
-    <row r="64" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="U64" s="70"/>
-      <c r="V64" s="71"/>
-      <c r="W64" s="71"/>
-      <c r="X64" s="71"/>
-      <c r="Y64" s="71"/>
-      <c r="Z64" s="71"/>
-      <c r="AA64" s="71"/>
-      <c r="AB64" s="71"/>
-      <c r="AC64" s="72"/>
-    </row>
-    <row r="65" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="U65" s="73"/>
-      <c r="V65" s="74"/>
-      <c r="W65" s="74"/>
-      <c r="X65" s="74"/>
-      <c r="Y65" s="74"/>
-      <c r="Z65" s="74"/>
-      <c r="AA65" s="74"/>
-      <c r="AB65" s="74"/>
-      <c r="AC65" s="75"/>
-    </row>
-    <row r="66" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="U66" s="26"/>
-      <c r="V66" s="26"/>
-      <c r="W66" s="26"/>
-      <c r="X66" s="26"/>
-      <c r="Y66" s="26"/>
-      <c r="Z66" s="26"/>
-      <c r="AA66" s="26"/>
-      <c r="AB66" s="26"/>
-      <c r="AC66" s="26"/>
-    </row>
-    <row r="67" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
-        <v>38</v>
-      </c>
-      <c r="C67" s="7">
-        <v>1</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U67" s="64" t="s">
-        <v>84</v>
-      </c>
-      <c r="V67" s="65"/>
-      <c r="W67" s="65"/>
-      <c r="X67" s="65"/>
-      <c r="Y67" s="65"/>
-      <c r="Z67" s="65"/>
-      <c r="AA67" s="65"/>
-      <c r="AB67" s="65"/>
-      <c r="AC67" s="65"/>
-      <c r="AD67" s="66"/>
+      <c r="V67" s="59"/>
+      <c r="W67" s="59"/>
+      <c r="X67" s="59"/>
+      <c r="Y67" s="59"/>
+      <c r="Z67" s="59"/>
+      <c r="AA67" s="59"/>
+      <c r="AB67" s="59"/>
+      <c r="AC67" s="59"/>
+      <c r="AD67" s="65"/>
     </row>
     <row r="68" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C68" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>39</v>
@@ -4318,384 +4294,351 @@
       <c r="G68" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U68" s="67" t="s">
-        <v>83</v>
-      </c>
-      <c r="V68" s="68"/>
-      <c r="W68" s="68"/>
-      <c r="X68" s="68"/>
-      <c r="Y68" s="68"/>
-      <c r="Z68" s="68"/>
-      <c r="AA68" s="68"/>
-      <c r="AB68" s="68"/>
-      <c r="AC68" s="68"/>
-      <c r="AD68" s="69"/>
+      <c r="H68" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="I68" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="J68" s="60" t="s">
+        <v>44</v>
+      </c>
+      <c r="K68" s="61"/>
+      <c r="U68" s="64" t="s">
+        <v>84</v>
+      </c>
+      <c r="V68" s="59"/>
+      <c r="W68" s="59"/>
+      <c r="X68" s="59"/>
+      <c r="Y68" s="59"/>
+      <c r="Z68" s="59"/>
+      <c r="AA68" s="59"/>
+      <c r="AB68" s="59"/>
+      <c r="AC68" s="59"/>
+      <c r="AD68" s="65"/>
     </row>
     <row r="69" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="C69" s="7">
-        <v>4</v>
+      <c r="C69" s="11">
+        <v>8</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F69" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="G69" s="52"/>
+      <c r="H69" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="H69" s="17" t="s">
+      <c r="I69" s="61"/>
+      <c r="J69" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="I69" s="17" t="s">
+      <c r="K69" s="61"/>
+      <c r="L69" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="J69" s="59" t="s">
+      <c r="M69" s="61"/>
+      <c r="N69" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="K69" s="60"/>
-      <c r="U69" s="67" t="s">
+      <c r="O69" s="61"/>
+      <c r="P69" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q69" s="62"/>
+      <c r="R69" s="62"/>
+      <c r="S69" s="61"/>
+      <c r="U69" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="V69" s="68"/>
-      <c r="W69" s="68"/>
-      <c r="X69" s="68"/>
-      <c r="Y69" s="68"/>
-      <c r="Z69" s="68"/>
-      <c r="AA69" s="68"/>
-      <c r="AB69" s="68"/>
-      <c r="AC69" s="68"/>
-      <c r="AD69" s="69"/>
-    </row>
-    <row r="70" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="C70" s="11">
-        <v>8</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F70" s="54" t="s">
-        <v>40</v>
-      </c>
-      <c r="G70" s="54"/>
-      <c r="H70" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="I70" s="60"/>
-      <c r="J70" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="K70" s="60"/>
-      <c r="L70" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="M70" s="60"/>
-      <c r="N70" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="O70" s="60"/>
-      <c r="P70" s="59" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q70" s="89"/>
-      <c r="R70" s="89"/>
-      <c r="S70" s="60"/>
-      <c r="U70" s="61" t="s">
+      <c r="V69" s="67"/>
+      <c r="W69" s="67"/>
+      <c r="X69" s="67"/>
+      <c r="Y69" s="67"/>
+      <c r="Z69" s="67"/>
+      <c r="AA69" s="67"/>
+      <c r="AB69" s="67"/>
+      <c r="AC69" s="67"/>
+      <c r="AD69" s="68"/>
+    </row>
+    <row r="71" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" s="7">
+        <v>1</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U71" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="V70" s="62"/>
-      <c r="W70" s="62"/>
-      <c r="X70" s="62"/>
-      <c r="Y70" s="62"/>
-      <c r="Z70" s="62"/>
-      <c r="AA70" s="62"/>
-      <c r="AB70" s="62"/>
-      <c r="AC70" s="62"/>
-      <c r="AD70" s="63"/>
+      <c r="V71" s="73"/>
+      <c r="W71" s="73"/>
+      <c r="X71" s="73"/>
+      <c r="Y71" s="83"/>
     </row>
     <row r="72" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
-        <v>45</v>
-      </c>
       <c r="C72" s="7">
+        <v>2</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F72" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="G72" s="61"/>
+      <c r="U72" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="V72" s="67"/>
+      <c r="W72" s="67"/>
+      <c r="X72" s="67"/>
+      <c r="Y72" s="68"/>
+    </row>
+    <row r="74" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>47</v>
+      </c>
+      <c r="C74" s="7">
         <v>1</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="U72" s="64" t="s">
-        <v>87</v>
-      </c>
-      <c r="V72" s="65"/>
-      <c r="W72" s="65"/>
-      <c r="X72" s="65"/>
-      <c r="Y72" s="66"/>
-    </row>
-    <row r="73" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="C73" s="7">
+      <c r="D74" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U74" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="V74" s="73"/>
+      <c r="W74" s="73"/>
+      <c r="X74" s="73"/>
+      <c r="Y74" s="73"/>
+      <c r="Z74" s="73"/>
+      <c r="AA74" s="73"/>
+      <c r="AB74" s="73"/>
+      <c r="AC74" s="73"/>
+      <c r="AD74" s="83"/>
+    </row>
+    <row r="75" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="C75" s="7">
         <v>2</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F73" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="G73" s="60"/>
-      <c r="U73" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="V73" s="62"/>
-      <c r="W73" s="62"/>
-      <c r="X73" s="62"/>
-      <c r="Y73" s="63"/>
-    </row>
-    <row r="75" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
-        <v>47</v>
-      </c>
-      <c r="C75" s="7">
-        <v>1</v>
-      </c>
-      <c r="D75" s="2" t="s">
+      <c r="E75" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="F75" s="60" t="s">
         <v>49</v>
       </c>
+      <c r="G75" s="61"/>
       <c r="U75" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="V75" s="65"/>
-      <c r="W75" s="65"/>
-      <c r="X75" s="65"/>
-      <c r="Y75" s="65"/>
-      <c r="Z75" s="65"/>
-      <c r="AA75" s="65"/>
-      <c r="AB75" s="65"/>
-      <c r="AC75" s="65"/>
-      <c r="AD75" s="66"/>
+      <c r="V75" s="59"/>
+      <c r="W75" s="59"/>
+      <c r="X75" s="59"/>
+      <c r="Y75" s="59"/>
+      <c r="Z75" s="59"/>
+      <c r="AA75" s="59"/>
+      <c r="AB75" s="59"/>
+      <c r="AC75" s="59"/>
+      <c r="AD75" s="65"/>
     </row>
     <row r="76" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C76" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F76" s="59" t="s">
+      <c r="F76" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="G76" s="60"/>
-      <c r="U76" s="67" t="s">
+      <c r="G76" s="52"/>
+      <c r="H76" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="I76" s="52"/>
+      <c r="J76" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K76" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="U76" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="V76" s="68"/>
-      <c r="W76" s="68"/>
-      <c r="X76" s="68"/>
-      <c r="Y76" s="68"/>
-      <c r="Z76" s="68"/>
-      <c r="AA76" s="68"/>
-      <c r="AB76" s="68"/>
-      <c r="AC76" s="68"/>
-      <c r="AD76" s="69"/>
-    </row>
-    <row r="77" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="C77" s="7">
+      <c r="V76" s="67"/>
+      <c r="W76" s="67"/>
+      <c r="X76" s="67"/>
+      <c r="Y76" s="67"/>
+      <c r="Z76" s="67"/>
+      <c r="AA76" s="67"/>
+      <c r="AB76" s="67"/>
+      <c r="AC76" s="67"/>
+      <c r="AD76" s="68"/>
+    </row>
+    <row r="78" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>51</v>
+      </c>
+      <c r="C78" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D78" s="59"/>
+      <c r="E78" s="59"/>
+      <c r="F78" s="59"/>
+      <c r="G78" s="59"/>
+      <c r="H78" s="59"/>
+      <c r="I78" s="59"/>
+      <c r="J78" s="59"/>
+      <c r="K78" s="59"/>
+      <c r="L78" s="59"/>
+      <c r="M78" s="59"/>
+      <c r="N78" s="59"/>
+      <c r="O78" s="59"/>
+      <c r="P78" s="59"/>
+      <c r="Q78" s="59"/>
+      <c r="R78" s="59"/>
+      <c r="S78" s="59"/>
+    </row>
+    <row r="80" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>98</v>
+      </c>
+      <c r="C80" s="17">
+        <v>1</v>
+      </c>
+      <c r="D80" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E80" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="U80" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C81" s="7">
+        <v>2</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F77" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="G77" s="54"/>
-      <c r="H77" s="54" t="s">
-        <v>3</v>
-      </c>
-      <c r="I77" s="54"/>
-      <c r="J77" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K77" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="U77" s="61" t="s">
-        <v>91</v>
-      </c>
-      <c r="V77" s="62"/>
-      <c r="W77" s="62"/>
-      <c r="X77" s="62"/>
-      <c r="Y77" s="62"/>
-      <c r="Z77" s="62"/>
-      <c r="AA77" s="62"/>
-      <c r="AB77" s="62"/>
-      <c r="AC77" s="62"/>
-      <c r="AD77" s="63"/>
-    </row>
-    <row r="79" spans="2:30" x14ac:dyDescent="0.3">
-      <c r="B79" t="s">
-        <v>51</v>
-      </c>
-      <c r="C79" s="68" t="s">
-        <v>52</v>
-      </c>
-      <c r="D79" s="68"/>
-      <c r="E79" s="68"/>
-      <c r="F79" s="68"/>
-      <c r="G79" s="68"/>
-      <c r="H79" s="68"/>
-      <c r="I79" s="68"/>
-      <c r="J79" s="68"/>
-      <c r="K79" s="68"/>
-      <c r="L79" s="68"/>
-      <c r="M79" s="68"/>
-      <c r="N79" s="68"/>
-      <c r="O79" s="68"/>
-      <c r="P79" s="68"/>
-      <c r="Q79" s="68"/>
-      <c r="R79" s="68"/>
-      <c r="S79" s="68"/>
-    </row>
-    <row r="81" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B81" t="s">
+      <c r="E81" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C81" s="17">
-        <v>1</v>
-      </c>
-      <c r="D81" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E81" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="U81" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="82" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="C82" s="7">
-        <v>2</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F82" s="59" t="s">
-        <v>250</v>
-      </c>
-      <c r="G82" s="60"/>
+      <c r="F81" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="G81" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="86">
-    <mergeCell ref="C55:S55"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="L70:M70"/>
-    <mergeCell ref="N70:O70"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="H59:I59"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="P70:S70"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="H48:S48"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="H53:S53"/>
+  <mergeCells count="82">
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="U72:Y72"/>
+    <mergeCell ref="U74:AD74"/>
+    <mergeCell ref="U75:AD75"/>
+    <mergeCell ref="U76:AD76"/>
+    <mergeCell ref="C78:S78"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="U66:AD66"/>
+    <mergeCell ref="U67:AD67"/>
+    <mergeCell ref="U68:AD68"/>
+    <mergeCell ref="U69:AD69"/>
+    <mergeCell ref="U71:Y71"/>
+    <mergeCell ref="U56:AC56"/>
+    <mergeCell ref="U57:AC57"/>
+    <mergeCell ref="U58:AC58"/>
+    <mergeCell ref="U61:AC61"/>
+    <mergeCell ref="U62:AC64"/>
+    <mergeCell ref="U49:AC49"/>
+    <mergeCell ref="U50:AC50"/>
+    <mergeCell ref="U51:AC51"/>
+    <mergeCell ref="U52:AC52"/>
+    <mergeCell ref="U54:AC54"/>
+    <mergeCell ref="U39:X40"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="U37:AB37"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="U15:X18"/>
+    <mergeCell ref="U21:X24"/>
+    <mergeCell ref="H22:S22"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="U30:AB30"/>
+    <mergeCell ref="U31:AB31"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="U26:X26"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="C26:S26"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
-    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="H46:K46"/>
     <mergeCell ref="I31:S31"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="C43:S43"/>
-    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C42:S42"/>
+    <mergeCell ref="F46:G46"/>
     <mergeCell ref="C33:S33"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="I30:K30"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="G23:K23"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="U30:AB30"/>
-    <mergeCell ref="U31:AB31"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="U15:X18"/>
-    <mergeCell ref="U21:X24"/>
-    <mergeCell ref="U26:X26"/>
-    <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U29:X29"/>
-    <mergeCell ref="C26:S26"/>
-    <mergeCell ref="H22:S22"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="U40:X41"/>
-    <mergeCell ref="U43:X43"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="U35:X35"/>
-    <mergeCell ref="U36:X36"/>
-    <mergeCell ref="U37:AB37"/>
-    <mergeCell ref="U38:AB38"/>
-    <mergeCell ref="U50:AC50"/>
-    <mergeCell ref="U51:AC51"/>
-    <mergeCell ref="U52:AC52"/>
-    <mergeCell ref="U53:AC53"/>
-    <mergeCell ref="U55:AC55"/>
-    <mergeCell ref="U57:AC57"/>
-    <mergeCell ref="U58:AC58"/>
-    <mergeCell ref="U59:AC59"/>
-    <mergeCell ref="U62:AC62"/>
-    <mergeCell ref="U63:AC65"/>
-    <mergeCell ref="U67:AD67"/>
-    <mergeCell ref="U68:AD68"/>
-    <mergeCell ref="U69:AD69"/>
-    <mergeCell ref="U70:AD70"/>
-    <mergeCell ref="U72:Y72"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="U73:Y73"/>
-    <mergeCell ref="U75:AD75"/>
-    <mergeCell ref="U76:AD76"/>
-    <mergeCell ref="U77:AD77"/>
-    <mergeCell ref="C79:S79"/>
-    <mergeCell ref="F73:G73"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F77:G77"/>
-    <mergeCell ref="H77:I77"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:S47"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:S52"/>
+    <mergeCell ref="C54:S54"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="N69:O69"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="P69:S69"/>
+    <mergeCell ref="F61:G61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4714,7 +4657,7 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
I/O formatting in process...
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aroma\Desktop\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BA4A8F-4DF8-4801-8B9F-306D8A313AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1825EF59-C940-4FC3-8C23-449DFB45A815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="262">
   <si>
     <t>POP</t>
   </si>
@@ -755,28 +755,7 @@
     <t>FMT</t>
   </si>
   <si>
-    <t>ZERO_PAD</t>
-  </si>
-  <si>
-    <t>FMT_RAW</t>
-  </si>
-  <si>
-    <t>PRECISION</t>
-  </si>
-  <si>
     <t>where:</t>
-  </si>
-  <si>
-    <t>u2</t>
-  </si>
-  <si>
-    <t>1 - formatted ouput, 0 - raw</t>
-  </si>
-  <si>
-    <t>1 - PAD with Zero</t>
-  </si>
-  <si>
-    <t>number of decimals after point</t>
   </si>
   <si>
     <t>By default instruction is 1 byte length</t>
@@ -827,12 +806,381 @@
   <si>
     <t>eight byte form: same as above, but all operands are u8, except ofs, which is i16, used by LOAD/STORE operations</t>
   </si>
+  <si>
+    <t>PAD</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <r>
+      <t>FMT</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>enum</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>u3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>raw</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFB5CEA8"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Just output bytes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>dec</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Decimal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>hex</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Hex</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>bin</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Binary</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>fp0</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Rounded float</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>fp2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 2 decimal precision float</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>fp4</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// 4 decimal precision float</t>
+    </r>
+  </si>
+  <si>
+    <t>Pad with zero up to max length</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -856,6 +1204,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFB5CEA8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1361,7 +1751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1445,12 +1835,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1459,14 +1843,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1479,12 +1863,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1494,25 +1893,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1530,47 +1956,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1937,7 +2331,7 @@
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F4" t="s">
         <v>102</v>
@@ -1945,22 +2339,22 @@
       <c r="I4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="57">
+      <c r="J4" s="55">
         <v>0</v>
       </c>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55">
+      <c r="K4" s="54"/>
+      <c r="L4" s="54">
         <v>1</v>
       </c>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55">
+      <c r="M4" s="54"/>
+      <c r="N4" s="54">
         <v>2</v>
       </c>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55">
+      <c r="O4" s="54"/>
+      <c r="P4" s="54">
         <v>3</v>
       </c>
-      <c r="Q4" s="55"/>
+      <c r="Q4" s="54"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="27" t="s">
@@ -1970,7 +2364,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F5" t="s">
         <v>103</v>
@@ -2010,31 +2404,31 @@
       <c r="I8" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="56" t="s">
+      <c r="J8" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56" t="s">
+      <c r="K8" s="52"/>
+      <c r="L8" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="M8" s="56"/>
-      <c r="N8" s="56" t="s">
+      <c r="M8" s="52"/>
+      <c r="N8" s="52" t="s">
         <v>126</v>
       </c>
-      <c r="O8" s="56"/>
-      <c r="P8" s="56" t="s">
+      <c r="O8" s="52"/>
+      <c r="P8" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="56"/>
+      <c r="Q8" s="52"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>105</v>
       </c>
-      <c r="F9" s="54" t="s">
+      <c r="F9" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="54"/>
+      <c r="G9" s="53"/>
       <c r="H9" s="8"/>
       <c r="I9" s="28" t="s">
         <v>134</v>
@@ -2044,8 +2438,8 @@
       <c r="C10" t="s">
         <v>106</v>
       </c>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="8"/>
       <c r="J10" t="s">
         <v>30</v>
@@ -2061,8 +2455,8 @@
       <c r="C11" t="s">
         <v>116</v>
       </c>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
       <c r="H11" s="8"/>
       <c r="J11" t="s">
         <v>125</v>
@@ -2131,20 +2525,20 @@
       <c r="I16" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="J16" s="56" t="s">
+      <c r="J16" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56" t="s">
+      <c r="K16" s="52"/>
+      <c r="L16" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56" t="s">
+      <c r="M16" s="52"/>
+      <c r="N16" s="52" t="s">
         <v>130</v>
       </c>
-      <c r="O16" s="56"/>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I17" s="28" t="s">
@@ -2155,10 +2549,10 @@
       <c r="C18" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="F18" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="54"/>
+      <c r="G18" s="53"/>
       <c r="H18" s="8"/>
       <c r="J18" t="s">
         <v>128</v>
@@ -2174,8 +2568,8 @@
       <c r="C19" t="s">
         <v>106</v>
       </c>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
+      <c r="F19" s="53"/>
+      <c r="G19" s="53"/>
       <c r="H19" s="8"/>
       <c r="J19" t="s">
         <v>127</v>
@@ -2191,8 +2585,8 @@
       <c r="C20" t="s">
         <v>124</v>
       </c>
-      <c r="F20" s="54"/>
-      <c r="G20" s="54"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
       <c r="H20" s="8"/>
       <c r="J20" t="s">
         <v>130</v>
@@ -2214,18 +2608,18 @@
       <c r="I22" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="J22" s="56" t="s">
+      <c r="J22" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56" t="s">
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="O22" s="56"/>
-      <c r="P22" s="56"/>
-      <c r="Q22" s="56"/>
+      <c r="O22" s="52"/>
+      <c r="P22" s="52"/>
+      <c r="Q22" s="52"/>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
@@ -2270,18 +2664,18 @@
       <c r="I28" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="J28" s="56" t="s">
+      <c r="J28" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="K28" s="56"/>
-      <c r="L28" s="56" t="s">
+      <c r="K28" s="52"/>
+      <c r="L28" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="56"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="52"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="52"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I29" s="28" t="s">
@@ -2306,13 +2700,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:Q28"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:Q16"/>
     <mergeCell ref="F9:G11"/>
     <mergeCell ref="F18:G20"/>
     <mergeCell ref="P4:Q4"/>
@@ -2323,6 +2710,13 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:Q28"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2330,10 +2724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A222D11D-FBDB-42C8-93C4-B5D16645D996}">
-  <dimension ref="A3:O70"/>
+  <dimension ref="A3:O78"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2383,10 +2777,10 @@
         <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2889,16 +3283,16 @@
       <c r="G62" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H62" s="55">
+      <c r="H62" s="54">
         <v>0</v>
       </c>
-      <c r="I62" s="55"/>
-      <c r="J62" s="55"/>
-      <c r="K62" s="58"/>
-      <c r="L62" s="59"/>
-      <c r="M62" s="60"/>
-      <c r="N62" s="60"/>
-      <c r="O62" s="60"/>
+      <c r="I62" s="54"/>
+      <c r="J62" s="54"/>
+      <c r="K62" s="56"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="58"/>
+      <c r="N62" s="58"/>
+      <c r="O62" s="58"/>
     </row>
     <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" s="37" t="s">
@@ -2941,64 +3335,95 @@
         <v>235</v>
       </c>
     </row>
-    <row r="66" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G66" s="27" t="s">
+    <row r="66" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G66" s="27"/>
+      <c r="H66" s="60" t="s">
         <v>237</v>
       </c>
-      <c r="H66" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="I66" s="7" t="s">
+      <c r="I66" s="62"/>
+      <c r="J66" s="61"/>
+      <c r="K66" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="67" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="G67" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="J66" s="56" t="s">
-        <v>240</v>
-      </c>
-      <c r="K66" s="56"/>
-    </row>
-    <row r="67" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G67" s="28" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="68" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H68" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="I68" s="49" t="s">
+    </row>
+    <row r="68" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="H68" s="92" t="s">
+        <v>253</v>
+      </c>
+      <c r="I68" s="91"/>
+      <c r="J68" s="90"/>
+      <c r="K68" s="90"/>
+      <c r="L68" s="90"/>
+    </row>
+    <row r="69" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="H69" s="93" t="s">
+        <v>254</v>
+      </c>
+      <c r="I69" s="91"/>
+      <c r="J69" s="90"/>
+      <c r="K69" s="90"/>
+      <c r="L69" s="90"/>
+    </row>
+    <row r="70" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="H70" s="93" t="s">
+        <v>255</v>
+      </c>
+      <c r="I70" s="91"/>
+      <c r="J70" s="90"/>
+      <c r="K70" s="90"/>
+      <c r="L70" s="90"/>
+    </row>
+    <row r="71" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="H71" s="93" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="72" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="H72" s="93" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="73" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="H73" s="93" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="74" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="H74" s="93" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="75" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="H75" s="93" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="76" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="H76" s="93" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="78" spans="7:12" x14ac:dyDescent="0.3">
+      <c r="H78" s="93" t="s">
+        <v>251</v>
+      </c>
+      <c r="I78" t="s">
         <v>178</v>
       </c>
-      <c r="J68" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="69" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H69" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="I69" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="J69" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="70" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H70" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="I70" s="50" t="s">
-        <v>242</v>
-      </c>
-      <c r="J70" t="s">
-        <v>245</v>
+      <c r="J78" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="J66:K66"/>
     <mergeCell ref="H62:K62"/>
     <mergeCell ref="L62:O62"/>
+    <mergeCell ref="H66:J66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3008,7 +3433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43404EB-A4C0-4EEB-BCD6-93EC84295AA2}">
   <dimension ref="A2:AD81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="U69" sqref="U69:AD69"/>
     </sheetView>
   </sheetViews>
@@ -3028,17 +3453,17 @@
   <sheetData>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -3046,47 +3471,47 @@
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="87" t="s">
+      <c r="C7" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="57">
+      <c r="D7" s="55">
         <v>0</v>
       </c>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55">
+      <c r="E7" s="54"/>
+      <c r="F7" s="54">
         <v>1</v>
       </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55">
+      <c r="G7" s="54"/>
+      <c r="H7" s="54">
         <v>2</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55">
+      <c r="I7" s="54"/>
+      <c r="J7" s="54">
         <v>3</v>
       </c>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55">
+      <c r="K7" s="54"/>
+      <c r="L7" s="54">
         <v>4</v>
       </c>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55">
+      <c r="M7" s="54"/>
+      <c r="N7" s="54">
         <v>5</v>
       </c>
-      <c r="O7" s="55"/>
-      <c r="P7" s="55">
+      <c r="O7" s="54"/>
+      <c r="P7" s="54">
         <v>6</v>
       </c>
-      <c r="Q7" s="55"/>
-      <c r="R7" s="55">
+      <c r="Q7" s="54"/>
+      <c r="R7" s="54">
         <v>7</v>
       </c>
-      <c r="S7" s="89"/>
+      <c r="S7" s="69"/>
     </row>
     <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="88"/>
+      <c r="C8" s="73"/>
       <c r="D8" s="4">
         <v>0</v>
       </c>
@@ -3193,12 +3618,12 @@
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="54" t="s">
+      <c r="U15" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="V15" s="54"/>
-      <c r="W15" s="54"/>
-      <c r="X15" s="54"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="53"/>
       <c r="AA15" t="s">
         <v>69</v>
       </c>
@@ -3219,10 +3644,10 @@
       <c r="G16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U16" s="54"/>
-      <c r="V16" s="54"/>
-      <c r="W16" s="54"/>
-      <c r="X16" s="54"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="53"/>
+      <c r="W16" s="53"/>
+      <c r="X16" s="53"/>
       <c r="AA16" t="s">
         <v>70</v>
       </c>
@@ -3255,10 +3680,10 @@
       <c r="K17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="54"/>
-      <c r="V17" s="54"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="54"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
       <c r="AA17" t="s">
         <v>71</v>
       </c>
@@ -3315,10 +3740,10 @@
       <c r="S18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="54"/>
-      <c r="V18" s="54"/>
-      <c r="W18" s="54"/>
-      <c r="X18" s="54"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="53"/>
+      <c r="W18" s="53"/>
+      <c r="X18" s="53"/>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -3338,12 +3763,12 @@
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U21" s="54" t="s">
-        <v>255</v>
-      </c>
-      <c r="V21" s="54"/>
-      <c r="W21" s="54"/>
-      <c r="X21" s="54"/>
+      <c r="U21" s="53" t="s">
+        <v>248</v>
+      </c>
+      <c r="V21" s="53"/>
+      <c r="W21" s="53"/>
+      <c r="X21" s="53"/>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C22" s="7">
@@ -3361,24 +3786,24 @@
       <c r="G22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="69" t="s">
+      <c r="H22" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="70"/>
-      <c r="J22" s="70"/>
-      <c r="K22" s="70"/>
-      <c r="L22" s="70"/>
-      <c r="M22" s="70"/>
-      <c r="N22" s="70"/>
-      <c r="O22" s="70"/>
-      <c r="P22" s="70"/>
-      <c r="Q22" s="70"/>
-      <c r="R22" s="70"/>
-      <c r="S22" s="70"/>
-      <c r="U22" s="54"/>
-      <c r="V22" s="54"/>
-      <c r="W22" s="54"/>
-      <c r="X22" s="54"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="59"/>
+      <c r="U22" s="53"/>
+      <c r="V22" s="53"/>
+      <c r="W22" s="53"/>
+      <c r="X22" s="53"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C23" s="7">
@@ -3393,58 +3818,58 @@
       <c r="F23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="61" t="s">
+      <c r="G23" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="91"/>
-      <c r="I23" s="91"/>
-      <c r="J23" s="91"/>
-      <c r="K23" s="62"/>
-      <c r="U23" s="54"/>
-      <c r="V23" s="54"/>
-      <c r="W23" s="54"/>
-      <c r="X23" s="54"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="61"/>
+      <c r="U23" s="53"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="53"/>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="U24" s="54"/>
-      <c r="V24" s="54"/>
-      <c r="W24" s="54"/>
-      <c r="X24" s="54"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="U24" s="53"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
+      <c r="X24" s="53"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="70" t="s">
+      <c r="C26" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
-      <c r="J26" s="70"/>
-      <c r="K26" s="70"/>
-      <c r="L26" s="70"/>
-      <c r="M26" s="70"/>
-      <c r="N26" s="70"/>
-      <c r="O26" s="70"/>
-      <c r="P26" s="70"/>
-      <c r="Q26" s="70"/>
-      <c r="R26" s="70"/>
-      <c r="S26" s="70"/>
-      <c r="U26" s="60" t="s">
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="59"/>
+      <c r="U26" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="V26" s="60"/>
-      <c r="W26" s="60"/>
-      <c r="X26" s="60"/>
+      <c r="V26" s="58"/>
+      <c r="W26" s="58"/>
+      <c r="X26" s="58"/>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
@@ -3459,12 +3884,12 @@
       <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U28" s="66" t="s">
+      <c r="U28" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="V28" s="67"/>
-      <c r="W28" s="67"/>
-      <c r="X28" s="67"/>
+      <c r="V28" s="71"/>
+      <c r="W28" s="71"/>
+      <c r="X28" s="71"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
@@ -3486,12 +3911,12 @@
       <c r="G29" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="69" t="s">
+      <c r="U29" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="V29" s="70"/>
-      <c r="W29" s="70"/>
-      <c r="X29" s="70"/>
+      <c r="V29" s="59"/>
+      <c r="W29" s="59"/>
+      <c r="X29" s="59"/>
       <c r="AB29" s="20"/>
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.3">
@@ -3507,25 +3932,25 @@
       <c r="F30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="56" t="s">
+      <c r="G30" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="56"/>
-      <c r="I30" s="90" t="s">
+      <c r="H30" s="52"/>
+      <c r="I30" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="90"/>
-      <c r="K30" s="90"/>
-      <c r="U30" s="69" t="s">
+      <c r="J30" s="63"/>
+      <c r="K30" s="63"/>
+      <c r="U30" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="V30" s="70"/>
-      <c r="W30" s="70"/>
-      <c r="X30" s="70"/>
-      <c r="Y30" s="70"/>
-      <c r="Z30" s="70"/>
-      <c r="AA30" s="70"/>
-      <c r="AB30" s="71"/>
+      <c r="V30" s="59"/>
+      <c r="W30" s="59"/>
+      <c r="X30" s="59"/>
+      <c r="Y30" s="59"/>
+      <c r="Z30" s="59"/>
+      <c r="AA30" s="59"/>
+      <c r="AB30" s="65"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C31" s="7">
@@ -3540,63 +3965,63 @@
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="56" t="s">
+      <c r="G31" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56" t="s">
+      <c r="H31" s="52"/>
+      <c r="I31" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="56"/>
-      <c r="M31" s="56"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
-      <c r="S31" s="56"/>
-      <c r="U31" s="63" t="s">
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="52"/>
+      <c r="O31" s="52"/>
+      <c r="P31" s="52"/>
+      <c r="Q31" s="52"/>
+      <c r="R31" s="52"/>
+      <c r="S31" s="52"/>
+      <c r="U31" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="V31" s="64"/>
-      <c r="W31" s="64"/>
-      <c r="X31" s="64"/>
-      <c r="Y31" s="64"/>
-      <c r="Z31" s="64"/>
-      <c r="AA31" s="64"/>
-      <c r="AB31" s="65"/>
+      <c r="V31" s="67"/>
+      <c r="W31" s="67"/>
+      <c r="X31" s="67"/>
+      <c r="Y31" s="67"/>
+      <c r="Z31" s="67"/>
+      <c r="AA31" s="67"/>
+      <c r="AB31" s="68"/>
     </row>
     <row r="33" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="70" t="s">
+      <c r="C33" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="70"/>
-      <c r="I33" s="70"/>
-      <c r="J33" s="70"/>
-      <c r="K33" s="70"/>
-      <c r="L33" s="70"/>
-      <c r="M33" s="70"/>
-      <c r="N33" s="70"/>
-      <c r="O33" s="70"/>
-      <c r="P33" s="70"/>
-      <c r="Q33" s="70"/>
-      <c r="R33" s="70"/>
-      <c r="S33" s="70"/>
-      <c r="U33" s="78" t="s">
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="59"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="59"/>
+      <c r="P33" s="59"/>
+      <c r="Q33" s="59"/>
+      <c r="R33" s="59"/>
+      <c r="S33" s="59"/>
+      <c r="U33" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="V33" s="79"/>
-      <c r="W33" s="79"/>
-      <c r="X33" s="80"/>
+      <c r="V33" s="81"/>
+      <c r="W33" s="81"/>
+      <c r="X33" s="82"/>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
@@ -3611,12 +4036,12 @@
       <c r="E35" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="U35" s="66" t="s">
+      <c r="U35" s="70" t="s">
         <v>60</v>
       </c>
-      <c r="V35" s="67"/>
-      <c r="W35" s="67"/>
-      <c r="X35" s="67"/>
+      <c r="V35" s="71"/>
+      <c r="W35" s="71"/>
+      <c r="X35" s="71"/>
       <c r="Y35" s="18"/>
       <c r="Z35" s="18"/>
       <c r="AA35" s="18"/>
@@ -3635,7 +4060,7 @@
       <c r="F36" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="G36" s="53" t="s">
+      <c r="G36" s="51" t="s">
         <v>3</v>
       </c>
       <c r="U36" s="22" t="s">
@@ -3653,30 +4078,30 @@
       <c r="E37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F37" s="52" t="s">
+      <c r="F37" s="50" t="s">
         <v>160</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="H37" s="56" t="s">
+        <v>249</v>
+      </c>
+      <c r="H37" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="56"/>
-      <c r="J37" s="56" t="s">
+      <c r="I37" s="52"/>
+      <c r="J37" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="K37" s="56"/>
-      <c r="U37" s="69" t="s">
+      <c r="K37" s="52"/>
+      <c r="U37" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="V37" s="70"/>
-      <c r="W37" s="70"/>
-      <c r="X37" s="70"/>
-      <c r="Y37" s="70"/>
-      <c r="Z37" s="70"/>
-      <c r="AA37" s="70"/>
-      <c r="AB37" s="71"/>
+      <c r="V37" s="59"/>
+      <c r="W37" s="59"/>
+      <c r="X37" s="59"/>
+      <c r="Y37" s="59"/>
+      <c r="Z37" s="59"/>
+      <c r="AA37" s="59"/>
+      <c r="AB37" s="65"/>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
@@ -3691,12 +4116,12 @@
       <c r="E39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U39" s="81" t="s">
+      <c r="U39" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="V39" s="82"/>
-      <c r="W39" s="82"/>
-      <c r="X39" s="83"/>
+      <c r="V39" s="75"/>
+      <c r="W39" s="75"/>
+      <c r="X39" s="76"/>
     </row>
     <row r="40" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C40" s="7">
@@ -3708,44 +4133,44 @@
       <c r="E40" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F40" s="61" t="s">
+      <c r="F40" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="G40" s="62"/>
-      <c r="U40" s="84"/>
-      <c r="V40" s="85"/>
-      <c r="W40" s="85"/>
-      <c r="X40" s="86"/>
+      <c r="G40" s="61"/>
+      <c r="U40" s="77"/>
+      <c r="V40" s="78"/>
+      <c r="W40" s="78"/>
+      <c r="X40" s="79"/>
     </row>
     <row r="42" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="70" t="s">
+      <c r="C42" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="G42" s="70"/>
-      <c r="H42" s="70"/>
-      <c r="I42" s="70"/>
-      <c r="J42" s="70"/>
-      <c r="K42" s="70"/>
-      <c r="L42" s="70"/>
-      <c r="M42" s="70"/>
-      <c r="N42" s="70"/>
-      <c r="O42" s="70"/>
-      <c r="P42" s="70"/>
-      <c r="Q42" s="70"/>
-      <c r="R42" s="70"/>
-      <c r="S42" s="70"/>
-      <c r="U42" s="78" t="s">
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="59"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="59"/>
+      <c r="P42" s="59"/>
+      <c r="Q42" s="59"/>
+      <c r="R42" s="59"/>
+      <c r="S42" s="59"/>
+      <c r="U42" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="V42" s="79"/>
-      <c r="W42" s="79"/>
-      <c r="X42" s="80"/>
+      <c r="V42" s="81"/>
+      <c r="W42" s="81"/>
+      <c r="X42" s="82"/>
     </row>
     <row r="43" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C43" s="12"/>
@@ -3805,16 +4230,16 @@
       <c r="E46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="56" t="s">
+      <c r="F46" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="56"/>
-      <c r="H46" s="90" t="s">
+      <c r="G46" s="52"/>
+      <c r="H46" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="I46" s="90"/>
-      <c r="J46" s="90"/>
-      <c r="K46" s="90"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
       <c r="U46" s="22" t="s">
         <v>68</v>
       </c>
@@ -3830,24 +4255,24 @@
       <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="56" t="s">
+      <c r="F47" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="56"/>
-      <c r="H47" s="56" t="s">
+      <c r="G47" s="52"/>
+      <c r="H47" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="56"/>
-      <c r="J47" s="56"/>
-      <c r="K47" s="56"/>
-      <c r="L47" s="56"/>
-      <c r="M47" s="56"/>
-      <c r="N47" s="56"/>
-      <c r="O47" s="56"/>
-      <c r="P47" s="56"/>
-      <c r="Q47" s="56"/>
-      <c r="R47" s="56"/>
-      <c r="S47" s="56"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
+      <c r="K47" s="52"/>
+      <c r="L47" s="52"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="52"/>
+      <c r="P47" s="52"/>
+      <c r="Q47" s="52"/>
+      <c r="R47" s="52"/>
+      <c r="S47" s="52"/>
       <c r="U47" s="23" t="s">
         <v>67</v>
       </c>
@@ -3872,17 +4297,17 @@
       <c r="E49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U49" s="66" t="s">
+      <c r="U49" s="70" t="s">
         <v>75</v>
       </c>
-      <c r="V49" s="67"/>
-      <c r="W49" s="67"/>
-      <c r="X49" s="67"/>
-      <c r="Y49" s="67"/>
-      <c r="Z49" s="67"/>
-      <c r="AA49" s="67"/>
-      <c r="AB49" s="67"/>
-      <c r="AC49" s="68"/>
+      <c r="V49" s="71"/>
+      <c r="W49" s="71"/>
+      <c r="X49" s="71"/>
+      <c r="Y49" s="71"/>
+      <c r="Z49" s="71"/>
+      <c r="AA49" s="71"/>
+      <c r="AB49" s="71"/>
+      <c r="AC49" s="83"/>
     </row>
     <row r="50" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C50" s="7">
@@ -3900,17 +4325,17 @@
       <c r="G50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U50" s="69" t="s">
+      <c r="U50" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="V50" s="70"/>
-      <c r="W50" s="70"/>
-      <c r="X50" s="70"/>
-      <c r="Y50" s="70"/>
-      <c r="Z50" s="70"/>
-      <c r="AA50" s="70"/>
-      <c r="AB50" s="70"/>
-      <c r="AC50" s="71"/>
+      <c r="V50" s="59"/>
+      <c r="W50" s="59"/>
+      <c r="X50" s="59"/>
+      <c r="Y50" s="59"/>
+      <c r="Z50" s="59"/>
+      <c r="AA50" s="59"/>
+      <c r="AB50" s="59"/>
+      <c r="AC50" s="65"/>
     </row>
     <row r="51" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C51" s="7">
@@ -3922,27 +4347,27 @@
       <c r="E51" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="56" t="s">
+      <c r="F51" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="56"/>
-      <c r="H51" s="90" t="s">
+      <c r="G51" s="52"/>
+      <c r="H51" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="90"/>
-      <c r="J51" s="90"/>
-      <c r="K51" s="90"/>
-      <c r="U51" s="69" t="s">
+      <c r="I51" s="63"/>
+      <c r="J51" s="63"/>
+      <c r="K51" s="63"/>
+      <c r="U51" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="V51" s="70"/>
-      <c r="W51" s="70"/>
-      <c r="X51" s="70"/>
-      <c r="Y51" s="70"/>
-      <c r="Z51" s="70"/>
-      <c r="AA51" s="70"/>
-      <c r="AB51" s="70"/>
-      <c r="AC51" s="71"/>
+      <c r="V51" s="59"/>
+      <c r="W51" s="59"/>
+      <c r="X51" s="59"/>
+      <c r="Y51" s="59"/>
+      <c r="Z51" s="59"/>
+      <c r="AA51" s="59"/>
+      <c r="AB51" s="59"/>
+      <c r="AC51" s="65"/>
     </row>
     <row r="52" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C52" s="11">
@@ -3954,70 +4379,70 @@
       <c r="E52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="56" t="s">
+      <c r="F52" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56" t="s">
+      <c r="G52" s="52"/>
+      <c r="H52" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="56"/>
-      <c r="J52" s="56"/>
-      <c r="K52" s="56"/>
-      <c r="L52" s="56"/>
-      <c r="M52" s="56"/>
-      <c r="N52" s="56"/>
-      <c r="O52" s="56"/>
-      <c r="P52" s="56"/>
-      <c r="Q52" s="56"/>
-      <c r="R52" s="56"/>
-      <c r="S52" s="56"/>
-      <c r="U52" s="63" t="s">
+      <c r="I52" s="52"/>
+      <c r="J52" s="52"/>
+      <c r="K52" s="52"/>
+      <c r="L52" s="52"/>
+      <c r="M52" s="52"/>
+      <c r="N52" s="52"/>
+      <c r="O52" s="52"/>
+      <c r="P52" s="52"/>
+      <c r="Q52" s="52"/>
+      <c r="R52" s="52"/>
+      <c r="S52" s="52"/>
+      <c r="U52" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="V52" s="64"/>
-      <c r="W52" s="64"/>
-      <c r="X52" s="64"/>
-      <c r="Y52" s="64"/>
-      <c r="Z52" s="64"/>
-      <c r="AA52" s="64"/>
-      <c r="AB52" s="64"/>
-      <c r="AC52" s="65"/>
+      <c r="V52" s="67"/>
+      <c r="W52" s="67"/>
+      <c r="X52" s="67"/>
+      <c r="Y52" s="67"/>
+      <c r="Z52" s="67"/>
+      <c r="AA52" s="67"/>
+      <c r="AB52" s="67"/>
+      <c r="AC52" s="68"/>
     </row>
     <row r="54" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="70" t="s">
+      <c r="C54" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="70"/>
-      <c r="E54" s="70"/>
-      <c r="F54" s="70"/>
-      <c r="G54" s="70"/>
-      <c r="H54" s="70"/>
-      <c r="I54" s="70"/>
-      <c r="J54" s="70"/>
-      <c r="K54" s="70"/>
-      <c r="L54" s="70"/>
-      <c r="M54" s="70"/>
-      <c r="N54" s="70"/>
-      <c r="O54" s="70"/>
-      <c r="P54" s="70"/>
-      <c r="Q54" s="70"/>
-      <c r="R54" s="70"/>
-      <c r="S54" s="70"/>
-      <c r="U54" s="78" t="s">
+      <c r="D54" s="59"/>
+      <c r="E54" s="59"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="59"/>
+      <c r="J54" s="59"/>
+      <c r="K54" s="59"/>
+      <c r="L54" s="59"/>
+      <c r="M54" s="59"/>
+      <c r="N54" s="59"/>
+      <c r="O54" s="59"/>
+      <c r="P54" s="59"/>
+      <c r="Q54" s="59"/>
+      <c r="R54" s="59"/>
+      <c r="S54" s="59"/>
+      <c r="U54" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="V54" s="79"/>
-      <c r="W54" s="79"/>
-      <c r="X54" s="79"/>
-      <c r="Y54" s="79"/>
-      <c r="Z54" s="79"/>
-      <c r="AA54" s="79"/>
-      <c r="AB54" s="79"/>
-      <c r="AC54" s="80"/>
+      <c r="V54" s="81"/>
+      <c r="W54" s="81"/>
+      <c r="X54" s="81"/>
+      <c r="Y54" s="81"/>
+      <c r="Z54" s="81"/>
+      <c r="AA54" s="81"/>
+      <c r="AB54" s="81"/>
+      <c r="AC54" s="82"/>
     </row>
     <row r="56" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
@@ -4032,17 +4457,17 @@
       <c r="E56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U56" s="66" t="s">
+      <c r="U56" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="V56" s="67"/>
-      <c r="W56" s="67"/>
-      <c r="X56" s="67"/>
-      <c r="Y56" s="67"/>
-      <c r="Z56" s="67"/>
-      <c r="AA56" s="67"/>
-      <c r="AB56" s="67"/>
-      <c r="AC56" s="68"/>
+      <c r="V56" s="71"/>
+      <c r="W56" s="71"/>
+      <c r="X56" s="71"/>
+      <c r="Y56" s="71"/>
+      <c r="Z56" s="71"/>
+      <c r="AA56" s="71"/>
+      <c r="AB56" s="71"/>
+      <c r="AC56" s="83"/>
     </row>
     <row r="57" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C57" s="7">
@@ -4054,21 +4479,21 @@
       <c r="E57" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F57" s="61" t="s">
+      <c r="F57" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="G57" s="62"/>
-      <c r="U57" s="69" t="s">
+      <c r="G57" s="61"/>
+      <c r="U57" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="V57" s="70"/>
-      <c r="W57" s="70"/>
-      <c r="X57" s="70"/>
-      <c r="Y57" s="70"/>
-      <c r="Z57" s="70"/>
-      <c r="AA57" s="70"/>
-      <c r="AB57" s="70"/>
-      <c r="AC57" s="71"/>
+      <c r="V57" s="59"/>
+      <c r="W57" s="59"/>
+      <c r="X57" s="59"/>
+      <c r="Y57" s="59"/>
+      <c r="Z57" s="59"/>
+      <c r="AA57" s="59"/>
+      <c r="AB57" s="59"/>
+      <c r="AC57" s="65"/>
     </row>
     <row r="58" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C58" s="7">
@@ -4080,25 +4505,25 @@
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="56" t="s">
+      <c r="F58" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G58" s="56"/>
-      <c r="H58" s="56" t="s">
+      <c r="G58" s="52"/>
+      <c r="H58" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="I58" s="56"/>
-      <c r="U58" s="63" t="s">
+      <c r="I58" s="52"/>
+      <c r="U58" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="V58" s="64"/>
-      <c r="W58" s="64"/>
-      <c r="X58" s="64"/>
-      <c r="Y58" s="64"/>
-      <c r="Z58" s="64"/>
-      <c r="AA58" s="64"/>
-      <c r="AB58" s="64"/>
-      <c r="AC58" s="65"/>
+      <c r="V58" s="67"/>
+      <c r="W58" s="67"/>
+      <c r="X58" s="67"/>
+      <c r="Y58" s="67"/>
+      <c r="Z58" s="67"/>
+      <c r="AA58" s="67"/>
+      <c r="AB58" s="67"/>
+      <c r="AC58" s="68"/>
     </row>
     <row r="60" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
@@ -4135,21 +4560,21 @@
       <c r="E61" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F61" s="61" t="s">
+      <c r="F61" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="G61" s="62"/>
-      <c r="U61" s="69" t="s">
+      <c r="G61" s="61"/>
+      <c r="U61" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="V61" s="70"/>
-      <c r="W61" s="70"/>
-      <c r="X61" s="70"/>
-      <c r="Y61" s="70"/>
-      <c r="Z61" s="70"/>
-      <c r="AA61" s="70"/>
-      <c r="AB61" s="70"/>
-      <c r="AC61" s="71"/>
+      <c r="V61" s="59"/>
+      <c r="W61" s="59"/>
+      <c r="X61" s="59"/>
+      <c r="Y61" s="59"/>
+      <c r="Z61" s="59"/>
+      <c r="AA61" s="59"/>
+      <c r="AB61" s="59"/>
+      <c r="AC61" s="65"/>
     </row>
     <row r="62" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="7">
@@ -4161,51 +4586,51 @@
       <c r="E62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="56" t="s">
+      <c r="F62" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="56"/>
-      <c r="H62" s="56" t="s">
+      <c r="G62" s="52"/>
+      <c r="H62" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="I62" s="56"/>
-      <c r="J62" s="56" t="s">
+      <c r="I62" s="52"/>
+      <c r="J62" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="K62" s="56"/>
-      <c r="U62" s="72" t="s">
+      <c r="K62" s="52"/>
+      <c r="U62" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="V62" s="73"/>
-      <c r="W62" s="73"/>
-      <c r="X62" s="73"/>
-      <c r="Y62" s="73"/>
-      <c r="Z62" s="73"/>
-      <c r="AA62" s="73"/>
-      <c r="AB62" s="73"/>
-      <c r="AC62" s="74"/>
+      <c r="V62" s="85"/>
+      <c r="W62" s="85"/>
+      <c r="X62" s="85"/>
+      <c r="Y62" s="85"/>
+      <c r="Z62" s="85"/>
+      <c r="AA62" s="85"/>
+      <c r="AB62" s="85"/>
+      <c r="AC62" s="86"/>
     </row>
     <row r="63" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="U63" s="72"/>
-      <c r="V63" s="73"/>
-      <c r="W63" s="73"/>
-      <c r="X63" s="73"/>
-      <c r="Y63" s="73"/>
-      <c r="Z63" s="73"/>
-      <c r="AA63" s="73"/>
-      <c r="AB63" s="73"/>
-      <c r="AC63" s="74"/>
+      <c r="U63" s="84"/>
+      <c r="V63" s="85"/>
+      <c r="W63" s="85"/>
+      <c r="X63" s="85"/>
+      <c r="Y63" s="85"/>
+      <c r="Z63" s="85"/>
+      <c r="AA63" s="85"/>
+      <c r="AB63" s="85"/>
+      <c r="AC63" s="86"/>
     </row>
     <row r="64" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="U64" s="75"/>
-      <c r="V64" s="76"/>
-      <c r="W64" s="76"/>
-      <c r="X64" s="76"/>
-      <c r="Y64" s="76"/>
-      <c r="Z64" s="76"/>
-      <c r="AA64" s="76"/>
-      <c r="AB64" s="76"/>
-      <c r="AC64" s="77"/>
+      <c r="U64" s="87"/>
+      <c r="V64" s="88"/>
+      <c r="W64" s="88"/>
+      <c r="X64" s="88"/>
+      <c r="Y64" s="88"/>
+      <c r="Z64" s="88"/>
+      <c r="AA64" s="88"/>
+      <c r="AB64" s="88"/>
+      <c r="AC64" s="89"/>
     </row>
     <row r="65" spans="2:30" x14ac:dyDescent="0.3">
       <c r="U65" s="26"/>
@@ -4231,18 +4656,18 @@
       <c r="E66" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U66" s="66" t="s">
+      <c r="U66" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="V66" s="67"/>
-      <c r="W66" s="67"/>
-      <c r="X66" s="67"/>
-      <c r="Y66" s="67"/>
-      <c r="Z66" s="67"/>
-      <c r="AA66" s="67"/>
-      <c r="AB66" s="67"/>
-      <c r="AC66" s="67"/>
-      <c r="AD66" s="68"/>
+      <c r="V66" s="71"/>
+      <c r="W66" s="71"/>
+      <c r="X66" s="71"/>
+      <c r="Y66" s="71"/>
+      <c r="Z66" s="71"/>
+      <c r="AA66" s="71"/>
+      <c r="AB66" s="71"/>
+      <c r="AC66" s="71"/>
+      <c r="AD66" s="83"/>
     </row>
     <row r="67" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C67" s="7">
@@ -4260,18 +4685,18 @@
       <c r="G67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U67" s="69" t="s">
+      <c r="U67" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="V67" s="70"/>
-      <c r="W67" s="70"/>
-      <c r="X67" s="70"/>
-      <c r="Y67" s="70"/>
-      <c r="Z67" s="70"/>
-      <c r="AA67" s="70"/>
-      <c r="AB67" s="70"/>
-      <c r="AC67" s="70"/>
-      <c r="AD67" s="71"/>
+      <c r="V67" s="59"/>
+      <c r="W67" s="59"/>
+      <c r="X67" s="59"/>
+      <c r="Y67" s="59"/>
+      <c r="Z67" s="59"/>
+      <c r="AA67" s="59"/>
+      <c r="AB67" s="59"/>
+      <c r="AC67" s="59"/>
+      <c r="AD67" s="65"/>
     </row>
     <row r="68" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C68" s="7">
@@ -4295,22 +4720,22 @@
       <c r="I68" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J68" s="61" t="s">
+      <c r="J68" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="K68" s="62"/>
-      <c r="U68" s="69" t="s">
+      <c r="K68" s="61"/>
+      <c r="U68" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="V68" s="70"/>
-      <c r="W68" s="70"/>
-      <c r="X68" s="70"/>
-      <c r="Y68" s="70"/>
-      <c r="Z68" s="70"/>
-      <c r="AA68" s="70"/>
-      <c r="AB68" s="70"/>
-      <c r="AC68" s="70"/>
-      <c r="AD68" s="71"/>
+      <c r="V68" s="59"/>
+      <c r="W68" s="59"/>
+      <c r="X68" s="59"/>
+      <c r="Y68" s="59"/>
+      <c r="Z68" s="59"/>
+      <c r="AA68" s="59"/>
+      <c r="AB68" s="59"/>
+      <c r="AC68" s="59"/>
+      <c r="AD68" s="65"/>
     </row>
     <row r="69" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C69" s="11">
@@ -4322,44 +4747,44 @@
       <c r="E69" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F69" s="56" t="s">
+      <c r="F69" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="56"/>
-      <c r="H69" s="61" t="s">
+      <c r="G69" s="52"/>
+      <c r="H69" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="I69" s="62"/>
-      <c r="J69" s="61" t="s">
+      <c r="I69" s="61"/>
+      <c r="J69" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="K69" s="62"/>
-      <c r="L69" s="61" t="s">
+      <c r="K69" s="61"/>
+      <c r="L69" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="M69" s="62"/>
-      <c r="N69" s="61" t="s">
+      <c r="M69" s="61"/>
+      <c r="N69" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="O69" s="62"/>
-      <c r="P69" s="61" t="s">
+      <c r="O69" s="61"/>
+      <c r="P69" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="Q69" s="91"/>
-      <c r="R69" s="91"/>
-      <c r="S69" s="62"/>
-      <c r="U69" s="63" t="s">
-        <v>257</v>
-      </c>
-      <c r="V69" s="64"/>
-      <c r="W69" s="64"/>
-      <c r="X69" s="64"/>
-      <c r="Y69" s="64"/>
-      <c r="Z69" s="64"/>
-      <c r="AA69" s="64"/>
-      <c r="AB69" s="64"/>
-      <c r="AC69" s="64"/>
-      <c r="AD69" s="65"/>
+      <c r="Q69" s="62"/>
+      <c r="R69" s="62"/>
+      <c r="S69" s="61"/>
+      <c r="U69" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="V69" s="67"/>
+      <c r="W69" s="67"/>
+      <c r="X69" s="67"/>
+      <c r="Y69" s="67"/>
+      <c r="Z69" s="67"/>
+      <c r="AA69" s="67"/>
+      <c r="AB69" s="67"/>
+      <c r="AC69" s="67"/>
+      <c r="AD69" s="68"/>
     </row>
     <row r="71" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
@@ -4374,13 +4799,13 @@
       <c r="E71" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U71" s="66" t="s">
+      <c r="U71" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="V71" s="67"/>
-      <c r="W71" s="67"/>
-      <c r="X71" s="67"/>
-      <c r="Y71" s="68"/>
+      <c r="V71" s="71"/>
+      <c r="W71" s="71"/>
+      <c r="X71" s="71"/>
+      <c r="Y71" s="83"/>
     </row>
     <row r="72" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C72" s="7">
@@ -4392,17 +4817,17 @@
       <c r="E72" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F72" s="61" t="s">
+      <c r="F72" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="G72" s="62"/>
-      <c r="U72" s="63" t="s">
+      <c r="G72" s="61"/>
+      <c r="U72" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="V72" s="64"/>
-      <c r="W72" s="64"/>
-      <c r="X72" s="64"/>
-      <c r="Y72" s="65"/>
+      <c r="V72" s="67"/>
+      <c r="W72" s="67"/>
+      <c r="X72" s="67"/>
+      <c r="Y72" s="68"/>
     </row>
     <row r="74" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
@@ -4417,18 +4842,18 @@
       <c r="E74" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U74" s="66" t="s">
+      <c r="U74" s="70" t="s">
         <v>87</v>
       </c>
-      <c r="V74" s="67"/>
-      <c r="W74" s="67"/>
-      <c r="X74" s="67"/>
-      <c r="Y74" s="67"/>
-      <c r="Z74" s="67"/>
-      <c r="AA74" s="67"/>
-      <c r="AB74" s="67"/>
-      <c r="AC74" s="67"/>
-      <c r="AD74" s="68"/>
+      <c r="V74" s="71"/>
+      <c r="W74" s="71"/>
+      <c r="X74" s="71"/>
+      <c r="Y74" s="71"/>
+      <c r="Z74" s="71"/>
+      <c r="AA74" s="71"/>
+      <c r="AB74" s="71"/>
+      <c r="AC74" s="71"/>
+      <c r="AD74" s="83"/>
     </row>
     <row r="75" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C75" s="7">
@@ -4440,22 +4865,22 @@
       <c r="E75" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F75" s="61" t="s">
+      <c r="F75" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="G75" s="62"/>
-      <c r="U75" s="69" t="s">
+      <c r="G75" s="61"/>
+      <c r="U75" s="64" t="s">
         <v>88</v>
       </c>
-      <c r="V75" s="70"/>
-      <c r="W75" s="70"/>
-      <c r="X75" s="70"/>
-      <c r="Y75" s="70"/>
-      <c r="Z75" s="70"/>
-      <c r="AA75" s="70"/>
-      <c r="AB75" s="70"/>
-      <c r="AC75" s="70"/>
-      <c r="AD75" s="71"/>
+      <c r="V75" s="59"/>
+      <c r="W75" s="59"/>
+      <c r="X75" s="59"/>
+      <c r="Y75" s="59"/>
+      <c r="Z75" s="59"/>
+      <c r="AA75" s="59"/>
+      <c r="AB75" s="59"/>
+      <c r="AC75" s="59"/>
+      <c r="AD75" s="65"/>
     </row>
     <row r="76" spans="2:30" x14ac:dyDescent="0.3">
       <c r="C76" s="7">
@@ -4467,56 +4892,56 @@
       <c r="E76" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F76" s="56" t="s">
+      <c r="F76" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="G76" s="56"/>
-      <c r="H76" s="56" t="s">
+      <c r="G76" s="52"/>
+      <c r="H76" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="I76" s="56"/>
+      <c r="I76" s="52"/>
       <c r="J76" s="7" t="s">
         <v>41</v>
       </c>
       <c r="K76" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U76" s="63" t="s">
+      <c r="U76" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="V76" s="64"/>
-      <c r="W76" s="64"/>
-      <c r="X76" s="64"/>
-      <c r="Y76" s="64"/>
-      <c r="Z76" s="64"/>
-      <c r="AA76" s="64"/>
-      <c r="AB76" s="64"/>
-      <c r="AC76" s="64"/>
-      <c r="AD76" s="65"/>
+      <c r="V76" s="67"/>
+      <c r="W76" s="67"/>
+      <c r="X76" s="67"/>
+      <c r="Y76" s="67"/>
+      <c r="Z76" s="67"/>
+      <c r="AA76" s="67"/>
+      <c r="AB76" s="67"/>
+      <c r="AC76" s="67"/>
+      <c r="AD76" s="68"/>
     </row>
     <row r="78" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>51</v>
       </c>
-      <c r="C78" s="70" t="s">
+      <c r="C78" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="D78" s="70"/>
-      <c r="E78" s="70"/>
-      <c r="F78" s="70"/>
-      <c r="G78" s="70"/>
-      <c r="H78" s="70"/>
-      <c r="I78" s="70"/>
-      <c r="J78" s="70"/>
-      <c r="K78" s="70"/>
-      <c r="L78" s="70"/>
-      <c r="M78" s="70"/>
-      <c r="N78" s="70"/>
-      <c r="O78" s="70"/>
-      <c r="P78" s="70"/>
-      <c r="Q78" s="70"/>
-      <c r="R78" s="70"/>
-      <c r="S78" s="70"/>
+      <c r="D78" s="59"/>
+      <c r="E78" s="59"/>
+      <c r="F78" s="59"/>
+      <c r="G78" s="59"/>
+      <c r="H78" s="59"/>
+      <c r="I78" s="59"/>
+      <c r="J78" s="59"/>
+      <c r="K78" s="59"/>
+      <c r="L78" s="59"/>
+      <c r="M78" s="59"/>
+      <c r="N78" s="59"/>
+      <c r="O78" s="59"/>
+      <c r="P78" s="59"/>
+      <c r="Q78" s="59"/>
+      <c r="R78" s="59"/>
+      <c r="S78" s="59"/>
     </row>
     <row r="80" spans="2:30" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
@@ -4529,10 +4954,10 @@
         <v>98</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="U80" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.3">
@@ -4545,41 +4970,49 @@
       <c r="E81" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F81" s="61" t="s">
-        <v>248</v>
-      </c>
-      <c r="G81" s="62"/>
+      <c r="F81" s="60" t="s">
+        <v>241</v>
+      </c>
+      <c r="G81" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="C54:S54"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="N69:O69"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="P69:S69"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:S47"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:S52"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="I31:S31"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C42:S42"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="C33:S33"/>
-    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="U72:Y72"/>
+    <mergeCell ref="U74:AD74"/>
+    <mergeCell ref="U75:AD75"/>
+    <mergeCell ref="U76:AD76"/>
+    <mergeCell ref="C78:S78"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="U71:Y71"/>
+    <mergeCell ref="U56:AC56"/>
+    <mergeCell ref="U57:AC57"/>
+    <mergeCell ref="U58:AC58"/>
+    <mergeCell ref="U61:AC61"/>
+    <mergeCell ref="U62:AC64"/>
+    <mergeCell ref="U66:AD66"/>
+    <mergeCell ref="U67:AD67"/>
+    <mergeCell ref="U68:AD68"/>
+    <mergeCell ref="U69:AD69"/>
+    <mergeCell ref="U49:AC49"/>
+    <mergeCell ref="U50:AC50"/>
+    <mergeCell ref="U51:AC51"/>
+    <mergeCell ref="U52:AC52"/>
+    <mergeCell ref="U54:AC54"/>
+    <mergeCell ref="U39:X40"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="U37:AB37"/>
+    <mergeCell ref="U15:X18"/>
+    <mergeCell ref="U21:X24"/>
+    <mergeCell ref="H22:S22"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="G24:K24"/>
     <mergeCell ref="U30:AB30"/>
     <mergeCell ref="U31:AB31"/>
     <mergeCell ref="P7:Q7"/>
@@ -4596,44 +5029,36 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="N7:O7"/>
-    <mergeCell ref="U15:X18"/>
-    <mergeCell ref="U21:X24"/>
-    <mergeCell ref="H22:S22"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="U39:X40"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="U35:X35"/>
-    <mergeCell ref="U37:AB37"/>
-    <mergeCell ref="U49:AC49"/>
-    <mergeCell ref="U50:AC50"/>
-    <mergeCell ref="U51:AC51"/>
-    <mergeCell ref="U52:AC52"/>
-    <mergeCell ref="U54:AC54"/>
-    <mergeCell ref="U71:Y71"/>
-    <mergeCell ref="U56:AC56"/>
-    <mergeCell ref="U57:AC57"/>
-    <mergeCell ref="U58:AC58"/>
-    <mergeCell ref="U61:AC61"/>
-    <mergeCell ref="U62:AC64"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="I31:S31"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C42:S42"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="C33:S33"/>
+    <mergeCell ref="G31:H31"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="J37:K37"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="U72:Y72"/>
-    <mergeCell ref="U74:AD74"/>
-    <mergeCell ref="U75:AD75"/>
-    <mergeCell ref="U76:AD76"/>
-    <mergeCell ref="C78:S78"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="U66:AD66"/>
-    <mergeCell ref="U67:AD67"/>
-    <mergeCell ref="U68:AD68"/>
-    <mergeCell ref="U69:AD69"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:S47"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:S52"/>
+    <mergeCell ref="C54:S54"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="N69:O69"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="P69:S69"/>
+    <mergeCell ref="F61:G61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4652,11 +5077,11 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="51"/>
+      <c r="B4" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
IN instruction unit tests pass
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aroma\Desktop\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBECCA4E-CF06-4389-BB5F-B6B5F26B234B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25699668-1906-4AAA-A14B-9D1E1C653848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
@@ -960,6 +960,18 @@
     </r>
   </si>
   <si>
+    <t>Pad with zero up to max length</t>
+  </si>
+  <si>
+    <t>four byte form: formatted output, but uses reg value for register index and inputs type defined by adt according to format fmt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outputs value to i/o channel ch, which is u4, from R[N.RS], use FMT from R[N.SRC], sets R[N.RS+1] to zero, if successfull </t>
+  </si>
+  <si>
+    <t>Better to use N.DST?</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">    </t>
     </r>
@@ -971,7 +983,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>dec</t>
+      <t>dec = 1</t>
     </r>
     <r>
       <rPr>
@@ -981,7 +993,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>,        </t>
+      <t>,    </t>
     </r>
     <r>
       <rPr>
@@ -1006,7 +1018,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>hex</t>
+      <t>hex = 2</t>
     </r>
     <r>
       <rPr>
@@ -1016,7 +1028,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>,        </t>
+      <t>,    </t>
     </r>
     <r>
       <rPr>
@@ -1041,7 +1053,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>bin</t>
+      <t>bin = 3</t>
     </r>
     <r>
       <rPr>
@@ -1051,7 +1063,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>,        </t>
+      <t>,    </t>
     </r>
     <r>
       <rPr>
@@ -1076,7 +1088,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>fp0</t>
+      <t>fp0 = 4</t>
     </r>
     <r>
       <rPr>
@@ -1086,7 +1098,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>,        </t>
+      <t>,    </t>
     </r>
     <r>
       <rPr>
@@ -1111,7 +1123,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>fp2</t>
+      <t>fp2 = 5</t>
     </r>
     <r>
       <rPr>
@@ -1121,7 +1133,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>,        </t>
+      <t>,    </t>
     </r>
     <r>
       <rPr>
@@ -1146,7 +1158,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>fp4</t>
+      <t>fp4 = 6</t>
     </r>
     <r>
       <rPr>
@@ -1156,7 +1168,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>,        </t>
+      <t>,    </t>
     </r>
     <r>
       <rPr>
@@ -1168,18 +1180,6 @@
       </rPr>
       <t>// 4 decimal precision float</t>
     </r>
-  </si>
-  <si>
-    <t>Pad with zero up to max length</t>
-  </si>
-  <si>
-    <t>four byte form: formatted output, but uses reg value for register index and inputs type defined by adt according to format fmt.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Outputs value to i/o channel ch, which is u4, from R[N.RS], use FMT from R[N.SRC], sets R[N.RS+1] to zero, if successfull </t>
-  </si>
-  <si>
-    <t>Better to use N.DST?</t>
   </si>
 </sst>
 </file>
@@ -1757,7 +1757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1858,14 +1858,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1896,6 +1896,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1905,81 +1914,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2356,19 +2349,19 @@
       <c r="J4" s="58">
         <v>0</v>
       </c>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57">
+      <c r="K4" s="56"/>
+      <c r="L4" s="56">
         <v>1</v>
       </c>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57">
+      <c r="M4" s="56"/>
+      <c r="N4" s="56">
         <v>2</v>
       </c>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57">
+      <c r="O4" s="56"/>
+      <c r="P4" s="56">
         <v>3</v>
       </c>
-      <c r="Q4" s="57"/>
+      <c r="Q4" s="56"/>
     </row>
     <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="27" t="s">
@@ -2418,31 +2411,31 @@
       <c r="I8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="55" t="s">
+      <c r="J8" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55" t="s">
+      <c r="K8" s="57"/>
+      <c r="L8" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="M8" s="55"/>
-      <c r="N8" s="55" t="s">
+      <c r="M8" s="57"/>
+      <c r="N8" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="O8" s="55"/>
-      <c r="P8" s="55" t="s">
+      <c r="O8" s="57"/>
+      <c r="P8" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="55"/>
+      <c r="Q8" s="57"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="56"/>
+      <c r="G9" s="55"/>
       <c r="H9" s="8"/>
       <c r="I9" s="28" t="s">
         <v>133</v>
@@ -2452,8 +2445,8 @@
       <c r="C10" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
       <c r="H10" s="8"/>
       <c r="J10" t="s">
         <v>30</v>
@@ -2469,8 +2462,8 @@
       <c r="C11" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
       <c r="H11" s="8"/>
       <c r="J11" t="s">
         <v>124</v>
@@ -2539,20 +2532,20 @@
       <c r="I16" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="55" t="s">
+      <c r="J16" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55" t="s">
+      <c r="K16" s="57"/>
+      <c r="L16" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55" t="s">
+      <c r="M16" s="57"/>
+      <c r="N16" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="55"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I17" s="28" t="s">
@@ -2563,10 +2556,10 @@
       <c r="C18" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="56" t="s">
+      <c r="F18" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="G18" s="56"/>
+      <c r="G18" s="55"/>
       <c r="H18" s="8"/>
       <c r="J18" t="s">
         <v>127</v>
@@ -2582,8 +2575,8 @@
       <c r="C19" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="56"/>
-      <c r="G19" s="56"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="55"/>
       <c r="H19" s="8"/>
       <c r="J19" t="s">
         <v>126</v>
@@ -2599,8 +2592,8 @@
       <c r="C20" t="s">
         <v>123</v>
       </c>
-      <c r="F20" s="56"/>
-      <c r="G20" s="56"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
       <c r="H20" s="8"/>
       <c r="J20" t="s">
         <v>129</v>
@@ -2622,18 +2615,18 @@
       <c r="I22" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="J22" s="55" t="s">
+      <c r="J22" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="K22" s="55"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="55"/>
-      <c r="N22" s="55" t="s">
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="O22" s="55"/>
-      <c r="P22" s="55"/>
-      <c r="Q22" s="55"/>
+      <c r="O22" s="57"/>
+      <c r="P22" s="57"/>
+      <c r="Q22" s="57"/>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
@@ -2678,18 +2671,18 @@
       <c r="I28" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="J28" s="55" t="s">
+      <c r="J28" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55" t="s">
+      <c r="K28" s="57"/>
+      <c r="L28" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="57"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.3">
       <c r="I29" s="28" t="s">
@@ -2714,6 +2707,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:Q28"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:Q16"/>
     <mergeCell ref="F9:G11"/>
     <mergeCell ref="F18:G20"/>
     <mergeCell ref="P4:Q4"/>
@@ -2724,13 +2724,6 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:Q28"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2738,10 +2731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A222D11D-FBDB-42C8-93C4-B5D16645D996}">
-  <dimension ref="A3:O78"/>
+  <dimension ref="A3:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="H78" sqref="H78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2753,7 +2746,7 @@
     <col min="9" max="9" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>127</v>
       </c>
@@ -2761,10 +2754,10 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="27"/>
     </row>
-    <row r="5" spans="1:4" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="40" t="s">
         <v>147</v>
       </c>
@@ -2774,129 +2767,195 @@
       <c r="D5" s="43" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G5"/>
+      <c r="H5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="56">
+        <v>0</v>
+      </c>
+      <c r="J5" s="56"/>
+      <c r="K5" s="56"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+    </row>
+    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1</v>
+      </c>
+      <c r="K6" s="5">
+        <v>2</v>
+      </c>
+      <c r="L6" s="48">
+        <v>3</v>
+      </c>
+      <c r="M6" s="47"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>244</v>
+        <v>151</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8" s="33" t="s">
         <v>153</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="39" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="H9" s="27"/>
+      <c r="I9" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="J9" s="63"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" s="33" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="33" t="s">
         <v>159</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="I11" s="53" t="s">
+        <v>252</v>
+      </c>
+      <c r="J11" s="52"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" s="33" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>253</v>
+      </c>
+      <c r="J12" s="52"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>258</v>
+      </c>
+      <c r="J13" s="52"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" s="33" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+      <c r="I14" s="54" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="I15" s="54" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" s="33" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>169</v>
+      </c>
+      <c r="I16" s="54" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B17" s="33" t="s">
         <v>172</v>
       </c>
@@ -2906,9 +2965,13 @@
       <c r="D17" s="34" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="33" t="s">
+      <c r="E17" s="93"/>
+      <c r="I17" s="54" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="94" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -2917,41 +2980,57 @@
       <c r="D18" s="34" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="93"/>
+      <c r="I18" s="54" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B19" s="33" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+      <c r="I19" s="54" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B20" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>166</v>
+        <v>244</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="D21" s="36" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+      <c r="I21" s="54" t="s">
+        <v>250</v>
+      </c>
+      <c r="J21" t="s">
+        <v>177</v>
+      </c>
+      <c r="K21" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>131</v>
       </c>
@@ -2959,8 +3038,17 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="93"/>
+      <c r="H24" s="93"/>
+      <c r="I24" s="93"/>
+      <c r="J24" s="93"/>
+      <c r="K24" s="93"/>
+      <c r="L24" s="93"/>
+      <c r="M24" s="93"/>
+      <c r="N24" s="93"/>
+    </row>
+    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="40" t="s">
         <v>147</v>
       </c>
@@ -2968,8 +3056,12 @@
         <v>183</v>
       </c>
       <c r="D25" s="42"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G25" s="93"/>
+      <c r="L25" s="93"/>
+      <c r="M25" s="93"/>
+      <c r="N25" s="93"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B26" s="37" t="s">
         <v>13</v>
       </c>
@@ -2977,8 +3069,12 @@
         <v>184</v>
       </c>
       <c r="D26" s="39"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G26" s="93"/>
+      <c r="L26" s="93"/>
+      <c r="M26" s="93"/>
+      <c r="N26" s="93"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B27" s="33" t="s">
         <v>19</v>
       </c>
@@ -2986,8 +3082,16 @@
         <v>185</v>
       </c>
       <c r="D27" s="34"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="93"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="93"/>
+      <c r="L27" s="93"/>
+      <c r="M27" s="93"/>
+      <c r="N27" s="93"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B28" s="33" t="s">
         <v>153</v>
       </c>
@@ -2995,8 +3099,16 @@
         <v>186</v>
       </c>
       <c r="D28" s="34"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G28" s="93"/>
+      <c r="H28" s="93"/>
+      <c r="I28" s="93"/>
+      <c r="J28" s="93"/>
+      <c r="K28" s="93"/>
+      <c r="L28" s="93"/>
+      <c r="M28" s="93"/>
+      <c r="N28" s="93"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29" s="33" t="s">
         <v>22</v>
       </c>
@@ -3004,8 +3116,16 @@
         <v>187</v>
       </c>
       <c r="D29" s="34"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G29" s="93"/>
+      <c r="H29" s="93"/>
+      <c r="I29" s="93"/>
+      <c r="J29" s="93"/>
+      <c r="K29" s="93"/>
+      <c r="L29" s="93"/>
+      <c r="M29" s="93"/>
+      <c r="N29" s="93"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B30" s="33" t="s">
         <v>29</v>
       </c>
@@ -3013,8 +3133,16 @@
         <v>188</v>
       </c>
       <c r="D30" s="34"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G30" s="93"/>
+      <c r="H30" s="93"/>
+      <c r="I30" s="93"/>
+      <c r="J30" s="93"/>
+      <c r="K30" s="93"/>
+      <c r="L30" s="93"/>
+      <c r="M30" s="93"/>
+      <c r="N30" s="93"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B31" s="33" t="s">
         <v>159</v>
       </c>
@@ -3022,8 +3150,16 @@
         <v>189</v>
       </c>
       <c r="D31" s="34"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G31" s="93"/>
+      <c r="H31" s="93"/>
+      <c r="I31" s="93"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="93"/>
+      <c r="L31" s="93"/>
+      <c r="M31" s="93"/>
+      <c r="N31" s="93"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B32" s="33" t="s">
         <v>9</v>
       </c>
@@ -3031,8 +3167,16 @@
         <v>190</v>
       </c>
       <c r="D32" s="34"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G32" s="93"/>
+      <c r="H32" s="93"/>
+      <c r="I32" s="93"/>
+      <c r="J32" s="93"/>
+      <c r="K32" s="93"/>
+      <c r="L32" s="93"/>
+      <c r="M32" s="93"/>
+      <c r="N32" s="93"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B33" s="33" t="s">
         <v>2</v>
       </c>
@@ -3040,8 +3184,16 @@
         <v>191</v>
       </c>
       <c r="D33" s="34"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G33" s="93"/>
+      <c r="H33" s="93"/>
+      <c r="I33" s="93"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="93"/>
+      <c r="M33" s="93"/>
+      <c r="N33" s="93"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B34" s="33" t="s">
         <v>39</v>
       </c>
@@ -3049,8 +3201,16 @@
         <v>192</v>
       </c>
       <c r="D34" s="34"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G34" s="93"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="93"/>
+      <c r="J34" s="93"/>
+      <c r="K34" s="93"/>
+      <c r="L34" s="93"/>
+      <c r="M34" s="93"/>
+      <c r="N34" s="93"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B35" s="33" t="s">
         <v>46</v>
       </c>
@@ -3058,8 +3218,16 @@
         <v>193</v>
       </c>
       <c r="D35" s="34"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G35" s="93"/>
+      <c r="H35" s="93"/>
+      <c r="I35" s="93"/>
+      <c r="J35" s="93"/>
+      <c r="K35" s="93"/>
+      <c r="L35" s="93"/>
+      <c r="M35" s="93"/>
+      <c r="N35" s="93"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B36" s="33" t="s">
         <v>48</v>
       </c>
@@ -3067,8 +3235,16 @@
         <v>194</v>
       </c>
       <c r="D36" s="34"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G36" s="93"/>
+      <c r="H36" s="93"/>
+      <c r="I36" s="93"/>
+      <c r="J36" s="93"/>
+      <c r="K36" s="93"/>
+      <c r="L36" s="93"/>
+      <c r="M36" s="93"/>
+      <c r="N36" s="93"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B37" s="33" t="s">
         <v>172</v>
       </c>
@@ -3076,8 +3252,16 @@
         <v>195</v>
       </c>
       <c r="D37" s="34"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G37" s="93"/>
+      <c r="H37" s="93"/>
+      <c r="I37" s="93"/>
+      <c r="J37" s="93"/>
+      <c r="K37" s="93"/>
+      <c r="L37" s="93"/>
+      <c r="M37" s="93"/>
+      <c r="N37" s="93"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B38" s="33" t="s">
         <v>4</v>
       </c>
@@ -3085,8 +3269,16 @@
         <v>196</v>
       </c>
       <c r="D38" s="34"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G38" s="93"/>
+      <c r="H38" s="93"/>
+      <c r="I38" s="93"/>
+      <c r="J38" s="93"/>
+      <c r="K38" s="93"/>
+      <c r="L38" s="93"/>
+      <c r="M38" s="93"/>
+      <c r="N38" s="93"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B39" s="33" t="s">
         <v>14</v>
       </c>
@@ -3094,8 +3286,16 @@
         <v>197</v>
       </c>
       <c r="D39" s="34"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G39" s="93"/>
+      <c r="H39" s="93"/>
+      <c r="I39" s="93"/>
+      <c r="J39" s="93"/>
+      <c r="K39" s="93"/>
+      <c r="L39" s="93"/>
+      <c r="M39" s="93"/>
+      <c r="N39" s="93"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B40" s="33" t="s">
         <v>15</v>
       </c>
@@ -3103,8 +3303,16 @@
         <v>198</v>
       </c>
       <c r="D40" s="34"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G40" s="93"/>
+      <c r="H40" s="93"/>
+      <c r="I40" s="93"/>
+      <c r="J40" s="93"/>
+      <c r="K40" s="93"/>
+      <c r="L40" s="93"/>
+      <c r="M40" s="93"/>
+      <c r="N40" s="93"/>
+    </row>
+    <row r="41" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="10" t="s">
         <v>97</v>
       </c>
@@ -3112,19 +3320,55 @@
         <v>199</v>
       </c>
       <c r="D41" s="36"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="G41" s="93"/>
+      <c r="H41" s="93"/>
+      <c r="I41" s="93"/>
+      <c r="J41" s="93"/>
+      <c r="K41" s="93"/>
+      <c r="L41" s="93"/>
+      <c r="M41" s="93"/>
+      <c r="N41" s="93"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G42" s="93"/>
+      <c r="H42" s="93"/>
+      <c r="I42" s="93"/>
+      <c r="J42" s="93"/>
+      <c r="K42" s="93"/>
+      <c r="L42" s="93"/>
+      <c r="M42" s="93"/>
+      <c r="N42" s="93"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G43" s="93"/>
+      <c r="H43" s="93"/>
+      <c r="I43" s="93"/>
+      <c r="J43" s="93"/>
+      <c r="K43" s="93"/>
+      <c r="L43" s="93"/>
+      <c r="M43" s="93"/>
+      <c r="N43" s="93"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
         <v>228</v>
       </c>
       <c r="B44" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G44" s="93"/>
+      <c r="H44" s="93"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
+    </row>
+    <row r="45" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="27"/>
     </row>
-    <row r="46" spans="1:4" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="29" t="s">
         <v>147</v>
       </c>
@@ -3135,7 +3379,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
         <v>13</v>
       </c>
@@ -3146,7 +3390,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B48" s="33" t="s">
         <v>19</v>
       </c>
@@ -3157,7 +3401,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49" s="33" t="s">
         <v>153</v>
       </c>
@@ -3168,7 +3412,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" s="33" t="s">
         <v>22</v>
       </c>
@@ -3179,7 +3423,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" s="33" t="s">
         <v>29</v>
       </c>
@@ -3190,7 +3434,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B52" s="33" t="s">
         <v>159</v>
       </c>
@@ -3201,7 +3445,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B53" s="33" t="s">
         <v>9</v>
       </c>
@@ -3212,7 +3456,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B54" s="33" t="s">
         <v>2</v>
       </c>
@@ -3223,7 +3467,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B55" s="33" t="s">
         <v>39</v>
       </c>
@@ -3234,7 +3478,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B56" s="33" t="s">
         <v>46</v>
       </c>
@@ -3245,7 +3489,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" s="33" t="s">
         <v>48</v>
       </c>
@@ -3256,7 +3500,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B58" s="33" t="s">
         <v>172</v>
       </c>
@@ -3267,7 +3511,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B59" s="10" t="s">
         <v>225</v>
       </c>
@@ -3276,7 +3520,7 @@
       </c>
       <c r="D59" s="36"/>
     </row>
-    <row r="61" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="27" t="s">
         <v>229</v>
       </c>
@@ -3284,7 +3528,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B62" s="45" t="s">
         <v>147</v>
       </c>
@@ -3294,21 +3538,8 @@
       <c r="D62" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="G62" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="H62" s="57">
-        <v>0</v>
-      </c>
-      <c r="I62" s="57"/>
-      <c r="J62" s="57"/>
-      <c r="K62" s="59"/>
-      <c r="L62" s="60"/>
-      <c r="M62" s="61"/>
-      <c r="N62" s="61"/>
-      <c r="O62" s="61"/>
-    </row>
-    <row r="63" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B63" s="37" t="s">
         <v>13</v>
       </c>
@@ -3318,27 +3549,8 @@
       <c r="D63" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="G63" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="H63" s="5">
-        <v>0</v>
-      </c>
-      <c r="I63" s="5">
-        <v>1</v>
-      </c>
-      <c r="J63" s="5">
-        <v>2</v>
-      </c>
-      <c r="K63" s="48">
-        <v>3</v>
-      </c>
-      <c r="L63" s="47"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-    </row>
-    <row r="64" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" s="10" t="s">
         <v>19</v>
       </c>
@@ -3349,86 +3561,11 @@
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G66" s="27"/>
-      <c r="H66" s="62" t="s">
-        <v>236</v>
-      </c>
-      <c r="I66" s="63"/>
-      <c r="J66" s="64"/>
-      <c r="K66" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="67" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="G67" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="68" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H68" s="53" t="s">
-        <v>252</v>
-      </c>
-      <c r="I68" s="52"/>
-    </row>
-    <row r="69" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H69" s="54" t="s">
-        <v>253</v>
-      </c>
-      <c r="I69" s="52"/>
-    </row>
-    <row r="70" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H70" s="54" t="s">
-        <v>254</v>
-      </c>
-      <c r="I70" s="52"/>
-    </row>
-    <row r="71" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H71" s="54" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="72" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H72" s="54" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="73" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H73" s="54" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="74" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H74" s="54" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="75" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H75" s="54" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="76" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H76" s="54" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="78" spans="7:11" x14ac:dyDescent="0.3">
-      <c r="H78" s="54" t="s">
-        <v>250</v>
-      </c>
-      <c r="I78" t="s">
-        <v>177</v>
-      </c>
-      <c r="J78" t="s">
-        <v>260</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="H62:K62"/>
-    <mergeCell ref="L62:O62"/>
-    <mergeCell ref="H66:J66"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="I9:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3438,7 +3575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43404EB-A4C0-4EEB-BCD6-93EC84295AA2}">
   <dimension ref="A2:AF83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
@@ -3477,47 +3614,47 @@
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="76" t="s">
+      <c r="C7" s="91" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="58">
         <v>0</v>
       </c>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57">
+      <c r="E7" s="56"/>
+      <c r="F7" s="56">
         <v>1</v>
       </c>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57">
+      <c r="G7" s="56"/>
+      <c r="H7" s="56">
         <v>2</v>
       </c>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57">
+      <c r="I7" s="56"/>
+      <c r="J7" s="56">
         <v>3</v>
       </c>
-      <c r="K7" s="57"/>
-      <c r="L7" s="57">
+      <c r="K7" s="56"/>
+      <c r="L7" s="56">
         <v>4</v>
       </c>
-      <c r="M7" s="57"/>
-      <c r="N7" s="57">
+      <c r="M7" s="56"/>
+      <c r="N7" s="56">
         <v>5</v>
       </c>
-      <c r="O7" s="57"/>
-      <c r="P7" s="57">
+      <c r="O7" s="56"/>
+      <c r="P7" s="56">
         <v>6</v>
       </c>
-      <c r="Q7" s="57"/>
-      <c r="R7" s="57">
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56">
         <v>7</v>
       </c>
-      <c r="S7" s="75"/>
+      <c r="S7" s="89"/>
     </row>
     <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="92"/>
       <c r="D8" s="4">
         <v>0</v>
       </c>
@@ -3624,12 +3761,12 @@
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="56" t="s">
+      <c r="U15" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="V15" s="56"/>
-      <c r="W15" s="56"/>
-      <c r="X15" s="56"/>
+      <c r="V15" s="55"/>
+      <c r="W15" s="55"/>
+      <c r="X15" s="55"/>
       <c r="AA15" t="s">
         <v>68</v>
       </c>
@@ -3650,10 +3787,10 @@
       <c r="G16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U16" s="56"/>
-      <c r="V16" s="56"/>
-      <c r="W16" s="56"/>
-      <c r="X16" s="56"/>
+      <c r="U16" s="55"/>
+      <c r="V16" s="55"/>
+      <c r="W16" s="55"/>
+      <c r="X16" s="55"/>
       <c r="AA16" t="s">
         <v>69</v>
       </c>
@@ -3686,10 +3823,10 @@
       <c r="K17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="56"/>
-      <c r="V17" s="56"/>
-      <c r="W17" s="56"/>
-      <c r="X17" s="56"/>
+      <c r="U17" s="55"/>
+      <c r="V17" s="55"/>
+      <c r="W17" s="55"/>
+      <c r="X17" s="55"/>
       <c r="AA17" t="s">
         <v>70</v>
       </c>
@@ -3746,10 +3883,10 @@
       <c r="S18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="56"/>
-      <c r="V18" s="56"/>
-      <c r="W18" s="56"/>
-      <c r="X18" s="56"/>
+      <c r="U18" s="55"/>
+      <c r="V18" s="55"/>
+      <c r="W18" s="55"/>
+      <c r="X18" s="55"/>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -3769,12 +3906,12 @@
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U21" s="56" t="s">
+      <c r="U21" s="55" t="s">
         <v>247</v>
       </c>
-      <c r="V21" s="56"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="56"/>
+      <c r="V21" s="55"/>
+      <c r="W21" s="55"/>
+      <c r="X21" s="55"/>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C22" s="7">
@@ -3792,24 +3929,24 @@
       <c r="G22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="68" t="s">
+      <c r="H22" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="69"/>
-      <c r="J22" s="69"/>
-      <c r="K22" s="69"/>
-      <c r="L22" s="69"/>
-      <c r="M22" s="69"/>
-      <c r="N22" s="69"/>
-      <c r="O22" s="69"/>
-      <c r="P22" s="69"/>
-      <c r="Q22" s="69"/>
-      <c r="R22" s="69"/>
-      <c r="S22" s="69"/>
-      <c r="U22" s="56"/>
-      <c r="V22" s="56"/>
-      <c r="W22" s="56"/>
-      <c r="X22" s="56"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="72"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="72"/>
+      <c r="Q22" s="72"/>
+      <c r="R22" s="72"/>
+      <c r="S22" s="72"/>
+      <c r="U22" s="55"/>
+      <c r="V22" s="55"/>
+      <c r="W22" s="55"/>
+      <c r="X22" s="55"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C23" s="7">
@@ -3831,10 +3968,10 @@
       <c r="I23" s="63"/>
       <c r="J23" s="63"/>
       <c r="K23" s="64"/>
-      <c r="U23" s="56"/>
-      <c r="V23" s="56"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="56"/>
+      <c r="U23" s="55"/>
+      <c r="V23" s="55"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="55"/>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.3">
       <c r="G24" s="61"/>
@@ -3842,34 +3979,34 @@
       <c r="I24" s="61"/>
       <c r="J24" s="61"/>
       <c r="K24" s="61"/>
-      <c r="U24" s="56"/>
-      <c r="V24" s="56"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="56"/>
+      <c r="U24" s="55"/>
+      <c r="V24" s="55"/>
+      <c r="W24" s="55"/>
+      <c r="X24" s="55"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="69" t="s">
+      <c r="C26" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="69"/>
-      <c r="N26" s="69"/>
-      <c r="O26" s="69"/>
-      <c r="P26" s="69"/>
-      <c r="Q26" s="69"/>
-      <c r="R26" s="69"/>
-      <c r="S26" s="69"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
+      <c r="J26" s="72"/>
+      <c r="K26" s="72"/>
+      <c r="L26" s="72"/>
+      <c r="M26" s="72"/>
+      <c r="N26" s="72"/>
+      <c r="O26" s="72"/>
+      <c r="P26" s="72"/>
+      <c r="Q26" s="72"/>
+      <c r="R26" s="72"/>
+      <c r="S26" s="72"/>
       <c r="U26" s="61" t="s">
         <v>53</v>
       </c>
@@ -3890,12 +4027,12 @@
       <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U28" s="71" t="s">
+      <c r="U28" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="V28" s="72"/>
-      <c r="W28" s="72"/>
-      <c r="X28" s="72"/>
+      <c r="V28" s="69"/>
+      <c r="W28" s="69"/>
+      <c r="X28" s="69"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
@@ -3917,12 +4054,12 @@
       <c r="G29" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="68" t="s">
+      <c r="U29" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="V29" s="69"/>
-      <c r="W29" s="69"/>
-      <c r="X29" s="69"/>
+      <c r="V29" s="72"/>
+      <c r="W29" s="72"/>
+      <c r="X29" s="72"/>
       <c r="AB29" s="20"/>
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.3">
@@ -3938,25 +4075,25 @@
       <c r="F30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="55" t="s">
+      <c r="G30" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="55"/>
-      <c r="I30" s="74" t="s">
+      <c r="H30" s="57"/>
+      <c r="I30" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="U30" s="68" t="s">
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="U30" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="V30" s="69"/>
-      <c r="W30" s="69"/>
-      <c r="X30" s="69"/>
-      <c r="Y30" s="69"/>
-      <c r="Z30" s="69"/>
-      <c r="AA30" s="69"/>
-      <c r="AB30" s="70"/>
+      <c r="V30" s="72"/>
+      <c r="W30" s="72"/>
+      <c r="X30" s="72"/>
+      <c r="Y30" s="72"/>
+      <c r="Z30" s="72"/>
+      <c r="AA30" s="72"/>
+      <c r="AB30" s="73"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C31" s="7">
@@ -3971,23 +4108,23 @@
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="55" t="s">
+      <c r="G31" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55" t="s">
+      <c r="H31" s="57"/>
+      <c r="I31" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="55"/>
-      <c r="N31" s="55"/>
-      <c r="O31" s="55"/>
-      <c r="P31" s="55"/>
-      <c r="Q31" s="55"/>
-      <c r="R31" s="55"/>
-      <c r="S31" s="55"/>
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="57"/>
+      <c r="Q31" s="57"/>
+      <c r="R31" s="57"/>
+      <c r="S31" s="57"/>
       <c r="U31" s="65" t="s">
         <v>57</v>
       </c>
@@ -4003,31 +4140,31 @@
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="69" t="s">
+      <c r="C33" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="69"/>
-      <c r="N33" s="69"/>
-      <c r="O33" s="69"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="69"/>
-      <c r="R33" s="69"/>
-      <c r="S33" s="69"/>
-      <c r="U33" s="84" t="s">
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="72"/>
+      <c r="M33" s="72"/>
+      <c r="N33" s="72"/>
+      <c r="O33" s="72"/>
+      <c r="P33" s="72"/>
+      <c r="Q33" s="72"/>
+      <c r="R33" s="72"/>
+      <c r="S33" s="72"/>
+      <c r="U33" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="V33" s="85"/>
-      <c r="W33" s="85"/>
-      <c r="X33" s="86"/>
+      <c r="V33" s="81"/>
+      <c r="W33" s="81"/>
+      <c r="X33" s="82"/>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
@@ -4042,12 +4179,12 @@
       <c r="E35" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="U35" s="71" t="s">
+      <c r="U35" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="V35" s="72"/>
-      <c r="W35" s="72"/>
-      <c r="X35" s="72"/>
+      <c r="V35" s="69"/>
+      <c r="W35" s="69"/>
+      <c r="X35" s="69"/>
       <c r="Y35" s="18"/>
       <c r="Z35" s="18"/>
       <c r="AA35" s="18"/>
@@ -4090,24 +4227,24 @@
       <c r="G37" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="H37" s="55" t="s">
+      <c r="H37" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55" t="s">
+      <c r="I37" s="57"/>
+      <c r="J37" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K37" s="55"/>
-      <c r="U37" s="68" t="s">
+      <c r="K37" s="57"/>
+      <c r="U37" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="V37" s="69"/>
-      <c r="W37" s="69"/>
-      <c r="X37" s="69"/>
-      <c r="Y37" s="69"/>
-      <c r="Z37" s="69"/>
-      <c r="AA37" s="69"/>
-      <c r="AB37" s="70"/>
+      <c r="V37" s="72"/>
+      <c r="W37" s="72"/>
+      <c r="X37" s="72"/>
+      <c r="Y37" s="72"/>
+      <c r="Z37" s="72"/>
+      <c r="AA37" s="72"/>
+      <c r="AB37" s="73"/>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
@@ -4122,12 +4259,12 @@
       <c r="E39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U39" s="78" t="s">
+      <c r="U39" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="V39" s="79"/>
-      <c r="W39" s="79"/>
-      <c r="X39" s="80"/>
+      <c r="V39" s="84"/>
+      <c r="W39" s="84"/>
+      <c r="X39" s="85"/>
     </row>
     <row r="40" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C40" s="7">
@@ -4143,40 +4280,40 @@
         <v>3</v>
       </c>
       <c r="G40" s="64"/>
-      <c r="U40" s="81"/>
-      <c r="V40" s="82"/>
-      <c r="W40" s="82"/>
-      <c r="X40" s="83"/>
+      <c r="U40" s="86"/>
+      <c r="V40" s="87"/>
+      <c r="W40" s="87"/>
+      <c r="X40" s="88"/>
     </row>
     <row r="42" spans="2:28" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="69" t="s">
+      <c r="C42" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="69"/>
-      <c r="K42" s="69"/>
-      <c r="L42" s="69"/>
-      <c r="M42" s="69"/>
-      <c r="N42" s="69"/>
-      <c r="O42" s="69"/>
-      <c r="P42" s="69"/>
-      <c r="Q42" s="69"/>
-      <c r="R42" s="69"/>
-      <c r="S42" s="69"/>
-      <c r="U42" s="84" t="s">
+      <c r="D42" s="72"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="72"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="72"/>
+      <c r="N42" s="72"/>
+      <c r="O42" s="72"/>
+      <c r="P42" s="72"/>
+      <c r="Q42" s="72"/>
+      <c r="R42" s="72"/>
+      <c r="S42" s="72"/>
+      <c r="U42" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="V42" s="85"/>
-      <c r="W42" s="85"/>
-      <c r="X42" s="86"/>
+      <c r="V42" s="81"/>
+      <c r="W42" s="81"/>
+      <c r="X42" s="82"/>
     </row>
     <row r="43" spans="2:28" x14ac:dyDescent="0.3">
       <c r="C43" s="12"/>
@@ -4236,16 +4373,16 @@
       <c r="E46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="55" t="s">
+      <c r="F46" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="55"/>
-      <c r="H46" s="74" t="s">
+      <c r="G46" s="57"/>
+      <c r="H46" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="I46" s="74"/>
-      <c r="J46" s="74"/>
-      <c r="K46" s="74"/>
+      <c r="I46" s="90"/>
+      <c r="J46" s="90"/>
+      <c r="K46" s="90"/>
       <c r="U46" s="22" t="s">
         <v>67</v>
       </c>
@@ -4261,24 +4398,24 @@
       <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="55" t="s">
+      <c r="F47" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="55"/>
-      <c r="H47" s="55" t="s">
+      <c r="G47" s="57"/>
+      <c r="H47" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="55"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="55"/>
-      <c r="L47" s="55"/>
-      <c r="M47" s="55"/>
-      <c r="N47" s="55"/>
-      <c r="O47" s="55"/>
-      <c r="P47" s="55"/>
-      <c r="Q47" s="55"/>
-      <c r="R47" s="55"/>
-      <c r="S47" s="55"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="57"/>
+      <c r="M47" s="57"/>
+      <c r="N47" s="57"/>
+      <c r="O47" s="57"/>
+      <c r="P47" s="57"/>
+      <c r="Q47" s="57"/>
+      <c r="R47" s="57"/>
+      <c r="S47" s="57"/>
       <c r="U47" s="23" t="s">
         <v>66</v>
       </c>
@@ -4303,17 +4440,17 @@
       <c r="E49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U49" s="71" t="s">
+      <c r="U49" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="V49" s="72"/>
-      <c r="W49" s="72"/>
-      <c r="X49" s="72"/>
-      <c r="Y49" s="72"/>
-      <c r="Z49" s="72"/>
-      <c r="AA49" s="72"/>
-      <c r="AB49" s="72"/>
-      <c r="AC49" s="73"/>
+      <c r="V49" s="69"/>
+      <c r="W49" s="69"/>
+      <c r="X49" s="69"/>
+      <c r="Y49" s="69"/>
+      <c r="Z49" s="69"/>
+      <c r="AA49" s="69"/>
+      <c r="AB49" s="69"/>
+      <c r="AC49" s="70"/>
     </row>
     <row r="50" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C50" s="7">
@@ -4331,17 +4468,17 @@
       <c r="G50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U50" s="68" t="s">
+      <c r="U50" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="V50" s="69"/>
-      <c r="W50" s="69"/>
-      <c r="X50" s="69"/>
-      <c r="Y50" s="69"/>
-      <c r="Z50" s="69"/>
-      <c r="AA50" s="69"/>
-      <c r="AB50" s="69"/>
-      <c r="AC50" s="70"/>
+      <c r="V50" s="72"/>
+      <c r="W50" s="72"/>
+      <c r="X50" s="72"/>
+      <c r="Y50" s="72"/>
+      <c r="Z50" s="72"/>
+      <c r="AA50" s="72"/>
+      <c r="AB50" s="72"/>
+      <c r="AC50" s="73"/>
     </row>
     <row r="51" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C51" s="7">
@@ -4353,27 +4490,27 @@
       <c r="E51" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="55" t="s">
+      <c r="F51" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="55"/>
-      <c r="H51" s="74" t="s">
+      <c r="G51" s="57"/>
+      <c r="H51" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="74"/>
-      <c r="J51" s="74"/>
-      <c r="K51" s="74"/>
-      <c r="U51" s="68" t="s">
+      <c r="I51" s="90"/>
+      <c r="J51" s="90"/>
+      <c r="K51" s="90"/>
+      <c r="U51" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="V51" s="69"/>
-      <c r="W51" s="69"/>
-      <c r="X51" s="69"/>
-      <c r="Y51" s="69"/>
-      <c r="Z51" s="69"/>
-      <c r="AA51" s="69"/>
-      <c r="AB51" s="69"/>
-      <c r="AC51" s="70"/>
+      <c r="V51" s="72"/>
+      <c r="W51" s="72"/>
+      <c r="X51" s="72"/>
+      <c r="Y51" s="72"/>
+      <c r="Z51" s="72"/>
+      <c r="AA51" s="72"/>
+      <c r="AB51" s="72"/>
+      <c r="AC51" s="73"/>
     </row>
     <row r="52" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C52" s="11">
@@ -4385,24 +4522,24 @@
       <c r="E52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="55" t="s">
+      <c r="F52" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="55"/>
-      <c r="H52" s="55" t="s">
+      <c r="G52" s="57"/>
+      <c r="H52" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="55"/>
-      <c r="J52" s="55"/>
-      <c r="K52" s="55"/>
-      <c r="L52" s="55"/>
-      <c r="M52" s="55"/>
-      <c r="N52" s="55"/>
-      <c r="O52" s="55"/>
-      <c r="P52" s="55"/>
-      <c r="Q52" s="55"/>
-      <c r="R52" s="55"/>
-      <c r="S52" s="55"/>
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="57"/>
+      <c r="N52" s="57"/>
+      <c r="O52" s="57"/>
+      <c r="P52" s="57"/>
+      <c r="Q52" s="57"/>
+      <c r="R52" s="57"/>
+      <c r="S52" s="57"/>
       <c r="U52" s="65" t="s">
         <v>73</v>
       </c>
@@ -4419,36 +4556,36 @@
       <c r="B54" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="69" t="s">
+      <c r="C54" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="69"/>
-      <c r="E54" s="69"/>
-      <c r="F54" s="69"/>
-      <c r="G54" s="69"/>
-      <c r="H54" s="69"/>
-      <c r="I54" s="69"/>
-      <c r="J54" s="69"/>
-      <c r="K54" s="69"/>
-      <c r="L54" s="69"/>
-      <c r="M54" s="69"/>
-      <c r="N54" s="69"/>
-      <c r="O54" s="69"/>
-      <c r="P54" s="69"/>
-      <c r="Q54" s="69"/>
-      <c r="R54" s="69"/>
-      <c r="S54" s="69"/>
-      <c r="U54" s="84" t="s">
+      <c r="D54" s="72"/>
+      <c r="E54" s="72"/>
+      <c r="F54" s="72"/>
+      <c r="G54" s="72"/>
+      <c r="H54" s="72"/>
+      <c r="I54" s="72"/>
+      <c r="J54" s="72"/>
+      <c r="K54" s="72"/>
+      <c r="L54" s="72"/>
+      <c r="M54" s="72"/>
+      <c r="N54" s="72"/>
+      <c r="O54" s="72"/>
+      <c r="P54" s="72"/>
+      <c r="Q54" s="72"/>
+      <c r="R54" s="72"/>
+      <c r="S54" s="72"/>
+      <c r="U54" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="V54" s="85"/>
-      <c r="W54" s="85"/>
-      <c r="X54" s="85"/>
-      <c r="Y54" s="85"/>
-      <c r="Z54" s="85"/>
-      <c r="AA54" s="85"/>
-      <c r="AB54" s="85"/>
-      <c r="AC54" s="86"/>
+      <c r="V54" s="81"/>
+      <c r="W54" s="81"/>
+      <c r="X54" s="81"/>
+      <c r="Y54" s="81"/>
+      <c r="Z54" s="81"/>
+      <c r="AA54" s="81"/>
+      <c r="AB54" s="81"/>
+      <c r="AC54" s="82"/>
     </row>
     <row r="56" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
@@ -4463,17 +4600,17 @@
       <c r="E56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U56" s="71" t="s">
+      <c r="U56" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="V56" s="72"/>
-      <c r="W56" s="72"/>
-      <c r="X56" s="72"/>
-      <c r="Y56" s="72"/>
-      <c r="Z56" s="72"/>
-      <c r="AA56" s="72"/>
-      <c r="AB56" s="72"/>
-      <c r="AC56" s="73"/>
+      <c r="V56" s="69"/>
+      <c r="W56" s="69"/>
+      <c r="X56" s="69"/>
+      <c r="Y56" s="69"/>
+      <c r="Z56" s="69"/>
+      <c r="AA56" s="69"/>
+      <c r="AB56" s="69"/>
+      <c r="AC56" s="70"/>
     </row>
     <row r="57" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C57" s="7">
@@ -4489,17 +4626,17 @@
         <v>3</v>
       </c>
       <c r="G57" s="64"/>
-      <c r="U57" s="68" t="s">
+      <c r="U57" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="V57" s="69"/>
-      <c r="W57" s="69"/>
-      <c r="X57" s="69"/>
-      <c r="Y57" s="69"/>
-      <c r="Z57" s="69"/>
-      <c r="AA57" s="69"/>
-      <c r="AB57" s="69"/>
-      <c r="AC57" s="70"/>
+      <c r="V57" s="72"/>
+      <c r="W57" s="72"/>
+      <c r="X57" s="72"/>
+      <c r="Y57" s="72"/>
+      <c r="Z57" s="72"/>
+      <c r="AA57" s="72"/>
+      <c r="AB57" s="72"/>
+      <c r="AC57" s="73"/>
     </row>
     <row r="58" spans="2:29" x14ac:dyDescent="0.3">
       <c r="C58" s="7">
@@ -4511,14 +4648,14 @@
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="55" t="s">
+      <c r="F58" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G58" s="55"/>
-      <c r="H58" s="55" t="s">
+      <c r="G58" s="57"/>
+      <c r="H58" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I58" s="55"/>
+      <c r="I58" s="57"/>
       <c r="U58" s="65" t="s">
         <v>79</v>
       </c>
@@ -4570,17 +4707,17 @@
         <v>3</v>
       </c>
       <c r="G61" s="64"/>
-      <c r="U61" s="68" t="s">
+      <c r="U61" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="V61" s="69"/>
-      <c r="W61" s="69"/>
-      <c r="X61" s="69"/>
-      <c r="Y61" s="69"/>
-      <c r="Z61" s="69"/>
-      <c r="AA61" s="69"/>
-      <c r="AB61" s="69"/>
-      <c r="AC61" s="70"/>
+      <c r="V61" s="72"/>
+      <c r="W61" s="72"/>
+      <c r="X61" s="72"/>
+      <c r="Y61" s="72"/>
+      <c r="Z61" s="72"/>
+      <c r="AA61" s="72"/>
+      <c r="AB61" s="72"/>
+      <c r="AC61" s="73"/>
     </row>
     <row r="62" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C62" s="7">
@@ -4592,51 +4729,51 @@
       <c r="E62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="55" t="s">
+      <c r="F62" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="55"/>
-      <c r="H62" s="55" t="s">
+      <c r="G62" s="57"/>
+      <c r="H62" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I62" s="55"/>
-      <c r="J62" s="55" t="s">
+      <c r="I62" s="57"/>
+      <c r="J62" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="K62" s="55"/>
-      <c r="U62" s="87" t="s">
+      <c r="K62" s="57"/>
+      <c r="U62" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="V62" s="88"/>
-      <c r="W62" s="88"/>
-      <c r="X62" s="88"/>
-      <c r="Y62" s="88"/>
-      <c r="Z62" s="88"/>
-      <c r="AA62" s="88"/>
-      <c r="AB62" s="88"/>
-      <c r="AC62" s="89"/>
+      <c r="V62" s="75"/>
+      <c r="W62" s="75"/>
+      <c r="X62" s="75"/>
+      <c r="Y62" s="75"/>
+      <c r="Z62" s="75"/>
+      <c r="AA62" s="75"/>
+      <c r="AB62" s="75"/>
+      <c r="AC62" s="76"/>
     </row>
     <row r="63" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="U63" s="87"/>
-      <c r="V63" s="88"/>
-      <c r="W63" s="88"/>
-      <c r="X63" s="88"/>
-      <c r="Y63" s="88"/>
-      <c r="Z63" s="88"/>
-      <c r="AA63" s="88"/>
-      <c r="AB63" s="88"/>
-      <c r="AC63" s="89"/>
+      <c r="U63" s="74"/>
+      <c r="V63" s="75"/>
+      <c r="W63" s="75"/>
+      <c r="X63" s="75"/>
+      <c r="Y63" s="75"/>
+      <c r="Z63" s="75"/>
+      <c r="AA63" s="75"/>
+      <c r="AB63" s="75"/>
+      <c r="AC63" s="76"/>
     </row>
     <row r="64" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="U64" s="90"/>
-      <c r="V64" s="91"/>
-      <c r="W64" s="91"/>
-      <c r="X64" s="91"/>
-      <c r="Y64" s="91"/>
-      <c r="Z64" s="91"/>
-      <c r="AA64" s="91"/>
-      <c r="AB64" s="91"/>
-      <c r="AC64" s="92"/>
+      <c r="U64" s="77"/>
+      <c r="V64" s="78"/>
+      <c r="W64" s="78"/>
+      <c r="X64" s="78"/>
+      <c r="Y64" s="78"/>
+      <c r="Z64" s="78"/>
+      <c r="AA64" s="78"/>
+      <c r="AB64" s="78"/>
+      <c r="AC64" s="79"/>
     </row>
     <row r="65" spans="2:32" x14ac:dyDescent="0.3">
       <c r="U65" s="26"/>
@@ -4662,18 +4799,18 @@
       <c r="E66" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U66" s="71" t="s">
+      <c r="U66" s="68" t="s">
         <v>82</v>
       </c>
-      <c r="V66" s="72"/>
-      <c r="W66" s="72"/>
-      <c r="X66" s="72"/>
-      <c r="Y66" s="72"/>
-      <c r="Z66" s="72"/>
-      <c r="AA66" s="72"/>
-      <c r="AB66" s="72"/>
-      <c r="AC66" s="72"/>
-      <c r="AD66" s="73"/>
+      <c r="V66" s="69"/>
+      <c r="W66" s="69"/>
+      <c r="X66" s="69"/>
+      <c r="Y66" s="69"/>
+      <c r="Z66" s="69"/>
+      <c r="AA66" s="69"/>
+      <c r="AB66" s="69"/>
+      <c r="AC66" s="69"/>
+      <c r="AD66" s="70"/>
     </row>
     <row r="67" spans="2:32" x14ac:dyDescent="0.3">
       <c r="C67" s="7">
@@ -4691,18 +4828,18 @@
       <c r="G67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U67" s="68" t="s">
+      <c r="U67" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="V67" s="69"/>
-      <c r="W67" s="69"/>
-      <c r="X67" s="69"/>
-      <c r="Y67" s="69"/>
-      <c r="Z67" s="69"/>
-      <c r="AA67" s="69"/>
-      <c r="AB67" s="69"/>
-      <c r="AC67" s="69"/>
-      <c r="AD67" s="70"/>
+      <c r="V67" s="72"/>
+      <c r="W67" s="72"/>
+      <c r="X67" s="72"/>
+      <c r="Y67" s="72"/>
+      <c r="Z67" s="72"/>
+      <c r="AA67" s="72"/>
+      <c r="AB67" s="72"/>
+      <c r="AC67" s="72"/>
+      <c r="AD67" s="73"/>
     </row>
     <row r="68" spans="2:32" x14ac:dyDescent="0.3">
       <c r="C68" s="7">
@@ -4730,18 +4867,18 @@
         <v>44</v>
       </c>
       <c r="K68" s="64"/>
-      <c r="U68" s="68" t="s">
+      <c r="U68" s="71" t="s">
         <v>83</v>
       </c>
-      <c r="V68" s="69"/>
-      <c r="W68" s="69"/>
-      <c r="X68" s="69"/>
-      <c r="Y68" s="69"/>
-      <c r="Z68" s="69"/>
-      <c r="AA68" s="69"/>
-      <c r="AB68" s="69"/>
-      <c r="AC68" s="69"/>
-      <c r="AD68" s="70"/>
+      <c r="V68" s="72"/>
+      <c r="W68" s="72"/>
+      <c r="X68" s="72"/>
+      <c r="Y68" s="72"/>
+      <c r="Z68" s="72"/>
+      <c r="AA68" s="72"/>
+      <c r="AB68" s="72"/>
+      <c r="AC68" s="72"/>
+      <c r="AD68" s="73"/>
     </row>
     <row r="69" spans="2:32" x14ac:dyDescent="0.3">
       <c r="C69" s="11">
@@ -4753,10 +4890,10 @@
       <c r="E69" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F69" s="55" t="s">
+      <c r="F69" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="55"/>
+      <c r="G69" s="57"/>
       <c r="H69" s="62" t="s">
         <v>41</v>
       </c>
@@ -4805,13 +4942,13 @@
       <c r="E71" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U71" s="71" t="s">
+      <c r="U71" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="V71" s="72"/>
-      <c r="W71" s="72"/>
-      <c r="X71" s="72"/>
-      <c r="Y71" s="73"/>
+      <c r="V71" s="69"/>
+      <c r="W71" s="69"/>
+      <c r="X71" s="69"/>
+      <c r="Y71" s="70"/>
     </row>
     <row r="72" spans="2:32" x14ac:dyDescent="0.3">
       <c r="C72" s="7">
@@ -4848,18 +4985,18 @@
       <c r="E74" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U74" s="71" t="s">
+      <c r="U74" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="V74" s="72"/>
-      <c r="W74" s="72"/>
-      <c r="X74" s="72"/>
-      <c r="Y74" s="72"/>
-      <c r="Z74" s="72"/>
-      <c r="AA74" s="72"/>
-      <c r="AB74" s="72"/>
-      <c r="AC74" s="72"/>
-      <c r="AD74" s="73"/>
+      <c r="V74" s="69"/>
+      <c r="W74" s="69"/>
+      <c r="X74" s="69"/>
+      <c r="Y74" s="69"/>
+      <c r="Z74" s="69"/>
+      <c r="AA74" s="69"/>
+      <c r="AB74" s="69"/>
+      <c r="AC74" s="69"/>
+      <c r="AD74" s="70"/>
     </row>
     <row r="75" spans="2:32" x14ac:dyDescent="0.3">
       <c r="C75" s="7">
@@ -4875,18 +5012,18 @@
         <v>49</v>
       </c>
       <c r="G75" s="64"/>
-      <c r="U75" s="68" t="s">
+      <c r="U75" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="V75" s="69"/>
-      <c r="W75" s="69"/>
-      <c r="X75" s="69"/>
-      <c r="Y75" s="69"/>
-      <c r="Z75" s="69"/>
-      <c r="AA75" s="69"/>
-      <c r="AB75" s="69"/>
-      <c r="AC75" s="69"/>
-      <c r="AD75" s="70"/>
+      <c r="V75" s="72"/>
+      <c r="W75" s="72"/>
+      <c r="X75" s="72"/>
+      <c r="Y75" s="72"/>
+      <c r="Z75" s="72"/>
+      <c r="AA75" s="72"/>
+      <c r="AB75" s="72"/>
+      <c r="AC75" s="72"/>
+      <c r="AD75" s="73"/>
     </row>
     <row r="76" spans="2:32" x14ac:dyDescent="0.3">
       <c r="C76" s="7">
@@ -4898,14 +5035,14 @@
       <c r="E76" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F76" s="55" t="s">
+      <c r="F76" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="G76" s="55"/>
-      <c r="H76" s="55" t="s">
+      <c r="G76" s="57"/>
+      <c r="H76" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="I76" s="55"/>
+      <c r="I76" s="57"/>
       <c r="J76" s="7" t="s">
         <v>41</v>
       </c>
@@ -4938,20 +5075,20 @@
       <c r="E78" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U78" s="71" t="s">
-        <v>262</v>
-      </c>
-      <c r="V78" s="72"/>
-      <c r="W78" s="72"/>
-      <c r="X78" s="72"/>
-      <c r="Y78" s="72"/>
-      <c r="Z78" s="72"/>
-      <c r="AA78" s="72"/>
-      <c r="AB78" s="72"/>
-      <c r="AC78" s="72"/>
-      <c r="AD78" s="73"/>
+      <c r="U78" s="68" t="s">
+        <v>256</v>
+      </c>
+      <c r="V78" s="69"/>
+      <c r="W78" s="69"/>
+      <c r="X78" s="69"/>
+      <c r="Y78" s="69"/>
+      <c r="Z78" s="69"/>
+      <c r="AA78" s="69"/>
+      <c r="AB78" s="69"/>
+      <c r="AC78" s="69"/>
+      <c r="AD78" s="70"/>
       <c r="AF78" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79" spans="2:32" x14ac:dyDescent="0.3">
@@ -4968,18 +5105,18 @@
         <v>49</v>
       </c>
       <c r="G79" s="64"/>
-      <c r="U79" s="93" t="s">
+      <c r="U79" s="71" t="s">
         <v>87</v>
       </c>
-      <c r="V79" s="95"/>
-      <c r="W79" s="95"/>
-      <c r="X79" s="95"/>
-      <c r="Y79" s="95"/>
-      <c r="Z79" s="95"/>
-      <c r="AA79" s="95"/>
-      <c r="AB79" s="95"/>
-      <c r="AC79" s="95"/>
-      <c r="AD79" s="94"/>
+      <c r="V79" s="72"/>
+      <c r="W79" s="72"/>
+      <c r="X79" s="72"/>
+      <c r="Y79" s="72"/>
+      <c r="Z79" s="72"/>
+      <c r="AA79" s="72"/>
+      <c r="AB79" s="72"/>
+      <c r="AC79" s="72"/>
+      <c r="AD79" s="73"/>
     </row>
     <row r="80" spans="2:32" x14ac:dyDescent="0.3">
       <c r="C80" s="7">
@@ -4991,14 +5128,14 @@
       <c r="E80" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F80" s="55" t="s">
+      <c r="F80" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="G80" s="55"/>
-      <c r="H80" s="55" t="s">
+      <c r="G80" s="57"/>
+      <c r="H80" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="I80" s="55"/>
+      <c r="I80" s="57"/>
       <c r="J80" s="7" t="s">
         <v>41</v>
       </c>
@@ -5006,7 +5143,7 @@
         <v>50</v>
       </c>
       <c r="U80" s="65" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="V80" s="66"/>
       <c r="W80" s="66"/>
@@ -5053,44 +5190,36 @@
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="U72:Y72"/>
-    <mergeCell ref="U74:AD74"/>
-    <mergeCell ref="U75:AD75"/>
-    <mergeCell ref="U76:AD76"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="U71:Y71"/>
-    <mergeCell ref="U56:AC56"/>
-    <mergeCell ref="U57:AC57"/>
-    <mergeCell ref="U58:AC58"/>
-    <mergeCell ref="U61:AC61"/>
-    <mergeCell ref="U62:AC64"/>
-    <mergeCell ref="U66:AD66"/>
-    <mergeCell ref="U67:AD67"/>
-    <mergeCell ref="U68:AD68"/>
-    <mergeCell ref="U69:AD69"/>
-    <mergeCell ref="U49:AC49"/>
-    <mergeCell ref="U50:AC50"/>
-    <mergeCell ref="U51:AC51"/>
-    <mergeCell ref="U52:AC52"/>
-    <mergeCell ref="U54:AC54"/>
-    <mergeCell ref="U39:X40"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="U35:X35"/>
-    <mergeCell ref="U37:AB37"/>
-    <mergeCell ref="U15:X18"/>
-    <mergeCell ref="U21:X24"/>
-    <mergeCell ref="H22:S22"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="P69:S69"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:S47"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:S52"/>
+    <mergeCell ref="C54:S54"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="N69:O69"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="I31:S31"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C42:S42"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="C33:S33"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
     <mergeCell ref="U30:AB30"/>
     <mergeCell ref="U31:AB31"/>
     <mergeCell ref="P7:Q7"/>
@@ -5107,39 +5236,47 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="N7:O7"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="I31:S31"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C42:S42"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="C33:S33"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="P69:S69"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:S47"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:S52"/>
+    <mergeCell ref="U15:X18"/>
+    <mergeCell ref="U21:X24"/>
+    <mergeCell ref="H22:S22"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="U39:X40"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="U37:AB37"/>
+    <mergeCell ref="U49:AC49"/>
+    <mergeCell ref="U50:AC50"/>
+    <mergeCell ref="U51:AC51"/>
+    <mergeCell ref="U52:AC52"/>
+    <mergeCell ref="U54:AC54"/>
+    <mergeCell ref="U71:Y71"/>
+    <mergeCell ref="U56:AC56"/>
+    <mergeCell ref="U57:AC57"/>
+    <mergeCell ref="U58:AC58"/>
+    <mergeCell ref="U61:AC61"/>
+    <mergeCell ref="U62:AC64"/>
+    <mergeCell ref="U66:AD66"/>
+    <mergeCell ref="U67:AD67"/>
+    <mergeCell ref="U68:AD68"/>
+    <mergeCell ref="U69:AD69"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="U72:Y72"/>
+    <mergeCell ref="U74:AD74"/>
+    <mergeCell ref="U75:AD75"/>
+    <mergeCell ref="U76:AD76"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="H80:I80"/>
     <mergeCell ref="U80:AD80"/>
     <mergeCell ref="U79:AD79"/>
     <mergeCell ref="U78:AD78"/>
-    <mergeCell ref="C54:S54"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="N69:O69"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ISA INT xx inplemented and tested in VM
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aroma\Desktop\vcda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar\Documents\Work\AI\CPU\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25699668-1906-4AAA-A14B-9D1E1C653848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE24D589-73DA-43F8-9E5B-3004D956A890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
+    <workbookView xWindow="23468" yWindow="0" windowWidth="15015" windowHeight="20963" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="270">
   <si>
     <t>POP</t>
   </si>
@@ -1181,12 +1181,30 @@
       <t>// 4 decimal precision float</t>
     </r>
   </si>
+  <si>
+    <t>R251</t>
+  </si>
+  <si>
+    <t>Interrupt Table Pointer</t>
+  </si>
+  <si>
+    <t>ITP</t>
+  </si>
+  <si>
+    <t>Base Pointer</t>
+  </si>
+  <si>
+    <t>Stack Pointer</t>
+  </si>
+  <si>
+    <t>Instruction Pointer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1252,6 +1270,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1857,15 +1882,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1887,6 +1913,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1896,25 +1934,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1932,47 +1997,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2309,28 +2336,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CDEC23-057C-4C1E-AB18-5AC9130DB945}">
   <dimension ref="B3:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="6.109375" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.21875" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
-    <col min="10" max="17" width="4.5546875" customWidth="1"/>
+    <col min="3" max="3" width="6.1328125" customWidth="1"/>
+    <col min="4" max="4" width="4.86328125" customWidth="1"/>
+    <col min="5" max="5" width="3.1328125" customWidth="1"/>
+    <col min="6" max="6" width="9.265625" customWidth="1"/>
+    <col min="7" max="7" width="21.73046875" customWidth="1"/>
+    <col min="8" max="8" width="5.86328125" customWidth="1"/>
+    <col min="9" max="9" width="14.19921875" customWidth="1"/>
+    <col min="10" max="17" width="4.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C4" s="27" t="s">
         <v>99</v>
       </c>
@@ -2346,24 +2373,24 @@
       <c r="I4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="58">
+      <c r="J4" s="59">
         <v>0</v>
       </c>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56">
+      <c r="K4" s="58"/>
+      <c r="L4" s="58">
         <v>1</v>
       </c>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56">
+      <c r="M4" s="58"/>
+      <c r="N4" s="58">
         <v>2</v>
       </c>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56">
+      <c r="O4" s="58"/>
+      <c r="P4" s="58">
         <v>3</v>
       </c>
-      <c r="Q4" s="56"/>
-    </row>
-    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q4" s="58"/>
+    </row>
+    <row r="5" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C5" s="27" t="s">
         <v>100</v>
       </c>
@@ -2404,49 +2431,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B8" s="27" t="s">
         <v>103</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="57" t="s">
+      <c r="J8" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57" t="s">
+      <c r="K8" s="56"/>
+      <c r="L8" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57" t="s">
+      <c r="M8" s="56"/>
+      <c r="N8" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="O8" s="57"/>
-      <c r="P8" s="57" t="s">
+      <c r="O8" s="56"/>
+      <c r="P8" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="57"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q8" s="56"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="55" t="s">
+      <c r="F9" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="55"/>
+      <c r="G9" s="57"/>
       <c r="H9" s="8"/>
       <c r="I9" s="28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="55"/>
-      <c r="G10" s="55"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="8"/>
       <c r="J10" t="s">
         <v>30</v>
@@ -2458,12 +2485,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="8"/>
       <c r="J11" t="s">
         <v>124</v>
@@ -2475,7 +2502,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
       <c r="J12" t="s">
         <v>125</v>
       </c>
@@ -2486,7 +2513,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>114</v>
       </c>
@@ -2503,7 +2530,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>113</v>
       </c>
@@ -2514,7 +2541,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
         <v>112</v>
       </c>
@@ -2522,7 +2549,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>111</v>
       </c>
@@ -2532,34 +2559,34 @@
       <c r="I16" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="57" t="s">
+      <c r="J16" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57" t="s">
+      <c r="K16" s="56"/>
+      <c r="L16" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57" t="s">
+      <c r="M16" s="56"/>
+      <c r="N16" s="56" t="s">
         <v>129</v>
       </c>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
-    </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I17" s="28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="55" t="s">
+      <c r="F18" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="G18" s="55"/>
+      <c r="G18" s="57"/>
       <c r="H18" s="8"/>
       <c r="J18" t="s">
         <v>127</v>
@@ -2571,12 +2598,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
       <c r="H19" s="8"/>
       <c r="J19" t="s">
         <v>126</v>
@@ -2588,12 +2615,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
-        <v>123</v>
-      </c>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
+        <v>264</v>
+      </c>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
       <c r="H20" s="8"/>
       <c r="J20" t="s">
         <v>129</v>
@@ -2605,46 +2632,46 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>122</v>
-      </c>
-      <c r="F22" t="s">
-        <v>117</v>
-      </c>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I22" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="J22" s="57" t="s">
+      <c r="J22" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="57" t="s">
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56" t="s">
         <v>130</v>
       </c>
-      <c r="O22" s="57"/>
-      <c r="P22" s="57"/>
-      <c r="Q22" s="57"/>
-    </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="56"/>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F23" t="s">
-        <v>118</v>
+        <v>266</v>
+      </c>
+      <c r="G23" s="94" t="s">
+        <v>265</v>
       </c>
       <c r="I23" s="28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F24" t="s">
-        <v>119</v>
+        <v>117</v>
+      </c>
+      <c r="G24" t="s">
+        <v>267</v>
       </c>
       <c r="J24" t="s">
         <v>128</v>
@@ -2656,7 +2683,16 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F25" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" t="s">
+        <v>268</v>
+      </c>
       <c r="J25" t="s">
         <v>130</v>
       </c>
@@ -2667,29 +2703,40 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.45">
+      <c r="C26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I28" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="J28" s="57" t="s">
+      <c r="J28" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57" t="s">
+      <c r="K28" s="56"/>
+      <c r="L28" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
-    </row>
-    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I29" s="28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:17" x14ac:dyDescent="0.45">
       <c r="J30" t="s">
         <v>131</v>
       </c>
@@ -2697,7 +2744,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:17" x14ac:dyDescent="0.45">
       <c r="J31" t="s">
         <v>132</v>
       </c>
@@ -2707,13 +2754,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:Q28"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:Q16"/>
     <mergeCell ref="F9:G11"/>
     <mergeCell ref="F18:G20"/>
     <mergeCell ref="P4:Q4"/>
@@ -2724,6 +2764,13 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:Q28"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2733,20 +2780,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A222D11D-FBDB-42C8-93C4-B5D16645D996}">
   <dimension ref="A3:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.88671875" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="34.86328125" customWidth="1"/>
+    <col min="7" max="7" width="7.46484375" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
         <v>127</v>
       </c>
@@ -2754,10 +2801,10 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="27"/>
     </row>
-    <row r="5" spans="1:16" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" s="27" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="40" t="s">
         <v>147</v>
       </c>
@@ -2771,18 +2818,18 @@
       <c r="H5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="56">
+      <c r="I5" s="58">
         <v>0</v>
       </c>
-      <c r="J5" s="56"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-    </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+    </row>
+    <row r="6" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="37" t="s">
         <v>13</v>
       </c>
@@ -2812,7 +2859,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
@@ -2823,7 +2870,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B8" s="33" t="s">
         <v>153</v>
       </c>
@@ -2834,7 +2881,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B9" s="33" t="s">
         <v>22</v>
       </c>
@@ -2845,16 +2892,16 @@
         <v>156</v>
       </c>
       <c r="H9" s="27"/>
-      <c r="I9" s="62" t="s">
+      <c r="I9" s="63" t="s">
         <v>236</v>
       </c>
-      <c r="J9" s="63"/>
-      <c r="K9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="65"/>
       <c r="L9" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B10" s="33" t="s">
         <v>29</v>
       </c>
@@ -2868,7 +2915,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B11" s="33" t="s">
         <v>159</v>
       </c>
@@ -2883,7 +2930,7 @@
       </c>
       <c r="J11" s="52"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B12" s="33" t="s">
         <v>9</v>
       </c>
@@ -2898,7 +2945,7 @@
       </c>
       <c r="J12" s="52"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
@@ -2913,7 +2960,7 @@
       </c>
       <c r="J13" s="52"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B14" s="33" t="s">
         <v>39</v>
       </c>
@@ -2927,7 +2974,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B15" s="33" t="s">
         <v>46</v>
       </c>
@@ -2941,7 +2988,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B16" s="33" t="s">
         <v>48</v>
       </c>
@@ -2955,7 +3002,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B17" s="33" t="s">
         <v>172</v>
       </c>
@@ -2965,13 +3012,12 @@
       <c r="D17" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="E17" s="93"/>
       <c r="I17" s="54" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="94" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B18" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="7" t="s">
@@ -2980,12 +3026,11 @@
       <c r="D18" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="E18" s="93"/>
       <c r="I18" s="54" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B19" s="33" t="s">
         <v>14</v>
       </c>
@@ -2999,7 +3044,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B20" s="33" t="s">
         <v>15</v>
       </c>
@@ -3010,7 +3055,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B21" s="10" t="s">
         <v>97</v>
       </c>
@@ -3030,7 +3075,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="27" t="s">
         <v>131</v>
       </c>
@@ -3038,17 +3083,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G24" s="93"/>
-      <c r="H24" s="93"/>
-      <c r="I24" s="93"/>
-      <c r="J24" s="93"/>
-      <c r="K24" s="93"/>
-      <c r="L24" s="93"/>
-      <c r="M24" s="93"/>
-      <c r="N24" s="93"/>
-    </row>
-    <row r="25" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="25" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B25" s="40" t="s">
         <v>147</v>
       </c>
@@ -3056,12 +3092,8 @@
         <v>183</v>
       </c>
       <c r="D25" s="42"/>
-      <c r="G25" s="93"/>
-      <c r="L25" s="93"/>
-      <c r="M25" s="93"/>
-      <c r="N25" s="93"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B26" s="37" t="s">
         <v>13</v>
       </c>
@@ -3069,12 +3101,8 @@
         <v>184</v>
       </c>
       <c r="D26" s="39"/>
-      <c r="G26" s="93"/>
-      <c r="L26" s="93"/>
-      <c r="M26" s="93"/>
-      <c r="N26" s="93"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B27" s="33" t="s">
         <v>19</v>
       </c>
@@ -3082,16 +3110,8 @@
         <v>185</v>
       </c>
       <c r="D27" s="34"/>
-      <c r="G27" s="93"/>
-      <c r="H27" s="93"/>
-      <c r="I27" s="93"/>
-      <c r="J27" s="93"/>
-      <c r="K27" s="93"/>
-      <c r="L27" s="93"/>
-      <c r="M27" s="93"/>
-      <c r="N27" s="93"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B28" s="33" t="s">
         <v>153</v>
       </c>
@@ -3099,16 +3119,8 @@
         <v>186</v>
       </c>
       <c r="D28" s="34"/>
-      <c r="G28" s="93"/>
-      <c r="H28" s="93"/>
-      <c r="I28" s="93"/>
-      <c r="J28" s="93"/>
-      <c r="K28" s="93"/>
-      <c r="L28" s="93"/>
-      <c r="M28" s="93"/>
-      <c r="N28" s="93"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B29" s="33" t="s">
         <v>22</v>
       </c>
@@ -3116,16 +3128,8 @@
         <v>187</v>
       </c>
       <c r="D29" s="34"/>
-      <c r="G29" s="93"/>
-      <c r="H29" s="93"/>
-      <c r="I29" s="93"/>
-      <c r="J29" s="93"/>
-      <c r="K29" s="93"/>
-      <c r="L29" s="93"/>
-      <c r="M29" s="93"/>
-      <c r="N29" s="93"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B30" s="33" t="s">
         <v>29</v>
       </c>
@@ -3133,16 +3137,8 @@
         <v>188</v>
       </c>
       <c r="D30" s="34"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="93"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="93"/>
-      <c r="L30" s="93"/>
-      <c r="M30" s="93"/>
-      <c r="N30" s="93"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B31" s="33" t="s">
         <v>159</v>
       </c>
@@ -3150,16 +3146,8 @@
         <v>189</v>
       </c>
       <c r="D31" s="34"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="93"/>
-      <c r="J31" s="93"/>
-      <c r="K31" s="93"/>
-      <c r="L31" s="93"/>
-      <c r="M31" s="93"/>
-      <c r="N31" s="93"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B32" s="33" t="s">
         <v>9</v>
       </c>
@@ -3167,16 +3155,8 @@
         <v>190</v>
       </c>
       <c r="D32" s="34"/>
-      <c r="G32" s="93"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="93"/>
-      <c r="J32" s="93"/>
-      <c r="K32" s="93"/>
-      <c r="L32" s="93"/>
-      <c r="M32" s="93"/>
-      <c r="N32" s="93"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B33" s="33" t="s">
         <v>2</v>
       </c>
@@ -3184,16 +3164,8 @@
         <v>191</v>
       </c>
       <c r="D33" s="34"/>
-      <c r="G33" s="93"/>
-      <c r="H33" s="93"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="93"/>
-      <c r="L33" s="93"/>
-      <c r="M33" s="93"/>
-      <c r="N33" s="93"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B34" s="33" t="s">
         <v>39</v>
       </c>
@@ -3201,16 +3173,8 @@
         <v>192</v>
       </c>
       <c r="D34" s="34"/>
-      <c r="G34" s="93"/>
-      <c r="H34" s="93"/>
-      <c r="I34" s="93"/>
-      <c r="J34" s="93"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="93"/>
-      <c r="N34" s="93"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B35" s="33" t="s">
         <v>46</v>
       </c>
@@ -3218,16 +3182,8 @@
         <v>193</v>
       </c>
       <c r="D35" s="34"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
-      <c r="K35" s="93"/>
-      <c r="L35" s="93"/>
-      <c r="M35" s="93"/>
-      <c r="N35" s="93"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B36" s="33" t="s">
         <v>48</v>
       </c>
@@ -3235,16 +3191,8 @@
         <v>194</v>
       </c>
       <c r="D36" s="34"/>
-      <c r="G36" s="93"/>
-      <c r="H36" s="93"/>
-      <c r="I36" s="93"/>
-      <c r="J36" s="93"/>
-      <c r="K36" s="93"/>
-      <c r="L36" s="93"/>
-      <c r="M36" s="93"/>
-      <c r="N36" s="93"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B37" s="33" t="s">
         <v>172</v>
       </c>
@@ -3252,16 +3200,8 @@
         <v>195</v>
       </c>
       <c r="D37" s="34"/>
-      <c r="G37" s="93"/>
-      <c r="H37" s="93"/>
-      <c r="I37" s="93"/>
-      <c r="J37" s="93"/>
-      <c r="K37" s="93"/>
-      <c r="L37" s="93"/>
-      <c r="M37" s="93"/>
-      <c r="N37" s="93"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B38" s="33" t="s">
         <v>4</v>
       </c>
@@ -3269,16 +3209,8 @@
         <v>196</v>
       </c>
       <c r="D38" s="34"/>
-      <c r="G38" s="93"/>
-      <c r="H38" s="93"/>
-      <c r="I38" s="93"/>
-      <c r="J38" s="93"/>
-      <c r="K38" s="93"/>
-      <c r="L38" s="93"/>
-      <c r="M38" s="93"/>
-      <c r="N38" s="93"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B39" s="33" t="s">
         <v>14</v>
       </c>
@@ -3286,16 +3218,8 @@
         <v>197</v>
       </c>
       <c r="D39" s="34"/>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
-      <c r="L39" s="93"/>
-      <c r="M39" s="93"/>
-      <c r="N39" s="93"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B40" s="33" t="s">
         <v>15</v>
       </c>
@@ -3303,16 +3227,8 @@
         <v>198</v>
       </c>
       <c r="D40" s="34"/>
-      <c r="G40" s="93"/>
-      <c r="H40" s="93"/>
-      <c r="I40" s="93"/>
-      <c r="J40" s="93"/>
-      <c r="K40" s="93"/>
-      <c r="L40" s="93"/>
-      <c r="M40" s="93"/>
-      <c r="N40" s="93"/>
-    </row>
-    <row r="41" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B41" s="10" t="s">
         <v>97</v>
       </c>
@@ -3320,55 +3236,19 @@
         <v>199</v>
       </c>
       <c r="D41" s="36"/>
-      <c r="G41" s="93"/>
-      <c r="H41" s="93"/>
-      <c r="I41" s="93"/>
-      <c r="J41" s="93"/>
-      <c r="K41" s="93"/>
-      <c r="L41" s="93"/>
-      <c r="M41" s="93"/>
-      <c r="N41" s="93"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G42" s="93"/>
-      <c r="H42" s="93"/>
-      <c r="I42" s="93"/>
-      <c r="J42" s="93"/>
-      <c r="K42" s="93"/>
-      <c r="L42" s="93"/>
-      <c r="M42" s="93"/>
-      <c r="N42" s="93"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="93"/>
-      <c r="J43" s="93"/>
-      <c r="K43" s="93"/>
-      <c r="L43" s="93"/>
-      <c r="M43" s="93"/>
-      <c r="N43" s="93"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="27" t="s">
         <v>228</v>
       </c>
       <c r="B44" t="s">
         <v>227</v>
       </c>
-      <c r="G44" s="93"/>
-      <c r="H44" s="93"/>
-      <c r="I44" s="93"/>
-      <c r="J44" s="93"/>
-      <c r="K44" s="93"/>
-      <c r="L44" s="93"/>
-      <c r="M44" s="93"/>
-      <c r="N44" s="93"/>
-    </row>
-    <row r="45" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A45" s="27"/>
     </row>
-    <row r="46" spans="1:14" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" s="27" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B46" s="29" t="s">
         <v>147</v>
       </c>
@@ -3379,7 +3259,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B47" s="9" t="s">
         <v>13</v>
       </c>
@@ -3390,7 +3270,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B48" s="33" t="s">
         <v>19</v>
       </c>
@@ -3401,7 +3281,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B49" s="33" t="s">
         <v>153</v>
       </c>
@@ -3412,7 +3292,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B50" s="33" t="s">
         <v>22</v>
       </c>
@@ -3423,7 +3303,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B51" s="33" t="s">
         <v>29</v>
       </c>
@@ -3434,7 +3314,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B52" s="33" t="s">
         <v>159</v>
       </c>
@@ -3445,7 +3325,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B53" s="33" t="s">
         <v>9</v>
       </c>
@@ -3456,7 +3336,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B54" s="33" t="s">
         <v>2</v>
       </c>
@@ -3467,7 +3347,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B55" s="33" t="s">
         <v>39</v>
       </c>
@@ -3478,7 +3358,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B56" s="33" t="s">
         <v>46</v>
       </c>
@@ -3489,7 +3369,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B57" s="33" t="s">
         <v>48</v>
       </c>
@@ -3500,7 +3380,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B58" s="33" t="s">
         <v>172</v>
       </c>
@@ -3511,7 +3391,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B59" s="10" t="s">
         <v>225</v>
       </c>
@@ -3520,7 +3400,7 @@
       </c>
       <c r="D59" s="36"/>
     </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A61" s="27" t="s">
         <v>229</v>
       </c>
@@ -3528,7 +3408,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B62" s="45" t="s">
         <v>147</v>
       </c>
@@ -3539,7 +3419,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B63" s="37" t="s">
         <v>13</v>
       </c>
@@ -3550,7 +3430,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B64" s="10" t="s">
         <v>19</v>
       </c>
@@ -3579,82 +3459,82 @@
       <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.21875" customWidth="1"/>
-    <col min="4" max="6" width="4.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.77734375" style="15" customWidth="1"/>
-    <col min="8" max="10" width="4.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="4.77734375" style="15" customWidth="1"/>
-    <col min="12" max="19" width="4.77734375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="2.109375" customWidth="1"/>
-    <col min="28" max="28" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="5.19921875" customWidth="1"/>
+    <col min="4" max="6" width="4.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.796875" style="15" customWidth="1"/>
+    <col min="8" max="10" width="4.796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="4.796875" style="15" customWidth="1"/>
+    <col min="12" max="19" width="4.796875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="2.1328125" customWidth="1"/>
+    <col min="28" max="28" width="11.53125" customWidth="1"/>
     <col min="29" max="29" width="12.33203125" customWidth="1"/>
     <col min="30" max="30" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="91" t="s">
+      <c r="C7" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="59">
         <v>0</v>
       </c>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56">
+      <c r="E7" s="58"/>
+      <c r="F7" s="58">
         <v>1</v>
       </c>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56">
+      <c r="G7" s="58"/>
+      <c r="H7" s="58">
         <v>2</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56">
+      <c r="I7" s="58"/>
+      <c r="J7" s="58">
         <v>3</v>
       </c>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56">
+      <c r="K7" s="58"/>
+      <c r="L7" s="58">
         <v>4</v>
       </c>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56">
+      <c r="M7" s="58"/>
+      <c r="N7" s="58">
         <v>5</v>
       </c>
-      <c r="O7" s="56"/>
-      <c r="P7" s="56">
+      <c r="O7" s="58"/>
+      <c r="P7" s="58">
         <v>6</v>
       </c>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56">
+      <c r="Q7" s="58"/>
+      <c r="R7" s="58">
         <v>7</v>
       </c>
-      <c r="S7" s="89"/>
-    </row>
-    <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S7" s="73"/>
+    </row>
+    <row r="8" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="92"/>
+      <c r="C8" s="77"/>
       <c r="D8" s="4">
         <v>0</v>
       </c>
@@ -3704,15 +3584,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>90</v>
       </c>
@@ -3723,7 +3603,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>91</v>
       </c>
@@ -3734,7 +3614,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>92</v>
       </c>
@@ -3745,10 +3625,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -3761,17 +3641,17 @@
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="55" t="s">
+      <c r="U15" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="V15" s="55"/>
-      <c r="W15" s="55"/>
-      <c r="X15" s="55"/>
+      <c r="V15" s="57"/>
+      <c r="W15" s="57"/>
+      <c r="X15" s="57"/>
       <c r="AA15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="C16" s="7">
         <v>2</v>
       </c>
@@ -3787,15 +3667,15 @@
       <c r="G16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U16" s="55"/>
-      <c r="V16" s="55"/>
-      <c r="W16" s="55"/>
-      <c r="X16" s="55"/>
+      <c r="U16" s="57"/>
+      <c r="V16" s="57"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
       <c r="AA16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C17" s="7">
         <v>4</v>
       </c>
@@ -3823,15 +3703,15 @@
       <c r="K17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="55"/>
-      <c r="V17" s="55"/>
-      <c r="W17" s="55"/>
-      <c r="X17" s="55"/>
+      <c r="U17" s="57"/>
+      <c r="V17" s="57"/>
+      <c r="W17" s="57"/>
+      <c r="X17" s="57"/>
       <c r="AA17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C18" s="7">
         <v>8</v>
       </c>
@@ -3883,17 +3763,17 @@
       <c r="S18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="55"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="55"/>
-      <c r="X18" s="55"/>
-    </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="U18" s="57"/>
+      <c r="V18" s="57"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="57"/>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -3906,14 +3786,14 @@
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U21" s="55" t="s">
+      <c r="U21" s="57" t="s">
         <v>247</v>
       </c>
-      <c r="V21" s="55"/>
-      <c r="W21" s="55"/>
-      <c r="X21" s="55"/>
-    </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V21" s="57"/>
+      <c r="W21" s="57"/>
+      <c r="X21" s="57"/>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C22" s="7">
         <v>2</v>
       </c>
@@ -3929,26 +3809,26 @@
       <c r="G22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="71" t="s">
+      <c r="H22" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="72"/>
-      <c r="N22" s="72"/>
-      <c r="O22" s="72"/>
-      <c r="P22" s="72"/>
-      <c r="Q22" s="72"/>
-      <c r="R22" s="72"/>
-      <c r="S22" s="72"/>
-      <c r="U22" s="55"/>
-      <c r="V22" s="55"/>
-      <c r="W22" s="55"/>
-      <c r="X22" s="55"/>
-    </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="67"/>
+      <c r="P22" s="67"/>
+      <c r="Q22" s="67"/>
+      <c r="R22" s="67"/>
+      <c r="S22" s="67"/>
+      <c r="U22" s="57"/>
+      <c r="V22" s="57"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C23" s="7">
         <v>4</v>
       </c>
@@ -3961,60 +3841,60 @@
       <c r="F23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="62" t="s">
+      <c r="G23" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="64"/>
-      <c r="U23" s="55"/>
-      <c r="V23" s="55"/>
-      <c r="W23" s="55"/>
-      <c r="X23" s="55"/>
-    </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.3">
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="U24" s="55"/>
-      <c r="V24" s="55"/>
-      <c r="W24" s="55"/>
-      <c r="X24" s="55"/>
-    </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="65"/>
+      <c r="U23" s="57"/>
+      <c r="V23" s="57"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.45">
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="U24" s="57"/>
+      <c r="V24" s="57"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="57"/>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="72" t="s">
+      <c r="C26" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="72"/>
-      <c r="K26" s="72"/>
-      <c r="L26" s="72"/>
-      <c r="M26" s="72"/>
-      <c r="N26" s="72"/>
-      <c r="O26" s="72"/>
-      <c r="P26" s="72"/>
-      <c r="Q26" s="72"/>
-      <c r="R26" s="72"/>
-      <c r="S26" s="72"/>
-      <c r="U26" s="61" t="s">
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="67"/>
+      <c r="P26" s="67"/>
+      <c r="Q26" s="67"/>
+      <c r="R26" s="67"/>
+      <c r="S26" s="67"/>
+      <c r="U26" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="V26" s="61"/>
-      <c r="W26" s="61"/>
-      <c r="X26" s="61"/>
-    </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V26" s="62"/>
+      <c r="W26" s="62"/>
+      <c r="X26" s="62"/>
+    </row>
+    <row r="28" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>21</v>
       </c>
@@ -4027,18 +3907,18 @@
       <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U28" s="68" t="s">
+      <c r="U28" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="V28" s="69"/>
-      <c r="W28" s="69"/>
-      <c r="X28" s="69"/>
+      <c r="V28" s="75"/>
+      <c r="W28" s="75"/>
+      <c r="X28" s="75"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
       <c r="AB28" s="19"/>
     </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C29" s="7">
         <v>2</v>
       </c>
@@ -4054,15 +3934,15 @@
       <c r="G29" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="71" t="s">
+      <c r="U29" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="V29" s="72"/>
-      <c r="W29" s="72"/>
-      <c r="X29" s="72"/>
+      <c r="V29" s="67"/>
+      <c r="W29" s="67"/>
+      <c r="X29" s="67"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C30" s="7">
         <v>4</v>
       </c>
@@ -4075,27 +3955,27 @@
       <c r="F30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="57" t="s">
+      <c r="G30" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="57"/>
-      <c r="I30" s="90" t="s">
+      <c r="H30" s="56"/>
+      <c r="I30" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="90"/>
-      <c r="K30" s="90"/>
-      <c r="U30" s="71" t="s">
+      <c r="J30" s="66"/>
+      <c r="K30" s="66"/>
+      <c r="U30" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="V30" s="72"/>
-      <c r="W30" s="72"/>
-      <c r="X30" s="72"/>
-      <c r="Y30" s="72"/>
-      <c r="Z30" s="72"/>
-      <c r="AA30" s="72"/>
-      <c r="AB30" s="73"/>
-    </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V30" s="67"/>
+      <c r="W30" s="67"/>
+      <c r="X30" s="67"/>
+      <c r="Y30" s="67"/>
+      <c r="Z30" s="67"/>
+      <c r="AA30" s="67"/>
+      <c r="AB30" s="69"/>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C31" s="7">
         <v>8</v>
       </c>
@@ -4108,65 +3988,65 @@
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="57" t="s">
+      <c r="G31" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57" t="s">
+      <c r="H31" s="56"/>
+      <c r="I31" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="57"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="57"/>
-      <c r="P31" s="57"/>
-      <c r="Q31" s="57"/>
-      <c r="R31" s="57"/>
-      <c r="S31" s="57"/>
-      <c r="U31" s="65" t="s">
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="56"/>
+      <c r="S31" s="56"/>
+      <c r="U31" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="V31" s="66"/>
-      <c r="W31" s="66"/>
-      <c r="X31" s="66"/>
-      <c r="Y31" s="66"/>
-      <c r="Z31" s="66"/>
-      <c r="AA31" s="66"/>
-      <c r="AB31" s="67"/>
-    </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V31" s="71"/>
+      <c r="W31" s="71"/>
+      <c r="X31" s="71"/>
+      <c r="Y31" s="71"/>
+      <c r="Z31" s="71"/>
+      <c r="AA31" s="71"/>
+      <c r="AB31" s="72"/>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="72" t="s">
+      <c r="C33" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
-      <c r="J33" s="72"/>
-      <c r="K33" s="72"/>
-      <c r="L33" s="72"/>
-      <c r="M33" s="72"/>
-      <c r="N33" s="72"/>
-      <c r="O33" s="72"/>
-      <c r="P33" s="72"/>
-      <c r="Q33" s="72"/>
-      <c r="R33" s="72"/>
-      <c r="S33" s="72"/>
-      <c r="U33" s="80" t="s">
+      <c r="D33" s="67"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="67"/>
+      <c r="K33" s="67"/>
+      <c r="L33" s="67"/>
+      <c r="M33" s="67"/>
+      <c r="N33" s="67"/>
+      <c r="O33" s="67"/>
+      <c r="P33" s="67"/>
+      <c r="Q33" s="67"/>
+      <c r="R33" s="67"/>
+      <c r="S33" s="67"/>
+      <c r="U33" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="V33" s="81"/>
-      <c r="W33" s="81"/>
-      <c r="X33" s="82"/>
-    </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V33" s="85"/>
+      <c r="W33" s="85"/>
+      <c r="X33" s="86"/>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>27</v>
       </c>
@@ -4179,18 +4059,18 @@
       <c r="E35" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="U35" s="68" t="s">
+      <c r="U35" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="V35" s="69"/>
-      <c r="W35" s="69"/>
-      <c r="X35" s="69"/>
+      <c r="V35" s="75"/>
+      <c r="W35" s="75"/>
+      <c r="X35" s="75"/>
       <c r="Y35" s="18"/>
       <c r="Z35" s="18"/>
       <c r="AA35" s="18"/>
       <c r="AB35" s="19"/>
     </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C36" s="7">
         <v>2</v>
       </c>
@@ -4211,7 +4091,7 @@
       </c>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C37" s="7">
         <v>4</v>
       </c>
@@ -4227,26 +4107,26 @@
       <c r="G37" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="H37" s="57" t="s">
+      <c r="H37" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57" t="s">
+      <c r="I37" s="56"/>
+      <c r="J37" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K37" s="57"/>
-      <c r="U37" s="71" t="s">
+      <c r="K37" s="56"/>
+      <c r="U37" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="V37" s="72"/>
-      <c r="W37" s="72"/>
-      <c r="X37" s="72"/>
-      <c r="Y37" s="72"/>
-      <c r="Z37" s="72"/>
-      <c r="AA37" s="72"/>
-      <c r="AB37" s="73"/>
-    </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V37" s="67"/>
+      <c r="W37" s="67"/>
+      <c r="X37" s="67"/>
+      <c r="Y37" s="67"/>
+      <c r="Z37" s="67"/>
+      <c r="AA37" s="67"/>
+      <c r="AB37" s="69"/>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>30</v>
       </c>
@@ -4259,14 +4139,14 @@
       <c r="E39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U39" s="83" t="s">
+      <c r="U39" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="V39" s="84"/>
-      <c r="W39" s="84"/>
-      <c r="X39" s="85"/>
-    </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V39" s="79"/>
+      <c r="W39" s="79"/>
+      <c r="X39" s="80"/>
+    </row>
+    <row r="40" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C40" s="7">
         <v>2</v>
       </c>
@@ -4276,49 +4156,49 @@
       <c r="E40" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F40" s="62" t="s">
+      <c r="F40" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G40" s="64"/>
-      <c r="U40" s="86"/>
-      <c r="V40" s="87"/>
-      <c r="W40" s="87"/>
-      <c r="X40" s="88"/>
-    </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="G40" s="65"/>
+      <c r="U40" s="81"/>
+      <c r="V40" s="82"/>
+      <c r="W40" s="82"/>
+      <c r="X40" s="83"/>
+    </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="72" t="s">
+      <c r="C42" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="72"/>
-      <c r="E42" s="72"/>
-      <c r="F42" s="72"/>
-      <c r="G42" s="72"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="72"/>
-      <c r="M42" s="72"/>
-      <c r="N42" s="72"/>
-      <c r="O42" s="72"/>
-      <c r="P42" s="72"/>
-      <c r="Q42" s="72"/>
-      <c r="R42" s="72"/>
-      <c r="S42" s="72"/>
-      <c r="U42" s="80" t="s">
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="67"/>
+      <c r="K42" s="67"/>
+      <c r="L42" s="67"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="67"/>
+      <c r="O42" s="67"/>
+      <c r="P42" s="67"/>
+      <c r="Q42" s="67"/>
+      <c r="R42" s="67"/>
+      <c r="S42" s="67"/>
+      <c r="U42" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="V42" s="81"/>
-      <c r="W42" s="81"/>
-      <c r="X42" s="82"/>
-    </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V42" s="85"/>
+      <c r="W42" s="85"/>
+      <c r="X42" s="86"/>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C43" s="12"/>
     </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>33</v>
       </c>
@@ -4342,7 +4222,7 @@
       <c r="AA44" s="18"/>
       <c r="AB44" s="19"/>
     </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C45" s="7">
         <v>2</v>
       </c>
@@ -4363,7 +4243,7 @@
       </c>
       <c r="AB45" s="20"/>
     </row>
-    <row r="46" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C46" s="7">
         <v>4</v>
       </c>
@@ -4373,22 +4253,22 @@
       <c r="E46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="57" t="s">
+      <c r="F46" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="57"/>
-      <c r="H46" s="90" t="s">
+      <c r="G46" s="56"/>
+      <c r="H46" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="I46" s="90"/>
-      <c r="J46" s="90"/>
-      <c r="K46" s="90"/>
+      <c r="I46" s="66"/>
+      <c r="J46" s="66"/>
+      <c r="K46" s="66"/>
       <c r="U46" s="22" t="s">
         <v>67</v>
       </c>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C47" s="11">
         <v>8</v>
       </c>
@@ -4398,24 +4278,24 @@
       <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="57" t="s">
+      <c r="F47" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57" t="s">
+      <c r="G47" s="56"/>
+      <c r="H47" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="57"/>
-      <c r="J47" s="57"/>
-      <c r="K47" s="57"/>
-      <c r="L47" s="57"/>
-      <c r="M47" s="57"/>
-      <c r="N47" s="57"/>
-      <c r="O47" s="57"/>
-      <c r="P47" s="57"/>
-      <c r="Q47" s="57"/>
-      <c r="R47" s="57"/>
-      <c r="S47" s="57"/>
+      <c r="I47" s="56"/>
+      <c r="J47" s="56"/>
+      <c r="K47" s="56"/>
+      <c r="L47" s="56"/>
+      <c r="M47" s="56"/>
+      <c r="N47" s="56"/>
+      <c r="O47" s="56"/>
+      <c r="P47" s="56"/>
+      <c r="Q47" s="56"/>
+      <c r="R47" s="56"/>
+      <c r="S47" s="56"/>
       <c r="U47" s="23" t="s">
         <v>66</v>
       </c>
@@ -4427,7 +4307,7 @@
       <c r="AA47" s="24"/>
       <c r="AB47" s="25"/>
     </row>
-    <row r="49" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
         <v>34</v>
       </c>
@@ -4440,19 +4320,19 @@
       <c r="E49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U49" s="68" t="s">
+      <c r="U49" s="74" t="s">
         <v>74</v>
       </c>
-      <c r="V49" s="69"/>
-      <c r="W49" s="69"/>
-      <c r="X49" s="69"/>
-      <c r="Y49" s="69"/>
-      <c r="Z49" s="69"/>
-      <c r="AA49" s="69"/>
-      <c r="AB49" s="69"/>
-      <c r="AC49" s="70"/>
-    </row>
-    <row r="50" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V49" s="75"/>
+      <c r="W49" s="75"/>
+      <c r="X49" s="75"/>
+      <c r="Y49" s="75"/>
+      <c r="Z49" s="75"/>
+      <c r="AA49" s="75"/>
+      <c r="AB49" s="75"/>
+      <c r="AC49" s="87"/>
+    </row>
+    <row r="50" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C50" s="7">
         <v>2</v>
       </c>
@@ -4468,19 +4348,19 @@
       <c r="G50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U50" s="71" t="s">
+      <c r="U50" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="V50" s="72"/>
-      <c r="W50" s="72"/>
-      <c r="X50" s="72"/>
-      <c r="Y50" s="72"/>
-      <c r="Z50" s="72"/>
-      <c r="AA50" s="72"/>
-      <c r="AB50" s="72"/>
-      <c r="AC50" s="73"/>
-    </row>
-    <row r="51" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V50" s="67"/>
+      <c r="W50" s="67"/>
+      <c r="X50" s="67"/>
+      <c r="Y50" s="67"/>
+      <c r="Z50" s="67"/>
+      <c r="AA50" s="67"/>
+      <c r="AB50" s="67"/>
+      <c r="AC50" s="69"/>
+    </row>
+    <row r="51" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C51" s="7">
         <v>4</v>
       </c>
@@ -4490,29 +4370,29 @@
       <c r="E51" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="57" t="s">
+      <c r="F51" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="57"/>
-      <c r="H51" s="90" t="s">
+      <c r="G51" s="56"/>
+      <c r="H51" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="90"/>
-      <c r="J51" s="90"/>
-      <c r="K51" s="90"/>
-      <c r="U51" s="71" t="s">
+      <c r="I51" s="66"/>
+      <c r="J51" s="66"/>
+      <c r="K51" s="66"/>
+      <c r="U51" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="V51" s="72"/>
-      <c r="W51" s="72"/>
-      <c r="X51" s="72"/>
-      <c r="Y51" s="72"/>
-      <c r="Z51" s="72"/>
-      <c r="AA51" s="72"/>
-      <c r="AB51" s="72"/>
-      <c r="AC51" s="73"/>
-    </row>
-    <row r="52" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V51" s="67"/>
+      <c r="W51" s="67"/>
+      <c r="X51" s="67"/>
+      <c r="Y51" s="67"/>
+      <c r="Z51" s="67"/>
+      <c r="AA51" s="67"/>
+      <c r="AB51" s="67"/>
+      <c r="AC51" s="69"/>
+    </row>
+    <row r="52" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C52" s="11">
         <v>8</v>
       </c>
@@ -4522,72 +4402,72 @@
       <c r="E52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="57" t="s">
+      <c r="F52" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57" t="s">
+      <c r="G52" s="56"/>
+      <c r="H52" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="57"/>
-      <c r="N52" s="57"/>
-      <c r="O52" s="57"/>
-      <c r="P52" s="57"/>
-      <c r="Q52" s="57"/>
-      <c r="R52" s="57"/>
-      <c r="S52" s="57"/>
-      <c r="U52" s="65" t="s">
+      <c r="I52" s="56"/>
+      <c r="J52" s="56"/>
+      <c r="K52" s="56"/>
+      <c r="L52" s="56"/>
+      <c r="M52" s="56"/>
+      <c r="N52" s="56"/>
+      <c r="O52" s="56"/>
+      <c r="P52" s="56"/>
+      <c r="Q52" s="56"/>
+      <c r="R52" s="56"/>
+      <c r="S52" s="56"/>
+      <c r="U52" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="V52" s="66"/>
-      <c r="W52" s="66"/>
-      <c r="X52" s="66"/>
-      <c r="Y52" s="66"/>
-      <c r="Z52" s="66"/>
-      <c r="AA52" s="66"/>
-      <c r="AB52" s="66"/>
-      <c r="AC52" s="67"/>
-    </row>
-    <row r="54" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V52" s="71"/>
+      <c r="W52" s="71"/>
+      <c r="X52" s="71"/>
+      <c r="Y52" s="71"/>
+      <c r="Z52" s="71"/>
+      <c r="AA52" s="71"/>
+      <c r="AB52" s="71"/>
+      <c r="AC52" s="72"/>
+    </row>
+    <row r="54" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="72" t="s">
+      <c r="C54" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="72"/>
-      <c r="E54" s="72"/>
-      <c r="F54" s="72"/>
-      <c r="G54" s="72"/>
-      <c r="H54" s="72"/>
-      <c r="I54" s="72"/>
-      <c r="J54" s="72"/>
-      <c r="K54" s="72"/>
-      <c r="L54" s="72"/>
-      <c r="M54" s="72"/>
-      <c r="N54" s="72"/>
-      <c r="O54" s="72"/>
-      <c r="P54" s="72"/>
-      <c r="Q54" s="72"/>
-      <c r="R54" s="72"/>
-      <c r="S54" s="72"/>
-      <c r="U54" s="80" t="s">
+      <c r="D54" s="67"/>
+      <c r="E54" s="67"/>
+      <c r="F54" s="67"/>
+      <c r="G54" s="67"/>
+      <c r="H54" s="67"/>
+      <c r="I54" s="67"/>
+      <c r="J54" s="67"/>
+      <c r="K54" s="67"/>
+      <c r="L54" s="67"/>
+      <c r="M54" s="67"/>
+      <c r="N54" s="67"/>
+      <c r="O54" s="67"/>
+      <c r="P54" s="67"/>
+      <c r="Q54" s="67"/>
+      <c r="R54" s="67"/>
+      <c r="S54" s="67"/>
+      <c r="U54" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="V54" s="81"/>
-      <c r="W54" s="81"/>
-      <c r="X54" s="81"/>
-      <c r="Y54" s="81"/>
-      <c r="Z54" s="81"/>
-      <c r="AA54" s="81"/>
-      <c r="AB54" s="81"/>
-      <c r="AC54" s="82"/>
-    </row>
-    <row r="56" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V54" s="85"/>
+      <c r="W54" s="85"/>
+      <c r="X54" s="85"/>
+      <c r="Y54" s="85"/>
+      <c r="Z54" s="85"/>
+      <c r="AA54" s="85"/>
+      <c r="AB54" s="85"/>
+      <c r="AC54" s="86"/>
+    </row>
+    <row r="56" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
         <v>8</v>
       </c>
@@ -4600,19 +4480,19 @@
       <c r="E56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U56" s="68" t="s">
+      <c r="U56" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="V56" s="69"/>
-      <c r="W56" s="69"/>
-      <c r="X56" s="69"/>
-      <c r="Y56" s="69"/>
-      <c r="Z56" s="69"/>
-      <c r="AA56" s="69"/>
-      <c r="AB56" s="69"/>
-      <c r="AC56" s="70"/>
-    </row>
-    <row r="57" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V56" s="75"/>
+      <c r="W56" s="75"/>
+      <c r="X56" s="75"/>
+      <c r="Y56" s="75"/>
+      <c r="Z56" s="75"/>
+      <c r="AA56" s="75"/>
+      <c r="AB56" s="75"/>
+      <c r="AC56" s="87"/>
+    </row>
+    <row r="57" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C57" s="7">
         <v>2</v>
       </c>
@@ -4622,23 +4502,23 @@
       <c r="E57" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F57" s="62" t="s">
+      <c r="F57" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G57" s="64"/>
-      <c r="U57" s="71" t="s">
+      <c r="G57" s="65"/>
+      <c r="U57" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="V57" s="72"/>
-      <c r="W57" s="72"/>
-      <c r="X57" s="72"/>
-      <c r="Y57" s="72"/>
-      <c r="Z57" s="72"/>
-      <c r="AA57" s="72"/>
-      <c r="AB57" s="72"/>
-      <c r="AC57" s="73"/>
-    </row>
-    <row r="58" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V57" s="67"/>
+      <c r="W57" s="67"/>
+      <c r="X57" s="67"/>
+      <c r="Y57" s="67"/>
+      <c r="Z57" s="67"/>
+      <c r="AA57" s="67"/>
+      <c r="AB57" s="67"/>
+      <c r="AC57" s="69"/>
+    </row>
+    <row r="58" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C58" s="7">
         <v>4</v>
       </c>
@@ -4648,27 +4528,27 @@
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="57" t="s">
+      <c r="F58" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G58" s="57"/>
-      <c r="H58" s="57" t="s">
+      <c r="G58" s="56"/>
+      <c r="H58" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I58" s="57"/>
-      <c r="U58" s="65" t="s">
+      <c r="I58" s="56"/>
+      <c r="U58" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="V58" s="66"/>
-      <c r="W58" s="66"/>
-      <c r="X58" s="66"/>
-      <c r="Y58" s="66"/>
-      <c r="Z58" s="66"/>
-      <c r="AA58" s="66"/>
-      <c r="AB58" s="66"/>
-      <c r="AC58" s="67"/>
-    </row>
-    <row r="60" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V58" s="71"/>
+      <c r="W58" s="71"/>
+      <c r="X58" s="71"/>
+      <c r="Y58" s="71"/>
+      <c r="Z58" s="71"/>
+      <c r="AA58" s="71"/>
+      <c r="AB58" s="71"/>
+      <c r="AC58" s="72"/>
+    </row>
+    <row r="60" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
         <v>0</v>
       </c>
@@ -4693,7 +4573,7 @@
       <c r="AB60" s="18"/>
       <c r="AC60" s="19"/>
     </row>
-    <row r="61" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C61" s="7">
         <v>2</v>
       </c>
@@ -4703,23 +4583,23 @@
       <c r="E61" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F61" s="62" t="s">
+      <c r="F61" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G61" s="64"/>
-      <c r="U61" s="71" t="s">
+      <c r="G61" s="65"/>
+      <c r="U61" s="68" t="s">
         <v>78</v>
       </c>
-      <c r="V61" s="72"/>
-      <c r="W61" s="72"/>
-      <c r="X61" s="72"/>
-      <c r="Y61" s="72"/>
-      <c r="Z61" s="72"/>
-      <c r="AA61" s="72"/>
-      <c r="AB61" s="72"/>
-      <c r="AC61" s="73"/>
-    </row>
-    <row r="62" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V61" s="67"/>
+      <c r="W61" s="67"/>
+      <c r="X61" s="67"/>
+      <c r="Y61" s="67"/>
+      <c r="Z61" s="67"/>
+      <c r="AA61" s="67"/>
+      <c r="AB61" s="67"/>
+      <c r="AC61" s="69"/>
+    </row>
+    <row r="62" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C62" s="7">
         <v>4</v>
       </c>
@@ -4729,53 +4609,53 @@
       <c r="E62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="57" t="s">
+      <c r="F62" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="57"/>
-      <c r="H62" s="57" t="s">
+      <c r="G62" s="56"/>
+      <c r="H62" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I62" s="57"/>
-      <c r="J62" s="57" t="s">
+      <c r="I62" s="56"/>
+      <c r="J62" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="K62" s="57"/>
-      <c r="U62" s="74" t="s">
+      <c r="K62" s="56"/>
+      <c r="U62" s="88" t="s">
         <v>80</v>
       </c>
-      <c r="V62" s="75"/>
-      <c r="W62" s="75"/>
-      <c r="X62" s="75"/>
-      <c r="Y62" s="75"/>
-      <c r="Z62" s="75"/>
-      <c r="AA62" s="75"/>
-      <c r="AB62" s="75"/>
-      <c r="AC62" s="76"/>
-    </row>
-    <row r="63" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="U63" s="74"/>
-      <c r="V63" s="75"/>
-      <c r="W63" s="75"/>
-      <c r="X63" s="75"/>
-      <c r="Y63" s="75"/>
-      <c r="Z63" s="75"/>
-      <c r="AA63" s="75"/>
-      <c r="AB63" s="75"/>
-      <c r="AC63" s="76"/>
-    </row>
-    <row r="64" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="U64" s="77"/>
-      <c r="V64" s="78"/>
-      <c r="W64" s="78"/>
-      <c r="X64" s="78"/>
-      <c r="Y64" s="78"/>
-      <c r="Z64" s="78"/>
-      <c r="AA64" s="78"/>
-      <c r="AB64" s="78"/>
-      <c r="AC64" s="79"/>
-    </row>
-    <row r="65" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V62" s="89"/>
+      <c r="W62" s="89"/>
+      <c r="X62" s="89"/>
+      <c r="Y62" s="89"/>
+      <c r="Z62" s="89"/>
+      <c r="AA62" s="89"/>
+      <c r="AB62" s="89"/>
+      <c r="AC62" s="90"/>
+    </row>
+    <row r="63" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="U63" s="88"/>
+      <c r="V63" s="89"/>
+      <c r="W63" s="89"/>
+      <c r="X63" s="89"/>
+      <c r="Y63" s="89"/>
+      <c r="Z63" s="89"/>
+      <c r="AA63" s="89"/>
+      <c r="AB63" s="89"/>
+      <c r="AC63" s="90"/>
+    </row>
+    <row r="64" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="U64" s="91"/>
+      <c r="V64" s="92"/>
+      <c r="W64" s="92"/>
+      <c r="X64" s="92"/>
+      <c r="Y64" s="92"/>
+      <c r="Z64" s="92"/>
+      <c r="AA64" s="92"/>
+      <c r="AB64" s="92"/>
+      <c r="AC64" s="93"/>
+    </row>
+    <row r="65" spans="2:32" x14ac:dyDescent="0.45">
       <c r="U65" s="26"/>
       <c r="V65" s="26"/>
       <c r="W65" s="26"/>
@@ -4786,7 +4666,7 @@
       <c r="AB65" s="26"/>
       <c r="AC65" s="26"/>
     </row>
-    <row r="66" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:32" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
         <v>38</v>
       </c>
@@ -4799,20 +4679,20 @@
       <c r="E66" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U66" s="68" t="s">
+      <c r="U66" s="74" t="s">
         <v>82</v>
       </c>
-      <c r="V66" s="69"/>
-      <c r="W66" s="69"/>
-      <c r="X66" s="69"/>
-      <c r="Y66" s="69"/>
-      <c r="Z66" s="69"/>
-      <c r="AA66" s="69"/>
-      <c r="AB66" s="69"/>
-      <c r="AC66" s="69"/>
-      <c r="AD66" s="70"/>
-    </row>
-    <row r="67" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V66" s="75"/>
+      <c r="W66" s="75"/>
+      <c r="X66" s="75"/>
+      <c r="Y66" s="75"/>
+      <c r="Z66" s="75"/>
+      <c r="AA66" s="75"/>
+      <c r="AB66" s="75"/>
+      <c r="AC66" s="75"/>
+      <c r="AD66" s="87"/>
+    </row>
+    <row r="67" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C67" s="7">
         <v>2</v>
       </c>
@@ -4828,20 +4708,20 @@
       <c r="G67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U67" s="71" t="s">
+      <c r="U67" s="68" t="s">
         <v>81</v>
       </c>
-      <c r="V67" s="72"/>
-      <c r="W67" s="72"/>
-      <c r="X67" s="72"/>
-      <c r="Y67" s="72"/>
-      <c r="Z67" s="72"/>
-      <c r="AA67" s="72"/>
-      <c r="AB67" s="72"/>
-      <c r="AC67" s="72"/>
-      <c r="AD67" s="73"/>
-    </row>
-    <row r="68" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V67" s="67"/>
+      <c r="W67" s="67"/>
+      <c r="X67" s="67"/>
+      <c r="Y67" s="67"/>
+      <c r="Z67" s="67"/>
+      <c r="AA67" s="67"/>
+      <c r="AB67" s="67"/>
+      <c r="AC67" s="67"/>
+      <c r="AD67" s="69"/>
+    </row>
+    <row r="68" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C68" s="7">
         <v>4</v>
       </c>
@@ -4863,24 +4743,24 @@
       <c r="I68" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J68" s="62" t="s">
+      <c r="J68" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="K68" s="64"/>
-      <c r="U68" s="71" t="s">
+      <c r="K68" s="65"/>
+      <c r="U68" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="V68" s="72"/>
-      <c r="W68" s="72"/>
-      <c r="X68" s="72"/>
-      <c r="Y68" s="72"/>
-      <c r="Z68" s="72"/>
-      <c r="AA68" s="72"/>
-      <c r="AB68" s="72"/>
-      <c r="AC68" s="72"/>
-      <c r="AD68" s="73"/>
-    </row>
-    <row r="69" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V68" s="67"/>
+      <c r="W68" s="67"/>
+      <c r="X68" s="67"/>
+      <c r="Y68" s="67"/>
+      <c r="Z68" s="67"/>
+      <c r="AA68" s="67"/>
+      <c r="AB68" s="67"/>
+      <c r="AC68" s="67"/>
+      <c r="AD68" s="69"/>
+    </row>
+    <row r="69" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C69" s="11">
         <v>8</v>
       </c>
@@ -4890,46 +4770,46 @@
       <c r="E69" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F69" s="57" t="s">
+      <c r="F69" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="57"/>
-      <c r="H69" s="62" t="s">
+      <c r="G69" s="56"/>
+      <c r="H69" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="I69" s="64"/>
-      <c r="J69" s="62" t="s">
+      <c r="I69" s="65"/>
+      <c r="J69" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="K69" s="64"/>
-      <c r="L69" s="62" t="s">
+      <c r="K69" s="65"/>
+      <c r="L69" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="M69" s="64"/>
-      <c r="N69" s="62" t="s">
+      <c r="M69" s="65"/>
+      <c r="N69" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="O69" s="64"/>
-      <c r="P69" s="62" t="s">
+      <c r="O69" s="65"/>
+      <c r="P69" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="Q69" s="63"/>
-      <c r="R69" s="63"/>
-      <c r="S69" s="64"/>
-      <c r="U69" s="65" t="s">
+      <c r="Q69" s="64"/>
+      <c r="R69" s="64"/>
+      <c r="S69" s="65"/>
+      <c r="U69" s="70" t="s">
         <v>249</v>
       </c>
-      <c r="V69" s="66"/>
-      <c r="W69" s="66"/>
-      <c r="X69" s="66"/>
-      <c r="Y69" s="66"/>
-      <c r="Z69" s="66"/>
-      <c r="AA69" s="66"/>
-      <c r="AB69" s="66"/>
-      <c r="AC69" s="66"/>
-      <c r="AD69" s="67"/>
-    </row>
-    <row r="71" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V69" s="71"/>
+      <c r="W69" s="71"/>
+      <c r="X69" s="71"/>
+      <c r="Y69" s="71"/>
+      <c r="Z69" s="71"/>
+      <c r="AA69" s="71"/>
+      <c r="AB69" s="71"/>
+      <c r="AC69" s="71"/>
+      <c r="AD69" s="72"/>
+    </row>
+    <row r="71" spans="2:32" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
         <v>45</v>
       </c>
@@ -4942,15 +4822,15 @@
       <c r="E71" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U71" s="68" t="s">
+      <c r="U71" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="V71" s="69"/>
-      <c r="W71" s="69"/>
-      <c r="X71" s="69"/>
-      <c r="Y71" s="70"/>
-    </row>
-    <row r="72" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V71" s="75"/>
+      <c r="W71" s="75"/>
+      <c r="X71" s="75"/>
+      <c r="Y71" s="87"/>
+    </row>
+    <row r="72" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C72" s="7">
         <v>2</v>
       </c>
@@ -4960,19 +4840,19 @@
       <c r="E72" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F72" s="62" t="s">
+      <c r="F72" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="G72" s="64"/>
-      <c r="U72" s="65" t="s">
+      <c r="G72" s="65"/>
+      <c r="U72" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="V72" s="66"/>
-      <c r="W72" s="66"/>
-      <c r="X72" s="66"/>
-      <c r="Y72" s="67"/>
-    </row>
-    <row r="74" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V72" s="71"/>
+      <c r="W72" s="71"/>
+      <c r="X72" s="71"/>
+      <c r="Y72" s="72"/>
+    </row>
+    <row r="74" spans="2:32" x14ac:dyDescent="0.45">
       <c r="B74" t="s">
         <v>47</v>
       </c>
@@ -4985,20 +4865,20 @@
       <c r="E74" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U74" s="68" t="s">
+      <c r="U74" s="74" t="s">
         <v>86</v>
       </c>
-      <c r="V74" s="69"/>
-      <c r="W74" s="69"/>
-      <c r="X74" s="69"/>
-      <c r="Y74" s="69"/>
-      <c r="Z74" s="69"/>
-      <c r="AA74" s="69"/>
-      <c r="AB74" s="69"/>
-      <c r="AC74" s="69"/>
-      <c r="AD74" s="70"/>
-    </row>
-    <row r="75" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V74" s="75"/>
+      <c r="W74" s="75"/>
+      <c r="X74" s="75"/>
+      <c r="Y74" s="75"/>
+      <c r="Z74" s="75"/>
+      <c r="AA74" s="75"/>
+      <c r="AB74" s="75"/>
+      <c r="AC74" s="75"/>
+      <c r="AD74" s="87"/>
+    </row>
+    <row r="75" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C75" s="7">
         <v>2</v>
       </c>
@@ -5008,24 +4888,24 @@
       <c r="E75" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F75" s="62" t="s">
+      <c r="F75" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="G75" s="64"/>
-      <c r="U75" s="71" t="s">
+      <c r="G75" s="65"/>
+      <c r="U75" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="V75" s="72"/>
-      <c r="W75" s="72"/>
-      <c r="X75" s="72"/>
-      <c r="Y75" s="72"/>
-      <c r="Z75" s="72"/>
-      <c r="AA75" s="72"/>
-      <c r="AB75" s="72"/>
-      <c r="AC75" s="72"/>
-      <c r="AD75" s="73"/>
-    </row>
-    <row r="76" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V75" s="67"/>
+      <c r="W75" s="67"/>
+      <c r="X75" s="67"/>
+      <c r="Y75" s="67"/>
+      <c r="Z75" s="67"/>
+      <c r="AA75" s="67"/>
+      <c r="AB75" s="67"/>
+      <c r="AC75" s="67"/>
+      <c r="AD75" s="69"/>
+    </row>
+    <row r="76" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C76" s="7">
         <v>4</v>
       </c>
@@ -5035,34 +4915,34 @@
       <c r="E76" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F76" s="57" t="s">
+      <c r="F76" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="G76" s="57"/>
-      <c r="H76" s="57" t="s">
+      <c r="G76" s="56"/>
+      <c r="H76" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="I76" s="57"/>
+      <c r="I76" s="56"/>
       <c r="J76" s="7" t="s">
         <v>41</v>
       </c>
       <c r="K76" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U76" s="65" t="s">
+      <c r="U76" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="V76" s="66"/>
-      <c r="W76" s="66"/>
-      <c r="X76" s="66"/>
-      <c r="Y76" s="66"/>
-      <c r="Z76" s="66"/>
-      <c r="AA76" s="66"/>
-      <c r="AB76" s="66"/>
-      <c r="AC76" s="66"/>
-      <c r="AD76" s="67"/>
-    </row>
-    <row r="78" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V76" s="71"/>
+      <c r="W76" s="71"/>
+      <c r="X76" s="71"/>
+      <c r="Y76" s="71"/>
+      <c r="Z76" s="71"/>
+      <c r="AA76" s="71"/>
+      <c r="AB76" s="71"/>
+      <c r="AC76" s="71"/>
+      <c r="AD76" s="72"/>
+    </row>
+    <row r="78" spans="2:32" x14ac:dyDescent="0.45">
       <c r="B78" t="s">
         <v>51</v>
       </c>
@@ -5075,23 +4955,23 @@
       <c r="E78" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U78" s="68" t="s">
+      <c r="U78" s="74" t="s">
         <v>256</v>
       </c>
-      <c r="V78" s="69"/>
-      <c r="W78" s="69"/>
-      <c r="X78" s="69"/>
-      <c r="Y78" s="69"/>
-      <c r="Z78" s="69"/>
-      <c r="AA78" s="69"/>
-      <c r="AB78" s="69"/>
-      <c r="AC78" s="69"/>
-      <c r="AD78" s="70"/>
+      <c r="V78" s="75"/>
+      <c r="W78" s="75"/>
+      <c r="X78" s="75"/>
+      <c r="Y78" s="75"/>
+      <c r="Z78" s="75"/>
+      <c r="AA78" s="75"/>
+      <c r="AB78" s="75"/>
+      <c r="AC78" s="75"/>
+      <c r="AD78" s="87"/>
       <c r="AF78" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="79" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C79" s="7">
         <v>2</v>
       </c>
@@ -5101,24 +4981,24 @@
       <c r="E79" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F79" s="62" t="s">
+      <c r="F79" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="G79" s="64"/>
-      <c r="U79" s="71" t="s">
+      <c r="G79" s="65"/>
+      <c r="U79" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="V79" s="72"/>
-      <c r="W79" s="72"/>
-      <c r="X79" s="72"/>
-      <c r="Y79" s="72"/>
-      <c r="Z79" s="72"/>
-      <c r="AA79" s="72"/>
-      <c r="AB79" s="72"/>
-      <c r="AC79" s="72"/>
-      <c r="AD79" s="73"/>
-    </row>
-    <row r="80" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V79" s="67"/>
+      <c r="W79" s="67"/>
+      <c r="X79" s="67"/>
+      <c r="Y79" s="67"/>
+      <c r="Z79" s="67"/>
+      <c r="AA79" s="67"/>
+      <c r="AB79" s="67"/>
+      <c r="AC79" s="67"/>
+      <c r="AD79" s="69"/>
+    </row>
+    <row r="80" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C80" s="7">
         <v>4</v>
       </c>
@@ -5128,35 +5008,35 @@
       <c r="E80" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F80" s="57" t="s">
+      <c r="F80" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="G80" s="57"/>
-      <c r="H80" s="57" t="s">
+      <c r="G80" s="56"/>
+      <c r="H80" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="I80" s="57"/>
+      <c r="I80" s="56"/>
       <c r="J80" s="7" t="s">
         <v>41</v>
       </c>
       <c r="K80" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U80" s="65" t="s">
+      <c r="U80" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="V80" s="66"/>
-      <c r="W80" s="66"/>
-      <c r="X80" s="66"/>
-      <c r="Y80" s="66"/>
-      <c r="Z80" s="66"/>
-      <c r="AA80" s="66"/>
-      <c r="AB80" s="66"/>
-      <c r="AC80" s="66"/>
-      <c r="AD80" s="67"/>
+      <c r="V80" s="71"/>
+      <c r="W80" s="71"/>
+      <c r="X80" s="71"/>
+      <c r="Y80" s="71"/>
+      <c r="Z80" s="71"/>
+      <c r="AA80" s="71"/>
+      <c r="AB80" s="71"/>
+      <c r="AC80" s="71"/>
+      <c r="AD80" s="72"/>
       <c r="AF80" s="49"/>
     </row>
-    <row r="82" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B82" t="s">
         <v>96</v>
       </c>
@@ -5173,7 +5053,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="83" spans="2:21" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:21" x14ac:dyDescent="0.45">
       <c r="C83" s="7">
         <v>2</v>
       </c>
@@ -5183,18 +5063,79 @@
       <c r="E83" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F83" s="62" t="s">
+      <c r="F83" s="63" t="s">
         <v>240</v>
       </c>
-      <c r="G83" s="64"/>
+      <c r="G83" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="U72:Y72"/>
+    <mergeCell ref="U74:AD74"/>
+    <mergeCell ref="U75:AD75"/>
+    <mergeCell ref="U76:AD76"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="H76:I76"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="U80:AD80"/>
+    <mergeCell ref="U79:AD79"/>
+    <mergeCell ref="U78:AD78"/>
+    <mergeCell ref="U71:Y71"/>
+    <mergeCell ref="U56:AC56"/>
+    <mergeCell ref="U57:AC57"/>
+    <mergeCell ref="U58:AC58"/>
+    <mergeCell ref="U61:AC61"/>
+    <mergeCell ref="U62:AC64"/>
+    <mergeCell ref="U66:AD66"/>
+    <mergeCell ref="U67:AD67"/>
+    <mergeCell ref="U68:AD68"/>
+    <mergeCell ref="U69:AD69"/>
+    <mergeCell ref="U49:AC49"/>
+    <mergeCell ref="U50:AC50"/>
+    <mergeCell ref="U51:AC51"/>
+    <mergeCell ref="U52:AC52"/>
+    <mergeCell ref="U54:AC54"/>
+    <mergeCell ref="U39:X40"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="U37:AB37"/>
+    <mergeCell ref="U15:X18"/>
+    <mergeCell ref="U21:X24"/>
+    <mergeCell ref="H22:S22"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="U30:AB30"/>
+    <mergeCell ref="U31:AB31"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="U26:X26"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="C26:S26"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="I31:S31"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C42:S42"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="C33:S33"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
     <mergeCell ref="P69:S69"/>
     <mergeCell ref="F61:G61"/>
     <mergeCell ref="F47:G47"/>
@@ -5211,72 +5152,11 @@
     <mergeCell ref="L69:M69"/>
     <mergeCell ref="N69:O69"/>
     <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="I31:S31"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C42:S42"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="C33:S33"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="U30:AB30"/>
-    <mergeCell ref="U31:AB31"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="U26:X26"/>
-    <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U29:X29"/>
-    <mergeCell ref="C26:S26"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="U15:X18"/>
-    <mergeCell ref="U21:X24"/>
-    <mergeCell ref="H22:S22"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="U39:X40"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="U35:X35"/>
-    <mergeCell ref="U37:AB37"/>
-    <mergeCell ref="U49:AC49"/>
-    <mergeCell ref="U50:AC50"/>
-    <mergeCell ref="U51:AC51"/>
-    <mergeCell ref="U52:AC52"/>
-    <mergeCell ref="U54:AC54"/>
-    <mergeCell ref="U71:Y71"/>
-    <mergeCell ref="U56:AC56"/>
-    <mergeCell ref="U57:AC57"/>
-    <mergeCell ref="U58:AC58"/>
-    <mergeCell ref="U61:AC61"/>
-    <mergeCell ref="U62:AC64"/>
-    <mergeCell ref="U66:AD66"/>
-    <mergeCell ref="U67:AD67"/>
-    <mergeCell ref="U68:AD68"/>
-    <mergeCell ref="U69:AD69"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="U72:Y72"/>
-    <mergeCell ref="U74:AD74"/>
-    <mergeCell ref="U75:AD75"/>
-    <mergeCell ref="U76:AD76"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="U80:AD80"/>
-    <mergeCell ref="U79:AD79"/>
-    <mergeCell ref="U78:AD78"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5291,14 +5171,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B4" s="49"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ALU LOAD/STORE debugged, unit tests pass
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aroma\Desktop\vcda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar\Documents\Work\AI\CPU\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572B596A-25DF-4C4A-BB57-764054930DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2E6F53-8C97-4FB3-BE9B-DD65953E5B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21075" activeTab="2" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="272">
   <si>
     <t>POP</t>
   </si>
@@ -681,9 +681,6 @@
   </si>
   <si>
     <t>SHR</t>
-  </si>
-  <si>
-    <t>Shift Right Logical</t>
   </si>
   <si>
     <t>MUL</t>
@@ -1198,6 +1195,15 @@
   </si>
   <si>
     <t>Instruction Pointer</t>
+  </si>
+  <si>
+    <t>Shift Right</t>
+  </si>
+  <si>
+    <t>LOAD: R[N.DST] = M[R[N.RS] + R[N.SRC]*ADT.sizeof() + ofs]</t>
+  </si>
+  <si>
+    <t>STORE:  M[R[N.RS] + R[N.SRC]*ADT.sizeof() + ofs] = R[N.DST]</t>
   </si>
 </sst>
 </file>
@@ -1782,7 +1788,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1887,14 +1893,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1916,6 +1922,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1925,25 +1943,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1961,44 +2006,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2336,28 +2351,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CDEC23-057C-4C1E-AB18-5AC9130DB945}">
   <dimension ref="B3:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="6.109375" customWidth="1"/>
-    <col min="4" max="4" width="4.88671875" customWidth="1"/>
-    <col min="5" max="5" width="3.109375" customWidth="1"/>
-    <col min="6" max="6" width="9.21875" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" customWidth="1"/>
-    <col min="10" max="17" width="4.5546875" customWidth="1"/>
+    <col min="3" max="3" width="6.1328125" customWidth="1"/>
+    <col min="4" max="4" width="4.86328125" customWidth="1"/>
+    <col min="5" max="5" width="3.1328125" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" customWidth="1"/>
+    <col min="7" max="7" width="21.796875" customWidth="1"/>
+    <col min="8" max="8" width="5.86328125" customWidth="1"/>
+    <col min="9" max="9" width="14.19921875" customWidth="1"/>
+    <col min="10" max="17" width="4.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="27" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C4" s="27" t="s">
         <v>99</v>
       </c>
@@ -2365,7 +2380,7 @@
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F4" t="s">
         <v>101</v>
@@ -2376,21 +2391,21 @@
       <c r="J4" s="60">
         <v>0</v>
       </c>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58">
+      <c r="K4" s="59"/>
+      <c r="L4" s="59">
         <v>1</v>
       </c>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58">
+      <c r="M4" s="59"/>
+      <c r="N4" s="59">
         <v>2</v>
       </c>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58">
+      <c r="O4" s="59"/>
+      <c r="P4" s="59">
         <v>3</v>
       </c>
-      <c r="Q4" s="58"/>
-    </row>
-    <row r="5" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q4" s="59"/>
+    </row>
+    <row r="5" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C5" s="27" t="s">
         <v>100</v>
       </c>
@@ -2398,7 +2413,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F5" t="s">
         <v>102</v>
@@ -2431,49 +2446,49 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B8" s="27" t="s">
         <v>103</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59" t="s">
+      <c r="K8" s="57"/>
+      <c r="L8" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="M8" s="59"/>
-      <c r="N8" s="59" t="s">
+      <c r="M8" s="57"/>
+      <c r="N8" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="O8" s="59"/>
-      <c r="P8" s="59" t="s">
+      <c r="O8" s="57"/>
+      <c r="P8" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="59"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q8" s="57"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="57" t="s">
+      <c r="F9" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="57"/>
+      <c r="G9" s="58"/>
       <c r="H9" s="8"/>
       <c r="I9" s="28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
       <c r="H10" s="8"/>
       <c r="J10" t="s">
         <v>30</v>
@@ -2485,12 +2500,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="58"/>
       <c r="H11" s="8"/>
       <c r="J11" t="s">
         <v>124</v>
@@ -2502,7 +2517,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.45">
       <c r="J12" t="s">
         <v>125</v>
       </c>
@@ -2513,7 +2528,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
         <v>114</v>
       </c>
@@ -2530,7 +2545,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>113</v>
       </c>
@@ -2541,7 +2556,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
         <v>112</v>
       </c>
@@ -2549,7 +2564,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
         <v>111</v>
       </c>
@@ -2559,34 +2574,34 @@
       <c r="I16" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="59" t="s">
+      <c r="J16" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59" t="s">
+      <c r="K16" s="57"/>
+      <c r="L16" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="M16" s="59"/>
-      <c r="N16" s="59" t="s">
+      <c r="M16" s="57"/>
+      <c r="N16" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="O16" s="59"/>
-      <c r="P16" s="59"/>
-      <c r="Q16" s="59"/>
-    </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I17" s="28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="57" t="s">
+      <c r="F18" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="G18" s="57"/>
+      <c r="G18" s="58"/>
       <c r="H18" s="8"/>
       <c r="J18" t="s">
         <v>127</v>
@@ -2598,12 +2613,12 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
       <c r="H19" s="8"/>
       <c r="J19" t="s">
         <v>126</v>
@@ -2615,12 +2630,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
-        <v>264</v>
-      </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
+        <v>263</v>
+      </c>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
       <c r="H20" s="8"/>
       <c r="J20" t="s">
         <v>129</v>
@@ -2632,38 +2647,38 @@
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I22" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="J22" s="59" t="s">
+      <c r="J22" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="59"/>
-      <c r="N22" s="59" t="s">
+      <c r="K22" s="57"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="O22" s="59"/>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="59"/>
-    </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="O22" s="57"/>
+      <c r="P22" s="57"/>
+      <c r="Q22" s="57"/>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
         <v>123</v>
       </c>
       <c r="F23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G23" s="56" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I23" s="28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
         <v>122</v>
       </c>
@@ -2671,7 +2686,7 @@
         <v>117</v>
       </c>
       <c r="G24" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J24" t="s">
         <v>128</v>
@@ -2683,7 +2698,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
         <v>121</v>
       </c>
@@ -2691,7 +2706,7 @@
         <v>118</v>
       </c>
       <c r="G25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J25" t="s">
         <v>130</v>
@@ -2703,7 +2718,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
         <v>120</v>
       </c>
@@ -2711,32 +2726,32 @@
         <v>119</v>
       </c>
       <c r="G26" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I28" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="J28" s="59" t="s">
+      <c r="J28" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="K28" s="59"/>
-      <c r="L28" s="59" t="s">
+      <c r="K28" s="57"/>
+      <c r="L28" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-    </row>
-    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="57"/>
+      <c r="Q28" s="57"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I29" s="28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:17" x14ac:dyDescent="0.45">
       <c r="J30" t="s">
         <v>131</v>
       </c>
@@ -2744,7 +2759,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:17" x14ac:dyDescent="0.45">
       <c r="J31" t="s">
         <v>132</v>
       </c>
@@ -2754,13 +2769,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:Q28"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:Q16"/>
     <mergeCell ref="F9:G11"/>
     <mergeCell ref="F18:G20"/>
     <mergeCell ref="P4:Q4"/>
@@ -2771,6 +2779,13 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:Q28"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2780,20 +2795,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A222D11D-FBDB-42C8-93C4-B5D16645D996}">
   <dimension ref="A3:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.88671875" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
+    <col min="4" max="4" width="34.86328125" customWidth="1"/>
+    <col min="7" max="7" width="7.46484375" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="27" t="s">
         <v>127</v>
       </c>
@@ -2801,10 +2816,10 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="27"/>
     </row>
-    <row r="5" spans="1:16" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" s="27" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="40" t="s">
         <v>147</v>
       </c>
@@ -2818,18 +2833,18 @@
       <c r="H5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="58">
+      <c r="I5" s="59">
         <v>0</v>
       </c>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
       <c r="L5" s="61"/>
       <c r="M5" s="62"/>
       <c r="N5" s="63"/>
       <c r="O5" s="63"/>
       <c r="P5" s="63"/>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="37" t="s">
         <v>13</v>
       </c>
@@ -2840,7 +2855,7 @@
         <v>150</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I6" s="5">
         <v>0</v>
@@ -2859,7 +2874,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B7" s="33" t="s">
         <v>19</v>
       </c>
@@ -2870,7 +2885,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B8" s="33" t="s">
         <v>153</v>
       </c>
@@ -2881,7 +2896,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B9" s="33" t="s">
         <v>22</v>
       </c>
@@ -2893,15 +2908,15 @@
       </c>
       <c r="H9" s="27"/>
       <c r="I9" s="64" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J9" s="65"/>
       <c r="K9" s="66"/>
       <c r="L9" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B10" s="33" t="s">
         <v>29</v>
       </c>
@@ -2912,10 +2927,10 @@
         <v>158</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B11" s="33" t="s">
         <v>159</v>
       </c>
@@ -2926,11 +2941,11 @@
         <v>161</v>
       </c>
       <c r="I11" s="53" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J11" s="52"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B12" s="33" t="s">
         <v>9</v>
       </c>
@@ -2941,11 +2956,11 @@
         <v>163</v>
       </c>
       <c r="I12" s="54" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J12" s="52"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B13" s="33" t="s">
         <v>2</v>
       </c>
@@ -2956,11 +2971,11 @@
         <v>171</v>
       </c>
       <c r="I13" s="54" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J13" s="52"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B14" s="33" t="s">
         <v>39</v>
       </c>
@@ -2971,10 +2986,10 @@
         <v>165</v>
       </c>
       <c r="I14" s="54" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B15" s="33" t="s">
         <v>46</v>
       </c>
@@ -2985,10 +3000,10 @@
         <v>167</v>
       </c>
       <c r="I15" s="54" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B16" s="33" t="s">
         <v>48</v>
       </c>
@@ -2999,10 +3014,10 @@
         <v>169</v>
       </c>
       <c r="I16" s="54" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B17" s="33" t="s">
         <v>172</v>
       </c>
@@ -3013,10 +3028,10 @@
         <v>174</v>
       </c>
       <c r="I17" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B18" s="55" t="s">
         <v>4</v>
       </c>
@@ -3027,10 +3042,10 @@
         <v>176</v>
       </c>
       <c r="I18" s="54" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B19" s="33" t="s">
         <v>14</v>
       </c>
@@ -3041,21 +3056,21 @@
         <v>178</v>
       </c>
       <c r="I19" s="54" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B20" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="D20" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="D20" s="34" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B21" s="10" t="s">
         <v>97</v>
       </c>
@@ -3066,16 +3081,16 @@
         <v>180</v>
       </c>
       <c r="I21" s="54" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J21" t="s">
         <v>177</v>
       </c>
       <c r="K21" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="27" t="s">
         <v>131</v>
       </c>
@@ -3083,8 +3098,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="25" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B25" s="40" t="s">
         <v>147</v>
       </c>
@@ -3093,7 +3108,7 @@
       </c>
       <c r="D25" s="42"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B26" s="37" t="s">
         <v>13</v>
       </c>
@@ -3102,7 +3117,7 @@
       </c>
       <c r="D26" s="39"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B27" s="33" t="s">
         <v>19</v>
       </c>
@@ -3111,7 +3126,7 @@
       </c>
       <c r="D27" s="34"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B28" s="33" t="s">
         <v>153</v>
       </c>
@@ -3120,7 +3135,7 @@
       </c>
       <c r="D28" s="34"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B29" s="33" t="s">
         <v>22</v>
       </c>
@@ -3129,7 +3144,7 @@
       </c>
       <c r="D29" s="34"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B30" s="33" t="s">
         <v>29</v>
       </c>
@@ -3138,7 +3153,7 @@
       </c>
       <c r="D30" s="34"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B31" s="33" t="s">
         <v>159</v>
       </c>
@@ -3147,7 +3162,7 @@
       </c>
       <c r="D31" s="34"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B32" s="33" t="s">
         <v>9</v>
       </c>
@@ -3156,7 +3171,7 @@
       </c>
       <c r="D32" s="34"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B33" s="33" t="s">
         <v>2</v>
       </c>
@@ -3165,7 +3180,7 @@
       </c>
       <c r="D33" s="34"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B34" s="33" t="s">
         <v>39</v>
       </c>
@@ -3174,7 +3189,7 @@
       </c>
       <c r="D34" s="34"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B35" s="33" t="s">
         <v>46</v>
       </c>
@@ -3183,7 +3198,7 @@
       </c>
       <c r="D35" s="34"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B36" s="33" t="s">
         <v>48</v>
       </c>
@@ -3192,7 +3207,7 @@
       </c>
       <c r="D36" s="34"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B37" s="33" t="s">
         <v>172</v>
       </c>
@@ -3201,7 +3216,7 @@
       </c>
       <c r="D37" s="34"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B38" s="33" t="s">
         <v>4</v>
       </c>
@@ -3210,7 +3225,7 @@
       </c>
       <c r="D38" s="34"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B39" s="33" t="s">
         <v>14</v>
       </c>
@@ -3219,7 +3234,7 @@
       </c>
       <c r="D39" s="34"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B40" s="33" t="s">
         <v>15</v>
       </c>
@@ -3228,7 +3243,7 @@
       </c>
       <c r="D40" s="34"/>
     </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B41" s="10" t="s">
         <v>97</v>
       </c>
@@ -3237,18 +3252,18 @@
       </c>
       <c r="D41" s="36"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="27" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B44" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A45" s="27"/>
     </row>
-    <row r="46" spans="1:4" s="27" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" s="27" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B46" s="29" t="s">
         <v>147</v>
       </c>
@@ -3259,7 +3274,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B47" s="9" t="s">
         <v>13</v>
       </c>
@@ -3270,7 +3285,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B48" s="33" t="s">
         <v>19</v>
       </c>
@@ -3281,7 +3296,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B49" s="33" t="s">
         <v>153</v>
       </c>
@@ -3292,7 +3307,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B50" s="33" t="s">
         <v>22</v>
       </c>
@@ -3303,7 +3318,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B51" s="33" t="s">
         <v>29</v>
       </c>
@@ -3314,7 +3329,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B52" s="33" t="s">
         <v>159</v>
       </c>
@@ -3325,7 +3340,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B53" s="33" t="s">
         <v>9</v>
       </c>
@@ -3333,82 +3348,82 @@
         <v>213</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B54" s="33" t="s">
         <v>2</v>
       </c>
       <c r="C54" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D54" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="D54" s="34" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B55" s="33" t="s">
         <v>39</v>
       </c>
       <c r="C55" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="D55" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="D55" s="34" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B56" s="33" t="s">
         <v>46</v>
       </c>
       <c r="C56" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D56" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="D56" s="34" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B57" s="33" t="s">
         <v>48</v>
       </c>
       <c r="C57" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D57" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="D57" s="34" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B58" s="33" t="s">
         <v>172</v>
       </c>
       <c r="C58" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="D58" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="D58" s="34" t="s">
+    </row>
+    <row r="59" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B59" s="10" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="10" t="s">
+      <c r="C59" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="C59" s="35" t="s">
-        <v>226</v>
-      </c>
       <c r="D59" s="36"/>
     </row>
-    <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A61" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="B61" t="s">
         <v>229</v>
       </c>
-      <c r="B61" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B62" s="45" t="s">
         <v>147</v>
       </c>
@@ -3419,26 +3434,26 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B63" s="37" t="s">
         <v>13</v>
       </c>
       <c r="C63" s="38" t="s">
+        <v>230</v>
+      </c>
+      <c r="D63" s="39" t="s">
         <v>231</v>
       </c>
-      <c r="D63" s="39" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B64" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C64" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="D64" s="36" t="s">
         <v>233</v>
-      </c>
-      <c r="D64" s="36" t="s">
-        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3453,88 +3468,88 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43404EB-A4C0-4EEB-BCD6-93EC84295AA2}">
-  <dimension ref="A2:AF83"/>
+  <dimension ref="A2:AF86"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="U72" sqref="U72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.21875" customWidth="1"/>
-    <col min="4" max="6" width="4.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.77734375" style="15" customWidth="1"/>
-    <col min="8" max="10" width="4.77734375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="4.77734375" style="15" customWidth="1"/>
-    <col min="12" max="19" width="4.77734375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="2.109375" customWidth="1"/>
-    <col min="28" max="28" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="5.19921875" customWidth="1"/>
+    <col min="4" max="6" width="4.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.796875" style="15" customWidth="1"/>
+    <col min="8" max="10" width="4.796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="4.796875" style="15" customWidth="1"/>
+    <col min="12" max="19" width="4.796875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="2.1328125" customWidth="1"/>
+    <col min="28" max="28" width="11.53125" customWidth="1"/>
     <col min="29" max="29" width="12.33203125" customWidth="1"/>
     <col min="30" max="30" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="77" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="60">
         <v>0</v>
       </c>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58">
+      <c r="E7" s="59"/>
+      <c r="F7" s="59">
         <v>1</v>
       </c>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58">
+      <c r="G7" s="59"/>
+      <c r="H7" s="59">
         <v>2</v>
       </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58">
+      <c r="I7" s="59"/>
+      <c r="J7" s="59">
         <v>3</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58">
+      <c r="K7" s="59"/>
+      <c r="L7" s="59">
         <v>4</v>
       </c>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58">
+      <c r="M7" s="59"/>
+      <c r="N7" s="59">
         <v>5</v>
       </c>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58">
+      <c r="O7" s="59"/>
+      <c r="P7" s="59">
         <v>6</v>
       </c>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="58">
+      <c r="Q7" s="59"/>
+      <c r="R7" s="59">
         <v>7</v>
       </c>
-      <c r="S7" s="91"/>
-    </row>
-    <row r="8" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="S7" s="74"/>
+    </row>
+    <row r="8" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="94"/>
+      <c r="C8" s="78"/>
       <c r="D8" s="4">
         <v>0</v>
       </c>
@@ -3584,15 +3599,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.45">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>90</v>
       </c>
@@ -3603,7 +3618,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>91</v>
       </c>
@@ -3614,7 +3629,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>92</v>
       </c>
@@ -3625,10 +3640,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.45">
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -3641,17 +3656,17 @@
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="57" t="s">
+      <c r="U15" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="V15" s="57"/>
-      <c r="W15" s="57"/>
-      <c r="X15" s="57"/>
+      <c r="V15" s="58"/>
+      <c r="W15" s="58"/>
+      <c r="X15" s="58"/>
       <c r="AA15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="C16" s="7">
         <v>2</v>
       </c>
@@ -3667,15 +3682,15 @@
       <c r="G16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U16" s="57"/>
-      <c r="V16" s="57"/>
-      <c r="W16" s="57"/>
-      <c r="X16" s="57"/>
+      <c r="U16" s="58"/>
+      <c r="V16" s="58"/>
+      <c r="W16" s="58"/>
+      <c r="X16" s="58"/>
       <c r="AA16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C17" s="7">
         <v>4</v>
       </c>
@@ -3703,15 +3718,15 @@
       <c r="K17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="57"/>
-      <c r="V17" s="57"/>
-      <c r="W17" s="57"/>
-      <c r="X17" s="57"/>
+      <c r="U17" s="58"/>
+      <c r="V17" s="58"/>
+      <c r="W17" s="58"/>
+      <c r="X17" s="58"/>
       <c r="AA17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C18" s="7">
         <v>8</v>
       </c>
@@ -3763,17 +3778,17 @@
       <c r="S18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="57"/>
-      <c r="V18" s="57"/>
-      <c r="W18" s="57"/>
-      <c r="X18" s="57"/>
-    </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="U18" s="58"/>
+      <c r="V18" s="58"/>
+      <c r="W18" s="58"/>
+      <c r="X18" s="58"/>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>18</v>
       </c>
@@ -3786,14 +3801,14 @@
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U21" s="57" t="s">
-        <v>247</v>
-      </c>
-      <c r="V21" s="57"/>
-      <c r="W21" s="57"/>
-      <c r="X21" s="57"/>
-    </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="U21" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="V21" s="58"/>
+      <c r="W21" s="58"/>
+      <c r="X21" s="58"/>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C22" s="7">
         <v>2</v>
       </c>
@@ -3809,26 +3824,26 @@
       <c r="G22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="73" t="s">
+      <c r="H22" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="74"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="74"/>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="74"/>
-      <c r="S22" s="74"/>
-      <c r="U22" s="57"/>
-      <c r="V22" s="57"/>
-      <c r="W22" s="57"/>
-      <c r="X22" s="57"/>
-    </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="I22" s="68"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="68"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="68"/>
+      <c r="P22" s="68"/>
+      <c r="Q22" s="68"/>
+      <c r="R22" s="68"/>
+      <c r="S22" s="68"/>
+      <c r="U22" s="58"/>
+      <c r="V22" s="58"/>
+      <c r="W22" s="58"/>
+      <c r="X22" s="58"/>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C23" s="7">
         <v>4</v>
       </c>
@@ -3848,45 +3863,45 @@
       <c r="I23" s="65"/>
       <c r="J23" s="65"/>
       <c r="K23" s="66"/>
-      <c r="U23" s="57"/>
-      <c r="V23" s="57"/>
-      <c r="W23" s="57"/>
-      <c r="X23" s="57"/>
-    </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="U23" s="58"/>
+      <c r="V23" s="58"/>
+      <c r="W23" s="58"/>
+      <c r="X23" s="58"/>
+    </row>
+    <row r="24" spans="2:28" x14ac:dyDescent="0.45">
       <c r="G24" s="63"/>
       <c r="H24" s="63"/>
       <c r="I24" s="63"/>
       <c r="J24" s="63"/>
       <c r="K24" s="63"/>
-      <c r="U24" s="57"/>
-      <c r="V24" s="57"/>
-      <c r="W24" s="57"/>
-      <c r="X24" s="57"/>
-    </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="U24" s="58"/>
+      <c r="V24" s="58"/>
+      <c r="W24" s="58"/>
+      <c r="X24" s="58"/>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="74"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="74"/>
-      <c r="K26" s="74"/>
-      <c r="L26" s="74"/>
-      <c r="M26" s="74"/>
-      <c r="N26" s="74"/>
-      <c r="O26" s="74"/>
-      <c r="P26" s="74"/>
-      <c r="Q26" s="74"/>
-      <c r="R26" s="74"/>
-      <c r="S26" s="74"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="68"/>
+      <c r="M26" s="68"/>
+      <c r="N26" s="68"/>
+      <c r="O26" s="68"/>
+      <c r="P26" s="68"/>
+      <c r="Q26" s="68"/>
+      <c r="R26" s="68"/>
+      <c r="S26" s="68"/>
       <c r="U26" s="63" t="s">
         <v>53</v>
       </c>
@@ -3894,7 +3909,7 @@
       <c r="W26" s="63"/>
       <c r="X26" s="63"/>
     </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>21</v>
       </c>
@@ -3907,18 +3922,18 @@
       <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U28" s="70" t="s">
+      <c r="U28" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="V28" s="71"/>
-      <c r="W28" s="71"/>
-      <c r="X28" s="71"/>
+      <c r="V28" s="76"/>
+      <c r="W28" s="76"/>
+      <c r="X28" s="76"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
       <c r="AB28" s="19"/>
     </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C29" s="7">
         <v>2</v>
       </c>
@@ -3934,15 +3949,15 @@
       <c r="G29" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="73" t="s">
+      <c r="U29" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="V29" s="74"/>
-      <c r="W29" s="74"/>
-      <c r="X29" s="74"/>
+      <c r="V29" s="68"/>
+      <c r="W29" s="68"/>
+      <c r="X29" s="68"/>
       <c r="AB29" s="20"/>
     </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C30" s="7">
         <v>4</v>
       </c>
@@ -3955,27 +3970,27 @@
       <c r="F30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="59" t="s">
+      <c r="G30" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="59"/>
-      <c r="I30" s="92" t="s">
+      <c r="H30" s="57"/>
+      <c r="I30" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="92"/>
-      <c r="K30" s="92"/>
-      <c r="U30" s="73" t="s">
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="U30" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="V30" s="74"/>
-      <c r="W30" s="74"/>
-      <c r="X30" s="74"/>
-      <c r="Y30" s="74"/>
-      <c r="Z30" s="74"/>
-      <c r="AA30" s="74"/>
-      <c r="AB30" s="75"/>
-    </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V30" s="68"/>
+      <c r="W30" s="68"/>
+      <c r="X30" s="68"/>
+      <c r="Y30" s="68"/>
+      <c r="Z30" s="68"/>
+      <c r="AA30" s="68"/>
+      <c r="AB30" s="70"/>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C31" s="7">
         <v>8</v>
       </c>
@@ -3988,65 +4003,65 @@
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="59" t="s">
+      <c r="G31" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59" t="s">
+      <c r="H31" s="57"/>
+      <c r="I31" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="59"/>
-      <c r="M31" s="59"/>
-      <c r="N31" s="59"/>
-      <c r="O31" s="59"/>
-      <c r="P31" s="59"/>
-      <c r="Q31" s="59"/>
-      <c r="R31" s="59"/>
-      <c r="S31" s="59"/>
-      <c r="U31" s="67" t="s">
+      <c r="J31" s="57"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="57"/>
+      <c r="M31" s="57"/>
+      <c r="N31" s="57"/>
+      <c r="O31" s="57"/>
+      <c r="P31" s="57"/>
+      <c r="Q31" s="57"/>
+      <c r="R31" s="57"/>
+      <c r="S31" s="57"/>
+      <c r="U31" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="V31" s="68"/>
-      <c r="W31" s="68"/>
-      <c r="X31" s="68"/>
-      <c r="Y31" s="68"/>
-      <c r="Z31" s="68"/>
-      <c r="AA31" s="68"/>
-      <c r="AB31" s="69"/>
-    </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V31" s="72"/>
+      <c r="W31" s="72"/>
+      <c r="X31" s="72"/>
+      <c r="Y31" s="72"/>
+      <c r="Z31" s="72"/>
+      <c r="AA31" s="72"/>
+      <c r="AB31" s="73"/>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="74" t="s">
+      <c r="C33" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="74"/>
-      <c r="K33" s="74"/>
-      <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
-      <c r="N33" s="74"/>
-      <c r="O33" s="74"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="74"/>
-      <c r="R33" s="74"/>
-      <c r="S33" s="74"/>
-      <c r="U33" s="82" t="s">
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="68"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
+      <c r="Q33" s="68"/>
+      <c r="R33" s="68"/>
+      <c r="S33" s="68"/>
+      <c r="U33" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="V33" s="83"/>
-      <c r="W33" s="83"/>
-      <c r="X33" s="84"/>
-    </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V33" s="86"/>
+      <c r="W33" s="86"/>
+      <c r="X33" s="87"/>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>27</v>
       </c>
@@ -4059,18 +4074,18 @@
       <c r="E35" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="U35" s="70" t="s">
+      <c r="U35" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="V35" s="71"/>
-      <c r="W35" s="71"/>
-      <c r="X35" s="71"/>
+      <c r="V35" s="76"/>
+      <c r="W35" s="76"/>
+      <c r="X35" s="76"/>
       <c r="Y35" s="18"/>
       <c r="Z35" s="18"/>
       <c r="AA35" s="18"/>
       <c r="AB35" s="19"/>
     </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C36" s="7">
         <v>2</v>
       </c>
@@ -4091,7 +4106,7 @@
       </c>
       <c r="AB36" s="20"/>
     </row>
-    <row r="37" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C37" s="7">
         <v>4</v>
       </c>
@@ -4105,28 +4120,28 @@
         <v>159</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="H37" s="59" t="s">
+        <v>247</v>
+      </c>
+      <c r="H37" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="59"/>
-      <c r="J37" s="59" t="s">
+      <c r="I37" s="57"/>
+      <c r="J37" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="K37" s="59"/>
-      <c r="U37" s="73" t="s">
+      <c r="K37" s="57"/>
+      <c r="U37" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="V37" s="74"/>
-      <c r="W37" s="74"/>
-      <c r="X37" s="74"/>
-      <c r="Y37" s="74"/>
-      <c r="Z37" s="74"/>
-      <c r="AA37" s="74"/>
-      <c r="AB37" s="75"/>
-    </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V37" s="68"/>
+      <c r="W37" s="68"/>
+      <c r="X37" s="68"/>
+      <c r="Y37" s="68"/>
+      <c r="Z37" s="68"/>
+      <c r="AA37" s="68"/>
+      <c r="AB37" s="70"/>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>30</v>
       </c>
@@ -4139,14 +4154,14 @@
       <c r="E39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U39" s="85" t="s">
+      <c r="U39" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="V39" s="86"/>
-      <c r="W39" s="86"/>
-      <c r="X39" s="87"/>
-    </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V39" s="80"/>
+      <c r="W39" s="80"/>
+      <c r="X39" s="81"/>
+    </row>
+    <row r="40" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C40" s="7">
         <v>2</v>
       </c>
@@ -4160,45 +4175,45 @@
         <v>3</v>
       </c>
       <c r="G40" s="66"/>
-      <c r="U40" s="88"/>
-      <c r="V40" s="89"/>
-      <c r="W40" s="89"/>
-      <c r="X40" s="90"/>
-    </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="U40" s="82"/>
+      <c r="V40" s="83"/>
+      <c r="W40" s="83"/>
+      <c r="X40" s="84"/>
+    </row>
+    <row r="42" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="74" t="s">
+      <c r="C42" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="74"/>
-      <c r="J42" s="74"/>
-      <c r="K42" s="74"/>
-      <c r="L42" s="74"/>
-      <c r="M42" s="74"/>
-      <c r="N42" s="74"/>
-      <c r="O42" s="74"/>
-      <c r="P42" s="74"/>
-      <c r="Q42" s="74"/>
-      <c r="R42" s="74"/>
-      <c r="S42" s="74"/>
-      <c r="U42" s="82" t="s">
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="68"/>
+      <c r="H42" s="68"/>
+      <c r="I42" s="68"/>
+      <c r="J42" s="68"/>
+      <c r="K42" s="68"/>
+      <c r="L42" s="68"/>
+      <c r="M42" s="68"/>
+      <c r="N42" s="68"/>
+      <c r="O42" s="68"/>
+      <c r="P42" s="68"/>
+      <c r="Q42" s="68"/>
+      <c r="R42" s="68"/>
+      <c r="S42" s="68"/>
+      <c r="U42" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="V42" s="83"/>
-      <c r="W42" s="83"/>
-      <c r="X42" s="84"/>
-    </row>
-    <row r="43" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="V42" s="86"/>
+      <c r="W42" s="86"/>
+      <c r="X42" s="87"/>
+    </row>
+    <row r="43" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C43" s="12"/>
     </row>
-    <row r="44" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>33</v>
       </c>
@@ -4222,7 +4237,7 @@
       <c r="AA44" s="18"/>
       <c r="AB44" s="19"/>
     </row>
-    <row r="45" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C45" s="7">
         <v>2</v>
       </c>
@@ -4243,7 +4258,7 @@
       </c>
       <c r="AB45" s="20"/>
     </row>
-    <row r="46" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C46" s="7">
         <v>4</v>
       </c>
@@ -4253,22 +4268,22 @@
       <c r="E46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="59" t="s">
+      <c r="F46" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="59"/>
-      <c r="H46" s="92" t="s">
+      <c r="G46" s="57"/>
+      <c r="H46" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="I46" s="92"/>
-      <c r="J46" s="92"/>
-      <c r="K46" s="92"/>
+      <c r="I46" s="67"/>
+      <c r="J46" s="67"/>
+      <c r="K46" s="67"/>
       <c r="U46" s="22" t="s">
         <v>67</v>
       </c>
       <c r="AB46" s="20"/>
     </row>
-    <row r="47" spans="2:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C47" s="11">
         <v>8</v>
       </c>
@@ -4278,24 +4293,24 @@
       <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="59" t="s">
+      <c r="F47" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="59"/>
-      <c r="H47" s="59" t="s">
+      <c r="G47" s="57"/>
+      <c r="H47" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="59"/>
-      <c r="J47" s="59"/>
-      <c r="K47" s="59"/>
-      <c r="L47" s="59"/>
-      <c r="M47" s="59"/>
-      <c r="N47" s="59"/>
-      <c r="O47" s="59"/>
-      <c r="P47" s="59"/>
-      <c r="Q47" s="59"/>
-      <c r="R47" s="59"/>
-      <c r="S47" s="59"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57"/>
+      <c r="L47" s="57"/>
+      <c r="M47" s="57"/>
+      <c r="N47" s="57"/>
+      <c r="O47" s="57"/>
+      <c r="P47" s="57"/>
+      <c r="Q47" s="57"/>
+      <c r="R47" s="57"/>
+      <c r="S47" s="57"/>
       <c r="U47" s="23" t="s">
         <v>66</v>
       </c>
@@ -4307,7 +4322,7 @@
       <c r="AA47" s="24"/>
       <c r="AB47" s="25"/>
     </row>
-    <row r="49" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
         <v>34</v>
       </c>
@@ -4320,19 +4335,19 @@
       <c r="E49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U49" s="70" t="s">
+      <c r="U49" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="V49" s="71"/>
-      <c r="W49" s="71"/>
-      <c r="X49" s="71"/>
-      <c r="Y49" s="71"/>
-      <c r="Z49" s="71"/>
-      <c r="AA49" s="71"/>
-      <c r="AB49" s="71"/>
-      <c r="AC49" s="72"/>
-    </row>
-    <row r="50" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V49" s="76"/>
+      <c r="W49" s="76"/>
+      <c r="X49" s="76"/>
+      <c r="Y49" s="76"/>
+      <c r="Z49" s="76"/>
+      <c r="AA49" s="76"/>
+      <c r="AB49" s="76"/>
+      <c r="AC49" s="88"/>
+    </row>
+    <row r="50" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C50" s="7">
         <v>2</v>
       </c>
@@ -4348,19 +4363,19 @@
       <c r="G50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U50" s="73" t="s">
+      <c r="U50" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="V50" s="74"/>
-      <c r="W50" s="74"/>
-      <c r="X50" s="74"/>
-      <c r="Y50" s="74"/>
-      <c r="Z50" s="74"/>
-      <c r="AA50" s="74"/>
-      <c r="AB50" s="74"/>
-      <c r="AC50" s="75"/>
-    </row>
-    <row r="51" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V50" s="68"/>
+      <c r="W50" s="68"/>
+      <c r="X50" s="68"/>
+      <c r="Y50" s="68"/>
+      <c r="Z50" s="68"/>
+      <c r="AA50" s="68"/>
+      <c r="AB50" s="68"/>
+      <c r="AC50" s="70"/>
+    </row>
+    <row r="51" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C51" s="7">
         <v>4</v>
       </c>
@@ -4370,29 +4385,29 @@
       <c r="E51" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="59" t="s">
+      <c r="F51" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="59"/>
-      <c r="H51" s="92" t="s">
+      <c r="G51" s="57"/>
+      <c r="H51" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="92"/>
-      <c r="J51" s="92"/>
-      <c r="K51" s="92"/>
-      <c r="U51" s="73" t="s">
+      <c r="I51" s="67"/>
+      <c r="J51" s="67"/>
+      <c r="K51" s="67"/>
+      <c r="U51" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="V51" s="74"/>
-      <c r="W51" s="74"/>
-      <c r="X51" s="74"/>
-      <c r="Y51" s="74"/>
-      <c r="Z51" s="74"/>
-      <c r="AA51" s="74"/>
-      <c r="AB51" s="74"/>
-      <c r="AC51" s="75"/>
-    </row>
-    <row r="52" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V51" s="68"/>
+      <c r="W51" s="68"/>
+      <c r="X51" s="68"/>
+      <c r="Y51" s="68"/>
+      <c r="Z51" s="68"/>
+      <c r="AA51" s="68"/>
+      <c r="AB51" s="68"/>
+      <c r="AC51" s="70"/>
+    </row>
+    <row r="52" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C52" s="11">
         <v>8</v>
       </c>
@@ -4402,72 +4417,72 @@
       <c r="E52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="59" t="s">
+      <c r="F52" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="59"/>
-      <c r="H52" s="59" t="s">
+      <c r="G52" s="57"/>
+      <c r="H52" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="59"/>
-      <c r="J52" s="59"/>
-      <c r="K52" s="59"/>
-      <c r="L52" s="59"/>
-      <c r="M52" s="59"/>
-      <c r="N52" s="59"/>
-      <c r="O52" s="59"/>
-      <c r="P52" s="59"/>
-      <c r="Q52" s="59"/>
-      <c r="R52" s="59"/>
-      <c r="S52" s="59"/>
-      <c r="U52" s="67" t="s">
+      <c r="I52" s="57"/>
+      <c r="J52" s="57"/>
+      <c r="K52" s="57"/>
+      <c r="L52" s="57"/>
+      <c r="M52" s="57"/>
+      <c r="N52" s="57"/>
+      <c r="O52" s="57"/>
+      <c r="P52" s="57"/>
+      <c r="Q52" s="57"/>
+      <c r="R52" s="57"/>
+      <c r="S52" s="57"/>
+      <c r="U52" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="V52" s="68"/>
-      <c r="W52" s="68"/>
-      <c r="X52" s="68"/>
-      <c r="Y52" s="68"/>
-      <c r="Z52" s="68"/>
-      <c r="AA52" s="68"/>
-      <c r="AB52" s="68"/>
-      <c r="AC52" s="69"/>
-    </row>
-    <row r="54" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V52" s="72"/>
+      <c r="W52" s="72"/>
+      <c r="X52" s="72"/>
+      <c r="Y52" s="72"/>
+      <c r="Z52" s="72"/>
+      <c r="AA52" s="72"/>
+      <c r="AB52" s="72"/>
+      <c r="AC52" s="73"/>
+    </row>
+    <row r="54" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="74" t="s">
+      <c r="C54" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
-      <c r="G54" s="74"/>
-      <c r="H54" s="74"/>
-      <c r="I54" s="74"/>
-      <c r="J54" s="74"/>
-      <c r="K54" s="74"/>
-      <c r="L54" s="74"/>
-      <c r="M54" s="74"/>
-      <c r="N54" s="74"/>
-      <c r="O54" s="74"/>
-      <c r="P54" s="74"/>
-      <c r="Q54" s="74"/>
-      <c r="R54" s="74"/>
-      <c r="S54" s="74"/>
-      <c r="U54" s="82" t="s">
+      <c r="D54" s="68"/>
+      <c r="E54" s="68"/>
+      <c r="F54" s="68"/>
+      <c r="G54" s="68"/>
+      <c r="H54" s="68"/>
+      <c r="I54" s="68"/>
+      <c r="J54" s="68"/>
+      <c r="K54" s="68"/>
+      <c r="L54" s="68"/>
+      <c r="M54" s="68"/>
+      <c r="N54" s="68"/>
+      <c r="O54" s="68"/>
+      <c r="P54" s="68"/>
+      <c r="Q54" s="68"/>
+      <c r="R54" s="68"/>
+      <c r="S54" s="68"/>
+      <c r="U54" s="85" t="s">
         <v>75</v>
       </c>
-      <c r="V54" s="83"/>
-      <c r="W54" s="83"/>
-      <c r="X54" s="83"/>
-      <c r="Y54" s="83"/>
-      <c r="Z54" s="83"/>
-      <c r="AA54" s="83"/>
-      <c r="AB54" s="83"/>
-      <c r="AC54" s="84"/>
-    </row>
-    <row r="56" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V54" s="86"/>
+      <c r="W54" s="86"/>
+      <c r="X54" s="86"/>
+      <c r="Y54" s="86"/>
+      <c r="Z54" s="86"/>
+      <c r="AA54" s="86"/>
+      <c r="AB54" s="86"/>
+      <c r="AC54" s="87"/>
+    </row>
+    <row r="56" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
         <v>8</v>
       </c>
@@ -4480,19 +4495,19 @@
       <c r="E56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U56" s="70" t="s">
+      <c r="U56" s="75" t="s">
         <v>76</v>
       </c>
-      <c r="V56" s="71"/>
-      <c r="W56" s="71"/>
-      <c r="X56" s="71"/>
-      <c r="Y56" s="71"/>
-      <c r="Z56" s="71"/>
-      <c r="AA56" s="71"/>
-      <c r="AB56" s="71"/>
-      <c r="AC56" s="72"/>
-    </row>
-    <row r="57" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V56" s="76"/>
+      <c r="W56" s="76"/>
+      <c r="X56" s="76"/>
+      <c r="Y56" s="76"/>
+      <c r="Z56" s="76"/>
+      <c r="AA56" s="76"/>
+      <c r="AB56" s="76"/>
+      <c r="AC56" s="88"/>
+    </row>
+    <row r="57" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C57" s="7">
         <v>2</v>
       </c>
@@ -4506,19 +4521,19 @@
         <v>3</v>
       </c>
       <c r="G57" s="66"/>
-      <c r="U57" s="73" t="s">
+      <c r="U57" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="V57" s="74"/>
-      <c r="W57" s="74"/>
-      <c r="X57" s="74"/>
-      <c r="Y57" s="74"/>
-      <c r="Z57" s="74"/>
-      <c r="AA57" s="74"/>
-      <c r="AB57" s="74"/>
-      <c r="AC57" s="75"/>
-    </row>
-    <row r="58" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V57" s="68"/>
+      <c r="W57" s="68"/>
+      <c r="X57" s="68"/>
+      <c r="Y57" s="68"/>
+      <c r="Z57" s="68"/>
+      <c r="AA57" s="68"/>
+      <c r="AB57" s="68"/>
+      <c r="AC57" s="70"/>
+    </row>
+    <row r="58" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C58" s="7">
         <v>4</v>
       </c>
@@ -4528,27 +4543,27 @@
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="59" t="s">
+      <c r="F58" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G58" s="59"/>
-      <c r="H58" s="59" t="s">
+      <c r="G58" s="57"/>
+      <c r="H58" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I58" s="59"/>
-      <c r="U58" s="67" t="s">
+      <c r="I58" s="57"/>
+      <c r="U58" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="V58" s="68"/>
-      <c r="W58" s="68"/>
-      <c r="X58" s="68"/>
-      <c r="Y58" s="68"/>
-      <c r="Z58" s="68"/>
-      <c r="AA58" s="68"/>
-      <c r="AB58" s="68"/>
-      <c r="AC58" s="69"/>
-    </row>
-    <row r="60" spans="2:29" x14ac:dyDescent="0.3">
+      <c r="V58" s="72"/>
+      <c r="W58" s="72"/>
+      <c r="X58" s="72"/>
+      <c r="Y58" s="72"/>
+      <c r="Z58" s="72"/>
+      <c r="AA58" s="72"/>
+      <c r="AB58" s="72"/>
+      <c r="AC58" s="73"/>
+    </row>
+    <row r="60" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
         <v>0</v>
       </c>
@@ -4573,7 +4588,7 @@
       <c r="AB60" s="18"/>
       <c r="AC60" s="19"/>
     </row>
-    <row r="61" spans="2:29" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C61" s="7">
         <v>2</v>
       </c>
@@ -4587,19 +4602,19 @@
         <v>3</v>
       </c>
       <c r="G61" s="66"/>
-      <c r="U61" s="73" t="s">
+      <c r="U61" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="V61" s="74"/>
-      <c r="W61" s="74"/>
-      <c r="X61" s="74"/>
-      <c r="Y61" s="74"/>
-      <c r="Z61" s="74"/>
-      <c r="AA61" s="74"/>
-      <c r="AB61" s="74"/>
-      <c r="AC61" s="75"/>
-    </row>
-    <row r="62" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V61" s="68"/>
+      <c r="W61" s="68"/>
+      <c r="X61" s="68"/>
+      <c r="Y61" s="68"/>
+      <c r="Z61" s="68"/>
+      <c r="AA61" s="68"/>
+      <c r="AB61" s="68"/>
+      <c r="AC61" s="70"/>
+    </row>
+    <row r="62" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C62" s="7">
         <v>4</v>
       </c>
@@ -4609,53 +4624,53 @@
       <c r="E62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="59" t="s">
+      <c r="F62" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="59"/>
-      <c r="H62" s="59" t="s">
+      <c r="G62" s="57"/>
+      <c r="H62" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I62" s="59"/>
-      <c r="J62" s="59" t="s">
+      <c r="I62" s="57"/>
+      <c r="J62" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="K62" s="59"/>
-      <c r="U62" s="76" t="s">
+      <c r="K62" s="57"/>
+      <c r="U62" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="V62" s="77"/>
-      <c r="W62" s="77"/>
-      <c r="X62" s="77"/>
-      <c r="Y62" s="77"/>
-      <c r="Z62" s="77"/>
-      <c r="AA62" s="77"/>
-      <c r="AB62" s="77"/>
-      <c r="AC62" s="78"/>
-    </row>
-    <row r="63" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="U63" s="76"/>
-      <c r="V63" s="77"/>
-      <c r="W63" s="77"/>
-      <c r="X63" s="77"/>
-      <c r="Y63" s="77"/>
-      <c r="Z63" s="77"/>
-      <c r="AA63" s="77"/>
-      <c r="AB63" s="77"/>
-      <c r="AC63" s="78"/>
-    </row>
-    <row r="64" spans="2:29" x14ac:dyDescent="0.3">
-      <c r="U64" s="79"/>
-      <c r="V64" s="80"/>
-      <c r="W64" s="80"/>
-      <c r="X64" s="80"/>
-      <c r="Y64" s="80"/>
-      <c r="Z64" s="80"/>
-      <c r="AA64" s="80"/>
-      <c r="AB64" s="80"/>
-      <c r="AC64" s="81"/>
-    </row>
-    <row r="65" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V62" s="90"/>
+      <c r="W62" s="90"/>
+      <c r="X62" s="90"/>
+      <c r="Y62" s="90"/>
+      <c r="Z62" s="90"/>
+      <c r="AA62" s="90"/>
+      <c r="AB62" s="90"/>
+      <c r="AC62" s="91"/>
+    </row>
+    <row r="63" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="U63" s="89"/>
+      <c r="V63" s="90"/>
+      <c r="W63" s="90"/>
+      <c r="X63" s="90"/>
+      <c r="Y63" s="90"/>
+      <c r="Z63" s="90"/>
+      <c r="AA63" s="90"/>
+      <c r="AB63" s="90"/>
+      <c r="AC63" s="91"/>
+    </row>
+    <row r="64" spans="2:29" x14ac:dyDescent="0.45">
+      <c r="U64" s="92"/>
+      <c r="V64" s="93"/>
+      <c r="W64" s="93"/>
+      <c r="X64" s="93"/>
+      <c r="Y64" s="93"/>
+      <c r="Z64" s="93"/>
+      <c r="AA64" s="93"/>
+      <c r="AB64" s="93"/>
+      <c r="AC64" s="94"/>
+    </row>
+    <row r="65" spans="2:30" x14ac:dyDescent="0.45">
       <c r="U65" s="26"/>
       <c r="V65" s="26"/>
       <c r="W65" s="26"/>
@@ -4666,7 +4681,7 @@
       <c r="AB65" s="26"/>
       <c r="AC65" s="26"/>
     </row>
-    <row r="66" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:30" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
         <v>38</v>
       </c>
@@ -4679,20 +4694,20 @@
       <c r="E66" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U66" s="70" t="s">
+      <c r="U66" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="V66" s="71"/>
-      <c r="W66" s="71"/>
-      <c r="X66" s="71"/>
-      <c r="Y66" s="71"/>
-      <c r="Z66" s="71"/>
-      <c r="AA66" s="71"/>
-      <c r="AB66" s="71"/>
-      <c r="AC66" s="71"/>
-      <c r="AD66" s="72"/>
-    </row>
-    <row r="67" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V66" s="76"/>
+      <c r="W66" s="76"/>
+      <c r="X66" s="76"/>
+      <c r="Y66" s="76"/>
+      <c r="Z66" s="76"/>
+      <c r="AA66" s="76"/>
+      <c r="AB66" s="76"/>
+      <c r="AC66" s="76"/>
+      <c r="AD66" s="88"/>
+    </row>
+    <row r="67" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C67" s="7">
         <v>2</v>
       </c>
@@ -4708,20 +4723,20 @@
       <c r="G67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U67" s="73" t="s">
+      <c r="U67" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="V67" s="74"/>
-      <c r="W67" s="74"/>
-      <c r="X67" s="74"/>
-      <c r="Y67" s="74"/>
-      <c r="Z67" s="74"/>
-      <c r="AA67" s="74"/>
-      <c r="AB67" s="74"/>
-      <c r="AC67" s="74"/>
-      <c r="AD67" s="75"/>
-    </row>
-    <row r="68" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V67" s="68"/>
+      <c r="W67" s="68"/>
+      <c r="X67" s="68"/>
+      <c r="Y67" s="68"/>
+      <c r="Z67" s="68"/>
+      <c r="AA67" s="68"/>
+      <c r="AB67" s="68"/>
+      <c r="AC67" s="68"/>
+      <c r="AD67" s="70"/>
+    </row>
+    <row r="68" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C68" s="7">
         <v>4</v>
       </c>
@@ -4747,20 +4762,20 @@
         <v>44</v>
       </c>
       <c r="K68" s="66"/>
-      <c r="U68" s="73" t="s">
+      <c r="U68" s="69" t="s">
         <v>83</v>
       </c>
-      <c r="V68" s="74"/>
-      <c r="W68" s="74"/>
-      <c r="X68" s="74"/>
-      <c r="Y68" s="74"/>
-      <c r="Z68" s="74"/>
-      <c r="AA68" s="74"/>
-      <c r="AB68" s="74"/>
-      <c r="AC68" s="74"/>
-      <c r="AD68" s="75"/>
-    </row>
-    <row r="69" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="V68" s="68"/>
+      <c r="W68" s="68"/>
+      <c r="X68" s="68"/>
+      <c r="Y68" s="68"/>
+      <c r="Z68" s="68"/>
+      <c r="AA68" s="68"/>
+      <c r="AB68" s="68"/>
+      <c r="AC68" s="68"/>
+      <c r="AD68" s="70"/>
+    </row>
+    <row r="69" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C69" s="11">
         <v>8</v>
       </c>
@@ -4770,10 +4785,10 @@
       <c r="E69" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F69" s="59" t="s">
+      <c r="F69" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="59"/>
+      <c r="G69" s="57"/>
       <c r="H69" s="64" t="s">
         <v>41</v>
       </c>
@@ -4796,89 +4811,132 @@
       <c r="Q69" s="65"/>
       <c r="R69" s="65"/>
       <c r="S69" s="66"/>
-      <c r="U69" s="67" t="s">
-        <v>249</v>
-      </c>
-      <c r="V69" s="68"/>
-      <c r="W69" s="68"/>
-      <c r="X69" s="68"/>
-      <c r="Y69" s="68"/>
-      <c r="Z69" s="68"/>
-      <c r="AA69" s="68"/>
-      <c r="AB69" s="68"/>
-      <c r="AC69" s="68"/>
-      <c r="AD69" s="69"/>
-    </row>
-    <row r="71" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
+      <c r="U69" s="71" t="s">
+        <v>248</v>
+      </c>
+      <c r="V69" s="72"/>
+      <c r="W69" s="72"/>
+      <c r="X69" s="72"/>
+      <c r="Y69" s="72"/>
+      <c r="Z69" s="72"/>
+      <c r="AA69" s="72"/>
+      <c r="AB69" s="72"/>
+      <c r="AC69" s="72"/>
+      <c r="AD69" s="73"/>
+    </row>
+    <row r="70" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C70" s="95"/>
+      <c r="D70" s="96"/>
+      <c r="E70" s="96"/>
+      <c r="F70" s="96"/>
+      <c r="G70" s="96"/>
+      <c r="H70" s="96"/>
+      <c r="I70" s="96"/>
+      <c r="J70" s="96"/>
+      <c r="K70" s="96"/>
+      <c r="L70" s="96"/>
+      <c r="M70" s="96"/>
+      <c r="N70" s="96"/>
+      <c r="O70" s="96"/>
+      <c r="P70" s="96"/>
+      <c r="Q70" s="96"/>
+      <c r="R70" s="96"/>
+      <c r="S70" s="96"/>
+      <c r="U70" s="97" t="s">
+        <v>270</v>
+      </c>
+      <c r="V70" s="97"/>
+      <c r="W70" s="97"/>
+      <c r="X70" s="97"/>
+      <c r="Y70" s="97"/>
+      <c r="Z70" s="97"/>
+      <c r="AA70" s="97"/>
+      <c r="AB70" s="97"/>
+      <c r="AC70" s="97"/>
+      <c r="AD70" s="97"/>
+    </row>
+    <row r="71" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C71" s="95"/>
+      <c r="D71" s="96"/>
+      <c r="E71" s="96"/>
+      <c r="F71" s="96"/>
+      <c r="G71" s="96"/>
+      <c r="H71" s="96"/>
+      <c r="I71" s="96"/>
+      <c r="J71" s="96"/>
+      <c r="K71" s="96"/>
+      <c r="L71" s="96"/>
+      <c r="M71" s="96"/>
+      <c r="N71" s="96"/>
+      <c r="O71" s="96"/>
+      <c r="P71" s="96"/>
+      <c r="Q71" s="96"/>
+      <c r="R71" s="96"/>
+      <c r="S71" s="96"/>
+      <c r="U71" s="97" t="s">
+        <v>271</v>
+      </c>
+      <c r="V71" s="97"/>
+      <c r="W71" s="97"/>
+      <c r="X71" s="97"/>
+      <c r="Y71" s="97"/>
+      <c r="Z71" s="97"/>
+      <c r="AA71" s="97"/>
+      <c r="AB71" s="97"/>
+      <c r="AC71" s="97"/>
+      <c r="AD71" s="97"/>
+    </row>
+    <row r="72" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C72" s="95"/>
+      <c r="D72" s="96"/>
+      <c r="E72" s="96"/>
+      <c r="F72" s="96"/>
+      <c r="G72" s="96"/>
+      <c r="H72" s="96"/>
+      <c r="I72" s="96"/>
+      <c r="J72" s="96"/>
+      <c r="K72" s="96"/>
+      <c r="L72" s="96"/>
+      <c r="M72" s="96"/>
+      <c r="N72" s="96"/>
+      <c r="O72" s="96"/>
+      <c r="P72" s="96"/>
+      <c r="Q72" s="96"/>
+      <c r="R72" s="96"/>
+      <c r="S72" s="96"/>
+      <c r="U72" s="97"/>
+      <c r="V72" s="97"/>
+      <c r="W72" s="97"/>
+      <c r="X72" s="97"/>
+      <c r="Y72" s="97"/>
+      <c r="Z72" s="97"/>
+      <c r="AA72" s="97"/>
+      <c r="AB72" s="97"/>
+      <c r="AC72" s="97"/>
+      <c r="AD72" s="97"/>
+    </row>
+    <row r="74" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="B74" t="s">
         <v>45</v>
-      </c>
-      <c r="C71" s="7">
-        <v>1</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="U71" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="V71" s="71"/>
-      <c r="W71" s="71"/>
-      <c r="X71" s="71"/>
-      <c r="Y71" s="72"/>
-    </row>
-    <row r="72" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="C72" s="7">
-        <v>2</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F72" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="G72" s="66"/>
-      <c r="U72" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="V72" s="68"/>
-      <c r="W72" s="68"/>
-      <c r="X72" s="68"/>
-      <c r="Y72" s="69"/>
-    </row>
-    <row r="74" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
-        <v>47</v>
       </c>
       <c r="C74" s="7">
         <v>1</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U74" s="70" t="s">
-        <v>86</v>
-      </c>
-      <c r="V74" s="71"/>
-      <c r="W74" s="71"/>
-      <c r="X74" s="71"/>
-      <c r="Y74" s="71"/>
-      <c r="Z74" s="71"/>
-      <c r="AA74" s="71"/>
-      <c r="AB74" s="71"/>
-      <c r="AC74" s="71"/>
-      <c r="AD74" s="72"/>
-    </row>
-    <row r="75" spans="2:32" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="U74" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="V74" s="76"/>
+      <c r="W74" s="76"/>
+      <c r="X74" s="76"/>
+      <c r="Y74" s="88"/>
+    </row>
+    <row r="75" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C75" s="7">
         <v>2</v>
       </c>
@@ -4886,195 +4944,304 @@
         <v>4</v>
       </c>
       <c r="E75" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F75" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G75" s="66"/>
+      <c r="U75" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="V75" s="72"/>
+      <c r="W75" s="72"/>
+      <c r="X75" s="72"/>
+      <c r="Y75" s="73"/>
+    </row>
+    <row r="77" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="B77" t="s">
+        <v>47</v>
+      </c>
+      <c r="C77" s="7">
+        <v>1</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F75" s="64" t="s">
+      <c r="E77" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G75" s="66"/>
-      <c r="U75" s="73" t="s">
+      <c r="U77" s="75" t="s">
+        <v>86</v>
+      </c>
+      <c r="V77" s="76"/>
+      <c r="W77" s="76"/>
+      <c r="X77" s="76"/>
+      <c r="Y77" s="76"/>
+      <c r="Z77" s="76"/>
+      <c r="AA77" s="76"/>
+      <c r="AB77" s="76"/>
+      <c r="AC77" s="76"/>
+      <c r="AD77" s="88"/>
+    </row>
+    <row r="78" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C78" s="7">
+        <v>2</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F78" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="G78" s="66"/>
+      <c r="U78" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="V75" s="74"/>
-      <c r="W75" s="74"/>
-      <c r="X75" s="74"/>
-      <c r="Y75" s="74"/>
-      <c r="Z75" s="74"/>
-      <c r="AA75" s="74"/>
-      <c r="AB75" s="74"/>
-      <c r="AC75" s="74"/>
-      <c r="AD75" s="75"/>
-    </row>
-    <row r="76" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="C76" s="7">
+      <c r="V78" s="68"/>
+      <c r="W78" s="68"/>
+      <c r="X78" s="68"/>
+      <c r="Y78" s="68"/>
+      <c r="Z78" s="68"/>
+      <c r="AA78" s="68"/>
+      <c r="AB78" s="68"/>
+      <c r="AC78" s="68"/>
+      <c r="AD78" s="70"/>
+    </row>
+    <row r="79" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C79" s="7">
         <v>4</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="E79" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F76" s="59" t="s">
+      <c r="F79" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="G76" s="59"/>
-      <c r="H76" s="59" t="s">
+      <c r="G79" s="57"/>
+      <c r="H79" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="I76" s="59"/>
-      <c r="J76" s="7" t="s">
+      <c r="I79" s="57"/>
+      <c r="J79" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="K76" s="7" t="s">
+      <c r="K79" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U76" s="67" t="s">
+      <c r="U79" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="V76" s="68"/>
-      <c r="W76" s="68"/>
-      <c r="X76" s="68"/>
-      <c r="Y76" s="68"/>
-      <c r="Z76" s="68"/>
-      <c r="AA76" s="68"/>
-      <c r="AB76" s="68"/>
-      <c r="AC76" s="68"/>
-      <c r="AD76" s="69"/>
-    </row>
-    <row r="78" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="B78" t="s">
+      <c r="V79" s="72"/>
+      <c r="W79" s="72"/>
+      <c r="X79" s="72"/>
+      <c r="Y79" s="72"/>
+      <c r="Z79" s="72"/>
+      <c r="AA79" s="72"/>
+      <c r="AB79" s="72"/>
+      <c r="AC79" s="72"/>
+      <c r="AD79" s="73"/>
+    </row>
+    <row r="81" spans="2:32" x14ac:dyDescent="0.45">
+      <c r="B81" t="s">
         <v>51</v>
       </c>
-      <c r="C78" s="7">
+      <c r="C81" s="7">
         <v>1</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E81" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U78" s="70" t="s">
+      <c r="U81" s="75" t="s">
+        <v>255</v>
+      </c>
+      <c r="V81" s="76"/>
+      <c r="W81" s="76"/>
+      <c r="X81" s="76"/>
+      <c r="Y81" s="76"/>
+      <c r="Z81" s="76"/>
+      <c r="AA81" s="76"/>
+      <c r="AB81" s="76"/>
+      <c r="AC81" s="76"/>
+      <c r="AD81" s="88"/>
+      <c r="AF81" t="s">
         <v>256</v>
       </c>
-      <c r="V78" s="71"/>
-      <c r="W78" s="71"/>
-      <c r="X78" s="71"/>
-      <c r="Y78" s="71"/>
-      <c r="Z78" s="71"/>
-      <c r="AA78" s="71"/>
-      <c r="AB78" s="71"/>
-      <c r="AC78" s="71"/>
-      <c r="AD78" s="72"/>
-      <c r="AF78" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="79" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="C79" s="7">
+    </row>
+    <row r="82" spans="2:32" x14ac:dyDescent="0.45">
+      <c r="C82" s="7">
         <v>2</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F79" s="64" t="s">
+      <c r="F82" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="G79" s="66"/>
-      <c r="U79" s="73" t="s">
+      <c r="G82" s="66"/>
+      <c r="U82" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="V79" s="74"/>
-      <c r="W79" s="74"/>
-      <c r="X79" s="74"/>
-      <c r="Y79" s="74"/>
-      <c r="Z79" s="74"/>
-      <c r="AA79" s="74"/>
-      <c r="AB79" s="74"/>
-      <c r="AC79" s="74"/>
-      <c r="AD79" s="75"/>
-    </row>
-    <row r="80" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="C80" s="7">
+      <c r="V82" s="68"/>
+      <c r="W82" s="68"/>
+      <c r="X82" s="68"/>
+      <c r="Y82" s="68"/>
+      <c r="Z82" s="68"/>
+      <c r="AA82" s="68"/>
+      <c r="AB82" s="68"/>
+      <c r="AC82" s="68"/>
+      <c r="AD82" s="70"/>
+    </row>
+    <row r="83" spans="2:32" x14ac:dyDescent="0.45">
+      <c r="C83" s="7">
         <v>4</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="E83" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F80" s="59" t="s">
+      <c r="F83" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="G80" s="59"/>
-      <c r="H80" s="59" t="s">
+      <c r="G83" s="57"/>
+      <c r="H83" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="I80" s="59"/>
-      <c r="J80" s="7" t="s">
+      <c r="I83" s="57"/>
+      <c r="J83" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="K80" s="7" t="s">
+      <c r="K83" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U80" s="67" t="s">
-        <v>255</v>
-      </c>
-      <c r="V80" s="68"/>
-      <c r="W80" s="68"/>
-      <c r="X80" s="68"/>
-      <c r="Y80" s="68"/>
-      <c r="Z80" s="68"/>
-      <c r="AA80" s="68"/>
-      <c r="AB80" s="68"/>
-      <c r="AC80" s="68"/>
-      <c r="AD80" s="69"/>
-      <c r="AF80" s="49"/>
-    </row>
-    <row r="82" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B82" t="s">
+      <c r="U83" s="71" t="s">
+        <v>254</v>
+      </c>
+      <c r="V83" s="72"/>
+      <c r="W83" s="72"/>
+      <c r="X83" s="72"/>
+      <c r="Y83" s="72"/>
+      <c r="Z83" s="72"/>
+      <c r="AA83" s="72"/>
+      <c r="AB83" s="72"/>
+      <c r="AC83" s="72"/>
+      <c r="AD83" s="73"/>
+      <c r="AF83" s="49"/>
+    </row>
+    <row r="85" spans="2:32" x14ac:dyDescent="0.45">
+      <c r="B85" t="s">
         <v>96</v>
       </c>
-      <c r="C82" s="17">
+      <c r="C85" s="17">
         <v>1</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E82" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="U82" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="83" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="C83" s="7">
+      <c r="E85" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="U85" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="86" spans="2:32" x14ac:dyDescent="0.45">
+      <c r="C86" s="7">
         <v>2</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="E86" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F83" s="64" t="s">
-        <v>240</v>
-      </c>
-      <c r="G83" s="66"/>
+      <c r="F86" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="G86" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="U75:Y75"/>
+    <mergeCell ref="U77:AD77"/>
+    <mergeCell ref="U78:AD78"/>
+    <mergeCell ref="U79:AD79"/>
+    <mergeCell ref="F75:G75"/>
+    <mergeCell ref="F78:G78"/>
+    <mergeCell ref="F79:G79"/>
+    <mergeCell ref="H79:I79"/>
+    <mergeCell ref="F82:G82"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="U83:AD83"/>
+    <mergeCell ref="U82:AD82"/>
+    <mergeCell ref="U81:AD81"/>
+    <mergeCell ref="U74:Y74"/>
+    <mergeCell ref="U56:AC56"/>
+    <mergeCell ref="U57:AC57"/>
+    <mergeCell ref="U58:AC58"/>
+    <mergeCell ref="U61:AC61"/>
+    <mergeCell ref="U62:AC64"/>
+    <mergeCell ref="U66:AD66"/>
+    <mergeCell ref="U67:AD67"/>
+    <mergeCell ref="U68:AD68"/>
+    <mergeCell ref="U69:AD69"/>
+    <mergeCell ref="U49:AC49"/>
+    <mergeCell ref="U50:AC50"/>
+    <mergeCell ref="U51:AC51"/>
+    <mergeCell ref="U52:AC52"/>
+    <mergeCell ref="U54:AC54"/>
+    <mergeCell ref="U39:X40"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="U37:AB37"/>
+    <mergeCell ref="U15:X18"/>
+    <mergeCell ref="U21:X24"/>
+    <mergeCell ref="H22:S22"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="U30:AB30"/>
+    <mergeCell ref="U31:AB31"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="U26:X26"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="C26:S26"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="I31:S31"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C42:S42"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="C33:S33"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
     <mergeCell ref="P69:S69"/>
     <mergeCell ref="F61:G61"/>
     <mergeCell ref="F47:G47"/>
@@ -5091,72 +5258,11 @@
     <mergeCell ref="L69:M69"/>
     <mergeCell ref="N69:O69"/>
     <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="I31:S31"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C42:S42"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="C33:S33"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="U30:AB30"/>
-    <mergeCell ref="U31:AB31"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="U26:X26"/>
-    <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U29:X29"/>
-    <mergeCell ref="C26:S26"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="U15:X18"/>
-    <mergeCell ref="U21:X24"/>
-    <mergeCell ref="H22:S22"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="U39:X40"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="U35:X35"/>
-    <mergeCell ref="U37:AB37"/>
-    <mergeCell ref="U49:AC49"/>
-    <mergeCell ref="U50:AC50"/>
-    <mergeCell ref="U51:AC51"/>
-    <mergeCell ref="U52:AC52"/>
-    <mergeCell ref="U54:AC54"/>
-    <mergeCell ref="U71:Y71"/>
-    <mergeCell ref="U56:AC56"/>
-    <mergeCell ref="U57:AC57"/>
-    <mergeCell ref="U58:AC58"/>
-    <mergeCell ref="U61:AC61"/>
-    <mergeCell ref="U62:AC64"/>
-    <mergeCell ref="U66:AD66"/>
-    <mergeCell ref="U67:AD67"/>
-    <mergeCell ref="U68:AD68"/>
-    <mergeCell ref="U69:AD69"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="U72:Y72"/>
-    <mergeCell ref="U74:AD74"/>
-    <mergeCell ref="U75:AD75"/>
-    <mergeCell ref="U76:AD76"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="H76:I76"/>
-    <mergeCell ref="F79:G79"/>
-    <mergeCell ref="F80:G80"/>
-    <mergeCell ref="H80:I80"/>
-    <mergeCell ref="U80:AD80"/>
-    <mergeCell ref="U79:AD79"/>
-    <mergeCell ref="U78:AD78"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5171,14 +5277,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B4" s="49"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ALU LOAD/STORE R[N.SRC] - Index register, ST_SRC - size of record, if 0 - index is not used
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar\Documents\Work\AI\CPU\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2E6F53-8C97-4FB3-BE9B-DD65953E5B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBF3D36-2C70-44EC-AC5C-88F036CBBBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21075" activeTab="2" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
@@ -1200,10 +1200,10 @@
     <t>Shift Right</t>
   </si>
   <si>
-    <t>LOAD: R[N.DST] = M[R[N.RS] + R[N.SRC]*ADT.sizeof() + ofs]</t>
-  </si>
-  <si>
-    <t>STORE:  M[R[N.RS] + R[N.SRC]*ADT.sizeof() + ofs] = R[N.DST]</t>
+    <t>STORE:  M[R[N.RS] + R[N.SRC]*ST_SRC + ofs] = R[N.DST]</t>
+  </si>
+  <si>
+    <t>LOAD: R[N.DST] = M[R[N.RS] + R[N.SRC]*ST_SRC + ofs], if ST_SRC is zero, R[N.SRC] is not used, can be any value.</t>
   </si>
 </sst>
 </file>
@@ -3471,7 +3471,7 @@
   <dimension ref="A2:AF86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="U72" sqref="U72"/>
+      <selection activeCell="U71" sqref="U71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4843,7 +4843,7 @@
       <c r="R70" s="96"/>
       <c r="S70" s="96"/>
       <c r="U70" s="97" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="V70" s="97"/>
       <c r="W70" s="97"/>
@@ -4874,7 +4874,7 @@
       <c r="R71" s="96"/>
       <c r="S71" s="96"/>
       <c r="U71" s="97" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="V71" s="97"/>
       <c r="W71" s="97"/>

</xml_diff>

<commit_message>
ALU Vector Mode optimizations
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar\Documents\Work\AI\CPU\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBF3D36-2C70-44EC-AC5C-88F036CBBBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA6114A-0365-4466-996B-849FF565CB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21075" activeTab="2" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="277">
   <si>
     <t>POP</t>
   </si>
@@ -1204,6 +1204,21 @@
   </si>
   <si>
     <t>LOAD: R[N.DST] = M[R[N.RS] + R[N.SRC]*ST_SRC + ofs], if ST_SRC is zero, R[N.SRC] is not used, can be any value.</t>
+  </si>
+  <si>
+    <t>LOOKUP: Searches for sub-sequence pointed by R[N.SRC], length R[N.SRC+1] in sequence pointed by R[N.RS], length R[N.SRC+1],</t>
+  </si>
+  <si>
+    <t>if found, store its pointer to R[N.DST] and 0 to R[N.DST+1]</t>
+  </si>
+  <si>
+    <t>if not found, store 1 to R[N.DST+1]</t>
+  </si>
+  <si>
+    <t>ST_RS and ST_SRC are used to advance pointers of main and sub-sequences in loop for comparison.</t>
+  </si>
+  <si>
+    <t>Note: basic ALU operations have scalar mode (VL == 0) or vector mode (VL &gt; 0). In vector mode ALU performs VL operations on its arguments. Argument will be read from register, if its stride is 0, or from memory, next argument value will be fetched from next register or memory, incrementing pointer by its stride. Same for destination.</t>
   </si>
 </sst>
 </file>
@@ -1788,7 +1803,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2014,6 +2029,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3468,10 +3486,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43404EB-A4C0-4EEB-BCD6-93EC84295AA2}">
-  <dimension ref="A2:AF86"/>
+  <dimension ref="A2:AF90"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="U71" sqref="U71"/>
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4856,22 +4874,24 @@
       <c r="AD70" s="97"/>
     </row>
     <row r="71" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C71" s="95"/>
-      <c r="D71" s="96"/>
-      <c r="E71" s="96"/>
-      <c r="F71" s="96"/>
-      <c r="G71" s="96"/>
-      <c r="H71" s="96"/>
-      <c r="I71" s="96"/>
-      <c r="J71" s="96"/>
-      <c r="K71" s="96"/>
-      <c r="L71" s="96"/>
-      <c r="M71" s="96"/>
-      <c r="N71" s="96"/>
-      <c r="O71" s="96"/>
-      <c r="P71" s="96"/>
-      <c r="Q71" s="96"/>
-      <c r="R71" s="96"/>
+      <c r="C71" s="98" t="s">
+        <v>276</v>
+      </c>
+      <c r="D71" s="98"/>
+      <c r="E71" s="98"/>
+      <c r="F71" s="98"/>
+      <c r="G71" s="98"/>
+      <c r="H71" s="98"/>
+      <c r="I71" s="98"/>
+      <c r="J71" s="98"/>
+      <c r="K71" s="98"/>
+      <c r="L71" s="98"/>
+      <c r="M71" s="98"/>
+      <c r="N71" s="98"/>
+      <c r="O71" s="98"/>
+      <c r="P71" s="98"/>
+      <c r="Q71" s="98"/>
+      <c r="R71" s="98"/>
       <c r="S71" s="96"/>
       <c r="U71" s="97" t="s">
         <v>270</v>
@@ -4887,24 +4907,26 @@
       <c r="AD71" s="97"/>
     </row>
     <row r="72" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C72" s="95"/>
-      <c r="D72" s="96"/>
-      <c r="E72" s="96"/>
-      <c r="F72" s="96"/>
-      <c r="G72" s="96"/>
-      <c r="H72" s="96"/>
-      <c r="I72" s="96"/>
-      <c r="J72" s="96"/>
-      <c r="K72" s="96"/>
-      <c r="L72" s="96"/>
-      <c r="M72" s="96"/>
-      <c r="N72" s="96"/>
-      <c r="O72" s="96"/>
-      <c r="P72" s="96"/>
-      <c r="Q72" s="96"/>
-      <c r="R72" s="96"/>
+      <c r="C72" s="98"/>
+      <c r="D72" s="98"/>
+      <c r="E72" s="98"/>
+      <c r="F72" s="98"/>
+      <c r="G72" s="98"/>
+      <c r="H72" s="98"/>
+      <c r="I72" s="98"/>
+      <c r="J72" s="98"/>
+      <c r="K72" s="98"/>
+      <c r="L72" s="98"/>
+      <c r="M72" s="98"/>
+      <c r="N72" s="98"/>
+      <c r="O72" s="98"/>
+      <c r="P72" s="98"/>
+      <c r="Q72" s="98"/>
+      <c r="R72" s="98"/>
       <c r="S72" s="96"/>
-      <c r="U72" s="97"/>
+      <c r="U72" s="97" t="s">
+        <v>272</v>
+      </c>
       <c r="V72" s="97"/>
       <c r="W72" s="97"/>
       <c r="X72" s="97"/>
@@ -4915,154 +4937,186 @@
       <c r="AC72" s="97"/>
       <c r="AD72" s="97"/>
     </row>
+    <row r="73" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C73" s="98"/>
+      <c r="D73" s="98"/>
+      <c r="E73" s="98"/>
+      <c r="F73" s="98"/>
+      <c r="G73" s="98"/>
+      <c r="H73" s="98"/>
+      <c r="I73" s="98"/>
+      <c r="J73" s="98"/>
+      <c r="K73" s="98"/>
+      <c r="L73" s="98"/>
+      <c r="M73" s="98"/>
+      <c r="N73" s="98"/>
+      <c r="O73" s="98"/>
+      <c r="P73" s="98"/>
+      <c r="Q73" s="98"/>
+      <c r="R73" s="98"/>
+      <c r="S73" s="96"/>
+      <c r="U73" s="97" t="s">
+        <v>275</v>
+      </c>
+      <c r="V73" s="97"/>
+      <c r="W73" s="97"/>
+      <c r="X73" s="97"/>
+      <c r="Y73" s="97"/>
+      <c r="Z73" s="97"/>
+      <c r="AA73" s="97"/>
+      <c r="AB73" s="97"/>
+      <c r="AC73" s="97"/>
+      <c r="AD73" s="97"/>
+    </row>
     <row r="74" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="B74" t="s">
+      <c r="C74" s="98"/>
+      <c r="D74" s="98"/>
+      <c r="E74" s="98"/>
+      <c r="F74" s="98"/>
+      <c r="G74" s="98"/>
+      <c r="H74" s="98"/>
+      <c r="I74" s="98"/>
+      <c r="J74" s="98"/>
+      <c r="K74" s="98"/>
+      <c r="L74" s="98"/>
+      <c r="M74" s="98"/>
+      <c r="N74" s="98"/>
+      <c r="O74" s="98"/>
+      <c r="P74" s="98"/>
+      <c r="Q74" s="98"/>
+      <c r="R74" s="98"/>
+      <c r="S74" s="96"/>
+      <c r="U74" s="97" t="s">
+        <v>273</v>
+      </c>
+      <c r="V74" s="97"/>
+      <c r="W74" s="97"/>
+      <c r="X74" s="97"/>
+      <c r="Y74" s="97"/>
+      <c r="Z74" s="97"/>
+      <c r="AA74" s="97"/>
+      <c r="AB74" s="97"/>
+      <c r="AC74" s="97"/>
+      <c r="AD74" s="97"/>
+    </row>
+    <row r="75" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C75" s="98"/>
+      <c r="D75" s="98"/>
+      <c r="E75" s="98"/>
+      <c r="F75" s="98"/>
+      <c r="G75" s="98"/>
+      <c r="H75" s="98"/>
+      <c r="I75" s="98"/>
+      <c r="J75" s="98"/>
+      <c r="K75" s="98"/>
+      <c r="L75" s="98"/>
+      <c r="M75" s="98"/>
+      <c r="N75" s="98"/>
+      <c r="O75" s="98"/>
+      <c r="P75" s="98"/>
+      <c r="Q75" s="98"/>
+      <c r="R75" s="98"/>
+      <c r="S75" s="96"/>
+      <c r="U75" s="97" t="s">
+        <v>274</v>
+      </c>
+      <c r="V75" s="97"/>
+      <c r="W75" s="97"/>
+      <c r="X75" s="97"/>
+      <c r="Y75" s="97"/>
+      <c r="Z75" s="97"/>
+      <c r="AA75" s="97"/>
+      <c r="AB75" s="97"/>
+      <c r="AC75" s="97"/>
+      <c r="AD75" s="97"/>
+    </row>
+    <row r="76" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C76" s="95"/>
+      <c r="D76" s="96"/>
+      <c r="E76" s="96"/>
+      <c r="F76" s="96"/>
+      <c r="G76" s="96"/>
+      <c r="H76" s="96"/>
+      <c r="I76" s="96"/>
+      <c r="J76" s="96"/>
+      <c r="K76" s="96"/>
+      <c r="L76" s="96"/>
+      <c r="M76" s="96"/>
+      <c r="N76" s="96"/>
+      <c r="O76" s="96"/>
+      <c r="P76" s="96"/>
+      <c r="Q76" s="96"/>
+      <c r="R76" s="96"/>
+      <c r="S76" s="96"/>
+      <c r="U76" s="97"/>
+      <c r="V76" s="97"/>
+      <c r="W76" s="97"/>
+      <c r="X76" s="97"/>
+      <c r="Y76" s="97"/>
+      <c r="Z76" s="97"/>
+      <c r="AA76" s="97"/>
+      <c r="AB76" s="97"/>
+      <c r="AC76" s="97"/>
+      <c r="AD76" s="97"/>
+    </row>
+    <row r="78" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="B78" t="s">
         <v>45</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C78" s="7">
         <v>1</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U74" s="75" t="s">
+      <c r="U78" s="75" t="s">
         <v>84</v>
       </c>
-      <c r="V74" s="76"/>
-      <c r="W74" s="76"/>
-      <c r="X74" s="76"/>
-      <c r="Y74" s="88"/>
-    </row>
-    <row r="75" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C75" s="7">
-        <v>2</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F75" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="G75" s="66"/>
-      <c r="U75" s="71" t="s">
-        <v>85</v>
-      </c>
-      <c r="V75" s="72"/>
-      <c r="W75" s="72"/>
-      <c r="X75" s="72"/>
-      <c r="Y75" s="73"/>
-    </row>
-    <row r="77" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="B77" t="s">
-        <v>47</v>
-      </c>
-      <c r="C77" s="7">
-        <v>1</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U77" s="75" t="s">
-        <v>86</v>
-      </c>
-      <c r="V77" s="76"/>
-      <c r="W77" s="76"/>
-      <c r="X77" s="76"/>
-      <c r="Y77" s="76"/>
-      <c r="Z77" s="76"/>
-      <c r="AA77" s="76"/>
-      <c r="AB77" s="76"/>
-      <c r="AC77" s="76"/>
-      <c r="AD77" s="88"/>
-    </row>
-    <row r="78" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C78" s="7">
-        <v>2</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F78" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="G78" s="66"/>
-      <c r="U78" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="V78" s="68"/>
-      <c r="W78" s="68"/>
-      <c r="X78" s="68"/>
-      <c r="Y78" s="68"/>
-      <c r="Z78" s="68"/>
-      <c r="AA78" s="68"/>
-      <c r="AB78" s="68"/>
-      <c r="AC78" s="68"/>
-      <c r="AD78" s="70"/>
+      <c r="V78" s="76"/>
+      <c r="W78" s="76"/>
+      <c r="X78" s="76"/>
+      <c r="Y78" s="88"/>
     </row>
     <row r="79" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C79" s="7">
+        <v>2</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E79" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F79" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="G79" s="57"/>
-      <c r="H79" s="57" t="s">
-        <v>3</v>
-      </c>
-      <c r="I79" s="57"/>
-      <c r="J79" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K79" s="7" t="s">
-        <v>50</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F79" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G79" s="66"/>
       <c r="U79" s="71" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="V79" s="72"/>
       <c r="W79" s="72"/>
       <c r="X79" s="72"/>
-      <c r="Y79" s="72"/>
-      <c r="Z79" s="72"/>
-      <c r="AA79" s="72"/>
-      <c r="AB79" s="72"/>
-      <c r="AC79" s="72"/>
-      <c r="AD79" s="73"/>
+      <c r="Y79" s="73"/>
     </row>
     <row r="81" spans="2:32" x14ac:dyDescent="0.45">
       <c r="B81" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C81" s="7">
         <v>1</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>172</v>
+        <v>48</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>49</v>
       </c>
       <c r="U81" s="75" t="s">
-        <v>255</v>
+        <v>86</v>
       </c>
       <c r="V81" s="76"/>
       <c r="W81" s="76"/>
@@ -5073,9 +5127,6 @@
       <c r="AB81" s="76"/>
       <c r="AC81" s="76"/>
       <c r="AD81" s="88"/>
-      <c r="AF81" t="s">
-        <v>256</v>
-      </c>
     </row>
     <row r="82" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C82" s="7">
@@ -5085,7 +5136,7 @@
         <v>4</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>172</v>
+        <v>48</v>
       </c>
       <c r="F82" s="64" t="s">
         <v>49</v>
@@ -5112,7 +5163,7 @@
         <v>5</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>172</v>
+        <v>48</v>
       </c>
       <c r="F83" s="57" t="s">
         <v>49</v>
@@ -5129,7 +5180,7 @@
         <v>50</v>
       </c>
       <c r="U83" s="71" t="s">
-        <v>254</v>
+        <v>88</v>
       </c>
       <c r="V83" s="72"/>
       <c r="W83" s="72"/>
@@ -5140,23 +5191,34 @@
       <c r="AB83" s="72"/>
       <c r="AC83" s="72"/>
       <c r="AD83" s="73"/>
-      <c r="AF83" s="49"/>
     </row>
     <row r="85" spans="2:32" x14ac:dyDescent="0.45">
       <c r="B85" t="s">
-        <v>96</v>
-      </c>
-      <c r="C85" s="17">
+        <v>51</v>
+      </c>
+      <c r="C85" s="7">
         <v>1</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E85" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="U85" t="s">
-        <v>241</v>
+        <v>172</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U85" s="75" t="s">
+        <v>255</v>
+      </c>
+      <c r="V85" s="76"/>
+      <c r="W85" s="76"/>
+      <c r="X85" s="76"/>
+      <c r="Y85" s="76"/>
+      <c r="Z85" s="76"/>
+      <c r="AA85" s="76"/>
+      <c r="AB85" s="76"/>
+      <c r="AC85" s="76"/>
+      <c r="AD85" s="88"/>
+      <c r="AF85" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="86" spans="2:32" x14ac:dyDescent="0.45">
@@ -5167,31 +5229,114 @@
         <v>4</v>
       </c>
       <c r="E86" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F86" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="G86" s="66"/>
+      <c r="U86" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="V86" s="68"/>
+      <c r="W86" s="68"/>
+      <c r="X86" s="68"/>
+      <c r="Y86" s="68"/>
+      <c r="Z86" s="68"/>
+      <c r="AA86" s="68"/>
+      <c r="AB86" s="68"/>
+      <c r="AC86" s="68"/>
+      <c r="AD86" s="70"/>
+    </row>
+    <row r="87" spans="2:32" x14ac:dyDescent="0.45">
+      <c r="C87" s="7">
+        <v>4</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F87" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="G87" s="57"/>
+      <c r="H87" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="I87" s="57"/>
+      <c r="J87" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K87" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="U87" s="71" t="s">
+        <v>254</v>
+      </c>
+      <c r="V87" s="72"/>
+      <c r="W87" s="72"/>
+      <c r="X87" s="72"/>
+      <c r="Y87" s="72"/>
+      <c r="Z87" s="72"/>
+      <c r="AA87" s="72"/>
+      <c r="AB87" s="72"/>
+      <c r="AC87" s="72"/>
+      <c r="AD87" s="73"/>
+      <c r="AF87" s="49"/>
+    </row>
+    <row r="89" spans="2:32" x14ac:dyDescent="0.45">
+      <c r="B89" t="s">
+        <v>96</v>
+      </c>
+      <c r="C89" s="17">
+        <v>1</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F86" s="64" t="s">
+      <c r="E89" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="G86" s="66"/>
+      <c r="U89" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="90" spans="2:32" x14ac:dyDescent="0.45">
+      <c r="C90" s="7">
+        <v>2</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F90" s="64" t="s">
+        <v>239</v>
+      </c>
+      <c r="G90" s="66"/>
     </row>
   </sheetData>
-  <mergeCells count="87">
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="U75:Y75"/>
-    <mergeCell ref="U77:AD77"/>
-    <mergeCell ref="U78:AD78"/>
-    <mergeCell ref="U79:AD79"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="F78:G78"/>
+  <mergeCells count="88">
+    <mergeCell ref="C71:R75"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="U79:Y79"/>
+    <mergeCell ref="U81:AD81"/>
+    <mergeCell ref="U82:AD82"/>
+    <mergeCell ref="U83:AD83"/>
     <mergeCell ref="F79:G79"/>
-    <mergeCell ref="H79:I79"/>
     <mergeCell ref="F82:G82"/>
     <mergeCell ref="F83:G83"/>
     <mergeCell ref="H83:I83"/>
-    <mergeCell ref="U83:AD83"/>
-    <mergeCell ref="U82:AD82"/>
-    <mergeCell ref="U81:AD81"/>
-    <mergeCell ref="U74:Y74"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F87:G87"/>
+    <mergeCell ref="H87:I87"/>
+    <mergeCell ref="U87:AD87"/>
+    <mergeCell ref="U86:AD86"/>
+    <mergeCell ref="U85:AD85"/>
+    <mergeCell ref="U78:Y78"/>
     <mergeCell ref="U56:AC56"/>
     <mergeCell ref="U57:AC57"/>
     <mergeCell ref="U58:AC58"/>

</xml_diff>

<commit_message>
Modification: RS -> ARG1, SRC -> ARG2
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar\Documents\Work\AI\CPU\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA6114A-0365-4466-996B-849FF565CB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AB67A9-E561-4F51-805B-0F24767DF3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="38596" windowHeight="21075" activeTab="2" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
+    <workbookView xWindow="23468" yWindow="0" windowWidth="15015" windowHeight="20963" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="281">
   <si>
     <t>POP</t>
   </si>
@@ -1219,6 +1219,18 @@
   </si>
   <si>
     <t>Note: basic ALU operations have scalar mode (VL == 0) or vector mode (VL &gt; 0). In vector mode ALU performs VL operations on its arguments. Argument will be read from register, if its stride is 0, or from memory, next argument value will be fetched from next register or memory, incrementing pointer by its stride. Same for destination.</t>
+  </si>
+  <si>
+    <t>ARG1</t>
+  </si>
+  <si>
+    <t>ARG2</t>
+  </si>
+  <si>
+    <t>ST_ARG1</t>
+  </si>
+  <si>
+    <t>ST_ARG2</t>
   </si>
 </sst>
 </file>
@@ -2367,10 +2379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CDEC23-057C-4C1E-AB18-5AC9130DB945}">
-  <dimension ref="B3:Q31"/>
+  <dimension ref="B3:Q33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2472,11 +2484,11 @@
         <v>107</v>
       </c>
       <c r="J8" s="57" t="s">
-        <v>30</v>
+        <v>277</v>
       </c>
       <c r="K8" s="57"/>
       <c r="L8" s="57" t="s">
-        <v>124</v>
+        <v>278</v>
       </c>
       <c r="M8" s="57"/>
       <c r="N8" s="57" t="s">
@@ -2670,13 +2682,13 @@
         <v>109</v>
       </c>
       <c r="J22" s="57" t="s">
-        <v>128</v>
+        <v>279</v>
       </c>
       <c r="K22" s="57"/>
       <c r="L22" s="57"/>
       <c r="M22" s="57"/>
       <c r="N22" s="57" t="s">
-        <v>130</v>
+        <v>280</v>
       </c>
       <c r="O22" s="57"/>
       <c r="P22" s="57"/>
@@ -2784,6 +2796,9 @@
       <c r="L31" t="s">
         <v>146</v>
       </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.45">
+      <c r="I33" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -3488,7 +3503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43404EB-A4C0-4EEB-BCD6-93EC84295AA2}">
   <dimension ref="A2:AF90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FMT.fpe for scientific e notation for floating point numbers
</commit_message>
<xml_diff>
--- a/ISA.xlsx
+++ b/ISA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ar\Documents\Work\AI\CPU\vcda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32AB67A9-E561-4F51-805B-0F24767DF3AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0487E1F-0752-44C4-934E-9B8E38A087AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23468" yWindow="0" windowWidth="15015" windowHeight="20963" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
+    <workbookView xWindow="19118" yWindow="0" windowWidth="19365" windowHeight="20963" activeTab="1" xr2:uid="{E2BD9803-269D-41CD-8E74-25CFF05574D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="EXT" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="281">
   <si>
     <t>POP</t>
   </si>
@@ -558,12 +559,6 @@
   </si>
   <si>
     <t>0xB</t>
-  </si>
-  <si>
-    <t>fp4</t>
-  </si>
-  <si>
-    <t>4-bit floating-point</t>
   </si>
   <si>
     <t>fp8</t>
@@ -1074,6 +1069,63 @@
     </r>
   </si>
   <si>
+    <t>R251</t>
+  </si>
+  <si>
+    <t>Interrupt Table Pointer</t>
+  </si>
+  <si>
+    <t>ITP</t>
+  </si>
+  <si>
+    <t>Base Pointer</t>
+  </si>
+  <si>
+    <t>Stack Pointer</t>
+  </si>
+  <si>
+    <t>Instruction Pointer</t>
+  </si>
+  <si>
+    <t>Shift Right</t>
+  </si>
+  <si>
+    <t>STORE:  M[R[N.RS] + R[N.SRC]*ST_SRC + ofs] = R[N.DST]</t>
+  </si>
+  <si>
+    <t>LOAD: R[N.DST] = M[R[N.RS] + R[N.SRC]*ST_SRC + ofs], if ST_SRC is zero, R[N.SRC] is not used, can be any value.</t>
+  </si>
+  <si>
+    <t>LOOKUP: Searches for sub-sequence pointed by R[N.SRC], length R[N.SRC+1] in sequence pointed by R[N.RS], length R[N.SRC+1],</t>
+  </si>
+  <si>
+    <t>if found, store its pointer to R[N.DST] and 0 to R[N.DST+1]</t>
+  </si>
+  <si>
+    <t>if not found, store 1 to R[N.DST+1]</t>
+  </si>
+  <si>
+    <t>ST_RS and ST_SRC are used to advance pointers of main and sub-sequences in loop for comparison.</t>
+  </si>
+  <si>
+    <t>Note: basic ALU operations have scalar mode (VL == 0) or vector mode (VL &gt; 0). In vector mode ALU performs VL operations on its arguments. Argument will be read from register, if its stride is 0, or from memory, next argument value will be fetched from next register or memory, incrementing pointer by its stride. Same for destination.</t>
+  </si>
+  <si>
+    <t>ARG1</t>
+  </si>
+  <si>
+    <t>ARG2</t>
+  </si>
+  <si>
+    <t>ST_ARG1</t>
+  </si>
+  <si>
+    <t>ST_ARG2</t>
+  </si>
+  <si>
+    <t>ALU_STRIDES</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">    </t>
     </r>
@@ -1085,7 +1137,42 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>fp0 = 4</t>
+      <t>fpe = 4</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// scientific e notation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>fp0 = 5</t>
     </r>
     <r>
       <rPr>
@@ -1120,7 +1207,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>fp2 = 5</t>
+      <t>fp2 = 6</t>
     </r>
     <r>
       <rPr>
@@ -1155,7 +1242,7 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>fp4 = 6</t>
+      <t>fp4 = 7</t>
     </r>
     <r>
       <rPr>
@@ -1177,60 +1264,6 @@
       </rPr>
       <t>// 4 decimal precision float</t>
     </r>
-  </si>
-  <si>
-    <t>R251</t>
-  </si>
-  <si>
-    <t>Interrupt Table Pointer</t>
-  </si>
-  <si>
-    <t>ITP</t>
-  </si>
-  <si>
-    <t>Base Pointer</t>
-  </si>
-  <si>
-    <t>Stack Pointer</t>
-  </si>
-  <si>
-    <t>Instruction Pointer</t>
-  </si>
-  <si>
-    <t>Shift Right</t>
-  </si>
-  <si>
-    <t>STORE:  M[R[N.RS] + R[N.SRC]*ST_SRC + ofs] = R[N.DST]</t>
-  </si>
-  <si>
-    <t>LOAD: R[N.DST] = M[R[N.RS] + R[N.SRC]*ST_SRC + ofs], if ST_SRC is zero, R[N.SRC] is not used, can be any value.</t>
-  </si>
-  <si>
-    <t>LOOKUP: Searches for sub-sequence pointed by R[N.SRC], length R[N.SRC+1] in sequence pointed by R[N.RS], length R[N.SRC+1],</t>
-  </si>
-  <si>
-    <t>if found, store its pointer to R[N.DST] and 0 to R[N.DST+1]</t>
-  </si>
-  <si>
-    <t>if not found, store 1 to R[N.DST+1]</t>
-  </si>
-  <si>
-    <t>ST_RS and ST_SRC are used to advance pointers of main and sub-sequences in loop for comparison.</t>
-  </si>
-  <si>
-    <t>Note: basic ALU operations have scalar mode (VL == 0) or vector mode (VL &gt; 0). In vector mode ALU performs VL operations on its arguments. Argument will be read from register, if its stride is 0, or from memory, next argument value will be fetched from next register or memory, incrementing pointer by its stride. Same for destination.</t>
-  </si>
-  <si>
-    <t>ARG1</t>
-  </si>
-  <si>
-    <t>ARG2</t>
-  </si>
-  <si>
-    <t>ST_ARG1</t>
-  </si>
-  <si>
-    <t>ST_ARG2</t>
   </si>
 </sst>
 </file>
@@ -1815,7 +1848,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1915,19 +1948,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1949,102 +1981,91 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -2381,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41CDEC23-057C-4C1E-AB18-5AC9130DB945}">
   <dimension ref="B3:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2410,7 +2431,7 @@
         <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F4" t="s">
         <v>101</v>
@@ -2418,22 +2439,22 @@
       <c r="I4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="60">
+      <c r="J4" s="59">
         <v>0</v>
       </c>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59">
+      <c r="K4" s="57"/>
+      <c r="L4" s="57">
         <v>1</v>
       </c>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59">
+      <c r="M4" s="57"/>
+      <c r="N4" s="57">
         <v>2</v>
       </c>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59">
+      <c r="O4" s="57"/>
+      <c r="P4" s="57">
         <v>3</v>
       </c>
-      <c r="Q4" s="59"/>
+      <c r="Q4" s="57"/>
     </row>
     <row r="5" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C5" s="27" t="s">
@@ -2443,7 +2464,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F5" t="s">
         <v>102</v>
@@ -2483,31 +2504,31 @@
       <c r="I8" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="J8" s="57" t="s">
-        <v>277</v>
-      </c>
-      <c r="K8" s="57"/>
-      <c r="L8" s="57" t="s">
-        <v>278</v>
-      </c>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57" t="s">
+      <c r="J8" s="58" t="s">
+        <v>272</v>
+      </c>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58" t="s">
+        <v>273</v>
+      </c>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="O8" s="57"/>
-      <c r="P8" s="57" t="s">
+      <c r="O8" s="58"/>
+      <c r="P8" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="57"/>
+      <c r="Q8" s="58"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="F9" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="G9" s="58"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="8"/>
       <c r="I9" s="28" t="s">
         <v>133</v>
@@ -2517,8 +2538,8 @@
       <c r="C10" t="s">
         <v>105</v>
       </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="8"/>
       <c r="J10" t="s">
         <v>30</v>
@@ -2534,8 +2555,8 @@
       <c r="C11" t="s">
         <v>115</v>
       </c>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="8"/>
       <c r="J11" t="s">
         <v>124</v>
@@ -2604,20 +2625,20 @@
       <c r="I16" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="57" t="s">
+      <c r="J16" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57" t="s">
+      <c r="K16" s="58"/>
+      <c r="L16" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57" t="s">
+      <c r="M16" s="58"/>
+      <c r="N16" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="58"/>
+      <c r="Q16" s="58"/>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I17" s="28" t="s">
@@ -2628,10 +2649,10 @@
       <c r="C18" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="58" t="s">
+      <c r="F18" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="G18" s="58"/>
+      <c r="G18" s="56"/>
       <c r="H18" s="8"/>
       <c r="J18" t="s">
         <v>127</v>
@@ -2647,8 +2668,8 @@
       <c r="C19" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="8"/>
       <c r="J19" t="s">
         <v>126</v>
@@ -2662,10 +2683,10 @@
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
-        <v>263</v>
-      </c>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
+        <v>258</v>
+      </c>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
       <c r="H20" s="8"/>
       <c r="J20" t="s">
         <v>129</v>
@@ -2679,30 +2700,30 @@
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I22" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="J22" s="57" t="s">
-        <v>279</v>
-      </c>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="57" t="s">
-        <v>280</v>
-      </c>
-      <c r="O22" s="57"/>
-      <c r="P22" s="57"/>
-      <c r="Q22" s="57"/>
+        <v>276</v>
+      </c>
+      <c r="J22" s="58" t="s">
+        <v>274</v>
+      </c>
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="58"/>
+      <c r="N22" s="58" t="s">
+        <v>275</v>
+      </c>
+      <c r="O22" s="58"/>
+      <c r="P22" s="58"/>
+      <c r="Q22" s="58"/>
     </row>
     <row r="23" spans="3:17" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
         <v>123</v>
       </c>
       <c r="F23" t="s">
-        <v>265</v>
-      </c>
-      <c r="G23" s="56" t="s">
-        <v>264</v>
+        <v>260</v>
+      </c>
+      <c r="G23" s="55" t="s">
+        <v>259</v>
       </c>
       <c r="I23" s="28" t="s">
         <v>133</v>
@@ -2716,7 +2737,7 @@
         <v>117</v>
       </c>
       <c r="G24" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="J24" t="s">
         <v>128</v>
@@ -2736,7 +2757,7 @@
         <v>118</v>
       </c>
       <c r="G25" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="J25" t="s">
         <v>130</v>
@@ -2756,25 +2777,25 @@
         <v>119</v>
       </c>
       <c r="G26" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="28" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I28" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="J28" s="57" t="s">
+      <c r="J28" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57" t="s">
+      <c r="K28" s="58"/>
+      <c r="L28" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="M28" s="57"/>
-      <c r="N28" s="57"/>
-      <c r="O28" s="57"/>
-      <c r="P28" s="57"/>
-      <c r="Q28" s="57"/>
+      <c r="M28" s="58"/>
+      <c r="N28" s="58"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="58"/>
+      <c r="Q28" s="58"/>
     </row>
     <row r="29" spans="3:17" x14ac:dyDescent="0.45">
       <c r="I29" s="28" t="s">
@@ -2802,6 +2823,13 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="N22:Q22"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="L28:Q28"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:Q16"/>
     <mergeCell ref="F9:G11"/>
     <mergeCell ref="F18:G20"/>
     <mergeCell ref="P4:Q4"/>
@@ -2812,15 +2840,9 @@
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="N22:Q22"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="L28:Q28"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:Q16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2828,8 +2850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A222D11D-FBDB-42C8-93C4-B5D16645D996}">
   <dimension ref="A3:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2846,7 +2868,7 @@
         <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -2866,16 +2888,16 @@
       <c r="H5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="59">
+      <c r="I5" s="57">
         <v>0</v>
       </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="62"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
     </row>
     <row r="6" spans="1:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="37" t="s">
@@ -2888,7 +2910,7 @@
         <v>150</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I6" s="5">
         <v>0</v>
@@ -2940,13 +2962,13 @@
         <v>156</v>
       </c>
       <c r="H9" s="27"/>
-      <c r="I9" s="64" t="s">
-        <v>235</v>
-      </c>
-      <c r="J9" s="65"/>
-      <c r="K9" s="66"/>
+      <c r="I9" s="63" t="s">
+        <v>233</v>
+      </c>
+      <c r="J9" s="64"/>
+      <c r="K9" s="65"/>
       <c r="L9" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.45">
@@ -2960,7 +2982,7 @@
         <v>158</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
@@ -2974,7 +2996,7 @@
         <v>161</v>
       </c>
       <c r="I11" s="53" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J11" s="52"/>
     </row>
@@ -2989,7 +3011,7 @@
         <v>163</v>
       </c>
       <c r="I12" s="54" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J12" s="52"/>
     </row>
@@ -3004,7 +3026,7 @@
         <v>171</v>
       </c>
       <c r="I13" s="54" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J13" s="52"/>
     </row>
@@ -3019,7 +3041,7 @@
         <v>165</v>
       </c>
       <c r="I14" s="54" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
@@ -3033,7 +3055,7 @@
         <v>167</v>
       </c>
       <c r="I15" s="54" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
@@ -3047,7 +3069,7 @@
         <v>169</v>
       </c>
       <c r="I16" s="54" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
@@ -3055,72 +3077,66 @@
         <v>172</v>
       </c>
       <c r="C17" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B18" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="I18" s="54" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B19" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="I19" s="54" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B20" s="94" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D20" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="I17" s="54" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B18" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="I20" s="54" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="I22" s="54" t="s">
+        <v>247</v>
+      </c>
+      <c r="J22" t="s">
         <v>175</v>
       </c>
-      <c r="D18" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="I18" s="54" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B19" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="I19" s="54" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B20" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>243</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>179</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="I21" s="54" t="s">
-        <v>249</v>
-      </c>
-      <c r="J21" t="s">
-        <v>177</v>
-      </c>
-      <c r="K21" t="s">
-        <v>253</v>
+      <c r="K22" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
@@ -3128,7 +3144,7 @@
         <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
@@ -3137,7 +3153,7 @@
         <v>147</v>
       </c>
       <c r="C25" s="41" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D25" s="42"/>
     </row>
@@ -3146,7 +3162,7 @@
         <v>13</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D26" s="39"/>
     </row>
@@ -3155,7 +3171,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D27" s="34"/>
     </row>
@@ -3164,7 +3180,7 @@
         <v>153</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D28" s="34"/>
     </row>
@@ -3173,7 +3189,7 @@
         <v>22</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D29" s="34"/>
     </row>
@@ -3182,7 +3198,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D30" s="34"/>
     </row>
@@ -3191,7 +3207,7 @@
         <v>159</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D31" s="34"/>
     </row>
@@ -3200,7 +3216,7 @@
         <v>9</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D32" s="34"/>
     </row>
@@ -3209,7 +3225,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D33" s="34"/>
     </row>
@@ -3218,7 +3234,7 @@
         <v>39</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D34" s="34"/>
     </row>
@@ -3227,7 +3243,7 @@
         <v>46</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D35" s="34"/>
     </row>
@@ -3236,7 +3252,7 @@
         <v>48</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D36" s="34"/>
     </row>
@@ -3245,7 +3261,7 @@
         <v>172</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D37" s="34"/>
     </row>
@@ -3254,7 +3270,7 @@
         <v>4</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D38" s="34"/>
     </row>
@@ -3263,7 +3279,7 @@
         <v>14</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D39" s="34"/>
     </row>
@@ -3272,7 +3288,7 @@
         <v>15</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D40" s="34"/>
     </row>
@@ -3281,16 +3297,16 @@
         <v>97</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D41" s="36"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="27" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B44" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -3301,7 +3317,7 @@
         <v>147</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D46" s="31" t="s">
         <v>149</v>
@@ -3312,10 +3328,10 @@
         <v>13</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
@@ -3323,10 +3339,10 @@
         <v>19</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D48" s="34" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
@@ -3334,10 +3350,10 @@
         <v>153</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D49" s="34" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
@@ -3345,10 +3361,10 @@
         <v>22</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D50" s="34" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
@@ -3356,10 +3372,10 @@
         <v>29</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D51" s="34" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.45">
@@ -3367,10 +3383,10 @@
         <v>159</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D52" s="34" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.45">
@@ -3378,10 +3394,10 @@
         <v>9</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D53" s="34" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.45">
@@ -3389,10 +3405,10 @@
         <v>2</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D54" s="34" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.45">
@@ -3400,10 +3416,10 @@
         <v>39</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D55" s="34" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.45">
@@ -3411,10 +3427,10 @@
         <v>46</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D56" s="34" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.45">
@@ -3422,10 +3438,10 @@
         <v>48</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D57" s="34" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.45">
@@ -3433,27 +3449,27 @@
         <v>172</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D58" s="34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B59" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C59" s="35" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D59" s="36"/>
     </row>
     <row r="61" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A61" s="27" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B61" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -3461,7 +3477,7 @@
         <v>147</v>
       </c>
       <c r="C62" s="46" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D62" s="42" t="s">
         <v>149</v>
@@ -3472,10 +3488,10 @@
         <v>13</v>
       </c>
       <c r="C63" s="38" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D63" s="39" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -3483,10 +3499,10 @@
         <v>19</v>
       </c>
       <c r="C64" s="35" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D64" s="36" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3503,7 +3519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B43404EB-A4C0-4EEB-BCD6-93EC84295AA2}">
   <dimension ref="A2:AF90"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
@@ -3524,17 +3540,17 @@
   <sheetData>
     <row r="2" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
@@ -3542,47 +3558,47 @@
       <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="77" t="s">
+      <c r="C7" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="60">
+      <c r="D7" s="59">
         <v>0</v>
       </c>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59">
+      <c r="E7" s="57"/>
+      <c r="F7" s="57">
         <v>1</v>
       </c>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59">
+      <c r="G7" s="57"/>
+      <c r="H7" s="57">
         <v>2</v>
       </c>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59">
+      <c r="I7" s="57"/>
+      <c r="J7" s="57">
         <v>3</v>
       </c>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59">
+      <c r="K7" s="57"/>
+      <c r="L7" s="57">
         <v>4</v>
       </c>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59">
+      <c r="M7" s="57"/>
+      <c r="N7" s="57">
         <v>5</v>
       </c>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59">
+      <c r="O7" s="57"/>
+      <c r="P7" s="57">
         <v>6</v>
       </c>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59">
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57">
         <v>7</v>
       </c>
-      <c r="S7" s="74"/>
+      <c r="S7" s="90"/>
     </row>
     <row r="8" spans="1:27" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="78"/>
+      <c r="C8" s="93"/>
       <c r="D8" s="4">
         <v>0</v>
       </c>
@@ -3689,12 +3705,12 @@
       <c r="E15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="U15" s="58" t="s">
+      <c r="U15" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="V15" s="58"/>
-      <c r="W15" s="58"/>
-      <c r="X15" s="58"/>
+      <c r="V15" s="56"/>
+      <c r="W15" s="56"/>
+      <c r="X15" s="56"/>
       <c r="AA15" t="s">
         <v>68</v>
       </c>
@@ -3715,10 +3731,10 @@
       <c r="G16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U16" s="58"/>
-      <c r="V16" s="58"/>
-      <c r="W16" s="58"/>
-      <c r="X16" s="58"/>
+      <c r="U16" s="56"/>
+      <c r="V16" s="56"/>
+      <c r="W16" s="56"/>
+      <c r="X16" s="56"/>
       <c r="AA16" t="s">
         <v>69</v>
       </c>
@@ -3751,10 +3767,10 @@
       <c r="K17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="U17" s="58"/>
-      <c r="V17" s="58"/>
-      <c r="W17" s="58"/>
-      <c r="X17" s="58"/>
+      <c r="U17" s="56"/>
+      <c r="V17" s="56"/>
+      <c r="W17" s="56"/>
+      <c r="X17" s="56"/>
       <c r="AA17" t="s">
         <v>70</v>
       </c>
@@ -3811,10 +3827,10 @@
       <c r="S18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="U18" s="58"/>
-      <c r="V18" s="58"/>
-      <c r="W18" s="58"/>
-      <c r="X18" s="58"/>
+      <c r="U18" s="56"/>
+      <c r="V18" s="56"/>
+      <c r="W18" s="56"/>
+      <c r="X18" s="56"/>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
@@ -3834,12 +3850,12 @@
       <c r="E21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U21" s="58" t="s">
-        <v>246</v>
-      </c>
-      <c r="V21" s="58"/>
-      <c r="W21" s="58"/>
-      <c r="X21" s="58"/>
+      <c r="U21" s="56" t="s">
+        <v>244</v>
+      </c>
+      <c r="V21" s="56"/>
+      <c r="W21" s="56"/>
+      <c r="X21" s="56"/>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C22" s="7">
@@ -3857,24 +3873,24 @@
       <c r="G22" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="69" t="s">
+      <c r="H22" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="68"/>
-      <c r="J22" s="68"/>
-      <c r="K22" s="68"/>
-      <c r="L22" s="68"/>
-      <c r="M22" s="68"/>
-      <c r="N22" s="68"/>
-      <c r="O22" s="68"/>
-      <c r="P22" s="68"/>
-      <c r="Q22" s="68"/>
-      <c r="R22" s="68"/>
-      <c r="S22" s="68"/>
-      <c r="U22" s="58"/>
-      <c r="V22" s="58"/>
-      <c r="W22" s="58"/>
-      <c r="X22" s="58"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="74"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="74"/>
+      <c r="O22" s="74"/>
+      <c r="P22" s="74"/>
+      <c r="Q22" s="74"/>
+      <c r="R22" s="74"/>
+      <c r="S22" s="74"/>
+      <c r="U22" s="56"/>
+      <c r="V22" s="56"/>
+      <c r="W22" s="56"/>
+      <c r="X22" s="56"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C23" s="7">
@@ -3889,58 +3905,58 @@
       <c r="F23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="64" t="s">
+      <c r="G23" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="65"/>
-      <c r="I23" s="65"/>
-      <c r="J23" s="65"/>
-      <c r="K23" s="66"/>
-      <c r="U23" s="58"/>
-      <c r="V23" s="58"/>
-      <c r="W23" s="58"/>
-      <c r="X23" s="58"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="65"/>
+      <c r="U23" s="56"/>
+      <c r="V23" s="56"/>
+      <c r="W23" s="56"/>
+      <c r="X23" s="56"/>
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.45">
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
-      <c r="I24" s="63"/>
-      <c r="J24" s="63"/>
-      <c r="K24" s="63"/>
-      <c r="U24" s="58"/>
-      <c r="V24" s="58"/>
-      <c r="W24" s="58"/>
-      <c r="X24" s="58"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="U24" s="56"/>
+      <c r="V24" s="56"/>
+      <c r="W24" s="56"/>
+      <c r="X24" s="56"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="68" t="s">
+      <c r="C26" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="68"/>
-      <c r="L26" s="68"/>
-      <c r="M26" s="68"/>
-      <c r="N26" s="68"/>
-      <c r="O26" s="68"/>
-      <c r="P26" s="68"/>
-      <c r="Q26" s="68"/>
-      <c r="R26" s="68"/>
-      <c r="S26" s="68"/>
-      <c r="U26" s="63" t="s">
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="74"/>
+      <c r="M26" s="74"/>
+      <c r="N26" s="74"/>
+      <c r="O26" s="74"/>
+      <c r="P26" s="74"/>
+      <c r="Q26" s="74"/>
+      <c r="R26" s="74"/>
+      <c r="S26" s="74"/>
+      <c r="U26" s="62" t="s">
         <v>53</v>
       </c>
-      <c r="V26" s="63"/>
-      <c r="W26" s="63"/>
-      <c r="X26" s="63"/>
+      <c r="V26" s="62"/>
+      <c r="W26" s="62"/>
+      <c r="X26" s="62"/>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
@@ -3955,12 +3971,12 @@
       <c r="E28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U28" s="75" t="s">
+      <c r="U28" s="70" t="s">
         <v>54</v>
       </c>
-      <c r="V28" s="76"/>
-      <c r="W28" s="76"/>
-      <c r="X28" s="76"/>
+      <c r="V28" s="71"/>
+      <c r="W28" s="71"/>
+      <c r="X28" s="71"/>
       <c r="Y28" s="18"/>
       <c r="Z28" s="18"/>
       <c r="AA28" s="18"/>
@@ -3982,12 +3998,12 @@
       <c r="G29" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="69" t="s">
+      <c r="U29" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="V29" s="68"/>
-      <c r="W29" s="68"/>
-      <c r="X29" s="68"/>
+      <c r="V29" s="74"/>
+      <c r="W29" s="74"/>
+      <c r="X29" s="74"/>
       <c r="AB29" s="20"/>
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.45">
@@ -4003,25 +4019,25 @@
       <c r="F30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G30" s="57" t="s">
+      <c r="G30" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="H30" s="57"/>
-      <c r="I30" s="67" t="s">
+      <c r="H30" s="58"/>
+      <c r="I30" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="67"/>
-      <c r="K30" s="67"/>
-      <c r="U30" s="69" t="s">
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+      <c r="U30" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="V30" s="68"/>
-      <c r="W30" s="68"/>
-      <c r="X30" s="68"/>
-      <c r="Y30" s="68"/>
-      <c r="Z30" s="68"/>
-      <c r="AA30" s="68"/>
-      <c r="AB30" s="70"/>
+      <c r="V30" s="74"/>
+      <c r="W30" s="74"/>
+      <c r="X30" s="74"/>
+      <c r="Y30" s="74"/>
+      <c r="Z30" s="74"/>
+      <c r="AA30" s="74"/>
+      <c r="AB30" s="75"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C31" s="7">
@@ -4036,63 +4052,63 @@
       <c r="F31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G31" s="57" t="s">
+      <c r="G31" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="H31" s="57"/>
-      <c r="I31" s="57" t="s">
+      <c r="H31" s="58"/>
+      <c r="I31" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="57"/>
-      <c r="K31" s="57"/>
-      <c r="L31" s="57"/>
-      <c r="M31" s="57"/>
-      <c r="N31" s="57"/>
-      <c r="O31" s="57"/>
-      <c r="P31" s="57"/>
-      <c r="Q31" s="57"/>
-      <c r="R31" s="57"/>
-      <c r="S31" s="57"/>
-      <c r="U31" s="71" t="s">
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="58"/>
+      <c r="Q31" s="58"/>
+      <c r="R31" s="58"/>
+      <c r="S31" s="58"/>
+      <c r="U31" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="V31" s="72"/>
-      <c r="W31" s="72"/>
-      <c r="X31" s="72"/>
-      <c r="Y31" s="72"/>
-      <c r="Z31" s="72"/>
-      <c r="AA31" s="72"/>
-      <c r="AB31" s="73"/>
+      <c r="V31" s="68"/>
+      <c r="W31" s="68"/>
+      <c r="X31" s="68"/>
+      <c r="Y31" s="68"/>
+      <c r="Z31" s="68"/>
+      <c r="AA31" s="68"/>
+      <c r="AB31" s="69"/>
     </row>
     <row r="33" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="68" t="s">
+      <c r="C33" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="68"/>
-      <c r="M33" s="68"/>
-      <c r="N33" s="68"/>
-      <c r="O33" s="68"/>
-      <c r="P33" s="68"/>
-      <c r="Q33" s="68"/>
-      <c r="R33" s="68"/>
-      <c r="S33" s="68"/>
-      <c r="U33" s="85" t="s">
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74"/>
+      <c r="M33" s="74"/>
+      <c r="N33" s="74"/>
+      <c r="O33" s="74"/>
+      <c r="P33" s="74"/>
+      <c r="Q33" s="74"/>
+      <c r="R33" s="74"/>
+      <c r="S33" s="74"/>
+      <c r="U33" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="V33" s="86"/>
-      <c r="W33" s="86"/>
-      <c r="X33" s="87"/>
+      <c r="V33" s="82"/>
+      <c r="W33" s="82"/>
+      <c r="X33" s="83"/>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
@@ -4107,12 +4123,12 @@
       <c r="E35" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="U35" s="75" t="s">
+      <c r="U35" s="70" t="s">
         <v>59</v>
       </c>
-      <c r="V35" s="76"/>
-      <c r="W35" s="76"/>
-      <c r="X35" s="76"/>
+      <c r="V35" s="71"/>
+      <c r="W35" s="71"/>
+      <c r="X35" s="71"/>
       <c r="Y35" s="18"/>
       <c r="Z35" s="18"/>
       <c r="AA35" s="18"/>
@@ -4153,26 +4169,26 @@
         <v>159</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="H37" s="57" t="s">
+        <v>245</v>
+      </c>
+      <c r="H37" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="57"/>
-      <c r="J37" s="57" t="s">
+      <c r="I37" s="58"/>
+      <c r="J37" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="K37" s="57"/>
-      <c r="U37" s="69" t="s">
+      <c r="K37" s="58"/>
+      <c r="U37" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="V37" s="68"/>
-      <c r="W37" s="68"/>
-      <c r="X37" s="68"/>
-      <c r="Y37" s="68"/>
-      <c r="Z37" s="68"/>
-      <c r="AA37" s="68"/>
-      <c r="AB37" s="70"/>
+      <c r="V37" s="74"/>
+      <c r="W37" s="74"/>
+      <c r="X37" s="74"/>
+      <c r="Y37" s="74"/>
+      <c r="Z37" s="74"/>
+      <c r="AA37" s="74"/>
+      <c r="AB37" s="75"/>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
@@ -4187,12 +4203,12 @@
       <c r="E39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U39" s="79" t="s">
+      <c r="U39" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="V39" s="80"/>
-      <c r="W39" s="80"/>
-      <c r="X39" s="81"/>
+      <c r="V39" s="85"/>
+      <c r="W39" s="85"/>
+      <c r="X39" s="86"/>
     </row>
     <row r="40" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C40" s="7">
@@ -4204,44 +4220,44 @@
       <c r="E40" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F40" s="64" t="s">
+      <c r="F40" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G40" s="66"/>
-      <c r="U40" s="82"/>
-      <c r="V40" s="83"/>
-      <c r="W40" s="83"/>
-      <c r="X40" s="84"/>
+      <c r="G40" s="65"/>
+      <c r="U40" s="87"/>
+      <c r="V40" s="88"/>
+      <c r="W40" s="88"/>
+      <c r="X40" s="89"/>
     </row>
     <row r="42" spans="2:28" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="68" t="s">
+      <c r="C42" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="68"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="68"/>
-      <c r="J42" s="68"/>
-      <c r="K42" s="68"/>
-      <c r="L42" s="68"/>
-      <c r="M42" s="68"/>
-      <c r="N42" s="68"/>
-      <c r="O42" s="68"/>
-      <c r="P42" s="68"/>
-      <c r="Q42" s="68"/>
-      <c r="R42" s="68"/>
-      <c r="S42" s="68"/>
-      <c r="U42" s="85" t="s">
+      <c r="D42" s="74"/>
+      <c r="E42" s="74"/>
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="74"/>
+      <c r="I42" s="74"/>
+      <c r="J42" s="74"/>
+      <c r="K42" s="74"/>
+      <c r="L42" s="74"/>
+      <c r="M42" s="74"/>
+      <c r="N42" s="74"/>
+      <c r="O42" s="74"/>
+      <c r="P42" s="74"/>
+      <c r="Q42" s="74"/>
+      <c r="R42" s="74"/>
+      <c r="S42" s="74"/>
+      <c r="U42" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="V42" s="86"/>
-      <c r="W42" s="86"/>
-      <c r="X42" s="87"/>
+      <c r="V42" s="82"/>
+      <c r="W42" s="82"/>
+      <c r="X42" s="83"/>
     </row>
     <row r="43" spans="2:28" x14ac:dyDescent="0.45">
       <c r="C43" s="12"/>
@@ -4301,16 +4317,16 @@
       <c r="E46" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F46" s="57" t="s">
+      <c r="F46" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G46" s="57"/>
-      <c r="H46" s="67" t="s">
+      <c r="G46" s="58"/>
+      <c r="H46" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="I46" s="67"/>
-      <c r="J46" s="67"/>
-      <c r="K46" s="67"/>
+      <c r="I46" s="91"/>
+      <c r="J46" s="91"/>
+      <c r="K46" s="91"/>
       <c r="U46" s="22" t="s">
         <v>67</v>
       </c>
@@ -4326,24 +4342,24 @@
       <c r="E47" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="57" t="s">
+      <c r="F47" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G47" s="57"/>
-      <c r="H47" s="57" t="s">
+      <c r="G47" s="58"/>
+      <c r="H47" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="I47" s="57"/>
-      <c r="J47" s="57"/>
-      <c r="K47" s="57"/>
-      <c r="L47" s="57"/>
-      <c r="M47" s="57"/>
-      <c r="N47" s="57"/>
-      <c r="O47" s="57"/>
-      <c r="P47" s="57"/>
-      <c r="Q47" s="57"/>
-      <c r="R47" s="57"/>
-      <c r="S47" s="57"/>
+      <c r="I47" s="58"/>
+      <c r="J47" s="58"/>
+      <c r="K47" s="58"/>
+      <c r="L47" s="58"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="58"/>
+      <c r="O47" s="58"/>
+      <c r="P47" s="58"/>
+      <c r="Q47" s="58"/>
+      <c r="R47" s="58"/>
+      <c r="S47" s="58"/>
       <c r="U47" s="23" t="s">
         <v>66</v>
       </c>
@@ -4368,17 +4384,17 @@
       <c r="E49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U49" s="75" t="s">
+      <c r="U49" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="V49" s="76"/>
-      <c r="W49" s="76"/>
-      <c r="X49" s="76"/>
-      <c r="Y49" s="76"/>
-      <c r="Z49" s="76"/>
-      <c r="AA49" s="76"/>
-      <c r="AB49" s="76"/>
-      <c r="AC49" s="88"/>
+      <c r="V49" s="71"/>
+      <c r="W49" s="71"/>
+      <c r="X49" s="71"/>
+      <c r="Y49" s="71"/>
+      <c r="Z49" s="71"/>
+      <c r="AA49" s="71"/>
+      <c r="AB49" s="71"/>
+      <c r="AC49" s="72"/>
     </row>
     <row r="50" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C50" s="7">
@@ -4396,17 +4412,17 @@
       <c r="G50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="U50" s="69" t="s">
+      <c r="U50" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="V50" s="68"/>
-      <c r="W50" s="68"/>
-      <c r="X50" s="68"/>
-      <c r="Y50" s="68"/>
-      <c r="Z50" s="68"/>
-      <c r="AA50" s="68"/>
-      <c r="AB50" s="68"/>
-      <c r="AC50" s="70"/>
+      <c r="V50" s="74"/>
+      <c r="W50" s="74"/>
+      <c r="X50" s="74"/>
+      <c r="Y50" s="74"/>
+      <c r="Z50" s="74"/>
+      <c r="AA50" s="74"/>
+      <c r="AB50" s="74"/>
+      <c r="AC50" s="75"/>
     </row>
     <row r="51" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C51" s="7">
@@ -4418,27 +4434,27 @@
       <c r="E51" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="57" t="s">
+      <c r="F51" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="G51" s="57"/>
-      <c r="H51" s="67" t="s">
+      <c r="G51" s="58"/>
+      <c r="H51" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="67"/>
-      <c r="J51" s="67"/>
-      <c r="K51" s="67"/>
-      <c r="U51" s="69" t="s">
+      <c r="I51" s="91"/>
+      <c r="J51" s="91"/>
+      <c r="K51" s="91"/>
+      <c r="U51" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="V51" s="68"/>
-      <c r="W51" s="68"/>
-      <c r="X51" s="68"/>
-      <c r="Y51" s="68"/>
-      <c r="Z51" s="68"/>
-      <c r="AA51" s="68"/>
-      <c r="AB51" s="68"/>
-      <c r="AC51" s="70"/>
+      <c r="V51" s="74"/>
+      <c r="W51" s="74"/>
+      <c r="X51" s="74"/>
+      <c r="Y51" s="74"/>
+      <c r="Z51" s="74"/>
+      <c r="AA51" s="74"/>
+      <c r="AB51" s="74"/>
+      <c r="AC51" s="75"/>
     </row>
     <row r="52" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C52" s="11">
@@ -4450,70 +4466,70 @@
       <c r="E52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F52" s="57" t="s">
+      <c r="F52" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="G52" s="57"/>
-      <c r="H52" s="57" t="s">
+      <c r="G52" s="58"/>
+      <c r="H52" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="57"/>
-      <c r="J52" s="57"/>
-      <c r="K52" s="57"/>
-      <c r="L52" s="57"/>
-      <c r="M52" s="57"/>
-      <c r="N52" s="57"/>
-      <c r="O52" s="57"/>
-      <c r="P52" s="57"/>
-      <c r="Q52" s="57"/>
-      <c r="R52" s="57"/>
-      <c r="S52" s="57"/>
-      <c r="U52" s="71" t="s">
+      <c r="I52" s="58"/>
+      <c r="J52" s="58"/>
+      <c r="K52" s="58"/>
+      <c r="L52" s="58"/>
+      <c r="M52" s="58"/>
+      <c r="N52" s="58"/>
+      <c r="O52" s="58"/>
+      <c r="P52" s="58"/>
+      <c r="Q52" s="58"/>
+      <c r="R52" s="58"/>
+      <c r="S52" s="58"/>
+      <c r="U52" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="V52" s="72"/>
-      <c r="W52" s="72"/>
-      <c r="X52" s="72"/>
-      <c r="Y52" s="72"/>
-      <c r="Z52" s="72"/>
-      <c r="AA52" s="72"/>
-      <c r="AB52" s="72"/>
-      <c r="AC52" s="73"/>
+      <c r="V52" s="68"/>
+      <c r="W52" s="68"/>
+      <c r="X52" s="68"/>
+      <c r="Y52" s="68"/>
+      <c r="Z52" s="68"/>
+      <c r="AA52" s="68"/>
+      <c r="AB52" s="68"/>
+      <c r="AC52" s="69"/>
     </row>
     <row r="54" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
         <v>36</v>
       </c>
-      <c r="C54" s="68" t="s">
+      <c r="C54" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="D54" s="68"/>
-      <c r="E54" s="68"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="68"/>
-      <c r="J54" s="68"/>
-      <c r="K54" s="68"/>
-      <c r="L54" s="68"/>
-      <c r="M54" s="68"/>
-      <c r="N54" s="68"/>
-      <c r="O54" s="68"/>
-      <c r="P54" s="68"/>
-      <c r="Q54" s="68"/>
-      <c r="R54" s="68"/>
-      <c r="S54" s="68"/>
-      <c r="U54" s="85" t="s">
+      <c r="D54" s="74"/>
+      <c r="E54" s="74"/>
+      <c r="F54" s="74"/>
+      <c r="G54" s="74"/>
+      <c r="H54" s="74"/>
+      <c r="I54" s="74"/>
+      <c r="J54" s="74"/>
+      <c r="K54" s="74"/>
+      <c r="L54" s="74"/>
+      <c r="M54" s="74"/>
+      <c r="N54" s="74"/>
+      <c r="O54" s="74"/>
+      <c r="P54" s="74"/>
+      <c r="Q54" s="74"/>
+      <c r="R54" s="74"/>
+      <c r="S54" s="74"/>
+      <c r="U54" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="V54" s="86"/>
-      <c r="W54" s="86"/>
-      <c r="X54" s="86"/>
-      <c r="Y54" s="86"/>
-      <c r="Z54" s="86"/>
-      <c r="AA54" s="86"/>
-      <c r="AB54" s="86"/>
-      <c r="AC54" s="87"/>
+      <c r="V54" s="82"/>
+      <c r="W54" s="82"/>
+      <c r="X54" s="82"/>
+      <c r="Y54" s="82"/>
+      <c r="Z54" s="82"/>
+      <c r="AA54" s="82"/>
+      <c r="AB54" s="82"/>
+      <c r="AC54" s="83"/>
     </row>
     <row r="56" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
@@ -4528,17 +4544,17 @@
       <c r="E56" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="U56" s="75" t="s">
+      <c r="U56" s="70" t="s">
         <v>76</v>
       </c>
-      <c r="V56" s="76"/>
-      <c r="W56" s="76"/>
-      <c r="X56" s="76"/>
-      <c r="Y56" s="76"/>
-      <c r="Z56" s="76"/>
-      <c r="AA56" s="76"/>
-      <c r="AB56" s="76"/>
-      <c r="AC56" s="88"/>
+      <c r="V56" s="71"/>
+      <c r="W56" s="71"/>
+      <c r="X56" s="71"/>
+      <c r="Y56" s="71"/>
+      <c r="Z56" s="71"/>
+      <c r="AA56" s="71"/>
+      <c r="AB56" s="71"/>
+      <c r="AC56" s="72"/>
     </row>
     <row r="57" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C57" s="7">
@@ -4550,21 +4566,21 @@
       <c r="E57" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F57" s="64" t="s">
+      <c r="F57" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G57" s="66"/>
-      <c r="U57" s="69" t="s">
+      <c r="G57" s="65"/>
+      <c r="U57" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="V57" s="68"/>
-      <c r="W57" s="68"/>
-      <c r="X57" s="68"/>
-      <c r="Y57" s="68"/>
-      <c r="Z57" s="68"/>
-      <c r="AA57" s="68"/>
-      <c r="AB57" s="68"/>
-      <c r="AC57" s="70"/>
+      <c r="V57" s="74"/>
+      <c r="W57" s="74"/>
+      <c r="X57" s="74"/>
+      <c r="Y57" s="74"/>
+      <c r="Z57" s="74"/>
+      <c r="AA57" s="74"/>
+      <c r="AB57" s="74"/>
+      <c r="AC57" s="75"/>
     </row>
     <row r="58" spans="2:29" x14ac:dyDescent="0.45">
       <c r="C58" s="7">
@@ -4576,25 +4592,25 @@
       <c r="E58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="57" t="s">
+      <c r="F58" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G58" s="57"/>
-      <c r="H58" s="57" t="s">
+      <c r="G58" s="58"/>
+      <c r="H58" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I58" s="57"/>
-      <c r="U58" s="71" t="s">
+      <c r="I58" s="58"/>
+      <c r="U58" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="V58" s="72"/>
-      <c r="W58" s="72"/>
-      <c r="X58" s="72"/>
-      <c r="Y58" s="72"/>
-      <c r="Z58" s="72"/>
-      <c r="AA58" s="72"/>
-      <c r="AB58" s="72"/>
-      <c r="AC58" s="73"/>
+      <c r="V58" s="68"/>
+      <c r="W58" s="68"/>
+      <c r="X58" s="68"/>
+      <c r="Y58" s="68"/>
+      <c r="Z58" s="68"/>
+      <c r="AA58" s="68"/>
+      <c r="AB58" s="68"/>
+      <c r="AC58" s="69"/>
     </row>
     <row r="60" spans="2:29" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
@@ -4631,21 +4647,21 @@
       <c r="E61" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F61" s="64" t="s">
+      <c r="F61" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G61" s="66"/>
-      <c r="U61" s="69" t="s">
+      <c r="G61" s="65"/>
+      <c r="U61" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="V61" s="68"/>
-      <c r="W61" s="68"/>
-      <c r="X61" s="68"/>
-      <c r="Y61" s="68"/>
-      <c r="Z61" s="68"/>
-      <c r="AA61" s="68"/>
-      <c r="AB61" s="68"/>
-      <c r="AC61" s="70"/>
+      <c r="V61" s="74"/>
+      <c r="W61" s="74"/>
+      <c r="X61" s="74"/>
+      <c r="Y61" s="74"/>
+      <c r="Z61" s="74"/>
+      <c r="AA61" s="74"/>
+      <c r="AB61" s="74"/>
+      <c r="AC61" s="75"/>
     </row>
     <row r="62" spans="2:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C62" s="7">
@@ -4657,51 +4673,51 @@
       <c r="E62" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F62" s="57" t="s">
+      <c r="F62" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="G62" s="57"/>
-      <c r="H62" s="57" t="s">
+      <c r="G62" s="58"/>
+      <c r="H62" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I62" s="57"/>
-      <c r="J62" s="57" t="s">
+      <c r="I62" s="58"/>
+      <c r="J62" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="K62" s="57"/>
-      <c r="U62" s="89" t="s">
+      <c r="K62" s="58"/>
+      <c r="U62" s="76" t="s">
         <v>80</v>
       </c>
-      <c r="V62" s="90"/>
-      <c r="W62" s="90"/>
-      <c r="X62" s="90"/>
-      <c r="Y62" s="90"/>
-      <c r="Z62" s="90"/>
-      <c r="AA62" s="90"/>
-      <c r="AB62" s="90"/>
-      <c r="AC62" s="91"/>
+      <c r="V62" s="66"/>
+      <c r="W62" s="66"/>
+      <c r="X62" s="66"/>
+      <c r="Y62" s="66"/>
+      <c r="Z62" s="66"/>
+      <c r="AA62" s="66"/>
+      <c r="AB62" s="66"/>
+      <c r="AC62" s="77"/>
     </row>
     <row r="63" spans="2:29" x14ac:dyDescent="0.45">
-      <c r="U63" s="89"/>
-      <c r="V63" s="90"/>
-      <c r="W63" s="90"/>
-      <c r="X63" s="90"/>
-      <c r="Y63" s="90"/>
-      <c r="Z63" s="90"/>
-      <c r="AA63" s="90"/>
-      <c r="AB63" s="90"/>
-      <c r="AC63" s="91"/>
+      <c r="U63" s="76"/>
+      <c r="V63" s="66"/>
+      <c r="W63" s="66"/>
+      <c r="X63" s="66"/>
+      <c r="Y63" s="66"/>
+      <c r="Z63" s="66"/>
+      <c r="AA63" s="66"/>
+      <c r="AB63" s="66"/>
+      <c r="AC63" s="77"/>
     </row>
     <row r="64" spans="2:29" x14ac:dyDescent="0.45">
-      <c r="U64" s="92"/>
-      <c r="V64" s="93"/>
-      <c r="W64" s="93"/>
-      <c r="X64" s="93"/>
-      <c r="Y64" s="93"/>
-      <c r="Z64" s="93"/>
-      <c r="AA64" s="93"/>
-      <c r="AB64" s="93"/>
-      <c r="AC64" s="94"/>
+      <c r="U64" s="78"/>
+      <c r="V64" s="79"/>
+      <c r="W64" s="79"/>
+      <c r="X64" s="79"/>
+      <c r="Y64" s="79"/>
+      <c r="Z64" s="79"/>
+      <c r="AA64" s="79"/>
+      <c r="AB64" s="79"/>
+      <c r="AC64" s="80"/>
     </row>
     <row r="65" spans="2:30" x14ac:dyDescent="0.45">
       <c r="U65" s="26"/>
@@ -4727,18 +4743,18 @@
       <c r="E66" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U66" s="75" t="s">
+      <c r="U66" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="V66" s="76"/>
-      <c r="W66" s="76"/>
-      <c r="X66" s="76"/>
-      <c r="Y66" s="76"/>
-      <c r="Z66" s="76"/>
-      <c r="AA66" s="76"/>
-      <c r="AB66" s="76"/>
-      <c r="AC66" s="76"/>
-      <c r="AD66" s="88"/>
+      <c r="V66" s="71"/>
+      <c r="W66" s="71"/>
+      <c r="X66" s="71"/>
+      <c r="Y66" s="71"/>
+      <c r="Z66" s="71"/>
+      <c r="AA66" s="71"/>
+      <c r="AB66" s="71"/>
+      <c r="AC66" s="71"/>
+      <c r="AD66" s="72"/>
     </row>
     <row r="67" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C67" s="7">
@@ -4756,18 +4772,18 @@
       <c r="G67" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U67" s="69" t="s">
+      <c r="U67" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="V67" s="68"/>
-      <c r="W67" s="68"/>
-      <c r="X67" s="68"/>
-      <c r="Y67" s="68"/>
-      <c r="Z67" s="68"/>
-      <c r="AA67" s="68"/>
-      <c r="AB67" s="68"/>
-      <c r="AC67" s="68"/>
-      <c r="AD67" s="70"/>
+      <c r="V67" s="74"/>
+      <c r="W67" s="74"/>
+      <c r="X67" s="74"/>
+      <c r="Y67" s="74"/>
+      <c r="Z67" s="74"/>
+      <c r="AA67" s="74"/>
+      <c r="AB67" s="74"/>
+      <c r="AC67" s="74"/>
+      <c r="AD67" s="75"/>
     </row>
     <row r="68" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C68" s="7">
@@ -4791,22 +4807,22 @@
       <c r="I68" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J68" s="64" t="s">
+      <c r="J68" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="K68" s="66"/>
-      <c r="U68" s="69" t="s">
+      <c r="K68" s="65"/>
+      <c r="U68" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="V68" s="68"/>
-      <c r="W68" s="68"/>
-      <c r="X68" s="68"/>
-      <c r="Y68" s="68"/>
-      <c r="Z68" s="68"/>
-      <c r="AA68" s="68"/>
-      <c r="AB68" s="68"/>
-      <c r="AC68" s="68"/>
-      <c r="AD68" s="70"/>
+      <c r="V68" s="74"/>
+      <c r="W68" s="74"/>
+      <c r="X68" s="74"/>
+      <c r="Y68" s="74"/>
+      <c r="Z68" s="74"/>
+      <c r="AA68" s="74"/>
+      <c r="AB68" s="74"/>
+      <c r="AC68" s="74"/>
+      <c r="AD68" s="75"/>
     </row>
     <row r="69" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C69" s="11">
@@ -4818,261 +4834,228 @@
       <c r="E69" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F69" s="57" t="s">
+      <c r="F69" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="57"/>
-      <c r="H69" s="64" t="s">
+      <c r="G69" s="58"/>
+      <c r="H69" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="I69" s="66"/>
-      <c r="J69" s="64" t="s">
+      <c r="I69" s="65"/>
+      <c r="J69" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="K69" s="66"/>
-      <c r="L69" s="64" t="s">
+      <c r="K69" s="65"/>
+      <c r="L69" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="M69" s="66"/>
-      <c r="N69" s="64" t="s">
+      <c r="M69" s="65"/>
+      <c r="N69" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="O69" s="66"/>
-      <c r="P69" s="64" t="s">
+      <c r="O69" s="65"/>
+      <c r="P69" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="Q69" s="65"/>
-      <c r="R69" s="65"/>
-      <c r="S69" s="66"/>
-      <c r="U69" s="71" t="s">
-        <v>248</v>
-      </c>
-      <c r="V69" s="72"/>
-      <c r="W69" s="72"/>
-      <c r="X69" s="72"/>
-      <c r="Y69" s="72"/>
-      <c r="Z69" s="72"/>
-      <c r="AA69" s="72"/>
-      <c r="AB69" s="72"/>
-      <c r="AC69" s="72"/>
-      <c r="AD69" s="73"/>
+      <c r="Q69" s="64"/>
+      <c r="R69" s="64"/>
+      <c r="S69" s="65"/>
+      <c r="U69" s="67" t="s">
+        <v>246</v>
+      </c>
+      <c r="V69" s="68"/>
+      <c r="W69" s="68"/>
+      <c r="X69" s="68"/>
+      <c r="Y69" s="68"/>
+      <c r="Z69" s="68"/>
+      <c r="AA69" s="68"/>
+      <c r="AB69" s="68"/>
+      <c r="AC69" s="68"/>
+      <c r="AD69" s="69"/>
     </row>
     <row r="70" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C70" s="95"/>
-      <c r="D70" s="96"/>
-      <c r="E70" s="96"/>
-      <c r="F70" s="96"/>
-      <c r="G70" s="96"/>
-      <c r="H70" s="96"/>
-      <c r="I70" s="96"/>
-      <c r="J70" s="96"/>
-      <c r="K70" s="96"/>
-      <c r="L70" s="96"/>
-      <c r="M70" s="96"/>
-      <c r="N70" s="96"/>
-      <c r="O70" s="96"/>
-      <c r="P70" s="96"/>
-      <c r="Q70" s="96"/>
-      <c r="R70" s="96"/>
-      <c r="S70" s="96"/>
-      <c r="U70" s="97" t="s">
+      <c r="C70" s="28"/>
+      <c r="G70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="U70" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="V70" s="12"/>
+      <c r="W70" s="12"/>
+      <c r="X70" s="12"/>
+      <c r="Y70" s="12"/>
+      <c r="Z70" s="12"/>
+      <c r="AA70" s="12"/>
+      <c r="AB70" s="12"/>
+      <c r="AC70" s="12"/>
+      <c r="AD70" s="12"/>
+    </row>
+    <row r="71" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C71" s="66" t="s">
         <v>271</v>
       </c>
-      <c r="V70" s="97"/>
-      <c r="W70" s="97"/>
-      <c r="X70" s="97"/>
-      <c r="Y70" s="97"/>
-      <c r="Z70" s="97"/>
-      <c r="AA70" s="97"/>
-      <c r="AB70" s="97"/>
-      <c r="AC70" s="97"/>
-      <c r="AD70" s="97"/>
-    </row>
-    <row r="71" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C71" s="98" t="s">
-        <v>276</v>
-      </c>
-      <c r="D71" s="98"/>
-      <c r="E71" s="98"/>
-      <c r="F71" s="98"/>
-      <c r="G71" s="98"/>
-      <c r="H71" s="98"/>
-      <c r="I71" s="98"/>
-      <c r="J71" s="98"/>
-      <c r="K71" s="98"/>
-      <c r="L71" s="98"/>
-      <c r="M71" s="98"/>
-      <c r="N71" s="98"/>
-      <c r="O71" s="98"/>
-      <c r="P71" s="98"/>
-      <c r="Q71" s="98"/>
-      <c r="R71" s="98"/>
-      <c r="S71" s="96"/>
-      <c r="U71" s="97" t="s">
+      <c r="D71" s="66"/>
+      <c r="E71" s="66"/>
+      <c r="F71" s="66"/>
+      <c r="G71" s="66"/>
+      <c r="H71" s="66"/>
+      <c r="I71" s="66"/>
+      <c r="J71" s="66"/>
+      <c r="K71" s="66"/>
+      <c r="L71" s="66"/>
+      <c r="M71" s="66"/>
+      <c r="N71" s="66"/>
+      <c r="O71" s="66"/>
+      <c r="P71" s="66"/>
+      <c r="Q71" s="66"/>
+      <c r="R71" s="66"/>
+      <c r="U71" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="V71" s="12"/>
+      <c r="W71" s="12"/>
+      <c r="X71" s="12"/>
+      <c r="Y71" s="12"/>
+      <c r="Z71" s="12"/>
+      <c r="AA71" s="12"/>
+      <c r="AB71" s="12"/>
+      <c r="AC71" s="12"/>
+      <c r="AD71" s="12"/>
+    </row>
+    <row r="72" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C72" s="66"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="66"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="66"/>
+      <c r="I72" s="66"/>
+      <c r="J72" s="66"/>
+      <c r="K72" s="66"/>
+      <c r="L72" s="66"/>
+      <c r="M72" s="66"/>
+      <c r="N72" s="66"/>
+      <c r="O72" s="66"/>
+      <c r="P72" s="66"/>
+      <c r="Q72" s="66"/>
+      <c r="R72" s="66"/>
+      <c r="U72" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="V72" s="12"/>
+      <c r="W72" s="12"/>
+      <c r="X72" s="12"/>
+      <c r="Y72" s="12"/>
+      <c r="Z72" s="12"/>
+      <c r="AA72" s="12"/>
+      <c r="AB72" s="12"/>
+      <c r="AC72" s="12"/>
+      <c r="AD72" s="12"/>
+    </row>
+    <row r="73" spans="2:30" x14ac:dyDescent="0.45">
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="66"/>
+      <c r="I73" s="66"/>
+      <c r="J73" s="66"/>
+      <c r="K73" s="66"/>
+      <c r="L73" s="66"/>
+      <c r="M73" s="66"/>
+      <c r="N73" s="66"/>
+      <c r="O73" s="66"/>
+      <c r="P73" s="66"/>
+      <c r="Q73" s="66"/>
+      <c r="R73" s="66"/>
+      <c r="U73" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="V71" s="97"/>
-      <c r="W71" s="97"/>
-      <c r="X71" s="97"/>
-      <c r="Y71" s="97"/>
-      <c r="Z71" s="97"/>
-      <c r="AA71" s="97"/>
-      <c r="AB71" s="97"/>
-      <c r="AC71" s="97"/>
-      <c r="AD71" s="97"/>
-    </row>
-    <row r="72" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C72" s="98"/>
-      <c r="D72" s="98"/>
-      <c r="E72" s="98"/>
-      <c r="F72" s="98"/>
-      <c r="G72" s="98"/>
-      <c r="H72" s="98"/>
-      <c r="I72" s="98"/>
-      <c r="J72" s="98"/>
-      <c r="K72" s="98"/>
-      <c r="L72" s="98"/>
-      <c r="M72" s="98"/>
-      <c r="N72" s="98"/>
-      <c r="O72" s="98"/>
-      <c r="P72" s="98"/>
-      <c r="Q72" s="98"/>
-      <c r="R72" s="98"/>
-      <c r="S72" s="96"/>
-      <c r="U72" s="97" t="s">
-        <v>272</v>
-      </c>
-      <c r="V72" s="97"/>
-      <c r="W72" s="97"/>
-      <c r="X72" s="97"/>
-      <c r="Y72" s="97"/>
-      <c r="Z72" s="97"/>
-      <c r="AA72" s="97"/>
-      <c r="AB72" s="97"/>
-      <c r="AC72" s="97"/>
-      <c r="AD72" s="97"/>
-    </row>
-    <row r="73" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C73" s="98"/>
-      <c r="D73" s="98"/>
-      <c r="E73" s="98"/>
-      <c r="F73" s="98"/>
-      <c r="G73" s="98"/>
-      <c r="H73" s="98"/>
-      <c r="I73" s="98"/>
-      <c r="J73" s="98"/>
-      <c r="K73" s="98"/>
-      <c r="L73" s="98"/>
-      <c r="M73" s="98"/>
-      <c r="N73" s="98"/>
-      <c r="O73" s="98"/>
-      <c r="P73" s="98"/>
-      <c r="Q73" s="98"/>
-      <c r="R73" s="98"/>
-      <c r="S73" s="96"/>
-      <c r="U73" s="97" t="s">
-        <v>275</v>
-      </c>
-      <c r="V73" s="97"/>
-      <c r="W73" s="97"/>
-      <c r="X73" s="97"/>
-      <c r="Y73" s="97"/>
-      <c r="Z73" s="97"/>
-      <c r="AA73" s="97"/>
-      <c r="AB73" s="97"/>
-      <c r="AC73" s="97"/>
-      <c r="AD73" s="97"/>
+      <c r="V73" s="12"/>
+      <c r="W73" s="12"/>
+      <c r="X73" s="12"/>
+      <c r="Y73" s="12"/>
+      <c r="Z73" s="12"/>
+      <c r="AA73" s="12"/>
+      <c r="AB73" s="12"/>
+      <c r="AC73" s="12"/>
+      <c r="AD73" s="12"/>
     </row>
     <row r="74" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C74" s="98"/>
-      <c r="D74" s="98"/>
-      <c r="E74" s="98"/>
-      <c r="F74" s="98"/>
-      <c r="G74" s="98"/>
-      <c r="H74" s="98"/>
-      <c r="I74" s="98"/>
-      <c r="J74" s="98"/>
-      <c r="K74" s="98"/>
-      <c r="L74" s="98"/>
-      <c r="M74" s="98"/>
-      <c r="N74" s="98"/>
-      <c r="O74" s="98"/>
-      <c r="P74" s="98"/>
-      <c r="Q74" s="98"/>
-      <c r="R74" s="98"/>
-      <c r="S74" s="96"/>
-      <c r="U74" s="97" t="s">
-        <v>273</v>
-      </c>
-      <c r="V74" s="97"/>
-      <c r="W74" s="97"/>
-      <c r="X74" s="97"/>
-      <c r="Y74" s="97"/>
-      <c r="Z74" s="97"/>
-      <c r="AA74" s="97"/>
-      <c r="AB74" s="97"/>
-      <c r="AC74" s="97"/>
-      <c r="AD74" s="97"/>
+      <c r="C74" s="66"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="66"/>
+      <c r="F74" s="66"/>
+      <c r="G74" s="66"/>
+      <c r="H74" s="66"/>
+      <c r="I74" s="66"/>
+      <c r="J74" s="66"/>
+      <c r="K74" s="66"/>
+      <c r="L74" s="66"/>
+      <c r="M74" s="66"/>
+      <c r="N74" s="66"/>
+      <c r="O74" s="66"/>
+      <c r="P74" s="66"/>
+      <c r="Q74" s="66"/>
+      <c r="R74" s="66"/>
+      <c r="U74" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="V74" s="12"/>
+      <c r="W74" s="12"/>
+      <c r="X74" s="12"/>
+      <c r="Y74" s="12"/>
+      <c r="Z74" s="12"/>
+      <c r="AA74" s="12"/>
+      <c r="AB74" s="12"/>
+      <c r="AC74" s="12"/>
+      <c r="AD74" s="12"/>
     </row>
     <row r="75" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C75" s="98"/>
-      <c r="D75" s="98"/>
-      <c r="E75" s="98"/>
-      <c r="F75" s="98"/>
-      <c r="G75" s="98"/>
-      <c r="H75" s="98"/>
-      <c r="I75" s="98"/>
-      <c r="J75" s="98"/>
-      <c r="K75" s="98"/>
-      <c r="L75" s="98"/>
-      <c r="M75" s="98"/>
-      <c r="N75" s="98"/>
-      <c r="O75" s="98"/>
-      <c r="P75" s="98"/>
-      <c r="Q75" s="98"/>
-      <c r="R75" s="98"/>
-      <c r="S75" s="96"/>
-      <c r="U75" s="97" t="s">
-        <v>274</v>
-      </c>
-      <c r="V75" s="97"/>
-      <c r="W75" s="97"/>
-      <c r="X75" s="97"/>
-      <c r="Y75" s="97"/>
-      <c r="Z75" s="97"/>
-      <c r="AA75" s="97"/>
-      <c r="AB75" s="97"/>
-      <c r="AC75" s="97"/>
-      <c r="AD75" s="97"/>
+      <c r="C75" s="66"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="66"/>
+      <c r="F75" s="66"/>
+      <c r="G75" s="66"/>
+      <c r="H75" s="66"/>
+      <c r="I75" s="66"/>
+      <c r="J75" s="66"/>
+      <c r="K75" s="66"/>
+      <c r="L75" s="66"/>
+      <c r="M75" s="66"/>
+      <c r="N75" s="66"/>
+      <c r="O75" s="66"/>
+      <c r="P75" s="66"/>
+      <c r="Q75" s="66"/>
+      <c r="R75" s="66"/>
+      <c r="U75" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="V75" s="12"/>
+      <c r="W75" s="12"/>
+      <c r="X75" s="12"/>
+      <c r="Y75" s="12"/>
+      <c r="Z75" s="12"/>
+      <c r="AA75" s="12"/>
+      <c r="AB75" s="12"/>
+      <c r="AC75" s="12"/>
+      <c r="AD75" s="12"/>
     </row>
     <row r="76" spans="2:30" x14ac:dyDescent="0.45">
-      <c r="C76" s="95"/>
-      <c r="D76" s="96"/>
-      <c r="E76" s="96"/>
-      <c r="F76" s="96"/>
-      <c r="G76" s="96"/>
-      <c r="H76" s="96"/>
-      <c r="I76" s="96"/>
-      <c r="J76" s="96"/>
-      <c r="K76" s="96"/>
-      <c r="L76" s="96"/>
-      <c r="M76" s="96"/>
-      <c r="N76" s="96"/>
-      <c r="O76" s="96"/>
-      <c r="P76" s="96"/>
-      <c r="Q76" s="96"/>
-      <c r="R76" s="96"/>
-      <c r="S76" s="96"/>
-      <c r="U76" s="97"/>
-      <c r="V76" s="97"/>
-      <c r="W76" s="97"/>
-      <c r="X76" s="97"/>
-      <c r="Y76" s="97"/>
-      <c r="Z76" s="97"/>
-      <c r="AA76" s="97"/>
-      <c r="AB76" s="97"/>
-      <c r="AC76" s="97"/>
-      <c r="AD76" s="97"/>
+      <c r="C76" s="28"/>
+      <c r="G76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="U76" s="12"/>
+      <c r="V76" s="12"/>
+      <c r="W76" s="12"/>
+      <c r="X76" s="12"/>
+      <c r="Y76" s="12"/>
+      <c r="Z76" s="12"/>
+      <c r="AA76" s="12"/>
+      <c r="AB76" s="12"/>
+      <c r="AC76" s="12"/>
+      <c r="AD76" s="12"/>
     </row>
     <row r="78" spans="2:30" x14ac:dyDescent="0.45">
       <c r="B78" t="s">
@@ -5087,13 +5070,13 @@
       <c r="E78" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U78" s="75" t="s">
+      <c r="U78" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="V78" s="76"/>
-      <c r="W78" s="76"/>
-      <c r="X78" s="76"/>
-      <c r="Y78" s="88"/>
+      <c r="V78" s="71"/>
+      <c r="W78" s="71"/>
+      <c r="X78" s="71"/>
+      <c r="Y78" s="72"/>
     </row>
     <row r="79" spans="2:30" x14ac:dyDescent="0.45">
       <c r="C79" s="7">
@@ -5105,17 +5088,17 @@
       <c r="E79" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F79" s="64" t="s">
+      <c r="F79" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="G79" s="66"/>
-      <c r="U79" s="71" t="s">
+      <c r="G79" s="65"/>
+      <c r="U79" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="V79" s="72"/>
-      <c r="W79" s="72"/>
-      <c r="X79" s="72"/>
-      <c r="Y79" s="73"/>
+      <c r="V79" s="68"/>
+      <c r="W79" s="68"/>
+      <c r="X79" s="68"/>
+      <c r="Y79" s="69"/>
     </row>
     <row r="81" spans="2:32" x14ac:dyDescent="0.45">
       <c r="B81" t="s">
@@ -5130,18 +5113,18 @@
       <c r="E81" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U81" s="75" t="s">
+      <c r="U81" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="V81" s="76"/>
-      <c r="W81" s="76"/>
-      <c r="X81" s="76"/>
-      <c r="Y81" s="76"/>
-      <c r="Z81" s="76"/>
-      <c r="AA81" s="76"/>
-      <c r="AB81" s="76"/>
-      <c r="AC81" s="76"/>
-      <c r="AD81" s="88"/>
+      <c r="V81" s="71"/>
+      <c r="W81" s="71"/>
+      <c r="X81" s="71"/>
+      <c r="Y81" s="71"/>
+      <c r="Z81" s="71"/>
+      <c r="AA81" s="71"/>
+      <c r="AB81" s="71"/>
+      <c r="AC81" s="71"/>
+      <c r="AD81" s="72"/>
     </row>
     <row r="82" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C82" s="7">
@@ -5153,22 +5136,22 @@
       <c r="E82" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F82" s="64" t="s">
+      <c r="F82" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="G82" s="66"/>
-      <c r="U82" s="69" t="s">
+      <c r="G82" s="65"/>
+      <c r="U82" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="V82" s="68"/>
-      <c r="W82" s="68"/>
-      <c r="X82" s="68"/>
-      <c r="Y82" s="68"/>
-      <c r="Z82" s="68"/>
-      <c r="AA82" s="68"/>
-      <c r="AB82" s="68"/>
-      <c r="AC82" s="68"/>
-      <c r="AD82" s="70"/>
+      <c r="V82" s="74"/>
+      <c r="W82" s="74"/>
+      <c r="X82" s="74"/>
+      <c r="Y82" s="74"/>
+      <c r="Z82" s="74"/>
+      <c r="AA82" s="74"/>
+      <c r="AB82" s="74"/>
+      <c r="AC82" s="74"/>
+      <c r="AD82" s="75"/>
     </row>
     <row r="83" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C83" s="7">
@@ -5180,32 +5163,32 @@
       <c r="E83" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F83" s="57" t="s">
+      <c r="F83" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="G83" s="57"/>
-      <c r="H83" s="57" t="s">
+      <c r="G83" s="58"/>
+      <c r="H83" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="I83" s="57"/>
+      <c r="I83" s="58"/>
       <c r="J83" s="7" t="s">
         <v>41</v>
       </c>
       <c r="K83" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U83" s="71" t="s">
+      <c r="U83" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="V83" s="72"/>
-      <c r="W83" s="72"/>
-      <c r="X83" s="72"/>
-      <c r="Y83" s="72"/>
-      <c r="Z83" s="72"/>
-      <c r="AA83" s="72"/>
-      <c r="AB83" s="72"/>
-      <c r="AC83" s="72"/>
-      <c r="AD83" s="73"/>
+      <c r="V83" s="68"/>
+      <c r="W83" s="68"/>
+      <c r="X83" s="68"/>
+      <c r="Y83" s="68"/>
+      <c r="Z83" s="68"/>
+      <c r="AA83" s="68"/>
+      <c r="AB83" s="68"/>
+      <c r="AC83" s="68"/>
+      <c r="AD83" s="69"/>
     </row>
     <row r="85" spans="2:32" x14ac:dyDescent="0.45">
       <c r="B85" t="s">
@@ -5220,20 +5203,20 @@
       <c r="E85" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="U85" s="75" t="s">
-        <v>255</v>
-      </c>
-      <c r="V85" s="76"/>
-      <c r="W85" s="76"/>
-      <c r="X85" s="76"/>
-      <c r="Y85" s="76"/>
-      <c r="Z85" s="76"/>
-      <c r="AA85" s="76"/>
-      <c r="AB85" s="76"/>
-      <c r="AC85" s="76"/>
-      <c r="AD85" s="88"/>
+      <c r="U85" s="70" t="s">
+        <v>253</v>
+      </c>
+      <c r="V85" s="71"/>
+      <c r="W85" s="71"/>
+      <c r="X85" s="71"/>
+      <c r="Y85" s="71"/>
+      <c r="Z85" s="71"/>
+      <c r="AA85" s="71"/>
+      <c r="AB85" s="71"/>
+      <c r="AC85" s="71"/>
+      <c r="AD85" s="72"/>
       <c r="AF85" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="86" spans="2:32" x14ac:dyDescent="0.45">
@@ -5246,22 +5229,22 @@
       <c r="E86" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F86" s="64" t="s">
+      <c r="F86" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="G86" s="66"/>
-      <c r="U86" s="69" t="s">
+      <c r="G86" s="65"/>
+      <c r="U86" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="V86" s="68"/>
-      <c r="W86" s="68"/>
-      <c r="X86" s="68"/>
-      <c r="Y86" s="68"/>
-      <c r="Z86" s="68"/>
-      <c r="AA86" s="68"/>
-      <c r="AB86" s="68"/>
-      <c r="AC86" s="68"/>
-      <c r="AD86" s="70"/>
+      <c r="V86" s="74"/>
+      <c r="W86" s="74"/>
+      <c r="X86" s="74"/>
+      <c r="Y86" s="74"/>
+      <c r="Z86" s="74"/>
+      <c r="AA86" s="74"/>
+      <c r="AB86" s="74"/>
+      <c r="AC86" s="74"/>
+      <c r="AD86" s="75"/>
     </row>
     <row r="87" spans="2:32" x14ac:dyDescent="0.45">
       <c r="C87" s="7">
@@ -5273,32 +5256,32 @@
       <c r="E87" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F87" s="57" t="s">
+      <c r="F87" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="G87" s="57"/>
-      <c r="H87" s="57" t="s">
+      <c r="G87" s="58"/>
+      <c r="H87" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="I87" s="57"/>
+      <c r="I87" s="58"/>
       <c r="J87" s="7" t="s">
         <v>41</v>
       </c>
       <c r="K87" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="U87" s="71" t="s">
-        <v>254</v>
-      </c>
-      <c r="V87" s="72"/>
-      <c r="W87" s="72"/>
-      <c r="X87" s="72"/>
-      <c r="Y87" s="72"/>
-      <c r="Z87" s="72"/>
-      <c r="AA87" s="72"/>
-      <c r="AB87" s="72"/>
-      <c r="AC87" s="72"/>
-      <c r="AD87" s="73"/>
+      <c r="U87" s="67" t="s">
+        <v>252</v>
+      </c>
+      <c r="V87" s="68"/>
+      <c r="W87" s="68"/>
+      <c r="X87" s="68"/>
+      <c r="Y87" s="68"/>
+      <c r="Z87" s="68"/>
+      <c r="AA87" s="68"/>
+      <c r="AB87" s="68"/>
+      <c r="AC87" s="68"/>
+      <c r="AD87" s="69"/>
       <c r="AF87" s="49"/>
     </row>
     <row r="89" spans="2:32" x14ac:dyDescent="0.45">
@@ -5312,10 +5295,10 @@
         <v>97</v>
       </c>
       <c r="E89" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="U89" t="s">
         <v>239</v>
-      </c>
-      <c r="U89" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="90" spans="2:32" x14ac:dyDescent="0.45">
@@ -5328,13 +5311,85 @@
       <c r="E90" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F90" s="64" t="s">
-        <v>239</v>
-      </c>
-      <c r="G90" s="66"/>
+      <c r="F90" s="63" t="s">
+        <v>237</v>
+      </c>
+      <c r="G90" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="88">
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="P69:S69"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:S47"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:S52"/>
+    <mergeCell ref="C54:S54"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="N69:O69"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H46:K46"/>
+    <mergeCell ref="I31:S31"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="C42:S42"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="C33:S33"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="U30:AB30"/>
+    <mergeCell ref="U31:AB31"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="U26:X26"/>
+    <mergeCell ref="U28:X28"/>
+    <mergeCell ref="U29:X29"/>
+    <mergeCell ref="C26:S26"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="G23:K23"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="U15:X18"/>
+    <mergeCell ref="U21:X24"/>
+    <mergeCell ref="H22:S22"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="G24:K24"/>
+    <mergeCell ref="U39:X40"/>
+    <mergeCell ref="U42:X42"/>
+    <mergeCell ref="U33:X33"/>
+    <mergeCell ref="U35:X35"/>
+    <mergeCell ref="U37:AB37"/>
+    <mergeCell ref="U49:AC49"/>
+    <mergeCell ref="U50:AC50"/>
+    <mergeCell ref="U51:AC51"/>
+    <mergeCell ref="U52:AC52"/>
+    <mergeCell ref="U54:AC54"/>
+    <mergeCell ref="U78:Y78"/>
+    <mergeCell ref="U56:AC56"/>
+    <mergeCell ref="U57:AC57"/>
+    <mergeCell ref="U58:AC58"/>
+    <mergeCell ref="U61:AC61"/>
+    <mergeCell ref="U62:AC64"/>
+    <mergeCell ref="U66:AD66"/>
+    <mergeCell ref="U67:AD67"/>
+    <mergeCell ref="U68:AD68"/>
+    <mergeCell ref="U69:AD69"/>
     <mergeCell ref="C71:R75"/>
     <mergeCell ref="F90:G90"/>
     <mergeCell ref="U79:Y79"/>
@@ -5351,78 +5406,6 @@
     <mergeCell ref="U87:AD87"/>
     <mergeCell ref="U86:AD86"/>
     <mergeCell ref="U85:AD85"/>
-    <mergeCell ref="U78:Y78"/>
-    <mergeCell ref="U56:AC56"/>
-    <mergeCell ref="U57:AC57"/>
-    <mergeCell ref="U58:AC58"/>
-    <mergeCell ref="U61:AC61"/>
-    <mergeCell ref="U62:AC64"/>
-    <mergeCell ref="U66:AD66"/>
-    <mergeCell ref="U67:AD67"/>
-    <mergeCell ref="U68:AD68"/>
-    <mergeCell ref="U69:AD69"/>
-    <mergeCell ref="U49:AC49"/>
-    <mergeCell ref="U50:AC50"/>
-    <mergeCell ref="U51:AC51"/>
-    <mergeCell ref="U52:AC52"/>
-    <mergeCell ref="U54:AC54"/>
-    <mergeCell ref="U39:X40"/>
-    <mergeCell ref="U42:X42"/>
-    <mergeCell ref="U33:X33"/>
-    <mergeCell ref="U35:X35"/>
-    <mergeCell ref="U37:AB37"/>
-    <mergeCell ref="U15:X18"/>
-    <mergeCell ref="U21:X24"/>
-    <mergeCell ref="H22:S22"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="G24:K24"/>
-    <mergeCell ref="U30:AB30"/>
-    <mergeCell ref="U31:AB31"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="U26:X26"/>
-    <mergeCell ref="U28:X28"/>
-    <mergeCell ref="U29:X29"/>
-    <mergeCell ref="C26:S26"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="G23:K23"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="H46:K46"/>
-    <mergeCell ref="I31:S31"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="C42:S42"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="C33:S33"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="P69:S69"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:S47"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:S52"/>
-    <mergeCell ref="C54:S54"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="N69:O69"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5441,7 +5424,7 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.45">

</xml_diff>